<commit_message>
FEAT: improves states transition on EOF character.
</commit_message>
<xml_diff>
--- a/docs/lexer/lexer-FSM.xlsx
+++ b/docs/lexer/lexer-FSM.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Red\docs\lexer\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E9B17D-15CC-4E0B-99C3-2B675C00EE9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="564"/>
+    <workbookView xWindow="743" yWindow="83" windowWidth="19447" windowHeight="13522" tabRatio="564" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Transitions" sheetId="3" r:id="rId1"/>
@@ -328,7 +334,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -499,7 +505,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -532,9 +538,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -567,6 +590,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -742,23 +782,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AH40" sqref="AH40"/>
+      <pane xSplit="1" topLeftCell="T1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AH43" sqref="AH43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.08984375" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="34" width="9.7265625" customWidth="1"/>
+    <col min="1" max="1" width="10.06640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="34" width="9.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="8"/>
       <c r="B1" s="7" t="s">
         <v>39</v>
@@ -860,7 +900,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -964,7 +1004,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -1068,7 +1108,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A4" s="6" t="s">
         <v>72</v>
       </c>
@@ -1172,7 +1212,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A5" s="6" t="s">
         <v>73</v>
       </c>
@@ -1272,11 +1312,11 @@
       <c r="AG5" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="AH5" s="1" t="s">
-        <v>75</v>
+      <c r="AH5" s="3" t="s">
+        <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A6" s="6" t="s">
         <v>2</v>
       </c>
@@ -1380,7 +1420,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A7" s="6" t="s">
         <v>3</v>
       </c>
@@ -1480,11 +1520,11 @@
       <c r="AG7" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="AH7" s="1" t="s">
-        <v>75</v>
+      <c r="AH7" s="3" t="s">
+        <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A8" s="6" t="s">
         <v>77</v>
       </c>
@@ -1588,7 +1628,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A9" s="6" t="s">
         <v>4</v>
       </c>
@@ -1689,10 +1729,10 @@
         <v>66</v>
       </c>
       <c r="AH9" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A10" s="6" t="s">
         <v>5</v>
       </c>
@@ -1793,10 +1833,10 @@
         <v>66</v>
       </c>
       <c r="AH10" s="1" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
         <v>6</v>
       </c>
@@ -1896,11 +1936,11 @@
       <c r="AG11" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="AH11" s="1" t="s">
-        <v>75</v>
+      <c r="AH11" s="3" t="s">
+        <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A12" s="6" t="s">
         <v>7</v>
       </c>
@@ -2001,10 +2041,10 @@
         <v>66</v>
       </c>
       <c r="AH12" s="1" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A13" s="6" t="s">
         <v>8</v>
       </c>
@@ -2105,10 +2145,10 @@
         <v>66</v>
       </c>
       <c r="AH13" s="1" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
         <v>9</v>
       </c>
@@ -2208,11 +2248,11 @@
       <c r="AG14" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="AH14" s="1" t="s">
-        <v>75</v>
+      <c r="AH14" s="3" t="s">
+        <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A15" s="6" t="s">
         <v>74</v>
       </c>
@@ -2316,7 +2356,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A16" s="6" t="s">
         <v>10</v>
       </c>
@@ -2416,11 +2456,11 @@
       <c r="AG16" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="AH16" s="1" t="s">
-        <v>75</v>
+      <c r="AH16" s="3" t="s">
+        <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A17" s="6" t="s">
         <v>11</v>
       </c>
@@ -2520,11 +2560,11 @@
       <c r="AG17" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="AH17" s="1" t="s">
-        <v>75</v>
+      <c r="AH17" s="3" t="s">
+        <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A18" s="6" t="s">
         <v>12</v>
       </c>
@@ -2624,11 +2664,11 @@
       <c r="AG18" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="AH18" s="1" t="s">
-        <v>75</v>
+      <c r="AH18" s="3" t="s">
+        <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A19" s="6" t="s">
         <v>13</v>
       </c>
@@ -2729,10 +2769,10 @@
         <v>66</v>
       </c>
       <c r="AH19" s="1" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A20" s="6" t="s">
         <v>14</v>
       </c>
@@ -2833,10 +2873,10 @@
         <v>66</v>
       </c>
       <c r="AH20" s="1" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A21" s="6" t="s">
         <v>90</v>
       </c>
@@ -2937,10 +2977,10 @@
         <v>66</v>
       </c>
       <c r="AH21" s="1" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A22" s="6" t="s">
         <v>15</v>
       </c>
@@ -3041,10 +3081,10 @@
         <v>66</v>
       </c>
       <c r="AH22" s="1" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A23" s="6" t="s">
         <v>16</v>
       </c>
@@ -3148,7 +3188,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A24" s="6" t="s">
         <v>17</v>
       </c>
@@ -3252,7 +3292,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A25" s="6" t="s">
         <v>18</v>
       </c>
@@ -3356,7 +3396,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A26" s="6" t="s">
         <v>19</v>
       </c>
@@ -3456,11 +3496,11 @@
       <c r="AG26" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="AH26" s="1" t="s">
-        <v>75</v>
+      <c r="AH26" s="3" t="s">
+        <v>66</v>
       </c>
     </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A27" s="6" t="s">
         <v>20</v>
       </c>
@@ -3564,7 +3604,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A28" s="6" t="s">
         <v>21</v>
       </c>
@@ -3664,11 +3704,11 @@
       <c r="AG28" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="AH28" s="1" t="s">
-        <v>75</v>
+      <c r="AH28" s="3" t="s">
+        <v>66</v>
       </c>
     </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A29" s="6" t="s">
         <v>22</v>
       </c>
@@ -3772,7 +3812,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A30" s="6" t="s">
         <v>24</v>
       </c>
@@ -3872,11 +3912,11 @@
       <c r="AG30" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="AH30" s="1" t="s">
-        <v>75</v>
+      <c r="AH30" s="3" t="s">
+        <v>66</v>
       </c>
     </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A31" s="6" t="s">
         <v>25</v>
       </c>
@@ -3980,7 +4020,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A32" s="6" t="s">
         <v>26</v>
       </c>
@@ -4084,7 +4124,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="33" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A33" s="6" t="s">
         <v>27</v>
       </c>
@@ -4185,10 +4225,10 @@
         <v>66</v>
       </c>
       <c r="AH33" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
-    <row r="34" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A34" s="6" t="s">
         <v>28</v>
       </c>
@@ -4288,11 +4328,11 @@
       <c r="AG34" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="AH34" s="1" t="s">
-        <v>75</v>
+      <c r="AH34" s="3" t="s">
+        <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A35" s="6" t="s">
         <v>29</v>
       </c>
@@ -4392,11 +4432,11 @@
       <c r="AG35" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="AH35" s="1" t="s">
-        <v>75</v>
+      <c r="AH35" s="3" t="s">
+        <v>66</v>
       </c>
     </row>
-    <row r="36" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A36" s="6" t="s">
         <v>30</v>
       </c>
@@ -4496,11 +4536,11 @@
       <c r="AG36" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="AH36" s="1" t="s">
-        <v>75</v>
+      <c r="AH36" s="3" t="s">
+        <v>66</v>
       </c>
     </row>
-    <row r="37" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A37" s="6" t="s">
         <v>31</v>
       </c>
@@ -4600,11 +4640,11 @@
       <c r="AG37" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="AH37" s="1" t="s">
-        <v>75</v>
+      <c r="AH37" s="3" t="s">
+        <v>66</v>
       </c>
     </row>
-    <row r="38" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A38" s="6" t="s">
         <v>32</v>
       </c>
@@ -4704,11 +4744,11 @@
       <c r="AG38" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="AH38" s="1" t="s">
-        <v>75</v>
+      <c r="AH38" s="3" t="s">
+        <v>66</v>
       </c>
     </row>
-    <row r="39" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A39" s="6" t="s">
         <v>33</v>
       </c>
@@ -4809,10 +4849,10 @@
         <v>66</v>
       </c>
       <c r="AH39" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
-    <row r="40" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A40" s="6" t="s">
         <v>34</v>
       </c>
@@ -4913,10 +4953,10 @@
         <v>66</v>
       </c>
       <c r="AH40" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
-    <row r="41" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A41" s="6" t="s">
         <v>100</v>
       </c>
@@ -5017,10 +5057,10 @@
         <v>66</v>
       </c>
       <c r="AH41" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
-    <row r="42" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A42" s="6" t="s">
         <v>35</v>
       </c>
@@ -5121,10 +5161,10 @@
         <v>66</v>
       </c>
       <c r="AH42" s="1" t="s">
-        <v>75</v>
+        <v>98</v>
       </c>
     </row>
-    <row r="43" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A43" s="6" t="s">
         <v>23</v>
       </c>
@@ -5225,7 +5265,7 @@
         <v>66</v>
       </c>
       <c r="AH43" s="1" t="s">
-        <v>75</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FIX: minor lexer transition fix on special decimal values.
</commit_message>
<xml_diff>
--- a/docs/lexer/lexer-FSM.xlsx
+++ b/docs/lexer/lexer-FSM.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Red\docs\lexer\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E9B17D-15CC-4E0B-99C3-2B675C00EE9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="743" yWindow="83" windowWidth="19447" windowHeight="13522" tabRatio="564" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="740" yWindow="80" windowWidth="19450" windowHeight="13520" tabRatio="564"/>
   </bookViews>
   <sheets>
     <sheet name="Transitions" sheetId="3" r:id="rId1"/>
@@ -334,7 +328,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -505,7 +499,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -538,26 +532,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -590,23 +567,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -782,20 +742,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="T1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AH43" sqref="AH43"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="V34" sqref="V34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.06640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.73046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="34" width="9.73046875" customWidth="1"/>
+    <col min="1" max="1" width="10.08984375" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" customWidth="1"/>
+    <col min="5" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="9.7265625" customWidth="1"/>
+    <col min="13" max="13" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="34" width="9.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -900,7 +863,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -1004,7 +967,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -1108,7 +1071,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A4" s="6" t="s">
         <v>72</v>
       </c>
@@ -1212,7 +1175,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A5" s="6" t="s">
         <v>73</v>
       </c>
@@ -1316,7 +1279,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A6" s="6" t="s">
         <v>2</v>
       </c>
@@ -1420,7 +1383,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A7" s="6" t="s">
         <v>3</v>
       </c>
@@ -1524,7 +1487,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A8" s="6" t="s">
         <v>77</v>
       </c>
@@ -1628,7 +1591,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A9" s="6" t="s">
         <v>4</v>
       </c>
@@ -1732,7 +1695,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A10" s="6" t="s">
         <v>5</v>
       </c>
@@ -1836,7 +1799,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
         <v>6</v>
       </c>
@@ -1940,7 +1903,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A12" s="6" t="s">
         <v>7</v>
       </c>
@@ -2044,7 +2007,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A13" s="6" t="s">
         <v>8</v>
       </c>
@@ -2148,7 +2111,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
         <v>9</v>
       </c>
@@ -2252,7 +2215,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A15" s="6" t="s">
         <v>74</v>
       </c>
@@ -2356,7 +2319,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A16" s="6" t="s">
         <v>10</v>
       </c>
@@ -2460,7 +2423,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A17" s="6" t="s">
         <v>11</v>
       </c>
@@ -2564,7 +2527,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A18" s="6" t="s">
         <v>12</v>
       </c>
@@ -2668,7 +2631,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A19" s="6" t="s">
         <v>13</v>
       </c>
@@ -2772,7 +2735,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A20" s="6" t="s">
         <v>14</v>
       </c>
@@ -2876,7 +2839,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A21" s="6" t="s">
         <v>90</v>
       </c>
@@ -2980,7 +2943,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A22" s="6" t="s">
         <v>15</v>
       </c>
@@ -3084,7 +3047,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A23" s="6" t="s">
         <v>16</v>
       </c>
@@ -3121,8 +3084,8 @@
       <c r="L23" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="M23" s="1" t="s">
-        <v>91</v>
+      <c r="M23" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="N23" s="1" t="s">
         <v>91</v>
@@ -3188,7 +3151,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A24" s="6" t="s">
         <v>17</v>
       </c>
@@ -3292,7 +3255,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A25" s="6" t="s">
         <v>18</v>
       </c>
@@ -3396,7 +3359,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A26" s="6" t="s">
         <v>19</v>
       </c>
@@ -3500,7 +3463,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A27" s="6" t="s">
         <v>20</v>
       </c>
@@ -3604,7 +3567,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A28" s="6" t="s">
         <v>21</v>
       </c>
@@ -3708,7 +3671,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A29" s="6" t="s">
         <v>22</v>
       </c>
@@ -3812,7 +3775,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A30" s="6" t="s">
         <v>24</v>
       </c>
@@ -3916,7 +3879,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A31" s="6" t="s">
         <v>25</v>
       </c>
@@ -4020,7 +3983,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A32" s="6" t="s">
         <v>26</v>
       </c>
@@ -4124,7 +4087,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="33" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A33" s="6" t="s">
         <v>27</v>
       </c>
@@ -4228,7 +4191,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A34" s="6" t="s">
         <v>28</v>
       </c>
@@ -4332,7 +4295,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A35" s="6" t="s">
         <v>29</v>
       </c>
@@ -4436,7 +4399,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A36" s="6" t="s">
         <v>30</v>
       </c>
@@ -4540,7 +4503,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="37" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A37" s="6" t="s">
         <v>31</v>
       </c>
@@ -4644,7 +4607,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="38" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A38" s="6" t="s">
         <v>32</v>
       </c>
@@ -4748,7 +4711,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="39" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A39" s="6" t="s">
         <v>33</v>
       </c>
@@ -4852,7 +4815,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A40" s="6" t="s">
         <v>34</v>
       </c>
@@ -4956,7 +4919,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A41" s="6" t="s">
         <v>100</v>
       </c>
@@ -5060,7 +5023,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="42" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A42" s="6" t="s">
         <v>35</v>
       </c>
@@ -5164,7 +5127,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="43" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A43" s="6" t="s">
         <v>23</v>
       </c>
@@ -5270,5 +5233,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
FIX: aligns S_BLANK transitions to S_START transitions.
</commit_message>
<xml_diff>
--- a/docs/lexer/lexer-FSM.xlsx
+++ b/docs/lexer/lexer-FSM.xlsx
@@ -1,13 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Red\docs\lexer\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49979050-B514-4C85-BA83-D9317A9C99C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="80" windowWidth="19450" windowHeight="13520" tabRatio="564"/>
+    <workbookView xWindow="3053" yWindow="210" windowWidth="19447" windowHeight="13522" tabRatio="564" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Transitions" sheetId="3" r:id="rId1"/>
+    <sheet name="Copy of lexer-FSM" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -328,7 +334,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -499,7 +505,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -532,9 +538,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -567,6 +590,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -742,23 +782,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="V34" sqref="V34"/>
+      <selection pane="topRight" activeCell="AF3" sqref="AF3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.08984375" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" customWidth="1"/>
-    <col min="5" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="12" width="9.7265625" customWidth="1"/>
-    <col min="13" max="13" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="14" max="34" width="9.7265625" customWidth="1"/>
+    <col min="1" max="1" width="10.06640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.73046875" customWidth="1"/>
+    <col min="5" max="5" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="9.73046875" customWidth="1"/>
+    <col min="13" max="13" width="9.9296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="34" width="9.73046875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -863,7 +903,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -967,7 +1007,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -978,91 +1018,91 @@
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>66</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>0</v>
+        <v>73</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>66</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="X3" s="2" t="s">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>66</v>
       </c>
       <c r="Y3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z3" s="2" t="s">
-        <v>0</v>
+        <v>72</v>
+      </c>
+      <c r="Z3" s="3" t="s">
+        <v>66</v>
       </c>
       <c r="AA3" s="2" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="AB3" s="2" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="AC3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AD3" s="2" t="s">
-        <v>0</v>
+        <v>33</v>
+      </c>
+      <c r="AD3" s="3" t="s">
+        <v>66</v>
       </c>
       <c r="AE3" s="2" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="AF3" s="2" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="AG3" s="3" t="s">
         <v>66</v>
@@ -1071,7 +1111,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A4" s="6" t="s">
         <v>72</v>
       </c>
@@ -1175,7 +1215,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A5" s="6" t="s">
         <v>73</v>
       </c>
@@ -1279,7 +1319,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A6" s="6" t="s">
         <v>2</v>
       </c>
@@ -1383,7 +1423,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A7" s="6" t="s">
         <v>3</v>
       </c>
@@ -1487,7 +1527,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A8" s="6" t="s">
         <v>77</v>
       </c>
@@ -1591,7 +1631,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A9" s="6" t="s">
         <v>4</v>
       </c>
@@ -1695,7 +1735,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A10" s="6" t="s">
         <v>5</v>
       </c>
@@ -1799,7 +1839,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
         <v>6</v>
       </c>
@@ -1903,7 +1943,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A12" s="6" t="s">
         <v>7</v>
       </c>
@@ -2007,7 +2047,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A13" s="6" t="s">
         <v>8</v>
       </c>
@@ -2111,7 +2151,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
         <v>9</v>
       </c>
@@ -2215,7 +2255,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A15" s="6" t="s">
         <v>74</v>
       </c>
@@ -2319,7 +2359,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A16" s="6" t="s">
         <v>10</v>
       </c>
@@ -2423,7 +2463,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A17" s="6" t="s">
         <v>11</v>
       </c>
@@ -2527,7 +2567,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A18" s="6" t="s">
         <v>12</v>
       </c>
@@ -2631,7 +2671,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A19" s="6" t="s">
         <v>13</v>
       </c>
@@ -2735,7 +2775,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="20" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A20" s="6" t="s">
         <v>14</v>
       </c>
@@ -2839,7 +2879,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="21" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A21" s="6" t="s">
         <v>90</v>
       </c>
@@ -2943,7 +2983,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="22" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A22" s="6" t="s">
         <v>15</v>
       </c>
@@ -3047,7 +3087,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A23" s="6" t="s">
         <v>16</v>
       </c>
@@ -3151,7 +3191,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="24" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A24" s="6" t="s">
         <v>17</v>
       </c>
@@ -3255,7 +3295,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A25" s="6" t="s">
         <v>18</v>
       </c>
@@ -3359,7 +3399,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A26" s="6" t="s">
         <v>19</v>
       </c>
@@ -3463,7 +3503,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A27" s="6" t="s">
         <v>20</v>
       </c>
@@ -3567,7 +3607,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="28" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A28" s="6" t="s">
         <v>21</v>
       </c>
@@ -3671,7 +3711,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A29" s="6" t="s">
         <v>22</v>
       </c>
@@ -3775,7 +3815,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A30" s="6" t="s">
         <v>24</v>
       </c>
@@ -3879,7 +3919,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="31" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A31" s="6" t="s">
         <v>25</v>
       </c>
@@ -3983,7 +4023,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="32" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A32" s="6" t="s">
         <v>26</v>
       </c>
@@ -4087,7 +4127,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="33" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A33" s="6" t="s">
         <v>27</v>
       </c>
@@ -4191,7 +4231,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A34" s="6" t="s">
         <v>28</v>
       </c>
@@ -4295,7 +4335,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A35" s="6" t="s">
         <v>29</v>
       </c>
@@ -4399,7 +4439,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A36" s="6" t="s">
         <v>30</v>
       </c>
@@ -4503,7 +4543,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="37" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A37" s="6" t="s">
         <v>31</v>
       </c>
@@ -4607,7 +4647,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="38" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A38" s="6" t="s">
         <v>32</v>
       </c>
@@ -4711,7 +4751,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="39" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A39" s="6" t="s">
         <v>33</v>
       </c>
@@ -4815,7 +4855,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A40" s="6" t="s">
         <v>34</v>
       </c>
@@ -4919,7 +4959,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A41" s="6" t="s">
         <v>100</v>
       </c>
@@ -5023,7 +5063,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="42" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A42" s="6" t="s">
         <v>35</v>
       </c>
@@ -5127,7 +5167,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="43" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A43" s="6" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
FIX: forces an exit T_PAIR state on reaching the input's end.
</commit_message>
<xml_diff>
--- a/docs/lexer/lexer-FSM.xlsx
+++ b/docs/lexer/lexer-FSM.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Red\docs\lexer\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AB89C3E-87AD-4E09-BF71-7DA0E95D4325}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3050" yWindow="210" windowWidth="19450" windowHeight="13520" tabRatio="564"/>
+    <workbookView xWindow="2242" yWindow="210" windowWidth="19448" windowHeight="13522" tabRatio="564" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Copy of lexer-FSM" sheetId="3" r:id="rId1"/>
@@ -325,7 +331,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -496,7 +502,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -529,9 +535,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -564,6 +587,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -739,23 +779,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C2" sqref="C2"/>
+      <selection pane="topRight" activeCell="AH28" sqref="AH28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.08984375" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" customWidth="1"/>
-    <col min="5" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="12" width="9.7265625" customWidth="1"/>
-    <col min="13" max="13" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="14" max="34" width="9.7265625" customWidth="1"/>
+    <col min="1" max="1" width="10.06640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.73046875" customWidth="1"/>
+    <col min="5" max="5" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="9.73046875" customWidth="1"/>
+    <col min="13" max="13" width="9.9296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="34" width="9.73046875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -860,7 +900,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -964,7 +1004,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
         <v>71</v>
       </c>
@@ -1068,7 +1108,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A4" s="6" t="s">
         <v>72</v>
       </c>
@@ -1172,7 +1212,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A5" s="6" t="s">
         <v>1</v>
       </c>
@@ -1276,7 +1316,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A6" s="6" t="s">
         <v>2</v>
       </c>
@@ -1380,7 +1420,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A7" s="6" t="s">
         <v>76</v>
       </c>
@@ -1484,7 +1524,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A8" s="6" t="s">
         <v>3</v>
       </c>
@@ -1588,7 +1628,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A9" s="6" t="s">
         <v>4</v>
       </c>
@@ -1692,7 +1732,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A10" s="6" t="s">
         <v>5</v>
       </c>
@@ -1796,7 +1836,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
         <v>6</v>
       </c>
@@ -1900,7 +1940,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A12" s="6" t="s">
         <v>7</v>
       </c>
@@ -2004,7 +2044,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A13" s="6" t="s">
         <v>8</v>
       </c>
@@ -2108,7 +2148,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
         <v>73</v>
       </c>
@@ -2212,7 +2252,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A15" s="6" t="s">
         <v>9</v>
       </c>
@@ -2316,7 +2356,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A16" s="6" t="s">
         <v>10</v>
       </c>
@@ -2420,7 +2460,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A17" s="6" t="s">
         <v>11</v>
       </c>
@@ -2524,7 +2564,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A18" s="6" t="s">
         <v>12</v>
       </c>
@@ -2628,7 +2668,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="19" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A19" s="6" t="s">
         <v>13</v>
       </c>
@@ -2732,7 +2772,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="20" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A20" s="6" t="s">
         <v>89</v>
       </c>
@@ -2836,7 +2876,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A21" s="6" t="s">
         <v>14</v>
       </c>
@@ -2940,7 +2980,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A22" s="6" t="s">
         <v>15</v>
       </c>
@@ -3044,7 +3084,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="23" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A23" s="6" t="s">
         <v>16</v>
       </c>
@@ -3148,7 +3188,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A24" s="6" t="s">
         <v>17</v>
       </c>
@@ -3252,7 +3292,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="25" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A25" s="6" t="s">
         <v>18</v>
       </c>
@@ -3356,7 +3396,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A26" s="6" t="s">
         <v>19</v>
       </c>
@@ -3460,7 +3500,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="27" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A27" s="6" t="s">
         <v>20</v>
       </c>
@@ -3564,7 +3604,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A28" s="6" t="s">
         <v>21</v>
       </c>
@@ -3665,10 +3705,10 @@
         <v>65</v>
       </c>
       <c r="AH28" s="1" t="s">
-        <v>74</v>
+        <v>94</v>
       </c>
     </row>
-    <row r="29" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A29" s="6" t="s">
         <v>23</v>
       </c>
@@ -3772,7 +3812,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A30" s="6" t="s">
         <v>24</v>
       </c>
@@ -3876,7 +3916,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="31" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A31" s="6" t="s">
         <v>25</v>
       </c>
@@ -3980,7 +4020,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="32" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A32" s="6" t="s">
         <v>26</v>
       </c>
@@ -4084,7 +4124,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="33" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A33" s="6" t="s">
         <v>27</v>
       </c>
@@ -4188,7 +4228,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A34" s="6" t="s">
         <v>28</v>
       </c>
@@ -4292,7 +4332,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="35" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A35" s="6" t="s">
         <v>29</v>
       </c>
@@ -4396,7 +4436,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A36" s="6" t="s">
         <v>30</v>
       </c>
@@ -4500,7 +4540,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="37" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A37" s="6" t="s">
         <v>31</v>
       </c>
@@ -4604,7 +4644,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="38" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A38" s="6" t="s">
         <v>32</v>
       </c>
@@ -4708,7 +4748,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="39" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A39" s="6" t="s">
         <v>33</v>
       </c>
@@ -4812,7 +4852,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="40" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A40" s="6" t="s">
         <v>99</v>
       </c>
@@ -4916,7 +4956,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="41" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A41" s="6" t="s">
         <v>34</v>
       </c>
@@ -5020,7 +5060,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="42" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A42" s="6" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
FIX: forces an exit T_TUPLE state on reaching the input's end.
</commit_message>
<xml_diff>
--- a/docs/lexer/lexer-FSM.xlsx
+++ b/docs/lexer/lexer-FSM.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Red\docs\lexer\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AB89C3E-87AD-4E09-BF71-7DA0E95D4325}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2242" yWindow="210" windowWidth="19448" windowHeight="13522" tabRatio="564" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2240" yWindow="210" windowWidth="19450" windowHeight="13520" tabRatio="564"/>
   </bookViews>
   <sheets>
     <sheet name="Copy of lexer-FSM" sheetId="3" r:id="rId1"/>
@@ -331,7 +325,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -502,7 +496,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -535,26 +529,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -587,23 +564,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -779,23 +739,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AH28" sqref="AH28"/>
+      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AH23" sqref="AH23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.06640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.73046875" customWidth="1"/>
-    <col min="5" max="5" width="9.73046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="12" width="9.73046875" customWidth="1"/>
-    <col min="13" max="13" width="9.9296875" bestFit="1" customWidth="1"/>
-    <col min="14" max="34" width="9.73046875" customWidth="1"/>
+    <col min="1" max="1" width="10.08984375" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" customWidth="1"/>
+    <col min="5" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="9.7265625" customWidth="1"/>
+    <col min="13" max="13" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="34" width="9.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -900,7 +860,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -1004,7 +964,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
         <v>71</v>
       </c>
@@ -1108,7 +1068,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A4" s="6" t="s">
         <v>72</v>
       </c>
@@ -1212,7 +1172,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A5" s="6" t="s">
         <v>1</v>
       </c>
@@ -1316,7 +1276,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A6" s="6" t="s">
         <v>2</v>
       </c>
@@ -1420,7 +1380,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A7" s="6" t="s">
         <v>76</v>
       </c>
@@ -1524,7 +1484,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A8" s="6" t="s">
         <v>3</v>
       </c>
@@ -1628,7 +1588,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A9" s="6" t="s">
         <v>4</v>
       </c>
@@ -1732,7 +1692,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A10" s="6" t="s">
         <v>5</v>
       </c>
@@ -1836,7 +1796,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
         <v>6</v>
       </c>
@@ -1940,7 +1900,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A12" s="6" t="s">
         <v>7</v>
       </c>
@@ -2044,7 +2004,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A13" s="6" t="s">
         <v>8</v>
       </c>
@@ -2148,7 +2108,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
         <v>73</v>
       </c>
@@ -2252,7 +2212,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A15" s="6" t="s">
         <v>9</v>
       </c>
@@ -2356,7 +2316,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A16" s="6" t="s">
         <v>10</v>
       </c>
@@ -2460,7 +2420,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A17" s="6" t="s">
         <v>11</v>
       </c>
@@ -2564,7 +2524,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A18" s="6" t="s">
         <v>12</v>
       </c>
@@ -2668,7 +2628,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A19" s="6" t="s">
         <v>13</v>
       </c>
@@ -2772,7 +2732,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A20" s="6" t="s">
         <v>89</v>
       </c>
@@ -2876,7 +2836,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A21" s="6" t="s">
         <v>14</v>
       </c>
@@ -2980,7 +2940,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A22" s="6" t="s">
         <v>15</v>
       </c>
@@ -3084,7 +3044,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A23" s="6" t="s">
         <v>16</v>
       </c>
@@ -3185,10 +3145,10 @@
         <v>65</v>
       </c>
       <c r="AH23" s="1" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
     </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A24" s="6" t="s">
         <v>17</v>
       </c>
@@ -3292,7 +3252,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A25" s="6" t="s">
         <v>18</v>
       </c>
@@ -3396,7 +3356,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A26" s="6" t="s">
         <v>19</v>
       </c>
@@ -3500,7 +3460,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A27" s="6" t="s">
         <v>20</v>
       </c>
@@ -3604,7 +3564,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A28" s="6" t="s">
         <v>21</v>
       </c>
@@ -3708,7 +3668,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A29" s="6" t="s">
         <v>23</v>
       </c>
@@ -3812,7 +3772,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A30" s="6" t="s">
         <v>24</v>
       </c>
@@ -3916,7 +3876,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A31" s="6" t="s">
         <v>25</v>
       </c>
@@ -4020,7 +3980,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A32" s="6" t="s">
         <v>26</v>
       </c>
@@ -4124,7 +4084,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="33" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A33" s="6" t="s">
         <v>27</v>
       </c>
@@ -4228,7 +4188,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A34" s="6" t="s">
         <v>28</v>
       </c>
@@ -4332,7 +4292,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="35" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A35" s="6" t="s">
         <v>29</v>
       </c>
@@ -4436,7 +4396,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A36" s="6" t="s">
         <v>30</v>
       </c>
@@ -4540,7 +4500,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="37" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A37" s="6" t="s">
         <v>31</v>
       </c>
@@ -4644,7 +4604,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="38" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A38" s="6" t="s">
         <v>32</v>
       </c>
@@ -4748,7 +4708,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="39" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A39" s="6" t="s">
         <v>33</v>
       </c>
@@ -4852,7 +4812,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="40" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A40" s="6" t="s">
         <v>99</v>
       </c>
@@ -4956,7 +4916,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="41" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A41" s="6" t="s">
         <v>34</v>
       </c>
@@ -5060,7 +5020,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="42" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A42" s="6" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
FEAT: various fixes and improvements to scanning char! values.
</commit_message>
<xml_diff>
--- a/docs/lexer/lexer-FSM.xlsx
+++ b/docs/lexer/lexer-FSM.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Red\docs\lexer\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33D64905-8DD2-42B9-8A00-ED6F08DF2480}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2240" yWindow="210" windowWidth="19450" windowHeight="13520" tabRatio="564"/>
+    <workbookView xWindow="1110" yWindow="98" windowWidth="21270" windowHeight="13634" tabRatio="564" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Copy of lexer-FSM" sheetId="3" r:id="rId1"/>
@@ -325,7 +331,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -496,7 +502,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -529,9 +535,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -564,6 +587,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -739,23 +779,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AH23" sqref="AH23"/>
+      <pane xSplit="1" topLeftCell="R1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AH15" sqref="AH15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.08984375" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" customWidth="1"/>
-    <col min="5" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="12" width="9.7265625" customWidth="1"/>
-    <col min="13" max="13" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="14" max="34" width="9.7265625" customWidth="1"/>
+    <col min="1" max="1" width="10.06640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.73046875" customWidth="1"/>
+    <col min="5" max="5" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="9.73046875" customWidth="1"/>
+    <col min="13" max="13" width="9.9296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="34" width="9.73046875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -860,7 +900,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -964,7 +1004,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
         <v>71</v>
       </c>
@@ -1068,7 +1108,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A4" s="6" t="s">
         <v>72</v>
       </c>
@@ -1172,7 +1212,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A5" s="6" t="s">
         <v>1</v>
       </c>
@@ -1276,7 +1316,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A6" s="6" t="s">
         <v>2</v>
       </c>
@@ -1380,7 +1420,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A7" s="6" t="s">
         <v>76</v>
       </c>
@@ -1484,7 +1524,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A8" s="6" t="s">
         <v>3</v>
       </c>
@@ -1588,7 +1628,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A9" s="6" t="s">
         <v>4</v>
       </c>
@@ -1692,7 +1732,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A10" s="6" t="s">
         <v>5</v>
       </c>
@@ -1796,7 +1836,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
         <v>6</v>
       </c>
@@ -1900,7 +1940,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A12" s="6" t="s">
         <v>7</v>
       </c>
@@ -2004,7 +2044,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A13" s="6" t="s">
         <v>8</v>
       </c>
@@ -2108,7 +2148,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
         <v>73</v>
       </c>
@@ -2212,7 +2252,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A15" s="6" t="s">
         <v>9</v>
       </c>
@@ -2312,11 +2352,11 @@
       <c r="AG15" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="AH15" s="3" t="s">
-        <v>65</v>
+      <c r="AH15" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
-    <row r="16" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A16" s="6" t="s">
         <v>10</v>
       </c>
@@ -2420,7 +2460,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A17" s="6" t="s">
         <v>11</v>
       </c>
@@ -2524,7 +2564,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A18" s="6" t="s">
         <v>12</v>
       </c>
@@ -2628,7 +2668,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="19" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A19" s="6" t="s">
         <v>13</v>
       </c>
@@ -2732,7 +2772,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="20" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A20" s="6" t="s">
         <v>89</v>
       </c>
@@ -2836,7 +2876,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A21" s="6" t="s">
         <v>14</v>
       </c>
@@ -2940,7 +2980,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A22" s="6" t="s">
         <v>15</v>
       </c>
@@ -3044,7 +3084,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="23" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A23" s="6" t="s">
         <v>16</v>
       </c>
@@ -3148,7 +3188,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="24" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A24" s="6" t="s">
         <v>17</v>
       </c>
@@ -3252,7 +3292,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="25" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A25" s="6" t="s">
         <v>18</v>
       </c>
@@ -3356,7 +3396,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A26" s="6" t="s">
         <v>19</v>
       </c>
@@ -3460,7 +3500,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="27" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A27" s="6" t="s">
         <v>20</v>
       </c>
@@ -3564,7 +3604,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A28" s="6" t="s">
         <v>21</v>
       </c>
@@ -3668,7 +3708,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A29" s="6" t="s">
         <v>23</v>
       </c>
@@ -3772,7 +3812,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A30" s="6" t="s">
         <v>24</v>
       </c>
@@ -3876,7 +3916,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="31" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A31" s="6" t="s">
         <v>25</v>
       </c>
@@ -3980,7 +4020,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="32" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A32" s="6" t="s">
         <v>26</v>
       </c>
@@ -4084,7 +4124,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="33" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A33" s="6" t="s">
         <v>27</v>
       </c>
@@ -4188,7 +4228,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A34" s="6" t="s">
         <v>28</v>
       </c>
@@ -4292,7 +4332,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="35" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A35" s="6" t="s">
         <v>29</v>
       </c>
@@ -4396,7 +4436,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A36" s="6" t="s">
         <v>30</v>
       </c>
@@ -4500,7 +4540,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="37" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A37" s="6" t="s">
         <v>31</v>
       </c>
@@ -4604,7 +4644,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="38" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A38" s="6" t="s">
         <v>32</v>
       </c>
@@ -4708,7 +4748,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="39" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A39" s="6" t="s">
         <v>33</v>
       </c>
@@ -4812,7 +4852,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="40" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A40" s="6" t="s">
         <v>99</v>
       </c>
@@ -4916,7 +4956,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="41" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A41" s="6" t="s">
         <v>34</v>
       </c>
@@ -5020,7 +5060,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="42" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A42" s="6" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
FEAT: merges T_STR_ALT state into T_STRING.
</commit_message>
<xml_diff>
--- a/docs/lexer/lexer-FSM.xlsx
+++ b/docs/lexer/lexer-FSM.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Red\docs\lexer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33D64905-8DD2-42B9-8A00-ED6F08DF2480}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6717E0A3-56BE-42E5-BC15-6678443DF7FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1110" yWindow="98" windowWidth="21270" windowHeight="13634" tabRatio="564" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Copy of lexer-FSM" sheetId="3" r:id="rId1"/>
+    <sheet name="transitions" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1427" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1427" uniqueCount="101">
   <si>
     <t>S_START</t>
   </si>
@@ -251,9 +251,6 @@
   </si>
   <si>
     <t>S_SKIP_MSTR</t>
-  </si>
-  <si>
-    <t>T_STR_ALT</t>
   </si>
   <si>
     <t>T_WORD</t>
@@ -783,8 +780,8 @@
   <dimension ref="A1:AH42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="R1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AH15" sqref="AH15"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -849,7 +846,7 @@
         <v>49</v>
       </c>
       <c r="R1" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="S1" s="7" t="s">
         <v>50</v>
@@ -888,7 +885,7 @@
         <v>61</v>
       </c>
       <c r="AE1" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AF1" s="7" t="s">
         <v>64</v>
@@ -1348,7 +1345,7 @@
         <v>2</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>2</v>
@@ -1529,10 +1526,10 @@
         <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>4</v>
@@ -1541,22 +1538,22 @@
         <v>4</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L8" s="2" t="s">
         <v>4</v>
@@ -1568,7 +1565,7 @@
         <v>4</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="P8" s="2" t="s">
         <v>4</v>
@@ -1598,10 +1595,10 @@
         <v>4</v>
       </c>
       <c r="Y8" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="Z8" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AA8" s="2" t="s">
         <v>4</v>
@@ -1625,7 +1622,7 @@
         <v>65</v>
       </c>
       <c r="AH8" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.45">
@@ -1633,10 +1630,10 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>4</v>
@@ -1645,22 +1642,22 @@
         <v>4</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L9" s="2" t="s">
         <v>4</v>
@@ -1672,7 +1669,7 @@
         <v>4</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="P9" s="2" t="s">
         <v>4</v>
@@ -1702,10 +1699,10 @@
         <v>4</v>
       </c>
       <c r="Y9" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="Z9" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AA9" s="2" t="s">
         <v>4</v>
@@ -1729,7 +1726,7 @@
         <v>65</v>
       </c>
       <c r="AH9" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.45">
@@ -1841,10 +1838,10 @@
         <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>6</v>
@@ -1853,25 +1850,25 @@
         <v>6</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M11" s="2" t="s">
         <v>6</v>
@@ -1910,10 +1907,10 @@
         <v>6</v>
       </c>
       <c r="Y11" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Z11" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AA11" s="2" t="s">
         <v>6</v>
@@ -1937,7 +1934,7 @@
         <v>65</v>
       </c>
       <c r="AH11" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.45">
@@ -1945,10 +1942,10 @@
         <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>12</v>
@@ -1963,7 +1960,7 @@
         <v>65</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I12" s="3" t="s">
         <v>65</v>
@@ -2014,10 +2011,10 @@
         <v>65</v>
       </c>
       <c r="Y12" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Z12" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AA12" s="2" t="s">
         <v>12</v>
@@ -2041,7 +2038,7 @@
         <v>65</v>
       </c>
       <c r="AH12" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.45">
@@ -2076,7 +2073,7 @@
         <v>65</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L13" s="3" t="s">
         <v>65</v>
@@ -2287,7 +2284,7 @@
         <v>9</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M15" s="2" t="s">
         <v>9</v>
@@ -2353,7 +2350,7 @@
         <v>65</v>
       </c>
       <c r="AH15" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.45">
@@ -2480,7 +2477,7 @@
         <v>11</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>11</v>
@@ -2569,10 +2566,10 @@
         <v>12</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>12</v>
@@ -2581,25 +2578,25 @@
         <v>12</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M18" s="2" t="s">
         <v>12</v>
@@ -2638,10 +2635,10 @@
         <v>12</v>
       </c>
       <c r="Y18" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Z18" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AA18" s="2" t="s">
         <v>12</v>
@@ -2665,7 +2662,7 @@
         <v>65</v>
       </c>
       <c r="AH18" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:34" x14ac:dyDescent="0.45">
@@ -2673,10 +2670,10 @@
         <v>13</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>13</v>
@@ -2685,25 +2682,25 @@
         <v>13</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M19" s="2" t="s">
         <v>7</v>
@@ -2730,25 +2727,25 @@
         <v>65</v>
       </c>
       <c r="U19" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="V19" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="W19" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="V19" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="W19" s="1" t="s">
-        <v>88</v>
-      </c>
       <c r="X19" s="4" t="s">
         <v>65</v>
       </c>
       <c r="Y19" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Z19" s="2" t="s">
         <v>22</v>
       </c>
       <c r="AA19" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AB19" s="3" t="s">
         <v>65</v>
@@ -2769,18 +2766,18 @@
         <v>65</v>
       </c>
       <c r="AH19" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A20" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>90</v>
-      </c>
       <c r="C20" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>14</v>
@@ -2789,25 +2786,25 @@
         <v>14</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="M20" s="2" t="s">
         <v>15</v>
@@ -2828,25 +2825,25 @@
         <v>65</v>
       </c>
       <c r="S20" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="T20" s="3" t="s">
         <v>65</v>
       </c>
       <c r="U20" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="V20" s="3" t="s">
         <v>65</v>
       </c>
       <c r="W20" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="X20" s="4" t="s">
         <v>65</v>
       </c>
       <c r="Y20" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="Z20" s="3" t="s">
         <v>65</v>
@@ -2873,7 +2870,7 @@
         <v>65</v>
       </c>
       <c r="AH20" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:34" x14ac:dyDescent="0.45">
@@ -2881,10 +2878,10 @@
         <v>14</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>14</v>
@@ -2893,25 +2890,25 @@
         <v>14</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="M21" s="2" t="s">
         <v>20</v>
@@ -2920,7 +2917,7 @@
         <v>65</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="P21" s="3" t="s">
         <v>65</v>
@@ -2932,19 +2929,19 @@
         <v>65</v>
       </c>
       <c r="S21" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="T21" s="3" t="s">
         <v>65</v>
       </c>
       <c r="U21" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="V21" s="3" t="s">
         <v>65</v>
       </c>
       <c r="W21" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="X21" s="3" t="s">
         <v>65</v>
@@ -2977,7 +2974,7 @@
         <v>65</v>
       </c>
       <c r="AH21" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:34" x14ac:dyDescent="0.45">
@@ -2985,46 +2982,46 @@
         <v>15</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="M22" s="2" t="s">
         <v>15</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="P22" s="2" t="s">
         <v>15</v>
@@ -3036,40 +3033,40 @@
         <v>15</v>
       </c>
       <c r="S22" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="T22" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="U22" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="V22" s="2" t="s">
         <v>15</v>
       </c>
       <c r="W22" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="X22" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="Y22" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="Z22" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AA22" s="2" t="s">
         <v>15</v>
       </c>
       <c r="AB22" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AC22" s="2" t="s">
         <v>15</v>
       </c>
       <c r="AD22" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AE22" s="2" t="s">
         <v>15</v>
@@ -3089,10 +3086,10 @@
         <v>16</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>16</v>
@@ -3101,25 +3098,25 @@
         <v>16</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="M23" s="3" t="s">
         <v>65</v>
@@ -3128,7 +3125,7 @@
         <v>65</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="P23" s="3" t="s">
         <v>65</v>
@@ -3140,13 +3137,13 @@
         <v>65</v>
       </c>
       <c r="S23" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="T23" s="3" t="s">
         <v>65</v>
       </c>
       <c r="U23" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="V23" s="3" t="s">
         <v>65</v>
@@ -3185,7 +3182,7 @@
         <v>65</v>
       </c>
       <c r="AH23" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:34" x14ac:dyDescent="0.45">
@@ -3193,10 +3190,10 @@
         <v>17</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>17</v>
@@ -3205,25 +3202,25 @@
         <v>17</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M24" s="2" t="s">
         <v>17</v>
@@ -3232,7 +3229,7 @@
         <v>17</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="P24" s="2" t="s">
         <v>17</v>
@@ -3250,34 +3247,34 @@
         <v>17</v>
       </c>
       <c r="U24" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="V24" s="2" t="s">
         <v>17</v>
       </c>
       <c r="W24" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="X24" s="2" t="s">
         <v>17</v>
       </c>
       <c r="Y24" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Z24" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AA24" s="2" t="s">
         <v>17</v>
       </c>
       <c r="AB24" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AC24" s="2" t="s">
         <v>17</v>
       </c>
       <c r="AD24" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AE24" s="2" t="s">
         <v>17</v>
@@ -3401,10 +3398,10 @@
         <v>19</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>19</v>
@@ -3413,25 +3410,25 @@
         <v>19</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="M26" s="3" t="s">
         <v>65</v>
@@ -3452,13 +3449,13 @@
         <v>65</v>
       </c>
       <c r="S26" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="T26" s="3" t="s">
         <v>65</v>
       </c>
       <c r="U26" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="V26" s="3" t="s">
         <v>65</v>
@@ -3470,7 +3467,7 @@
         <v>65</v>
       </c>
       <c r="Y26" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Z26" s="3" t="s">
         <v>65</v>
@@ -3609,10 +3606,10 @@
         <v>21</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>21</v>
@@ -3621,25 +3618,25 @@
         <v>21</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M28" s="3" t="s">
         <v>65</v>
@@ -3666,7 +3663,7 @@
         <v>65</v>
       </c>
       <c r="U28" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="V28" s="3" t="s">
         <v>65</v>
@@ -3678,7 +3675,7 @@
         <v>65</v>
       </c>
       <c r="Y28" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Z28" s="3" t="s">
         <v>65</v>
@@ -3705,7 +3702,7 @@
         <v>65</v>
       </c>
       <c r="AH28" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" spans="1:34" x14ac:dyDescent="0.45">
@@ -3817,10 +3814,10 @@
         <v>24</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>24</v>
@@ -3829,28 +3826,28 @@
         <v>24</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="N30" s="2" t="s">
         <v>24</v>
@@ -3868,13 +3865,13 @@
         <v>65</v>
       </c>
       <c r="S30" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="T30" s="3" t="s">
         <v>65</v>
       </c>
       <c r="U30" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="V30" s="3" t="s">
         <v>65</v>
@@ -3886,7 +3883,7 @@
         <v>65</v>
       </c>
       <c r="Y30" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Z30" s="3" t="s">
         <v>65</v>
@@ -3921,10 +3918,10 @@
         <v>25</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>25</v>
@@ -3933,28 +3930,28 @@
         <v>25</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="N31" s="2" t="s">
         <v>25</v>
@@ -3972,13 +3969,13 @@
         <v>65</v>
       </c>
       <c r="S31" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="T31" s="3" t="s">
         <v>65</v>
       </c>
       <c r="U31" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="V31" s="3" t="s">
         <v>65</v>
@@ -3990,7 +3987,7 @@
         <v>65</v>
       </c>
       <c r="Y31" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Z31" s="3" t="s">
         <v>65</v>
@@ -4025,10 +4022,10 @@
         <v>26</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>27</v>
@@ -4037,25 +4034,25 @@
         <v>27</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M32" s="2" t="s">
         <v>27</v>
@@ -4064,7 +4061,7 @@
         <v>27</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="P32" s="2" t="s">
         <v>27</v>
@@ -4085,7 +4082,7 @@
         <v>65</v>
       </c>
       <c r="V32" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="W32" s="2" t="s">
         <v>27</v>
@@ -4094,10 +4091,10 @@
         <v>27</v>
       </c>
       <c r="Y32" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="Z32" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AA32" s="2" t="s">
         <v>27</v>
@@ -4121,7 +4118,7 @@
         <v>65</v>
       </c>
       <c r="AH32" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:34" x14ac:dyDescent="0.45">
@@ -4189,7 +4186,7 @@
         <v>27</v>
       </c>
       <c r="V33" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="W33" s="2" t="s">
         <v>27</v>
@@ -4745,7 +4742,7 @@
         <v>65</v>
       </c>
       <c r="AH38" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="39" spans="1:34" x14ac:dyDescent="0.45">
@@ -4753,10 +4750,10 @@
         <v>33</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>33</v>
@@ -4765,25 +4762,25 @@
         <v>33</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L39" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M39" s="3" t="s">
         <v>65</v>
@@ -4792,7 +4789,7 @@
         <v>33</v>
       </c>
       <c r="O39" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="P39" s="2" t="s">
         <v>33</v>
@@ -4804,10 +4801,10 @@
         <v>33</v>
       </c>
       <c r="S39" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="T39" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="U39" s="2" t="s">
         <v>33</v>
@@ -4822,7 +4819,7 @@
         <v>65</v>
       </c>
       <c r="Y39" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="Z39" s="2" t="s">
         <v>22</v>
@@ -4849,18 +4846,18 @@
         <v>65</v>
       </c>
       <c r="AH39" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="40" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A40" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>34</v>
@@ -4869,25 +4866,25 @@
         <v>34</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M40" s="5" t="s">
         <v>34</v>
@@ -4911,7 +4908,7 @@
         <v>34</v>
       </c>
       <c r="T40" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="U40" s="3" t="s">
         <v>65</v>
@@ -4926,7 +4923,7 @@
         <v>34</v>
       </c>
       <c r="Y40" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="Z40" s="5" t="s">
         <v>34</v>
@@ -4953,7 +4950,7 @@
         <v>65</v>
       </c>
       <c r="AH40" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="41" spans="1:34" x14ac:dyDescent="0.45">
@@ -4961,10 +4958,10 @@
         <v>34</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>34</v>
@@ -4973,25 +4970,25 @@
         <v>34</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L41" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M41" s="2" t="s">
         <v>34</v>
@@ -5015,10 +5012,10 @@
         <v>34</v>
       </c>
       <c r="T41" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="U41" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="V41" s="3" t="s">
         <v>65</v>
@@ -5027,10 +5024,10 @@
         <v>34</v>
       </c>
       <c r="X41" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Y41" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Z41" s="2" t="s">
         <v>34</v>
@@ -5057,7 +5054,7 @@
         <v>65</v>
       </c>
       <c r="AH41" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="42" spans="1:34" x14ac:dyDescent="0.45">
@@ -5065,10 +5062,10 @@
         <v>22</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>22</v>
@@ -5077,25 +5074,25 @@
         <v>22</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L42" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="M42" s="3" t="s">
         <v>65</v>
@@ -5116,13 +5113,13 @@
         <v>22</v>
       </c>
       <c r="S42" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="T42" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="U42" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="V42" s="3" t="s">
         <v>65</v>
@@ -5134,7 +5131,7 @@
         <v>65</v>
       </c>
       <c r="Y42" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="Z42" s="3" t="s">
         <v>65</v>
@@ -5161,7 +5158,7 @@
         <v>65</v>
       </c>
       <c r="AH42" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FEAT: adds support for scanning base 16 binary! values.
</commit_message>
<xml_diff>
--- a/docs/lexer/lexer-FSM.xlsx
+++ b/docs/lexer/lexer-FSM.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Red\docs\lexer\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6717E0A3-56BE-42E5-BC15-6678443DF7FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1110" yWindow="98" windowWidth="21270" windowHeight="13634" tabRatio="564" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1110" yWindow="100" windowWidth="21270" windowHeight="13630" tabRatio="564" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="transitions" sheetId="3" r:id="rId1"/>
+    <sheet name="bin16 transitions" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1427" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1450" uniqueCount="111">
   <si>
     <t>S_START</t>
   </si>
@@ -323,13 +318,43 @@
   </si>
   <si>
     <t>C_BIN</t>
+  </si>
+  <si>
+    <t>C_BIN_SKIP</t>
+  </si>
+  <si>
+    <t>C_BIN_BLANK</t>
+  </si>
+  <si>
+    <t>C_BIN_LINE</t>
+  </si>
+  <si>
+    <t>C_BIN_HEXA</t>
+  </si>
+  <si>
+    <t>S_BIN_1ST</t>
+  </si>
+  <si>
+    <t>S_BIN_START</t>
+  </si>
+  <si>
+    <t>T_BIN_BYTE</t>
+  </si>
+  <si>
+    <t>T_BIN_ERROR</t>
+  </si>
+  <si>
+    <t>S_BIN_CMT</t>
+  </si>
+  <si>
+    <t>C_BIN_CMT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -374,6 +399,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -412,7 +445,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -437,6 +470,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -499,7 +535,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -532,26 +568,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -584,23 +603,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -776,23 +778,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K6" sqref="K6"/>
+      <selection pane="topRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.06640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.73046875" customWidth="1"/>
-    <col min="5" max="5" width="9.73046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="12" width="9.73046875" customWidth="1"/>
-    <col min="13" max="13" width="9.9296875" bestFit="1" customWidth="1"/>
-    <col min="14" max="34" width="9.73046875" customWidth="1"/>
+    <col min="1" max="1" width="10.08984375" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" customWidth="1"/>
+    <col min="5" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="9.7265625" customWidth="1"/>
+    <col min="13" max="13" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="34" width="9.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -897,7 +899,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -1001,7 +1003,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
         <v>71</v>
       </c>
@@ -1105,7 +1107,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A4" s="6" t="s">
         <v>72</v>
       </c>
@@ -1209,7 +1211,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A5" s="6" t="s">
         <v>1</v>
       </c>
@@ -1313,7 +1315,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A6" s="6" t="s">
         <v>2</v>
       </c>
@@ -1417,7 +1419,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A7" s="6" t="s">
         <v>76</v>
       </c>
@@ -1521,7 +1523,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A8" s="6" t="s">
         <v>3</v>
       </c>
@@ -1625,7 +1627,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A9" s="6" t="s">
         <v>4</v>
       </c>
@@ -1729,7 +1731,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A10" s="6" t="s">
         <v>5</v>
       </c>
@@ -1833,7 +1835,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
         <v>6</v>
       </c>
@@ -1937,7 +1939,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
         <v>7</v>
       </c>
@@ -1965,11 +1967,11 @@
       <c r="I12" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="J12" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="K12" s="2" t="s">
+      <c r="J12" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>65</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>9</v>
@@ -2041,7 +2043,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
         <v>8</v>
       </c>
@@ -2090,8 +2092,8 @@
       <c r="P13" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="Q13" s="3" t="s">
-        <v>65</v>
+      <c r="Q13" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="R13" s="2" t="s">
         <v>8</v>
@@ -2145,7 +2147,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
         <v>73</v>
       </c>
@@ -2249,7 +2251,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A15" s="6" t="s">
         <v>9</v>
       </c>
@@ -2353,7 +2355,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A16" s="6" t="s">
         <v>10</v>
       </c>
@@ -2457,7 +2459,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A17" s="6" t="s">
         <v>11</v>
       </c>
@@ -2561,7 +2563,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A18" s="6" t="s">
         <v>12</v>
       </c>
@@ -2665,7 +2667,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A19" s="6" t="s">
         <v>13</v>
       </c>
@@ -2769,7 +2771,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A20" s="6" t="s">
         <v>88</v>
       </c>
@@ -2873,7 +2875,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A21" s="6" t="s">
         <v>14</v>
       </c>
@@ -2977,7 +2979,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A22" s="6" t="s">
         <v>15</v>
       </c>
@@ -3081,7 +3083,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A23" s="6" t="s">
         <v>16</v>
       </c>
@@ -3185,7 +3187,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A24" s="6" t="s">
         <v>17</v>
       </c>
@@ -3289,7 +3291,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A25" s="6" t="s">
         <v>18</v>
       </c>
@@ -3393,7 +3395,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A26" s="6" t="s">
         <v>19</v>
       </c>
@@ -3497,7 +3499,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A27" s="6" t="s">
         <v>20</v>
       </c>
@@ -3601,7 +3603,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A28" s="6" t="s">
         <v>21</v>
       </c>
@@ -3705,7 +3707,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A29" s="6" t="s">
         <v>23</v>
       </c>
@@ -3809,7 +3811,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A30" s="6" t="s">
         <v>24</v>
       </c>
@@ -3913,7 +3915,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A31" s="6" t="s">
         <v>25</v>
       </c>
@@ -4017,7 +4019,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A32" s="6" t="s">
         <v>26</v>
       </c>
@@ -4121,7 +4123,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="33" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A33" s="6" t="s">
         <v>27</v>
       </c>
@@ -4225,7 +4227,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A34" s="6" t="s">
         <v>28</v>
       </c>
@@ -4329,7 +4331,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="35" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A35" s="6" t="s">
         <v>29</v>
       </c>
@@ -4433,7 +4435,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A36" s="6" t="s">
         <v>30</v>
       </c>
@@ -4537,7 +4539,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="37" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A37" s="6" t="s">
         <v>31</v>
       </c>
@@ -4641,7 +4643,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="38" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A38" s="6" t="s">
         <v>32</v>
       </c>
@@ -4745,7 +4747,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="39" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A39" s="6" t="s">
         <v>33</v>
       </c>
@@ -4849,7 +4851,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="40" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A40" s="6" t="s">
         <v>98</v>
       </c>
@@ -4953,7 +4955,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="41" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A41" s="6" t="s">
         <v>34</v>
       </c>
@@ -5057,7 +5059,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="42" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A42" s="6" t="s">
         <v>22</v>
       </c>
@@ -5160,6 +5162,109 @@
       <c r="AH42" s="1" t="s">
         <v>99</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="8"/>
+      <c r="B1" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
FEAT: adds support for scanning base 64 binary! values.
Note: embedded blanks characters not supported yet.
</commit_message>
<xml_diff>
--- a/docs/lexer/lexer-FSM.xlsx
+++ b/docs/lexer/lexer-FSM.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Red\docs\lexer\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74624EB6-3245-4806-B2F2-C62F2B0910E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1110" yWindow="100" windowWidth="21270" windowHeight="13630" tabRatio="564" activeTab="1"/>
+    <workbookView xWindow="1110" yWindow="98" windowWidth="21270" windowHeight="13634" tabRatio="564" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="transitions" sheetId="3" r:id="rId1"/>
@@ -353,7 +359,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -535,7 +541,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -568,9 +574,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -603,6 +626,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -778,23 +818,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AF13" sqref="AF13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.08984375" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" customWidth="1"/>
-    <col min="5" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="12" width="9.7265625" customWidth="1"/>
-    <col min="13" max="13" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="14" max="34" width="9.7265625" customWidth="1"/>
+    <col min="1" max="1" width="10.06640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.73046875" customWidth="1"/>
+    <col min="5" max="5" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="9.73046875" customWidth="1"/>
+    <col min="13" max="13" width="9.9296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="34" width="9.73046875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -899,7 +939,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -1003,7 +1043,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
         <v>71</v>
       </c>
@@ -1107,7 +1147,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A4" s="6" t="s">
         <v>72</v>
       </c>
@@ -1211,7 +1251,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A5" s="6" t="s">
         <v>1</v>
       </c>
@@ -1315,7 +1355,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A6" s="6" t="s">
         <v>2</v>
       </c>
@@ -1419,7 +1459,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A7" s="6" t="s">
         <v>76</v>
       </c>
@@ -1523,7 +1563,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A8" s="6" t="s">
         <v>3</v>
       </c>
@@ -1627,7 +1667,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A9" s="6" t="s">
         <v>4</v>
       </c>
@@ -1731,7 +1771,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A10" s="6" t="s">
         <v>5</v>
       </c>
@@ -1835,7 +1875,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
         <v>6</v>
       </c>
@@ -1939,7 +1979,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A12" s="6" t="s">
         <v>7</v>
       </c>
@@ -2043,7 +2083,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A13" s="6" t="s">
         <v>8</v>
       </c>
@@ -2137,8 +2177,8 @@
       <c r="AE13" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="AF13" s="3" t="s">
-        <v>65</v>
+      <c r="AF13" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="AG13" s="3" t="s">
         <v>65</v>
@@ -2147,7 +2187,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
         <v>73</v>
       </c>
@@ -2251,7 +2291,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A15" s="6" t="s">
         <v>9</v>
       </c>
@@ -2355,7 +2395,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A16" s="6" t="s">
         <v>10</v>
       </c>
@@ -2459,7 +2499,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A17" s="6" t="s">
         <v>11</v>
       </c>
@@ -2563,7 +2603,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A18" s="6" t="s">
         <v>12</v>
       </c>
@@ -2667,7 +2707,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A19" s="6" t="s">
         <v>13</v>
       </c>
@@ -2771,7 +2811,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A20" s="6" t="s">
         <v>88</v>
       </c>
@@ -2875,7 +2915,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A21" s="6" t="s">
         <v>14</v>
       </c>
@@ -2979,7 +3019,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A22" s="6" t="s">
         <v>15</v>
       </c>
@@ -3083,7 +3123,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="23" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A23" s="6" t="s">
         <v>16</v>
       </c>
@@ -3187,7 +3227,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A24" s="6" t="s">
         <v>17</v>
       </c>
@@ -3291,7 +3331,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="25" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A25" s="6" t="s">
         <v>18</v>
       </c>
@@ -3395,7 +3435,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A26" s="6" t="s">
         <v>19</v>
       </c>
@@ -3499,7 +3539,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="27" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A27" s="6" t="s">
         <v>20</v>
       </c>
@@ -3603,7 +3643,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A28" s="6" t="s">
         <v>21</v>
       </c>
@@ -3707,7 +3747,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="29" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A29" s="6" t="s">
         <v>23</v>
       </c>
@@ -3811,7 +3851,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A30" s="6" t="s">
         <v>24</v>
       </c>
@@ -3915,7 +3955,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="31" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A31" s="6" t="s">
         <v>25</v>
       </c>
@@ -4019,7 +4059,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="32" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A32" s="6" t="s">
         <v>26</v>
       </c>
@@ -4123,7 +4163,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="33" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A33" s="6" t="s">
         <v>27</v>
       </c>
@@ -4227,7 +4267,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A34" s="6" t="s">
         <v>28</v>
       </c>
@@ -4331,7 +4371,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="35" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A35" s="6" t="s">
         <v>29</v>
       </c>
@@ -4435,7 +4475,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A36" s="6" t="s">
         <v>30</v>
       </c>
@@ -4539,7 +4579,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="37" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A37" s="6" t="s">
         <v>31</v>
       </c>
@@ -4643,7 +4683,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="38" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A38" s="6" t="s">
         <v>32</v>
       </c>
@@ -4747,7 +4787,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="39" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A39" s="6" t="s">
         <v>33</v>
       </c>
@@ -4851,7 +4891,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="40" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A40" s="6" t="s">
         <v>98</v>
       </c>
@@ -4955,7 +4995,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="41" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A41" s="6" t="s">
         <v>34</v>
       </c>
@@ -5059,7 +5099,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="42" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A42" s="6" t="s">
         <v>22</v>
       </c>
@@ -5170,22 +5210,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="8.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.9296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.06640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="8"/>
       <c r="B1" s="7" t="s">
         <v>101</v>
@@ -5203,7 +5243,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
         <v>106</v>
       </c>
@@ -5223,7 +5263,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
         <v>105</v>
       </c>
@@ -5243,7 +5283,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="6" t="s">
         <v>109</v>
       </c>
@@ -5263,7 +5303,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FIX: C_X character class was not allowed in binary! values.
Can be present in base64-encoded binaries.
</commit_message>
<xml_diff>
--- a/docs/lexer/lexer-FSM.xlsx
+++ b/docs/lexer/lexer-FSM.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Red\docs\lexer\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74624EB6-3245-4806-B2F2-C62F2B0910E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1110" yWindow="98" windowWidth="21270" windowHeight="13634" tabRatio="564" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1110" yWindow="100" windowWidth="21270" windowHeight="13630" tabRatio="564"/>
   </bookViews>
   <sheets>
     <sheet name="transitions" sheetId="3" r:id="rId1"/>
@@ -359,7 +353,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -541,7 +535,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -574,26 +568,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -626,23 +603,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -818,23 +778,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AF13" sqref="AF13"/>
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.06640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.73046875" customWidth="1"/>
-    <col min="5" max="5" width="9.73046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="12" width="9.73046875" customWidth="1"/>
-    <col min="13" max="13" width="9.9296875" bestFit="1" customWidth="1"/>
-    <col min="14" max="34" width="9.73046875" customWidth="1"/>
+    <col min="1" max="1" width="10.08984375" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" customWidth="1"/>
+    <col min="5" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="9.7265625" customWidth="1"/>
+    <col min="13" max="13" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="34" width="9.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -939,7 +899,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -1043,7 +1003,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
         <v>71</v>
       </c>
@@ -1147,7 +1107,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A4" s="6" t="s">
         <v>72</v>
       </c>
@@ -1251,7 +1211,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A5" s="6" t="s">
         <v>1</v>
       </c>
@@ -1355,7 +1315,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A6" s="6" t="s">
         <v>2</v>
       </c>
@@ -1459,7 +1419,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A7" s="6" t="s">
         <v>76</v>
       </c>
@@ -1563,7 +1523,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A8" s="6" t="s">
         <v>3</v>
       </c>
@@ -1667,7 +1627,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A9" s="6" t="s">
         <v>4</v>
       </c>
@@ -1771,7 +1731,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A10" s="6" t="s">
         <v>5</v>
       </c>
@@ -1875,7 +1835,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
         <v>6</v>
       </c>
@@ -1979,7 +1939,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A12" s="6" t="s">
         <v>7</v>
       </c>
@@ -2083,7 +2043,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
         <v>8</v>
       </c>
@@ -2129,8 +2089,8 @@
       <c r="O13" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="P13" s="3" t="s">
-        <v>65</v>
+      <c r="P13" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="Q13" s="2" t="s">
         <v>8</v>
@@ -2187,7 +2147,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
         <v>73</v>
       </c>
@@ -2291,7 +2251,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A15" s="6" t="s">
         <v>9</v>
       </c>
@@ -2395,7 +2355,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A16" s="6" t="s">
         <v>10</v>
       </c>
@@ -2499,7 +2459,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A17" s="6" t="s">
         <v>11</v>
       </c>
@@ -2603,7 +2563,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A18" s="6" t="s">
         <v>12</v>
       </c>
@@ -2707,7 +2667,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A19" s="6" t="s">
         <v>13</v>
       </c>
@@ -2811,7 +2771,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A20" s="6" t="s">
         <v>88</v>
       </c>
@@ -2915,7 +2875,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A21" s="6" t="s">
         <v>14</v>
       </c>
@@ -3019,7 +2979,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A22" s="6" t="s">
         <v>15</v>
       </c>
@@ -3123,7 +3083,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A23" s="6" t="s">
         <v>16</v>
       </c>
@@ -3227,7 +3187,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A24" s="6" t="s">
         <v>17</v>
       </c>
@@ -3331,7 +3291,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A25" s="6" t="s">
         <v>18</v>
       </c>
@@ -3435,7 +3395,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A26" s="6" t="s">
         <v>19</v>
       </c>
@@ -3539,7 +3499,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A27" s="6" t="s">
         <v>20</v>
       </c>
@@ -3643,7 +3603,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A28" s="6" t="s">
         <v>21</v>
       </c>
@@ -3747,7 +3707,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A29" s="6" t="s">
         <v>23</v>
       </c>
@@ -3851,7 +3811,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A30" s="6" t="s">
         <v>24</v>
       </c>
@@ -3955,7 +3915,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A31" s="6" t="s">
         <v>25</v>
       </c>
@@ -4059,7 +4019,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A32" s="6" t="s">
         <v>26</v>
       </c>
@@ -4163,7 +4123,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="33" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A33" s="6" t="s">
         <v>27</v>
       </c>
@@ -4267,7 +4227,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A34" s="6" t="s">
         <v>28</v>
       </c>
@@ -4371,7 +4331,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="35" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A35" s="6" t="s">
         <v>29</v>
       </c>
@@ -4475,7 +4435,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A36" s="6" t="s">
         <v>30</v>
       </c>
@@ -4579,7 +4539,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="37" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A37" s="6" t="s">
         <v>31</v>
       </c>
@@ -4683,7 +4643,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="38" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A38" s="6" t="s">
         <v>32</v>
       </c>
@@ -4787,7 +4747,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="39" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A39" s="6" t="s">
         <v>33</v>
       </c>
@@ -4891,7 +4851,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="40" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A40" s="6" t="s">
         <v>98</v>
       </c>
@@ -4995,7 +4955,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="41" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A41" s="6" t="s">
         <v>34</v>
       </c>
@@ -5099,7 +5059,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="42" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A42" s="6" t="s">
         <v>22</v>
       </c>
@@ -5210,19 +5170,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.9296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.06640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.19921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -5243,7 +5203,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
         <v>106</v>
       </c>
@@ -5263,7 +5223,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
         <v>105</v>
       </c>
@@ -5283,7 +5243,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A4" s="6" t="s">
         <v>109</v>
       </c>
@@ -5303,7 +5263,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A5" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FEAT: preliminary support for scanning path! values.
</commit_message>
<xml_diff>
--- a/docs/lexer/lexer-FSM.xlsx
+++ b/docs/lexer/lexer-FSM.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1518" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1620" uniqueCount="116">
   <si>
     <t>S_START</t>
   </si>
@@ -354,6 +354,15 @@
   </si>
   <si>
     <t>S_FILE_STR</t>
+  </si>
+  <si>
+    <t>S_PATH</t>
+  </si>
+  <si>
+    <t>S_PATH_NUM</t>
+  </si>
+  <si>
+    <t>S_PATH_WORD</t>
   </si>
 </sst>
 </file>
@@ -414,7 +423,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -424,6 +433,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -451,7 +466,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -479,6 +494,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -785,11 +803,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH44"/>
+  <dimension ref="A1:AH47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L8" sqref="L8"/>
+      <selection pane="topRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -905,8 +923,8 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -2881,7 +2899,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="21" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A21" s="6" t="s">
         <v>12</v>
       </c>
@@ -3817,7 +3835,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A30" s="6" t="s">
         <v>20</v>
       </c>
@@ -3860,8 +3878,8 @@
       <c r="N30" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="O30" s="3" t="s">
-        <v>64</v>
+      <c r="O30" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="P30" s="3" t="s">
         <v>64</v>
@@ -4025,7 +4043,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="32" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A32" s="6" t="s">
         <v>23</v>
       </c>
@@ -4068,8 +4086,8 @@
       <c r="N32" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="O32" s="3" t="s">
-        <v>64</v>
+      <c r="O32" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="P32" s="3" t="s">
         <v>64</v>
@@ -4129,7 +4147,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A33" s="6" t="s">
         <v>24</v>
       </c>
@@ -4172,8 +4190,8 @@
       <c r="N33" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="O33" s="3" t="s">
-        <v>64</v>
+      <c r="O33" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="P33" s="3" t="s">
         <v>64</v>
@@ -5375,6 +5393,318 @@
       </c>
       <c r="AH44" s="1" t="s">
         <v>98</v>
+      </c>
+    </row>
+    <row r="45" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A45" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J45" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="K45" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="L45" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M45" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N45" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="O45" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="P45" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q45" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="R45" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="S45" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="T45" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="U45" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="V45" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="W45" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="X45" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y45" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z45" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA45" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AB45" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC45" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD45" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE45" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AF45" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AG45" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AH45" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="46" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A46" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="L46" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="M46" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N46" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O46" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="P46" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q46" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="R46" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="S46" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="T46" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="U46" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="V46" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="W46" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="X46" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y46" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z46" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA46" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB46" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC46" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD46" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE46" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF46" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG46" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AH46" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="47" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A47" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="L47" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="M47" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="N47" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="O47" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="P47" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q47" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="R47" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="S47" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="T47" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="U47" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="V47" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="W47" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="X47" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y47" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z47" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA47" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AB47" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC47" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AD47" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AE47" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AF47" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AG47" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AH47" s="1" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FIX: C_SIGN lexical class was not leading to terminal states on reaching delimiters.
</commit_message>
<xml_diff>
--- a/docs/lexer/lexer-FSM.xlsx
+++ b/docs/lexer/lexer-FSM.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Red\docs\lexer\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB8DCC6D-EBF8-4D93-8AB7-022EA2A6F7AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1110" yWindow="100" windowWidth="21270" windowHeight="13630" tabRatio="564"/>
+    <workbookView xWindow="1110" yWindow="98" windowWidth="21270" windowHeight="13634" tabRatio="564" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="transitions" sheetId="3" r:id="rId1"/>
@@ -368,7 +374,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -559,7 +565,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -592,9 +598,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -627,6 +650,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -802,23 +842,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B2" sqref="B2"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Y40" sqref="Y40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.08984375" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" customWidth="1"/>
-    <col min="5" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="12" width="9.7265625" customWidth="1"/>
-    <col min="13" max="13" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="14" max="34" width="9.7265625" customWidth="1"/>
+    <col min="1" max="1" width="10.06640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.73046875" customWidth="1"/>
+    <col min="5" max="5" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="9.73046875" customWidth="1"/>
+    <col min="13" max="13" width="9.9296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="34" width="9.73046875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -923,7 +963,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
@@ -1027,7 +1067,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
         <v>70</v>
       </c>
@@ -1131,7 +1171,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A4" s="6" t="s">
         <v>71</v>
       </c>
@@ -1235,7 +1275,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A5" s="6" t="s">
         <v>1</v>
       </c>
@@ -1339,7 +1379,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A6" s="6" t="s">
         <v>2</v>
       </c>
@@ -1443,7 +1483,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A7" s="6" t="s">
         <v>75</v>
       </c>
@@ -1547,7 +1587,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A8" s="6" t="s">
         <v>3</v>
       </c>
@@ -1651,7 +1691,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A9" s="6" t="s">
         <v>4</v>
       </c>
@@ -1755,7 +1795,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A10" s="6" t="s">
         <v>110</v>
       </c>
@@ -1859,7 +1899,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
         <v>111</v>
       </c>
@@ -1963,7 +2003,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A12" s="6" t="s">
         <v>112</v>
       </c>
@@ -2067,7 +2107,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A13" s="6" t="s">
         <v>5</v>
       </c>
@@ -2171,7 +2211,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
         <v>6</v>
       </c>
@@ -2275,7 +2315,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A15" s="6" t="s">
         <v>7</v>
       </c>
@@ -2379,7 +2419,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A16" s="6" t="s">
         <v>72</v>
       </c>
@@ -2483,7 +2523,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A17" s="6" t="s">
         <v>8</v>
       </c>
@@ -2587,7 +2627,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A18" s="6" t="s">
         <v>9</v>
       </c>
@@ -2691,7 +2731,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A19" s="6" t="s">
         <v>10</v>
       </c>
@@ -2795,7 +2835,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A20" s="6" t="s">
         <v>11</v>
       </c>
@@ -2899,7 +2939,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A21" s="6" t="s">
         <v>12</v>
       </c>
@@ -3003,7 +3043,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A22" s="6" t="s">
         <v>87</v>
       </c>
@@ -3107,7 +3147,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A23" s="6" t="s">
         <v>13</v>
       </c>
@@ -3211,7 +3251,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="24" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A24" s="6" t="s">
         <v>14</v>
       </c>
@@ -3315,7 +3355,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A25" s="6" t="s">
         <v>15</v>
       </c>
@@ -3419,7 +3459,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A26" s="6" t="s">
         <v>16</v>
       </c>
@@ -3523,7 +3563,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A27" s="6" t="s">
         <v>17</v>
       </c>
@@ -3627,7 +3667,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A28" s="6" t="s">
         <v>18</v>
       </c>
@@ -3731,7 +3771,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A29" s="6" t="s">
         <v>19</v>
       </c>
@@ -3835,7 +3875,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A30" s="6" t="s">
         <v>20</v>
       </c>
@@ -3939,7 +3979,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="31" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A31" s="6" t="s">
         <v>22</v>
       </c>
@@ -4043,7 +4083,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A32" s="6" t="s">
         <v>23</v>
       </c>
@@ -4147,7 +4187,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A33" s="6" t="s">
         <v>24</v>
       </c>
@@ -4251,7 +4291,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A34" s="6" t="s">
         <v>25</v>
       </c>
@@ -4355,7 +4395,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="35" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A35" s="6" t="s">
         <v>26</v>
       </c>
@@ -4459,7 +4499,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A36" s="6" t="s">
         <v>27</v>
       </c>
@@ -4563,7 +4603,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A37" s="6" t="s">
         <v>28</v>
       </c>
@@ -4667,7 +4707,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="38" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A38" s="6" t="s">
         <v>29</v>
       </c>
@@ -4771,7 +4811,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A39" s="6" t="s">
         <v>30</v>
       </c>
@@ -4875,15 +4915,15 @@
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A40" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>32</v>
+      <c r="B40" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>12</v>
@@ -4891,26 +4931,26 @@
       <c r="E40" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F40" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="I40" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="J40" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="K40" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="L40" s="2" t="s">
-        <v>32</v>
+      <c r="F40" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="L40" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="M40" s="3" t="s">
         <v>64</v>
@@ -4933,8 +4973,8 @@
       <c r="S40" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="T40" s="2" t="s">
-        <v>32</v>
+      <c r="T40" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="U40" s="3" t="s">
         <v>64</v>
@@ -4948,8 +4988,8 @@
       <c r="X40" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Y40" s="2" t="s">
-        <v>32</v>
+      <c r="Y40" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="Z40" s="2" t="s">
         <v>32</v>
@@ -4979,7 +5019,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="41" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A41" s="6" t="s">
         <v>32</v>
       </c>
@@ -5083,7 +5123,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="42" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A42" s="6" t="s">
         <v>97</v>
       </c>
@@ -5187,7 +5227,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="43" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A43" s="6" t="s">
         <v>33</v>
       </c>
@@ -5291,7 +5331,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="44" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A44" s="6" t="s">
         <v>21</v>
       </c>
@@ -5395,7 +5435,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="45" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A45" s="11" t="s">
         <v>113</v>
       </c>
@@ -5499,7 +5539,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="46" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A46" s="6" t="s">
         <v>114</v>
       </c>
@@ -5603,7 +5643,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="47" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A47" s="6" t="s">
         <v>115</v>
       </c>
@@ -5714,19 +5754,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="8.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.9296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.06640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -5747,7 +5787,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
         <v>105</v>
       </c>
@@ -5767,7 +5807,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
         <v>104</v>
       </c>
@@ -5787,7 +5827,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="6" t="s">
         <v>108</v>
       </c>
@@ -5807,7 +5847,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FEAT: completes any-path! support in lexer.
</commit_message>
<xml_diff>
--- a/docs/lexer/lexer-FSM.xlsx
+++ b/docs/lexer/lexer-FSM.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Red\docs\lexer\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB8DCC6D-EBF8-4D93-8AB7-022EA2A6F7AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1110" yWindow="98" windowWidth="21270" windowHeight="13634" tabRatio="564" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1110" yWindow="100" windowWidth="21270" windowHeight="13630" tabRatio="564"/>
   </bookViews>
   <sheets>
     <sheet name="transitions" sheetId="3" r:id="rId1"/>
@@ -374,7 +368,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -565,7 +559,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -598,26 +592,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -650,23 +627,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -842,23 +802,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Y40" sqref="Y40"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S30" sqref="S30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.06640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.73046875" customWidth="1"/>
-    <col min="5" max="5" width="9.73046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="12" width="9.73046875" customWidth="1"/>
-    <col min="13" max="13" width="9.9296875" bestFit="1" customWidth="1"/>
-    <col min="14" max="34" width="9.73046875" customWidth="1"/>
+    <col min="1" max="1" width="10.08984375" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" customWidth="1"/>
+    <col min="5" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="9.7265625" customWidth="1"/>
+    <col min="13" max="13" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="34" width="9.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -963,7 +923,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
@@ -1067,7 +1027,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
         <v>70</v>
       </c>
@@ -1171,7 +1131,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A4" s="6" t="s">
         <v>71</v>
       </c>
@@ -1275,7 +1235,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A5" s="6" t="s">
         <v>1</v>
       </c>
@@ -1379,7 +1339,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A6" s="6" t="s">
         <v>2</v>
       </c>
@@ -1483,7 +1443,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A7" s="6" t="s">
         <v>75</v>
       </c>
@@ -1587,7 +1547,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A8" s="6" t="s">
         <v>3</v>
       </c>
@@ -1691,7 +1651,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A9" s="6" t="s">
         <v>4</v>
       </c>
@@ -1795,7 +1755,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A10" s="6" t="s">
         <v>110</v>
       </c>
@@ -1899,7 +1859,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
         <v>111</v>
       </c>
@@ -2003,7 +1963,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A12" s="6" t="s">
         <v>112</v>
       </c>
@@ -2107,7 +2067,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A13" s="6" t="s">
         <v>5</v>
       </c>
@@ -2211,7 +2171,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
         <v>6</v>
       </c>
@@ -2315,7 +2275,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A15" s="6" t="s">
         <v>7</v>
       </c>
@@ -2419,7 +2379,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A16" s="6" t="s">
         <v>72</v>
       </c>
@@ -2523,7 +2483,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A17" s="6" t="s">
         <v>8</v>
       </c>
@@ -2627,7 +2587,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A18" s="6" t="s">
         <v>9</v>
       </c>
@@ -2731,7 +2691,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A19" s="6" t="s">
         <v>10</v>
       </c>
@@ -2835,7 +2795,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A20" s="6" t="s">
         <v>11</v>
       </c>
@@ -2939,7 +2899,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A21" s="6" t="s">
         <v>12</v>
       </c>
@@ -3043,7 +3003,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A22" s="6" t="s">
         <v>87</v>
       </c>
@@ -3147,7 +3107,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A23" s="6" t="s">
         <v>13</v>
       </c>
@@ -3251,7 +3211,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A24" s="6" t="s">
         <v>14</v>
       </c>
@@ -3355,7 +3315,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A25" s="6" t="s">
         <v>15</v>
       </c>
@@ -3459,7 +3419,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A26" s="6" t="s">
         <v>16</v>
       </c>
@@ -3563,7 +3523,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A27" s="6" t="s">
         <v>17</v>
       </c>
@@ -3667,7 +3627,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A28" s="6" t="s">
         <v>18</v>
       </c>
@@ -3771,7 +3731,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A29" s="6" t="s">
         <v>19</v>
       </c>
@@ -3875,7 +3835,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A30" s="6" t="s">
         <v>20</v>
       </c>
@@ -3930,8 +3890,8 @@
       <c r="R30" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="S30" s="3" t="s">
-        <v>64</v>
+      <c r="S30" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="T30" s="3" t="s">
         <v>64</v>
@@ -3979,7 +3939,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A31" s="6" t="s">
         <v>22</v>
       </c>
@@ -4083,7 +4043,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A32" s="6" t="s">
         <v>23</v>
       </c>
@@ -4187,7 +4147,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A33" s="6" t="s">
         <v>24</v>
       </c>
@@ -4291,7 +4251,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A34" s="6" t="s">
         <v>25</v>
       </c>
@@ -4395,7 +4355,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="35" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A35" s="6" t="s">
         <v>26</v>
       </c>
@@ -4499,7 +4459,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A36" s="6" t="s">
         <v>27</v>
       </c>
@@ -4603,7 +4563,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A37" s="6" t="s">
         <v>28</v>
       </c>
@@ -4707,7 +4667,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="38" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A38" s="6" t="s">
         <v>29</v>
       </c>
@@ -4811,7 +4771,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A39" s="6" t="s">
         <v>30</v>
       </c>
@@ -4915,7 +4875,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A40" s="6" t="s">
         <v>31</v>
       </c>
@@ -5019,7 +4979,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="41" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A41" s="6" t="s">
         <v>32</v>
       </c>
@@ -5123,7 +5083,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="42" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A42" s="6" t="s">
         <v>97</v>
       </c>
@@ -5227,7 +5187,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="43" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A43" s="6" t="s">
         <v>33</v>
       </c>
@@ -5331,7 +5291,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="44" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A44" s="6" t="s">
         <v>21</v>
       </c>
@@ -5435,7 +5395,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="45" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A45" s="11" t="s">
         <v>113</v>
       </c>
@@ -5539,7 +5499,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="46" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A46" s="6" t="s">
         <v>114</v>
       </c>
@@ -5643,7 +5603,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="47" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A47" s="6" t="s">
         <v>115</v>
       </c>
@@ -5686,8 +5646,8 @@
       <c r="N47" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="O47" s="2" t="s">
-        <v>97</v>
+      <c r="O47" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="P47" s="2" t="s">
         <v>115</v>
@@ -5754,19 +5714,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.9296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.06640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.19921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -5787,7 +5747,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
         <v>105</v>
       </c>
@@ -5807,7 +5767,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
         <v>104</v>
       </c>
@@ -5827,7 +5787,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A4" s="6" t="s">
         <v>108</v>
       </c>
@@ -5847,7 +5807,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A5" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FEAT: adds extra path states for accurate handling of supported element types.
</commit_message>
<xml_diff>
--- a/docs/lexer/lexer-FSM.xlsx
+++ b/docs/lexer/lexer-FSM.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1620" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1688" uniqueCount="118">
   <si>
     <t>S_START</t>
   </si>
@@ -363,6 +363,12 @@
   </si>
   <si>
     <t>S_PATH_WORD</t>
+  </si>
+  <si>
+    <t>S_PATH_SHARP</t>
+  </si>
+  <si>
+    <t>S_PATH_SIGN</t>
   </si>
 </sst>
 </file>
@@ -803,16 +809,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH47"/>
+  <dimension ref="A1:AH49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S30" sqref="S30"/>
+      <selection pane="bottomLeft" activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.08984375" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.36328125" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.7265625" customWidth="1"/>
     <col min="5" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
@@ -5433,7 +5439,7 @@
         <v>71</v>
       </c>
       <c r="M45" s="2" t="s">
-        <v>6</v>
+        <v>116</v>
       </c>
       <c r="N45" s="2" t="s">
         <v>115</v>
@@ -5481,7 +5487,7 @@
         <v>64</v>
       </c>
       <c r="AC45" s="2" t="s">
-        <v>31</v>
+        <v>117</v>
       </c>
       <c r="AD45" s="3" t="s">
         <v>64</v>
@@ -5499,7 +5505,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="46" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A46" s="6" t="s">
         <v>114</v>
       </c>
@@ -5536,8 +5542,8 @@
       <c r="L46" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="M46" s="2" t="s">
-        <v>6</v>
+      <c r="M46" s="3" t="s">
+        <v>64</v>
       </c>
       <c r="N46" s="2" t="s">
         <v>12</v>
@@ -5704,6 +5710,214 @@
         <v>64</v>
       </c>
       <c r="AH47" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="48" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A48" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H48" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I48" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J48" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="K48" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="L48" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M48" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N48" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O48" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="P48" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q48" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="R48" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="S48" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="T48" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="U48" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="V48" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="W48" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="X48" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y48" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="Z48" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AA48" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB48" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC48" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD48" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE48" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF48" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AG48" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AH48" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="49" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A49" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="L49" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="M49" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="N49" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="O49" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="P49" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q49" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="R49" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="S49" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="T49" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="U49" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="V49" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="W49" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="X49" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y49" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z49" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA49" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB49" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC49" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD49" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE49" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF49" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AG49" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AH49" s="1" t="s">
         <v>76</v>
       </c>
     </row>

</xml_diff>

<commit_message>
FEAT: defines character classes for the date! lexer.
</commit_message>
<xml_diff>
--- a/docs/lexer/lexer-FSM.xlsx
+++ b/docs/lexer/lexer-FSM.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1110" yWindow="100" windowWidth="21270" windowHeight="13630" tabRatio="564"/>
+    <workbookView xWindow="1110" yWindow="100" windowWidth="21270" windowHeight="13630" tabRatio="564" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="transitions" sheetId="3" r:id="rId1"/>
-    <sheet name="bin16 transitions" sheetId="4" r:id="rId2"/>
+    <sheet name="date! transitions" sheetId="5" r:id="rId2"/>
+    <sheet name="bin16 transitions" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1688" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1754" uniqueCount="177">
   <si>
     <t>S_START</t>
   </si>
@@ -369,6 +370,183 @@
   </si>
   <si>
     <t>S_PATH_SIGN</t>
+  </si>
+  <si>
+    <t>C_DT_DIGIT</t>
+  </si>
+  <si>
+    <t>C_DT_ALPHA</t>
+  </si>
+  <si>
+    <t>C_DT_SLASH</t>
+  </si>
+  <si>
+    <t>C_DT_DASH</t>
+  </si>
+  <si>
+    <t>C_DT_PLUS</t>
+  </si>
+  <si>
+    <t>C_DT_COLON</t>
+  </si>
+  <si>
+    <t>C_DT_DOT</t>
+  </si>
+  <si>
+    <t>C_DT_T</t>
+  </si>
+  <si>
+    <t>C_DT_W</t>
+  </si>
+  <si>
+    <t>C_DT_Z</t>
+  </si>
+  <si>
+    <t>C_DT_ILLEGAL</t>
+  </si>
+  <si>
+    <t>C_DT_EOF</t>
+  </si>
+  <si>
+    <t>S_DT_START</t>
+  </si>
+  <si>
+    <t>S_DT_D</t>
+  </si>
+  <si>
+    <t>S_DT_DD</t>
+  </si>
+  <si>
+    <t>S_DT_YYY</t>
+  </si>
+  <si>
+    <t>F_DT_YEARL</t>
+  </si>
+  <si>
+    <t>F_DT_YEAR2</t>
+  </si>
+  <si>
+    <t>F_DT_DAYL</t>
+  </si>
+  <si>
+    <t>S_DT_YM</t>
+  </si>
+  <si>
+    <t>S_DT_YMM</t>
+  </si>
+  <si>
+    <t>F_DT_YMONTH</t>
+  </si>
+  <si>
+    <t>F_DT_DDD</t>
+  </si>
+  <si>
+    <t>S_DT_YV</t>
+  </si>
+  <si>
+    <t>S_DT_YW</t>
+  </si>
+  <si>
+    <t>S_DT_YWW</t>
+  </si>
+  <si>
+    <t>F_DT_WEEK</t>
+  </si>
+  <si>
+    <t>S_DT_W</t>
+  </si>
+  <si>
+    <t>S_DT_WW</t>
+  </si>
+  <si>
+    <t>F_DT_YWW</t>
+  </si>
+  <si>
+    <t>S_DT_WD</t>
+  </si>
+  <si>
+    <t>F_DT_YWWD</t>
+  </si>
+  <si>
+    <t>S_DT_YMON</t>
+  </si>
+  <si>
+    <t>S_DT_YMD</t>
+  </si>
+  <si>
+    <t>S_DT_YMDD</t>
+  </si>
+  <si>
+    <t>F_DT_YMDAY</t>
+  </si>
+  <si>
+    <t>S_DT_DM</t>
+  </si>
+  <si>
+    <t>S_DT_DMM</t>
+  </si>
+  <si>
+    <t>F_DT_DMONTH</t>
+  </si>
+  <si>
+    <t>S_DT_DMON</t>
+  </si>
+  <si>
+    <t>S_DT_DMY</t>
+  </si>
+  <si>
+    <t>S_DT_DMYY</t>
+  </si>
+  <si>
+    <t>S_DT_DMYYY</t>
+  </si>
+  <si>
+    <t>S_DT_DMYYYY</t>
+  </si>
+  <si>
+    <t>F_DT_DMYEAR</t>
+  </si>
+  <si>
+    <t>S_TM_START</t>
+  </si>
+  <si>
+    <t>S_TM_H</t>
+  </si>
+  <si>
+    <t>F_TM_HH</t>
+  </si>
+  <si>
+    <t>S_TM_M</t>
+  </si>
+  <si>
+    <t>F_TM_MM</t>
+  </si>
+  <si>
+    <t>S_TM_S</t>
+  </si>
+  <si>
+    <t>F_TM_SS</t>
+  </si>
+  <si>
+    <t>S_TM_N</t>
+  </si>
+  <si>
+    <t>F_TM_NNN</t>
+  </si>
+  <si>
+    <t>S_TZ_START</t>
+  </si>
+  <si>
+    <t>S_TZ_H</t>
+  </si>
+  <si>
+    <t>F_TZ_HH</t>
+  </si>
+  <si>
+    <t>S_TZ_M</t>
+  </si>
+  <si>
+    <t>F_TZ_MM</t>
   </si>
 </sst>
 </file>
@@ -449,7 +627,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -468,11 +646,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -502,7 +711,19 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -811,9 +1032,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E49" sqref="E49"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -827,7 +1048,7 @@
     <col min="14" max="34" width="9.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="8"/>
       <c r="B1" s="7" t="s">
         <v>37</v>
@@ -929,7 +1150,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
@@ -1033,8 +1254,8 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A3" s="12" t="s">
         <v>70</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1137,8 +1358,8 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A4" s="12" t="s">
         <v>71</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -1241,8 +1462,8 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A5" s="6" t="s">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A5" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -1345,8 +1566,8 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A6" s="6" t="s">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A6" s="12" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -1449,8 +1670,8 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A7" s="6" t="s">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A7" s="12" t="s">
         <v>75</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -1553,8 +1774,8 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A8" s="12" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1657,8 +1878,8 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A9" s="6" t="s">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A9" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1761,8 +1982,8 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A10" s="6" t="s">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A10" s="12" t="s">
         <v>110</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -1865,8 +2086,8 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A11" s="6" t="s">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A11" s="12" t="s">
         <v>111</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -1969,8 +2190,8 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A12" s="6" t="s">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A12" s="12" t="s">
         <v>112</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -2073,8 +2294,8 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A13" s="6" t="s">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A13" s="12" t="s">
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -2177,8 +2398,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A14" s="6" t="s">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A14" s="12" t="s">
         <v>6</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -2281,8 +2502,8 @@
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A15" s="6" t="s">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A15" s="12" t="s">
         <v>7</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -2385,8 +2606,8 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A16" s="6" t="s">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A16" s="12" t="s">
         <v>72</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -2489,8 +2710,8 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A17" s="6" t="s">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A17" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -2593,8 +2814,8 @@
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A18" s="6" t="s">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A18" s="12" t="s">
         <v>9</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -2697,8 +2918,8 @@
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A19" s="6" t="s">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A19" s="12" t="s">
         <v>10</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -2801,8 +3022,8 @@
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A20" s="6" t="s">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A20" s="12" t="s">
         <v>11</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -2905,8 +3126,8 @@
         <v>84</v>
       </c>
     </row>
-    <row r="21" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A21" s="6" t="s">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A21" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -3009,8 +3230,8 @@
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A22" s="6" t="s">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A22" s="12" t="s">
         <v>87</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -3113,8 +3334,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A23" s="6" t="s">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A23" s="12" t="s">
         <v>13</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -3217,8 +3438,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="24" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A24" s="6" t="s">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A24" s="12" t="s">
         <v>14</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -3321,8 +3542,8 @@
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A25" s="6" t="s">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A25" s="12" t="s">
         <v>15</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -3425,8 +3646,8 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A26" s="6" t="s">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A26" s="12" t="s">
         <v>16</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -3529,8 +3750,8 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A27" s="6" t="s">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A27" s="12" t="s">
         <v>17</v>
       </c>
       <c r="B27" s="3" t="s">
@@ -3633,8 +3854,8 @@
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A28" s="6" t="s">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A28" s="12" t="s">
         <v>18</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -3737,8 +3958,8 @@
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A29" s="6" t="s">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="B29" s="3" t="s">
@@ -3842,7 +4063,7 @@
       </c>
     </row>
     <row r="30" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="12" t="s">
         <v>20</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -3945,8 +4166,8 @@
         <v>92</v>
       </c>
     </row>
-    <row r="31" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A31" s="6" t="s">
+    <row r="31" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A31" s="12" t="s">
         <v>22</v>
       </c>
       <c r="B31" s="3" t="s">
@@ -4049,8 +4270,8 @@
         <v>64</v>
       </c>
     </row>
-    <row r="32" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A32" s="6" t="s">
+    <row r="32" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A32" s="12" t="s">
         <v>23</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -4153,8 +4374,8 @@
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A33" s="6" t="s">
+    <row r="33" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A33" s="12" t="s">
         <v>24</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -4257,8 +4478,8 @@
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A34" s="6" t="s">
+    <row r="34" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A34" s="12" t="s">
         <v>25</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -4361,8 +4582,8 @@
         <v>76</v>
       </c>
     </row>
-    <row r="35" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A35" s="6" t="s">
+    <row r="35" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A35" s="12" t="s">
         <v>26</v>
       </c>
       <c r="B35" s="2" t="s">
@@ -4465,8 +4686,8 @@
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A36" s="6" t="s">
+    <row r="36" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A36" s="12" t="s">
         <v>27</v>
       </c>
       <c r="B36" s="2" t="s">
@@ -4569,8 +4790,8 @@
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A37" s="6" t="s">
+    <row r="37" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A37" s="12" t="s">
         <v>28</v>
       </c>
       <c r="B37" s="2" t="s">
@@ -4673,8 +4894,8 @@
         <v>64</v>
       </c>
     </row>
-    <row r="38" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A38" s="6" t="s">
+    <row r="38" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A38" s="12" t="s">
         <v>29</v>
       </c>
       <c r="B38" s="2" t="s">
@@ -4777,8 +4998,8 @@
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A39" s="6" t="s">
+    <row r="39" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A39" s="12" t="s">
         <v>30</v>
       </c>
       <c r="B39" s="2" t="s">
@@ -4881,8 +5102,8 @@
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A40" s="6" t="s">
+    <row r="40" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A40" s="12" t="s">
         <v>31</v>
       </c>
       <c r="B40" s="1" t="s">
@@ -4985,8 +5206,8 @@
         <v>76</v>
       </c>
     </row>
-    <row r="41" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A41" s="6" t="s">
+    <row r="41" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A41" s="12" t="s">
         <v>32</v>
       </c>
       <c r="B41" s="1" t="s">
@@ -5089,8 +5310,8 @@
         <v>76</v>
       </c>
     </row>
-    <row r="42" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A42" s="6" t="s">
+    <row r="42" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A42" s="12" t="s">
         <v>97</v>
       </c>
       <c r="B42" s="1" t="s">
@@ -5193,8 +5414,8 @@
         <v>76</v>
       </c>
     </row>
-    <row r="43" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A43" s="6" t="s">
+    <row r="43" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A43" s="12" t="s">
         <v>33</v>
       </c>
       <c r="B43" s="1" t="s">
@@ -5297,8 +5518,8 @@
         <v>95</v>
       </c>
     </row>
-    <row r="44" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A44" s="6" t="s">
+    <row r="44" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A44" s="12" t="s">
         <v>21</v>
       </c>
       <c r="B44" s="1" t="s">
@@ -5401,8 +5622,8 @@
         <v>98</v>
       </c>
     </row>
-    <row r="45" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A45" s="11" t="s">
+    <row r="45" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A45" s="13" t="s">
         <v>113</v>
       </c>
       <c r="B45" s="3" t="s">
@@ -5506,7 +5727,7 @@
       </c>
     </row>
     <row r="46" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A46" s="6" t="s">
+      <c r="A46" s="12" t="s">
         <v>114</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -5610,7 +5831,7 @@
       </c>
     </row>
     <row r="47" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A47" s="6" t="s">
+      <c r="A47" s="12" t="s">
         <v>115</v>
       </c>
       <c r="B47" s="1" t="s">
@@ -5714,7 +5935,7 @@
       </c>
     </row>
     <row r="48" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A48" s="6" t="s">
+      <c r="A48" s="12" t="s">
         <v>116</v>
       </c>
       <c r="B48" s="1" t="s">
@@ -5818,7 +6039,7 @@
       </c>
     </row>
     <row r="49" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A49" s="6" t="s">
+      <c r="A49" s="12" t="s">
         <v>117</v>
       </c>
       <c r="B49" s="1" t="s">
@@ -5928,6 +6149,1999 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M128"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="14"/>
+      <c r="B1" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A4" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A5" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A6" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A7" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A8" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A9" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A10" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A11" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A12" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A13" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A14" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A15" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A16" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A17" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A18" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A19" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A20" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A21" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A22" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A23" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A24" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A25" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A26" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A27" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A28" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A29" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A30" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A31" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A32" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A33" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A34" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A35" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A36" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A37" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A38" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A39" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+      <c r="M39" s="2"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A40" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A41" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A42" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
+      <c r="M42" s="2"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A43" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A44" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A45" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A46" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+      <c r="L46" s="2"/>
+      <c r="M46" s="2"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A47" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+      <c r="L47" s="2"/>
+      <c r="M47" s="2"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A48" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="2"/>
+      <c r="L48" s="2"/>
+      <c r="M48" s="2"/>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A49" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="K49" s="2"/>
+      <c r="L49" s="2"/>
+      <c r="M49" s="2"/>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A50" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="2"/>
+      <c r="L50" s="2"/>
+      <c r="M50" s="2"/>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+      <c r="K51" s="2"/>
+      <c r="L51" s="2"/>
+      <c r="M51" s="2"/>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2"/>
+      <c r="K52" s="2"/>
+      <c r="L52" s="2"/>
+      <c r="M52" s="2"/>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2"/>
+      <c r="I53" s="2"/>
+      <c r="J53" s="2"/>
+      <c r="K53" s="2"/>
+      <c r="L53" s="2"/>
+      <c r="M53" s="2"/>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2"/>
+      <c r="I54" s="2"/>
+      <c r="J54" s="2"/>
+      <c r="K54" s="2"/>
+      <c r="L54" s="2"/>
+      <c r="M54" s="2"/>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+      <c r="G55" s="2"/>
+      <c r="H55" s="2"/>
+      <c r="I55" s="2"/>
+      <c r="J55" s="2"/>
+      <c r="K55" s="2"/>
+      <c r="L55" s="2"/>
+      <c r="M55" s="2"/>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2"/>
+      <c r="I56" s="2"/>
+      <c r="J56" s="2"/>
+      <c r="K56" s="2"/>
+      <c r="L56" s="2"/>
+      <c r="M56" s="2"/>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B57" s="2"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+      <c r="G57" s="2"/>
+      <c r="H57" s="2"/>
+      <c r="I57" s="2"/>
+      <c r="J57" s="2"/>
+      <c r="K57" s="2"/>
+      <c r="L57" s="2"/>
+      <c r="M57" s="2"/>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+      <c r="G58" s="2"/>
+      <c r="H58" s="2"/>
+      <c r="I58" s="2"/>
+      <c r="J58" s="2"/>
+      <c r="K58" s="2"/>
+      <c r="L58" s="2"/>
+      <c r="M58" s="2"/>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
+      <c r="F59" s="2"/>
+      <c r="G59" s="2"/>
+      <c r="H59" s="2"/>
+      <c r="I59" s="2"/>
+      <c r="J59" s="2"/>
+      <c r="K59" s="2"/>
+      <c r="L59" s="2"/>
+      <c r="M59" s="2"/>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B60" s="2"/>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2"/>
+      <c r="F60" s="2"/>
+      <c r="G60" s="2"/>
+      <c r="H60" s="2"/>
+      <c r="I60" s="2"/>
+      <c r="J60" s="2"/>
+      <c r="K60" s="2"/>
+      <c r="L60" s="2"/>
+      <c r="M60" s="2"/>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B61" s="2"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
+      <c r="F61" s="2"/>
+      <c r="G61" s="2"/>
+      <c r="H61" s="2"/>
+      <c r="I61" s="2"/>
+      <c r="J61" s="2"/>
+      <c r="K61" s="2"/>
+      <c r="L61" s="2"/>
+      <c r="M61" s="2"/>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B62" s="2"/>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="2"/>
+      <c r="F62" s="2"/>
+      <c r="G62" s="2"/>
+      <c r="H62" s="2"/>
+      <c r="I62" s="2"/>
+      <c r="J62" s="2"/>
+      <c r="K62" s="2"/>
+      <c r="L62" s="2"/>
+      <c r="M62" s="2"/>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B63" s="2"/>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="2"/>
+      <c r="G63" s="2"/>
+      <c r="H63" s="2"/>
+      <c r="I63" s="2"/>
+      <c r="J63" s="2"/>
+      <c r="K63" s="2"/>
+      <c r="L63" s="2"/>
+      <c r="M63" s="2"/>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B64" s="2"/>
+      <c r="C64" s="2"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
+      <c r="G64" s="2"/>
+      <c r="H64" s="2"/>
+      <c r="I64" s="2"/>
+      <c r="J64" s="2"/>
+      <c r="K64" s="2"/>
+      <c r="L64" s="2"/>
+      <c r="M64" s="2"/>
+    </row>
+    <row r="65" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B65" s="2"/>
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+      <c r="G65" s="2"/>
+      <c r="H65" s="2"/>
+      <c r="I65" s="2"/>
+      <c r="J65" s="2"/>
+      <c r="K65" s="2"/>
+      <c r="L65" s="2"/>
+      <c r="M65" s="2"/>
+    </row>
+    <row r="66" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B66" s="2"/>
+      <c r="C66" s="2"/>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2"/>
+      <c r="F66" s="2"/>
+      <c r="G66" s="2"/>
+      <c r="H66" s="2"/>
+      <c r="I66" s="2"/>
+      <c r="J66" s="2"/>
+      <c r="K66" s="2"/>
+      <c r="L66" s="2"/>
+      <c r="M66" s="2"/>
+    </row>
+    <row r="67" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B67" s="2"/>
+      <c r="C67" s="2"/>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2"/>
+      <c r="F67" s="2"/>
+      <c r="G67" s="2"/>
+      <c r="H67" s="2"/>
+      <c r="I67" s="2"/>
+      <c r="J67" s="2"/>
+      <c r="K67" s="2"/>
+      <c r="L67" s="2"/>
+      <c r="M67" s="2"/>
+    </row>
+    <row r="68" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B68" s="2"/>
+      <c r="C68" s="2"/>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2"/>
+      <c r="F68" s="2"/>
+      <c r="G68" s="2"/>
+      <c r="H68" s="2"/>
+      <c r="I68" s="2"/>
+      <c r="J68" s="2"/>
+      <c r="K68" s="2"/>
+      <c r="L68" s="2"/>
+      <c r="M68" s="2"/>
+    </row>
+    <row r="69" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B69" s="2"/>
+      <c r="C69" s="2"/>
+      <c r="D69" s="2"/>
+      <c r="E69" s="2"/>
+      <c r="F69" s="2"/>
+      <c r="G69" s="2"/>
+      <c r="H69" s="2"/>
+      <c r="I69" s="2"/>
+      <c r="J69" s="2"/>
+      <c r="K69" s="2"/>
+      <c r="L69" s="2"/>
+      <c r="M69" s="2"/>
+    </row>
+    <row r="70" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B70" s="2"/>
+      <c r="C70" s="2"/>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2"/>
+      <c r="F70" s="2"/>
+      <c r="G70" s="2"/>
+      <c r="H70" s="2"/>
+      <c r="I70" s="2"/>
+      <c r="J70" s="2"/>
+      <c r="K70" s="2"/>
+      <c r="L70" s="2"/>
+      <c r="M70" s="2"/>
+    </row>
+    <row r="71" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B71" s="2"/>
+      <c r="C71" s="2"/>
+      <c r="D71" s="2"/>
+      <c r="E71" s="2"/>
+      <c r="F71" s="2"/>
+      <c r="G71" s="2"/>
+      <c r="H71" s="2"/>
+      <c r="I71" s="2"/>
+      <c r="J71" s="2"/>
+      <c r="K71" s="2"/>
+      <c r="L71" s="2"/>
+      <c r="M71" s="2"/>
+    </row>
+    <row r="72" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B72" s="2"/>
+      <c r="C72" s="2"/>
+      <c r="D72" s="2"/>
+      <c r="E72" s="2"/>
+      <c r="F72" s="2"/>
+      <c r="G72" s="2"/>
+      <c r="H72" s="2"/>
+      <c r="I72" s="2"/>
+      <c r="J72" s="2"/>
+      <c r="K72" s="2"/>
+      <c r="L72" s="2"/>
+      <c r="M72" s="2"/>
+    </row>
+    <row r="73" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B73" s="2"/>
+      <c r="C73" s="2"/>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
+      <c r="G73" s="2"/>
+      <c r="H73" s="2"/>
+      <c r="I73" s="2"/>
+      <c r="J73" s="2"/>
+      <c r="K73" s="2"/>
+      <c r="L73" s="2"/>
+      <c r="M73" s="2"/>
+    </row>
+    <row r="74" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B74" s="2"/>
+      <c r="C74" s="2"/>
+      <c r="D74" s="2"/>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
+      <c r="G74" s="2"/>
+      <c r="H74" s="2"/>
+      <c r="I74" s="2"/>
+      <c r="J74" s="2"/>
+      <c r="K74" s="2"/>
+      <c r="L74" s="2"/>
+      <c r="M74" s="2"/>
+    </row>
+    <row r="75" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B75" s="2"/>
+      <c r="C75" s="2"/>
+      <c r="D75" s="2"/>
+      <c r="E75" s="2"/>
+      <c r="F75" s="2"/>
+      <c r="G75" s="2"/>
+      <c r="H75" s="2"/>
+      <c r="I75" s="2"/>
+      <c r="J75" s="2"/>
+      <c r="K75" s="2"/>
+      <c r="L75" s="2"/>
+      <c r="M75" s="2"/>
+    </row>
+    <row r="76" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B76" s="2"/>
+      <c r="C76" s="2"/>
+      <c r="D76" s="2"/>
+      <c r="E76" s="2"/>
+      <c r="F76" s="2"/>
+      <c r="G76" s="2"/>
+      <c r="H76" s="2"/>
+      <c r="I76" s="2"/>
+      <c r="J76" s="2"/>
+      <c r="K76" s="2"/>
+      <c r="L76" s="2"/>
+      <c r="M76" s="2"/>
+    </row>
+    <row r="77" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B77" s="2"/>
+      <c r="C77" s="2"/>
+      <c r="D77" s="2"/>
+      <c r="E77" s="2"/>
+      <c r="F77" s="2"/>
+      <c r="G77" s="2"/>
+      <c r="H77" s="2"/>
+      <c r="I77" s="2"/>
+      <c r="J77" s="2"/>
+      <c r="K77" s="2"/>
+      <c r="L77" s="2"/>
+      <c r="M77" s="2"/>
+    </row>
+    <row r="78" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B78" s="2"/>
+      <c r="C78" s="2"/>
+      <c r="D78" s="2"/>
+      <c r="E78" s="2"/>
+      <c r="F78" s="2"/>
+      <c r="G78" s="2"/>
+      <c r="H78" s="2"/>
+      <c r="I78" s="2"/>
+      <c r="J78" s="2"/>
+      <c r="K78" s="2"/>
+      <c r="L78" s="2"/>
+      <c r="M78" s="2"/>
+    </row>
+    <row r="79" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B79" s="2"/>
+      <c r="C79" s="2"/>
+      <c r="D79" s="2"/>
+      <c r="E79" s="2"/>
+      <c r="F79" s="2"/>
+      <c r="G79" s="2"/>
+      <c r="H79" s="2"/>
+      <c r="I79" s="2"/>
+      <c r="J79" s="2"/>
+      <c r="K79" s="2"/>
+      <c r="L79" s="2"/>
+      <c r="M79" s="2"/>
+    </row>
+    <row r="80" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B80" s="2"/>
+      <c r="C80" s="2"/>
+      <c r="D80" s="2"/>
+      <c r="E80" s="2"/>
+      <c r="F80" s="2"/>
+      <c r="G80" s="2"/>
+      <c r="H80" s="2"/>
+      <c r="I80" s="2"/>
+      <c r="J80" s="2"/>
+      <c r="K80" s="2"/>
+      <c r="L80" s="2"/>
+      <c r="M80" s="2"/>
+    </row>
+    <row r="81" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B81" s="2"/>
+      <c r="C81" s="2"/>
+      <c r="D81" s="2"/>
+      <c r="E81" s="2"/>
+      <c r="F81" s="2"/>
+      <c r="G81" s="2"/>
+      <c r="H81" s="2"/>
+      <c r="I81" s="2"/>
+      <c r="J81" s="2"/>
+      <c r="K81" s="2"/>
+      <c r="L81" s="2"/>
+      <c r="M81" s="2"/>
+    </row>
+    <row r="82" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B82" s="2"/>
+      <c r="C82" s="2"/>
+      <c r="D82" s="2"/>
+      <c r="E82" s="2"/>
+      <c r="F82" s="2"/>
+      <c r="G82" s="2"/>
+      <c r="H82" s="2"/>
+      <c r="I82" s="2"/>
+      <c r="J82" s="2"/>
+      <c r="K82" s="2"/>
+      <c r="L82" s="2"/>
+      <c r="M82" s="2"/>
+    </row>
+    <row r="83" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B83" s="2"/>
+      <c r="C83" s="2"/>
+      <c r="D83" s="2"/>
+      <c r="E83" s="2"/>
+      <c r="F83" s="2"/>
+      <c r="G83" s="2"/>
+      <c r="H83" s="2"/>
+      <c r="I83" s="2"/>
+      <c r="J83" s="2"/>
+      <c r="K83" s="2"/>
+      <c r="L83" s="2"/>
+      <c r="M83" s="2"/>
+    </row>
+    <row r="84" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B84" s="2"/>
+      <c r="C84" s="2"/>
+      <c r="D84" s="2"/>
+      <c r="E84" s="2"/>
+      <c r="F84" s="2"/>
+      <c r="G84" s="2"/>
+      <c r="H84" s="2"/>
+      <c r="I84" s="2"/>
+      <c r="J84" s="2"/>
+      <c r="K84" s="2"/>
+      <c r="L84" s="2"/>
+      <c r="M84" s="2"/>
+    </row>
+    <row r="85" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B85" s="2"/>
+      <c r="C85" s="2"/>
+      <c r="D85" s="2"/>
+      <c r="E85" s="2"/>
+      <c r="F85" s="2"/>
+      <c r="G85" s="2"/>
+      <c r="H85" s="2"/>
+      <c r="I85" s="2"/>
+      <c r="J85" s="2"/>
+      <c r="K85" s="2"/>
+      <c r="L85" s="2"/>
+      <c r="M85" s="2"/>
+    </row>
+    <row r="86" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B86" s="2"/>
+      <c r="C86" s="2"/>
+      <c r="D86" s="2"/>
+      <c r="E86" s="2"/>
+      <c r="F86" s="2"/>
+      <c r="G86" s="2"/>
+      <c r="H86" s="2"/>
+      <c r="I86" s="2"/>
+      <c r="J86" s="2"/>
+      <c r="K86" s="2"/>
+      <c r="L86" s="2"/>
+      <c r="M86" s="2"/>
+    </row>
+    <row r="87" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B87" s="2"/>
+      <c r="C87" s="2"/>
+      <c r="D87" s="2"/>
+      <c r="E87" s="2"/>
+      <c r="F87" s="2"/>
+      <c r="G87" s="2"/>
+      <c r="H87" s="2"/>
+      <c r="I87" s="2"/>
+      <c r="J87" s="2"/>
+      <c r="K87" s="2"/>
+      <c r="L87" s="2"/>
+      <c r="M87" s="2"/>
+    </row>
+    <row r="88" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B88" s="2"/>
+      <c r="C88" s="2"/>
+      <c r="D88" s="2"/>
+      <c r="E88" s="2"/>
+      <c r="F88" s="2"/>
+      <c r="G88" s="2"/>
+      <c r="H88" s="2"/>
+      <c r="I88" s="2"/>
+      <c r="J88" s="2"/>
+      <c r="K88" s="2"/>
+      <c r="L88" s="2"/>
+      <c r="M88" s="2"/>
+    </row>
+    <row r="89" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B89" s="2"/>
+      <c r="C89" s="2"/>
+      <c r="D89" s="2"/>
+      <c r="E89" s="2"/>
+      <c r="F89" s="2"/>
+      <c r="G89" s="2"/>
+      <c r="H89" s="2"/>
+      <c r="I89" s="2"/>
+      <c r="J89" s="2"/>
+      <c r="K89" s="2"/>
+      <c r="L89" s="2"/>
+      <c r="M89" s="2"/>
+    </row>
+    <row r="90" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B90" s="2"/>
+      <c r="C90" s="2"/>
+      <c r="D90" s="2"/>
+      <c r="E90" s="2"/>
+      <c r="F90" s="2"/>
+      <c r="G90" s="2"/>
+      <c r="H90" s="2"/>
+      <c r="I90" s="2"/>
+      <c r="J90" s="2"/>
+      <c r="K90" s="2"/>
+      <c r="L90" s="2"/>
+      <c r="M90" s="2"/>
+    </row>
+    <row r="91" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B91" s="2"/>
+      <c r="C91" s="2"/>
+      <c r="D91" s="2"/>
+      <c r="E91" s="2"/>
+      <c r="F91" s="2"/>
+      <c r="G91" s="2"/>
+      <c r="H91" s="2"/>
+      <c r="I91" s="2"/>
+      <c r="J91" s="2"/>
+      <c r="K91" s="2"/>
+      <c r="L91" s="2"/>
+      <c r="M91" s="2"/>
+    </row>
+    <row r="92" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B92" s="2"/>
+      <c r="C92" s="2"/>
+      <c r="D92" s="2"/>
+      <c r="E92" s="2"/>
+      <c r="F92" s="2"/>
+      <c r="G92" s="2"/>
+      <c r="H92" s="2"/>
+      <c r="I92" s="2"/>
+      <c r="J92" s="2"/>
+      <c r="K92" s="2"/>
+      <c r="L92" s="2"/>
+      <c r="M92" s="2"/>
+    </row>
+    <row r="93" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B93" s="2"/>
+      <c r="C93" s="2"/>
+      <c r="D93" s="2"/>
+      <c r="E93" s="2"/>
+      <c r="F93" s="2"/>
+      <c r="G93" s="2"/>
+      <c r="H93" s="2"/>
+      <c r="I93" s="2"/>
+      <c r="J93" s="2"/>
+      <c r="K93" s="2"/>
+      <c r="L93" s="2"/>
+      <c r="M93" s="2"/>
+    </row>
+    <row r="94" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B94" s="2"/>
+      <c r="C94" s="2"/>
+      <c r="D94" s="2"/>
+      <c r="E94" s="2"/>
+      <c r="F94" s="2"/>
+      <c r="G94" s="2"/>
+      <c r="H94" s="2"/>
+      <c r="I94" s="2"/>
+      <c r="J94" s="2"/>
+      <c r="K94" s="2"/>
+      <c r="L94" s="2"/>
+      <c r="M94" s="2"/>
+    </row>
+    <row r="95" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B95" s="2"/>
+      <c r="C95" s="2"/>
+      <c r="D95" s="2"/>
+      <c r="E95" s="2"/>
+      <c r="F95" s="2"/>
+      <c r="G95" s="2"/>
+      <c r="H95" s="2"/>
+      <c r="I95" s="2"/>
+      <c r="J95" s="2"/>
+      <c r="K95" s="2"/>
+      <c r="L95" s="2"/>
+      <c r="M95" s="2"/>
+    </row>
+    <row r="96" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B96" s="2"/>
+      <c r="C96" s="2"/>
+      <c r="D96" s="2"/>
+      <c r="E96" s="2"/>
+      <c r="F96" s="2"/>
+      <c r="G96" s="2"/>
+      <c r="H96" s="2"/>
+      <c r="I96" s="2"/>
+      <c r="J96" s="2"/>
+      <c r="K96" s="2"/>
+      <c r="L96" s="2"/>
+      <c r="M96" s="2"/>
+    </row>
+    <row r="97" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B97" s="2"/>
+      <c r="C97" s="2"/>
+      <c r="D97" s="2"/>
+      <c r="E97" s="2"/>
+      <c r="F97" s="2"/>
+      <c r="G97" s="2"/>
+      <c r="H97" s="2"/>
+      <c r="I97" s="2"/>
+      <c r="J97" s="2"/>
+      <c r="K97" s="2"/>
+      <c r="L97" s="2"/>
+      <c r="M97" s="2"/>
+    </row>
+    <row r="98" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B98" s="2"/>
+      <c r="C98" s="2"/>
+      <c r="D98" s="2"/>
+      <c r="E98" s="2"/>
+      <c r="F98" s="2"/>
+      <c r="G98" s="2"/>
+      <c r="H98" s="2"/>
+      <c r="I98" s="2"/>
+      <c r="J98" s="2"/>
+      <c r="K98" s="2"/>
+      <c r="L98" s="2"/>
+      <c r="M98" s="2"/>
+    </row>
+    <row r="99" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B99" s="2"/>
+      <c r="C99" s="2"/>
+      <c r="D99" s="2"/>
+      <c r="E99" s="2"/>
+      <c r="F99" s="2"/>
+      <c r="G99" s="2"/>
+      <c r="H99" s="2"/>
+      <c r="I99" s="2"/>
+      <c r="J99" s="2"/>
+      <c r="K99" s="2"/>
+      <c r="L99" s="2"/>
+      <c r="M99" s="2"/>
+    </row>
+    <row r="100" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B100" s="2"/>
+      <c r="C100" s="2"/>
+      <c r="D100" s="2"/>
+      <c r="E100" s="2"/>
+      <c r="F100" s="2"/>
+      <c r="G100" s="2"/>
+      <c r="H100" s="2"/>
+      <c r="I100" s="2"/>
+      <c r="J100" s="2"/>
+      <c r="K100" s="2"/>
+      <c r="L100" s="2"/>
+      <c r="M100" s="2"/>
+    </row>
+    <row r="101" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B101" s="2"/>
+      <c r="C101" s="2"/>
+      <c r="D101" s="2"/>
+      <c r="E101" s="2"/>
+      <c r="F101" s="2"/>
+      <c r="G101" s="2"/>
+      <c r="H101" s="2"/>
+      <c r="I101" s="2"/>
+      <c r="J101" s="2"/>
+      <c r="K101" s="2"/>
+      <c r="L101" s="2"/>
+      <c r="M101" s="2"/>
+    </row>
+    <row r="102" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B102" s="2"/>
+      <c r="C102" s="2"/>
+      <c r="D102" s="2"/>
+      <c r="E102" s="2"/>
+      <c r="F102" s="2"/>
+      <c r="G102" s="2"/>
+      <c r="H102" s="2"/>
+      <c r="I102" s="2"/>
+      <c r="J102" s="2"/>
+      <c r="K102" s="2"/>
+      <c r="L102" s="2"/>
+      <c r="M102" s="2"/>
+    </row>
+    <row r="103" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B103" s="2"/>
+      <c r="C103" s="2"/>
+      <c r="D103" s="2"/>
+      <c r="E103" s="2"/>
+      <c r="F103" s="2"/>
+      <c r="G103" s="2"/>
+      <c r="H103" s="2"/>
+      <c r="I103" s="2"/>
+      <c r="J103" s="2"/>
+      <c r="K103" s="2"/>
+      <c r="L103" s="2"/>
+      <c r="M103" s="2"/>
+    </row>
+    <row r="104" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B104" s="2"/>
+      <c r="C104" s="2"/>
+      <c r="D104" s="2"/>
+      <c r="E104" s="2"/>
+      <c r="F104" s="2"/>
+      <c r="G104" s="2"/>
+      <c r="H104" s="2"/>
+      <c r="I104" s="2"/>
+      <c r="J104" s="2"/>
+      <c r="K104" s="2"/>
+      <c r="L104" s="2"/>
+      <c r="M104" s="2"/>
+    </row>
+    <row r="105" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B105" s="2"/>
+      <c r="C105" s="2"/>
+      <c r="D105" s="2"/>
+      <c r="E105" s="2"/>
+      <c r="F105" s="2"/>
+      <c r="G105" s="2"/>
+      <c r="H105" s="2"/>
+      <c r="I105" s="2"/>
+      <c r="J105" s="2"/>
+      <c r="K105" s="2"/>
+      <c r="L105" s="2"/>
+      <c r="M105" s="2"/>
+    </row>
+    <row r="106" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B106" s="2"/>
+      <c r="C106" s="2"/>
+      <c r="D106" s="2"/>
+      <c r="E106" s="2"/>
+      <c r="F106" s="2"/>
+      <c r="G106" s="2"/>
+      <c r="H106" s="2"/>
+      <c r="I106" s="2"/>
+      <c r="J106" s="2"/>
+      <c r="K106" s="2"/>
+      <c r="L106" s="2"/>
+      <c r="M106" s="2"/>
+    </row>
+    <row r="107" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B107" s="2"/>
+      <c r="C107" s="2"/>
+      <c r="D107" s="2"/>
+      <c r="E107" s="2"/>
+      <c r="F107" s="2"/>
+      <c r="G107" s="2"/>
+      <c r="H107" s="2"/>
+      <c r="I107" s="2"/>
+      <c r="J107" s="2"/>
+      <c r="K107" s="2"/>
+      <c r="L107" s="2"/>
+      <c r="M107" s="2"/>
+    </row>
+    <row r="108" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B108" s="2"/>
+      <c r="C108" s="2"/>
+      <c r="D108" s="2"/>
+      <c r="E108" s="2"/>
+      <c r="F108" s="2"/>
+      <c r="G108" s="2"/>
+      <c r="H108" s="2"/>
+      <c r="I108" s="2"/>
+      <c r="J108" s="2"/>
+      <c r="K108" s="2"/>
+      <c r="L108" s="2"/>
+      <c r="M108" s="2"/>
+    </row>
+    <row r="109" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B109" s="2"/>
+      <c r="C109" s="2"/>
+      <c r="D109" s="2"/>
+      <c r="E109" s="2"/>
+      <c r="F109" s="2"/>
+      <c r="G109" s="2"/>
+      <c r="H109" s="2"/>
+      <c r="I109" s="2"/>
+      <c r="J109" s="2"/>
+      <c r="K109" s="2"/>
+      <c r="L109" s="2"/>
+      <c r="M109" s="2"/>
+    </row>
+    <row r="110" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B110" s="2"/>
+      <c r="C110" s="2"/>
+      <c r="D110" s="2"/>
+      <c r="E110" s="2"/>
+      <c r="F110" s="2"/>
+      <c r="G110" s="2"/>
+      <c r="H110" s="2"/>
+      <c r="I110" s="2"/>
+      <c r="J110" s="2"/>
+      <c r="K110" s="2"/>
+      <c r="L110" s="2"/>
+      <c r="M110" s="2"/>
+    </row>
+    <row r="111" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B111" s="2"/>
+      <c r="C111" s="2"/>
+      <c r="D111" s="2"/>
+      <c r="E111" s="2"/>
+      <c r="F111" s="2"/>
+      <c r="G111" s="2"/>
+      <c r="H111" s="2"/>
+      <c r="I111" s="2"/>
+      <c r="J111" s="2"/>
+      <c r="K111" s="2"/>
+      <c r="L111" s="2"/>
+      <c r="M111" s="2"/>
+    </row>
+    <row r="112" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B112" s="2"/>
+      <c r="C112" s="2"/>
+      <c r="D112" s="2"/>
+      <c r="E112" s="2"/>
+      <c r="F112" s="2"/>
+      <c r="G112" s="2"/>
+      <c r="H112" s="2"/>
+      <c r="I112" s="2"/>
+      <c r="J112" s="2"/>
+      <c r="K112" s="2"/>
+      <c r="L112" s="2"/>
+      <c r="M112" s="2"/>
+    </row>
+    <row r="113" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B113" s="2"/>
+      <c r="C113" s="2"/>
+      <c r="D113" s="2"/>
+      <c r="E113" s="2"/>
+      <c r="F113" s="2"/>
+      <c r="G113" s="2"/>
+      <c r="H113" s="2"/>
+      <c r="I113" s="2"/>
+      <c r="J113" s="2"/>
+      <c r="K113" s="2"/>
+      <c r="L113" s="2"/>
+      <c r="M113" s="2"/>
+    </row>
+    <row r="114" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B114" s="2"/>
+      <c r="C114" s="2"/>
+      <c r="D114" s="2"/>
+      <c r="E114" s="2"/>
+      <c r="F114" s="2"/>
+      <c r="G114" s="2"/>
+      <c r="H114" s="2"/>
+      <c r="I114" s="2"/>
+      <c r="J114" s="2"/>
+      <c r="K114" s="2"/>
+      <c r="L114" s="2"/>
+      <c r="M114" s="2"/>
+    </row>
+    <row r="115" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B115" s="2"/>
+      <c r="C115" s="2"/>
+      <c r="D115" s="2"/>
+      <c r="E115" s="2"/>
+      <c r="F115" s="2"/>
+      <c r="G115" s="2"/>
+      <c r="H115" s="2"/>
+      <c r="I115" s="2"/>
+      <c r="J115" s="2"/>
+      <c r="K115" s="2"/>
+      <c r="L115" s="2"/>
+      <c r="M115" s="2"/>
+    </row>
+    <row r="116" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B116" s="2"/>
+      <c r="C116" s="2"/>
+      <c r="D116" s="2"/>
+      <c r="E116" s="2"/>
+      <c r="F116" s="2"/>
+      <c r="G116" s="2"/>
+      <c r="H116" s="2"/>
+      <c r="I116" s="2"/>
+      <c r="J116" s="2"/>
+      <c r="K116" s="2"/>
+      <c r="L116" s="2"/>
+      <c r="M116" s="2"/>
+    </row>
+    <row r="117" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B117" s="2"/>
+      <c r="C117" s="2"/>
+      <c r="D117" s="2"/>
+      <c r="E117" s="2"/>
+      <c r="F117" s="2"/>
+      <c r="G117" s="2"/>
+      <c r="H117" s="2"/>
+      <c r="I117" s="2"/>
+      <c r="J117" s="2"/>
+      <c r="K117" s="2"/>
+      <c r="L117" s="2"/>
+      <c r="M117" s="2"/>
+    </row>
+    <row r="118" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B118" s="2"/>
+      <c r="C118" s="2"/>
+      <c r="D118" s="2"/>
+      <c r="E118" s="2"/>
+      <c r="F118" s="2"/>
+      <c r="G118" s="2"/>
+      <c r="H118" s="2"/>
+      <c r="I118" s="2"/>
+      <c r="J118" s="2"/>
+      <c r="K118" s="2"/>
+      <c r="L118" s="2"/>
+      <c r="M118" s="2"/>
+    </row>
+    <row r="119" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B119" s="2"/>
+      <c r="C119" s="2"/>
+      <c r="D119" s="2"/>
+      <c r="E119" s="2"/>
+      <c r="F119" s="2"/>
+      <c r="G119" s="2"/>
+      <c r="H119" s="2"/>
+      <c r="I119" s="2"/>
+      <c r="J119" s="2"/>
+      <c r="K119" s="2"/>
+      <c r="L119" s="2"/>
+      <c r="M119" s="2"/>
+    </row>
+    <row r="120" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B120" s="2"/>
+      <c r="C120" s="2"/>
+      <c r="D120" s="2"/>
+      <c r="E120" s="2"/>
+      <c r="F120" s="2"/>
+      <c r="G120" s="2"/>
+      <c r="H120" s="2"/>
+      <c r="I120" s="2"/>
+      <c r="J120" s="2"/>
+      <c r="K120" s="2"/>
+      <c r="L120" s="2"/>
+      <c r="M120" s="2"/>
+    </row>
+    <row r="121" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B121" s="2"/>
+      <c r="C121" s="2"/>
+      <c r="D121" s="2"/>
+      <c r="E121" s="2"/>
+      <c r="F121" s="2"/>
+      <c r="G121" s="2"/>
+      <c r="H121" s="2"/>
+      <c r="I121" s="2"/>
+      <c r="J121" s="2"/>
+      <c r="K121" s="2"/>
+      <c r="L121" s="2"/>
+      <c r="M121" s="2"/>
+    </row>
+    <row r="122" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B122" s="2"/>
+      <c r="C122" s="2"/>
+      <c r="D122" s="2"/>
+      <c r="E122" s="2"/>
+      <c r="F122" s="2"/>
+      <c r="G122" s="2"/>
+      <c r="H122" s="2"/>
+      <c r="I122" s="2"/>
+      <c r="J122" s="2"/>
+      <c r="K122" s="2"/>
+      <c r="L122" s="2"/>
+      <c r="M122" s="2"/>
+    </row>
+    <row r="123" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B123" s="2"/>
+      <c r="C123" s="2"/>
+      <c r="D123" s="2"/>
+      <c r="E123" s="2"/>
+      <c r="F123" s="2"/>
+      <c r="G123" s="2"/>
+      <c r="H123" s="2"/>
+      <c r="I123" s="2"/>
+      <c r="J123" s="2"/>
+      <c r="K123" s="2"/>
+      <c r="L123" s="2"/>
+      <c r="M123" s="2"/>
+    </row>
+    <row r="124" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B124" s="2"/>
+      <c r="C124" s="2"/>
+      <c r="D124" s="2"/>
+      <c r="E124" s="2"/>
+      <c r="F124" s="2"/>
+      <c r="G124" s="2"/>
+      <c r="H124" s="2"/>
+      <c r="I124" s="2"/>
+      <c r="J124" s="2"/>
+      <c r="K124" s="2"/>
+      <c r="L124" s="2"/>
+      <c r="M124" s="2"/>
+    </row>
+    <row r="125" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B125" s="2"/>
+      <c r="C125" s="2"/>
+      <c r="D125" s="2"/>
+      <c r="E125" s="2"/>
+      <c r="F125" s="2"/>
+      <c r="G125" s="2"/>
+      <c r="H125" s="2"/>
+      <c r="I125" s="2"/>
+      <c r="J125" s="2"/>
+      <c r="K125" s="2"/>
+      <c r="L125" s="2"/>
+      <c r="M125" s="2"/>
+    </row>
+    <row r="126" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B126" s="2"/>
+      <c r="C126" s="2"/>
+      <c r="D126" s="2"/>
+      <c r="E126" s="2"/>
+      <c r="F126" s="2"/>
+      <c r="G126" s="2"/>
+      <c r="H126" s="2"/>
+      <c r="I126" s="2"/>
+      <c r="J126" s="2"/>
+      <c r="K126" s="2"/>
+      <c r="L126" s="2"/>
+      <c r="M126" s="2"/>
+    </row>
+    <row r="127" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B127" s="2"/>
+      <c r="C127" s="2"/>
+      <c r="D127" s="2"/>
+      <c r="E127" s="2"/>
+      <c r="F127" s="2"/>
+      <c r="G127" s="2"/>
+      <c r="H127" s="2"/>
+      <c r="I127" s="2"/>
+      <c r="J127" s="2"/>
+      <c r="K127" s="2"/>
+      <c r="L127" s="2"/>
+      <c r="M127" s="2"/>
+    </row>
+    <row r="128" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B128" s="2"/>
+      <c r="C128" s="2"/>
+      <c r="D128" s="2"/>
+      <c r="E128" s="2"/>
+      <c r="F128" s="2"/>
+      <c r="G128" s="2"/>
+      <c r="H128" s="2"/>
+      <c r="I128" s="2"/>
+      <c r="J128" s="2"/>
+      <c r="K128" s="2"/>
+      <c r="L128" s="2"/>
+      <c r="M128" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>

</xml_diff>

<commit_message>
FEAT: various fixes and improvements to date! parsing FSM.
</commit_message>
<xml_diff>
--- a/docs/lexer/lexer-FSM.xlsx
+++ b/docs/lexer/lexer-FSM.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Red\docs\lexer\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{519605FB-0D00-448F-BE8A-3770BAF54A9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1110" yWindow="100" windowWidth="21270" windowHeight="13630" tabRatio="564" activeTab="1"/>
+    <workbookView xWindow="1035" yWindow="105" windowWidth="21270" windowHeight="13635" tabRatio="564" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="transitions" sheetId="3" r:id="rId1"/>
@@ -15,8 +21,43 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>dk</author>
+  </authors>
+  <commentList>
+    <comment ref="D6" authorId="0" shapeId="0" xr:uid="{960FFBA6-8FB5-44E2-B372-614E04387ADE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>dk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+ FIXME: /////...
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1754" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1810" uniqueCount="175">
   <si>
     <t>S_START</t>
   </si>
@@ -375,9 +416,6 @@
     <t>C_DT_DIGIT</t>
   </si>
   <si>
-    <t>C_DT_ALPHA</t>
-  </si>
-  <si>
     <t>C_DT_SLASH</t>
   </si>
   <si>
@@ -453,15 +491,6 @@
     <t>F_DT_WEEK</t>
   </si>
   <si>
-    <t>S_DT_W</t>
-  </si>
-  <si>
-    <t>S_DT_WW</t>
-  </si>
-  <si>
-    <t>F_DT_YWW</t>
-  </si>
-  <si>
     <t>S_DT_WD</t>
   </si>
   <si>
@@ -547,13 +576,19 @@
   </si>
   <si>
     <t>F_TZ_MM</t>
+  </si>
+  <si>
+    <t>F_DT_YEARL2</t>
+  </si>
+  <si>
+    <t>C_DT_LETTER</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -606,8 +641,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -623,6 +671,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -681,7 +735,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -724,6 +778,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -786,7 +843,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -819,9 +876,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -854,6 +928,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1029,7 +1120,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1037,18 +1128,18 @@
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.36328125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" customWidth="1"/>
-    <col min="5" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="12" width="9.7265625" customWidth="1"/>
-    <col min="13" max="13" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="14" max="34" width="9.7265625" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.73046875" customWidth="1"/>
+    <col min="5" max="5" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="9.73046875" customWidth="1"/>
+    <col min="13" max="13" width="9.9296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="34" width="9.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="8"/>
       <c r="B1" s="7" t="s">
         <v>37</v>
@@ -1150,7 +1241,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
@@ -1254,7 +1345,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A3" s="12" t="s">
         <v>70</v>
       </c>
@@ -1358,7 +1449,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A4" s="12" t="s">
         <v>71</v>
       </c>
@@ -1462,7 +1553,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A5" s="12" t="s">
         <v>1</v>
       </c>
@@ -1566,7 +1657,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A6" s="12" t="s">
         <v>2</v>
       </c>
@@ -1670,7 +1761,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A7" s="12" t="s">
         <v>75</v>
       </c>
@@ -1774,7 +1865,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A8" s="12" t="s">
         <v>3</v>
       </c>
@@ -1878,7 +1969,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A9" s="12" t="s">
         <v>4</v>
       </c>
@@ -1982,7 +2073,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A10" s="12" t="s">
         <v>110</v>
       </c>
@@ -2086,7 +2177,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A11" s="12" t="s">
         <v>111</v>
       </c>
@@ -2190,7 +2281,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A12" s="12" t="s">
         <v>112</v>
       </c>
@@ -2294,7 +2385,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A13" s="12" t="s">
         <v>5</v>
       </c>
@@ -2398,7 +2489,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A14" s="12" t="s">
         <v>6</v>
       </c>
@@ -2502,7 +2593,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A15" s="12" t="s">
         <v>7</v>
       </c>
@@ -2606,7 +2697,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A16" s="12" t="s">
         <v>72</v>
       </c>
@@ -2710,7 +2801,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A17" s="12" t="s">
         <v>8</v>
       </c>
@@ -2814,7 +2905,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A18" s="12" t="s">
         <v>9</v>
       </c>
@@ -2918,7 +3009,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A19" s="12" t="s">
         <v>10</v>
       </c>
@@ -3022,7 +3113,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A20" s="12" t="s">
         <v>11</v>
       </c>
@@ -3126,7 +3217,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A21" s="12" t="s">
         <v>12</v>
       </c>
@@ -3230,7 +3321,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A22" s="12" t="s">
         <v>87</v>
       </c>
@@ -3334,7 +3425,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A23" s="12" t="s">
         <v>13</v>
       </c>
@@ -3438,7 +3529,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A24" s="12" t="s">
         <v>14</v>
       </c>
@@ -3542,7 +3633,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A25" s="12" t="s">
         <v>15</v>
       </c>
@@ -3646,7 +3737,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A26" s="12" t="s">
         <v>16</v>
       </c>
@@ -3750,7 +3841,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A27" s="12" t="s">
         <v>17</v>
       </c>
@@ -3854,7 +3945,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A28" s="12" t="s">
         <v>18</v>
       </c>
@@ -3958,7 +4049,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A29" s="12" t="s">
         <v>19</v>
       </c>
@@ -4062,7 +4153,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A30" s="12" t="s">
         <v>20</v>
       </c>
@@ -4166,7 +4257,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A31" s="12" t="s">
         <v>22</v>
       </c>
@@ -4270,7 +4361,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A32" s="12" t="s">
         <v>23</v>
       </c>
@@ -4374,7 +4465,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A33" s="12" t="s">
         <v>24</v>
       </c>
@@ -4478,7 +4569,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A34" s="12" t="s">
         <v>25</v>
       </c>
@@ -4582,7 +4673,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="35" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A35" s="12" t="s">
         <v>26</v>
       </c>
@@ -4686,7 +4777,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A36" s="12" t="s">
         <v>27</v>
       </c>
@@ -4790,7 +4881,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A37" s="12" t="s">
         <v>28</v>
       </c>
@@ -4894,7 +4985,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="38" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A38" s="12" t="s">
         <v>29</v>
       </c>
@@ -4998,7 +5089,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A39" s="12" t="s">
         <v>30</v>
       </c>
@@ -5102,7 +5193,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A40" s="12" t="s">
         <v>31</v>
       </c>
@@ -5206,7 +5297,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="41" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A41" s="12" t="s">
         <v>32</v>
       </c>
@@ -5310,7 +5401,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="42" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A42" s="12" t="s">
         <v>97</v>
       </c>
@@ -5414,7 +5505,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="43" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A43" s="12" t="s">
         <v>33</v>
       </c>
@@ -5518,7 +5609,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="44" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A44" s="12" t="s">
         <v>21</v>
       </c>
@@ -5622,7 +5713,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="45" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A45" s="13" t="s">
         <v>113</v>
       </c>
@@ -5726,7 +5817,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="46" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A46" s="12" t="s">
         <v>114</v>
       </c>
@@ -5830,7 +5921,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="47" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A47" s="12" t="s">
         <v>115</v>
       </c>
@@ -5934,7 +6025,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="48" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A48" s="12" t="s">
         <v>116</v>
       </c>
@@ -6038,7 +6129,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="49" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A49" s="12" t="s">
         <v>117</v>
       </c>
@@ -6149,64 +6240,65 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M128"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:M125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="14"/>
       <c r="B1" s="7" t="s">
         <v>118</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="M1" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="M1" s="7" t="s">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A2" s="13" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A2" s="13" t="s">
+      <c r="B2" s="2" t="s">
         <v>130</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>131</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -6220,16 +6312,20 @@
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>132</v>
-      </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
+      <c r="D3" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>135</v>
+      </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
@@ -6239,16 +6335,20 @@
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>133</v>
-      </c>
       <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>135</v>
+      </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -6258,16 +6358,20 @@
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>134</v>
-      </c>
       <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
@@ -6277,48 +6381,68 @@
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A6" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>146</v>
+      </c>
       <c r="D6" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="E6" s="2"/>
+        <v>133</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>173</v>
+      </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
+      <c r="I6" s="2" t="s">
+        <v>146</v>
+      </c>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A7" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>146</v>
+      </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
+      <c r="I7" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>140</v>
+      </c>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A8" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A8" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>153</v>
+      </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -6330,14 +6454,20 @@
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B9" s="2"/>
       <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>138</v>
+      </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
@@ -6347,14 +6477,20 @@
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>138</v>
+      </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
@@ -6364,11 +6500,13 @@
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A11" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="B11" s="2"/>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A11" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>147</v>
+      </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -6381,9 +6519,9 @@
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A12" s="15" t="s">
-        <v>140</v>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A12" s="16" t="s">
+        <v>139</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -6392,17 +6530,21 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
+      <c r="I12" s="2" t="s">
+        <v>159</v>
+      </c>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -6415,11 +6557,13 @@
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -6430,28 +6574,34 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M14" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="B15" s="2"/>
+        <v>142</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>144</v>
+      </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
+      <c r="I15" s="2" t="s">
+        <v>159</v>
+      </c>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A16" s="15" t="s">
-        <v>144</v>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A16" s="16" t="s">
+        <v>143</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -6466,9 +6616,9 @@
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A17" s="15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -6481,11 +6631,13 @@
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A18" s="15" t="s">
-        <v>146</v>
+      <c r="M17" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A18" s="16" t="s">
+        <v>145</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -6500,14 +6652,20 @@
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A19" s="15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
+      <c r="C19" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>138</v>
+      </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
@@ -6517,14 +6675,20 @@
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A20" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="B20" s="2"/>
       <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
+      <c r="D20" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>149</v>
+      </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
@@ -6532,16 +6696,22 @@
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M20" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A21" s="15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
+      <c r="D21" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>149</v>
+      </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
@@ -6549,33 +6719,45 @@
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A22" s="15" t="s">
-        <v>150</v>
+      <c r="M21" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A22" s="16" t="s">
+        <v>149</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
+      <c r="D22" s="2" t="s">
+        <v>159</v>
+      </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
+      <c r="I22" s="2" t="s">
+        <v>159</v>
+      </c>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A23" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="B23" s="2"/>
       <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
+      <c r="D23" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>152</v>
+      </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
@@ -6585,14 +6767,18 @@
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A24" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
+      <c r="D24" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>152</v>
+      </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
@@ -6602,11 +6788,13 @@
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A25" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="B25" s="2"/>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A25" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>154</v>
+      </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -6619,14 +6807,20 @@
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A26" s="15" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
+      <c r="C26" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>152</v>
+      </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
@@ -6636,11 +6830,13 @@
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A27" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -6651,13 +6847,17 @@
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
-      <c r="M27" s="2"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M27" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A28" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="B28" s="2"/>
+        <v>155</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>155</v>
+      </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -6668,13 +6868,17 @@
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
-      <c r="M28" s="2"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M28" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A29" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="B29" s="2"/>
+        <v>156</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>156</v>
+      </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -6685,15 +6889,19 @@
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
-      <c r="M29" s="2"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M29" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A30" s="15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
+      <c r="D30" s="2" t="s">
+        <v>158</v>
+      </c>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
@@ -6702,11 +6910,13 @@
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
-      <c r="M30" s="2"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A31" s="15" t="s">
-        <v>159</v>
+      <c r="M30" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A31" s="16" t="s">
+        <v>158</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -6721,9 +6931,9 @@
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A32" s="15" t="s">
-        <v>160</v>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A32" s="16" t="s">
+        <v>149</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -6738,9 +6948,9 @@
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A33" s="15" t="s">
-        <v>161</v>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A33" s="13" t="s">
+        <v>159</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -6755,9 +6965,9 @@
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A34" s="15" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -6772,9 +6982,9 @@
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A35" s="15" t="s">
-        <v>153</v>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A35" s="16" t="s">
+        <v>161</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -6789,9 +6999,9 @@
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A36" s="13" t="s">
-        <v>163</v>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A36" s="16" t="s">
+        <v>161</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -6806,9 +7016,9 @@
       <c r="L36" s="2"/>
       <c r="M36" s="2"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A37" s="15" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -6823,9 +7033,9 @@
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A38" s="15" t="s">
-        <v>165</v>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A38" s="16" t="s">
+        <v>163</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -6840,9 +7050,9 @@
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A39" s="15" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -6857,9 +7067,9 @@
       <c r="L39" s="2"/>
       <c r="M39" s="2"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A40" s="15" t="s">
-        <v>166</v>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A40" s="16" t="s">
+        <v>165</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -6874,9 +7084,9 @@
       <c r="L40" s="2"/>
       <c r="M40" s="2"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A41" s="15" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -6891,9 +7101,9 @@
       <c r="L41" s="2"/>
       <c r="M41" s="2"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A42" s="15" t="s">
-        <v>168</v>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A42" s="16" t="s">
+        <v>167</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -6908,9 +7118,9 @@
       <c r="L42" s="2"/>
       <c r="M42" s="2"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A43" s="15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -6925,9 +7135,9 @@
       <c r="L43" s="2"/>
       <c r="M43" s="2"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A44" s="15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -6942,9 +7152,9 @@
       <c r="L44" s="2"/>
       <c r="M44" s="2"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A45" s="15" t="s">
-        <v>171</v>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A45" s="16" t="s">
+        <v>170</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -6959,9 +7169,9 @@
       <c r="L45" s="2"/>
       <c r="M45" s="2"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A46" s="15" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -6976,9 +7186,9 @@
       <c r="L46" s="2"/>
       <c r="M46" s="2"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A47" s="15" t="s">
-        <v>173</v>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A47" s="16" t="s">
+        <v>172</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -6993,10 +7203,7 @@
       <c r="L47" s="2"/>
       <c r="M47" s="2"/>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A48" s="15" t="s">
-        <v>174</v>
-      </c>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.45">
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
@@ -7010,10 +7217,7 @@
       <c r="L48" s="2"/>
       <c r="M48" s="2"/>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A49" s="15" t="s">
-        <v>175</v>
-      </c>
+    <row r="49" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
@@ -7027,10 +7231,7 @@
       <c r="L49" s="2"/>
       <c r="M49" s="2"/>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A50" s="15" t="s">
-        <v>176</v>
-      </c>
+    <row r="50" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
@@ -7044,7 +7245,7 @@
       <c r="L50" s="2"/>
       <c r="M50" s="2"/>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
@@ -7058,7 +7259,7 @@
       <c r="L51" s="2"/>
       <c r="M51" s="2"/>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
@@ -7072,7 +7273,7 @@
       <c r="L52" s="2"/>
       <c r="M52" s="2"/>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
@@ -7086,7 +7287,7 @@
       <c r="L53" s="2"/>
       <c r="M53" s="2"/>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
@@ -7100,7 +7301,7 @@
       <c r="L54" s="2"/>
       <c r="M54" s="2"/>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
@@ -7114,7 +7315,7 @@
       <c r="L55" s="2"/>
       <c r="M55" s="2"/>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
@@ -7128,7 +7329,7 @@
       <c r="L56" s="2"/>
       <c r="M56" s="2"/>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
@@ -7142,7 +7343,7 @@
       <c r="L57" s="2"/>
       <c r="M57" s="2"/>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
@@ -7156,7 +7357,7 @@
       <c r="L58" s="2"/>
       <c r="M58" s="2"/>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
@@ -7170,7 +7371,7 @@
       <c r="L59" s="2"/>
       <c r="M59" s="2"/>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
@@ -7184,7 +7385,7 @@
       <c r="L60" s="2"/>
       <c r="M60" s="2"/>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
@@ -7198,7 +7399,7 @@
       <c r="L61" s="2"/>
       <c r="M61" s="2"/>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
@@ -7212,7 +7413,7 @@
       <c r="L62" s="2"/>
       <c r="M62" s="2"/>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
@@ -7226,7 +7427,7 @@
       <c r="L63" s="2"/>
       <c r="M63" s="2"/>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
@@ -7240,7 +7441,7 @@
       <c r="L64" s="2"/>
       <c r="M64" s="2"/>
     </row>
-    <row r="65" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
@@ -7254,7 +7455,7 @@
       <c r="L65" s="2"/>
       <c r="M65" s="2"/>
     </row>
-    <row r="66" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
@@ -7268,7 +7469,7 @@
       <c r="L66" s="2"/>
       <c r="M66" s="2"/>
     </row>
-    <row r="67" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
@@ -7282,7 +7483,7 @@
       <c r="L67" s="2"/>
       <c r="M67" s="2"/>
     </row>
-    <row r="68" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
@@ -7296,7 +7497,7 @@
       <c r="L68" s="2"/>
       <c r="M68" s="2"/>
     </row>
-    <row r="69" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
@@ -7310,7 +7511,7 @@
       <c r="L69" s="2"/>
       <c r="M69" s="2"/>
     </row>
-    <row r="70" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
@@ -7324,7 +7525,7 @@
       <c r="L70" s="2"/>
       <c r="M70" s="2"/>
     </row>
-    <row r="71" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
@@ -7338,7 +7539,7 @@
       <c r="L71" s="2"/>
       <c r="M71" s="2"/>
     </row>
-    <row r="72" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
@@ -7352,7 +7553,7 @@
       <c r="L72" s="2"/>
       <c r="M72" s="2"/>
     </row>
-    <row r="73" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
@@ -7366,7 +7567,7 @@
       <c r="L73" s="2"/>
       <c r="M73" s="2"/>
     </row>
-    <row r="74" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
@@ -7380,7 +7581,7 @@
       <c r="L74" s="2"/>
       <c r="M74" s="2"/>
     </row>
-    <row r="75" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
@@ -7394,7 +7595,7 @@
       <c r="L75" s="2"/>
       <c r="M75" s="2"/>
     </row>
-    <row r="76" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
       <c r="D76" s="2"/>
@@ -7408,7 +7609,7 @@
       <c r="L76" s="2"/>
       <c r="M76" s="2"/>
     </row>
-    <row r="77" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
       <c r="D77" s="2"/>
@@ -7422,7 +7623,7 @@
       <c r="L77" s="2"/>
       <c r="M77" s="2"/>
     </row>
-    <row r="78" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
       <c r="D78" s="2"/>
@@ -7436,7 +7637,7 @@
       <c r="L78" s="2"/>
       <c r="M78" s="2"/>
     </row>
-    <row r="79" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
       <c r="D79" s="2"/>
@@ -7450,7 +7651,7 @@
       <c r="L79" s="2"/>
       <c r="M79" s="2"/>
     </row>
-    <row r="80" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
       <c r="D80" s="2"/>
@@ -7464,7 +7665,7 @@
       <c r="L80" s="2"/>
       <c r="M80" s="2"/>
     </row>
-    <row r="81" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
       <c r="D81" s="2"/>
@@ -7478,7 +7679,7 @@
       <c r="L81" s="2"/>
       <c r="M81" s="2"/>
     </row>
-    <row r="82" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
       <c r="D82" s="2"/>
@@ -7492,7 +7693,7 @@
       <c r="L82" s="2"/>
       <c r="M82" s="2"/>
     </row>
-    <row r="83" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
       <c r="D83" s="2"/>
@@ -7506,7 +7707,7 @@
       <c r="L83" s="2"/>
       <c r="M83" s="2"/>
     </row>
-    <row r="84" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
       <c r="D84" s="2"/>
@@ -7520,7 +7721,7 @@
       <c r="L84" s="2"/>
       <c r="M84" s="2"/>
     </row>
-    <row r="85" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
       <c r="D85" s="2"/>
@@ -7534,7 +7735,7 @@
       <c r="L85" s="2"/>
       <c r="M85" s="2"/>
     </row>
-    <row r="86" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
       <c r="D86" s="2"/>
@@ -7548,7 +7749,7 @@
       <c r="L86" s="2"/>
       <c r="M86" s="2"/>
     </row>
-    <row r="87" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
       <c r="D87" s="2"/>
@@ -7562,7 +7763,7 @@
       <c r="L87" s="2"/>
       <c r="M87" s="2"/>
     </row>
-    <row r="88" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
       <c r="D88" s="2"/>
@@ -7576,7 +7777,7 @@
       <c r="L88" s="2"/>
       <c r="M88" s="2"/>
     </row>
-    <row r="89" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
       <c r="D89" s="2"/>
@@ -7590,7 +7791,7 @@
       <c r="L89" s="2"/>
       <c r="M89" s="2"/>
     </row>
-    <row r="90" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
       <c r="D90" s="2"/>
@@ -7604,7 +7805,7 @@
       <c r="L90" s="2"/>
       <c r="M90" s="2"/>
     </row>
-    <row r="91" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
       <c r="D91" s="2"/>
@@ -7618,7 +7819,7 @@
       <c r="L91" s="2"/>
       <c r="M91" s="2"/>
     </row>
-    <row r="92" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="92" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
       <c r="D92" s="2"/>
@@ -7632,7 +7833,7 @@
       <c r="L92" s="2"/>
       <c r="M92" s="2"/>
     </row>
-    <row r="93" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
       <c r="D93" s="2"/>
@@ -7646,7 +7847,7 @@
       <c r="L93" s="2"/>
       <c r="M93" s="2"/>
     </row>
-    <row r="94" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="94" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
       <c r="D94" s="2"/>
@@ -7660,7 +7861,7 @@
       <c r="L94" s="2"/>
       <c r="M94" s="2"/>
     </row>
-    <row r="95" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="95" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
       <c r="D95" s="2"/>
@@ -7674,7 +7875,7 @@
       <c r="L95" s="2"/>
       <c r="M95" s="2"/>
     </row>
-    <row r="96" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="96" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
       <c r="D96" s="2"/>
@@ -7688,7 +7889,7 @@
       <c r="L96" s="2"/>
       <c r="M96" s="2"/>
     </row>
-    <row r="97" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="97" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
       <c r="D97" s="2"/>
@@ -7702,7 +7903,7 @@
       <c r="L97" s="2"/>
       <c r="M97" s="2"/>
     </row>
-    <row r="98" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="98" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
       <c r="D98" s="2"/>
@@ -7716,7 +7917,7 @@
       <c r="L98" s="2"/>
       <c r="M98" s="2"/>
     </row>
-    <row r="99" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="99" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
       <c r="D99" s="2"/>
@@ -7730,7 +7931,7 @@
       <c r="L99" s="2"/>
       <c r="M99" s="2"/>
     </row>
-    <row r="100" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
       <c r="D100" s="2"/>
@@ -7744,7 +7945,7 @@
       <c r="L100" s="2"/>
       <c r="M100" s="2"/>
     </row>
-    <row r="101" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="101" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
       <c r="D101" s="2"/>
@@ -7758,7 +7959,7 @@
       <c r="L101" s="2"/>
       <c r="M101" s="2"/>
     </row>
-    <row r="102" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="102" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
       <c r="D102" s="2"/>
@@ -7772,7 +7973,7 @@
       <c r="L102" s="2"/>
       <c r="M102" s="2"/>
     </row>
-    <row r="103" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="103" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
       <c r="D103" s="2"/>
@@ -7786,7 +7987,7 @@
       <c r="L103" s="2"/>
       <c r="M103" s="2"/>
     </row>
-    <row r="104" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
       <c r="D104" s="2"/>
@@ -7800,7 +8001,7 @@
       <c r="L104" s="2"/>
       <c r="M104" s="2"/>
     </row>
-    <row r="105" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="105" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
       <c r="D105" s="2"/>
@@ -7814,7 +8015,7 @@
       <c r="L105" s="2"/>
       <c r="M105" s="2"/>
     </row>
-    <row r="106" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="106" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
       <c r="D106" s="2"/>
@@ -7828,7 +8029,7 @@
       <c r="L106" s="2"/>
       <c r="M106" s="2"/>
     </row>
-    <row r="107" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="107" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
       <c r="D107" s="2"/>
@@ -7842,7 +8043,7 @@
       <c r="L107" s="2"/>
       <c r="M107" s="2"/>
     </row>
-    <row r="108" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="108" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
       <c r="D108" s="2"/>
@@ -7856,7 +8057,7 @@
       <c r="L108" s="2"/>
       <c r="M108" s="2"/>
     </row>
-    <row r="109" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="109" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
       <c r="D109" s="2"/>
@@ -7870,7 +8071,7 @@
       <c r="L109" s="2"/>
       <c r="M109" s="2"/>
     </row>
-    <row r="110" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="110" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
       <c r="D110" s="2"/>
@@ -7884,7 +8085,7 @@
       <c r="L110" s="2"/>
       <c r="M110" s="2"/>
     </row>
-    <row r="111" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="111" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
       <c r="D111" s="2"/>
@@ -7898,7 +8099,7 @@
       <c r="L111" s="2"/>
       <c r="M111" s="2"/>
     </row>
-    <row r="112" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="112" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
       <c r="D112" s="2"/>
@@ -7912,7 +8113,7 @@
       <c r="L112" s="2"/>
       <c r="M112" s="2"/>
     </row>
-    <row r="113" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="113" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
       <c r="D113" s="2"/>
@@ -7926,7 +8127,7 @@
       <c r="L113" s="2"/>
       <c r="M113" s="2"/>
     </row>
-    <row r="114" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="114" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
       <c r="D114" s="2"/>
@@ -7940,7 +8141,7 @@
       <c r="L114" s="2"/>
       <c r="M114" s="2"/>
     </row>
-    <row r="115" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="115" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
       <c r="D115" s="2"/>
@@ -7954,7 +8155,7 @@
       <c r="L115" s="2"/>
       <c r="M115" s="2"/>
     </row>
-    <row r="116" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="116" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
       <c r="D116" s="2"/>
@@ -7968,7 +8169,7 @@
       <c r="L116" s="2"/>
       <c r="M116" s="2"/>
     </row>
-    <row r="117" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="117" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
       <c r="D117" s="2"/>
@@ -7982,7 +8183,7 @@
       <c r="L117" s="2"/>
       <c r="M117" s="2"/>
     </row>
-    <row r="118" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="118" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
       <c r="D118" s="2"/>
@@ -7996,7 +8197,7 @@
       <c r="L118" s="2"/>
       <c r="M118" s="2"/>
     </row>
-    <row r="119" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="119" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
       <c r="D119" s="2"/>
@@ -8010,7 +8211,7 @@
       <c r="L119" s="2"/>
       <c r="M119" s="2"/>
     </row>
-    <row r="120" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="120" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
       <c r="D120" s="2"/>
@@ -8024,7 +8225,7 @@
       <c r="L120" s="2"/>
       <c r="M120" s="2"/>
     </row>
-    <row r="121" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="121" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
       <c r="D121" s="2"/>
@@ -8038,7 +8239,7 @@
       <c r="L121" s="2"/>
       <c r="M121" s="2"/>
     </row>
-    <row r="122" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="122" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
       <c r="D122" s="2"/>
@@ -8052,7 +8253,7 @@
       <c r="L122" s="2"/>
       <c r="M122" s="2"/>
     </row>
-    <row r="123" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="123" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
       <c r="D123" s="2"/>
@@ -8066,7 +8267,7 @@
       <c r="L123" s="2"/>
       <c r="M123" s="2"/>
     </row>
-    <row r="124" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="124" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
       <c r="D124" s="2"/>
@@ -8080,7 +8281,7 @@
       <c r="L124" s="2"/>
       <c r="M124" s="2"/>
     </row>
-    <row r="125" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="125" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
       <c r="D125" s="2"/>
@@ -8094,67 +8295,26 @@
       <c r="L125" s="2"/>
       <c r="M125" s="2"/>
     </row>
-    <row r="126" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B126" s="2"/>
-      <c r="C126" s="2"/>
-      <c r="D126" s="2"/>
-      <c r="E126" s="2"/>
-      <c r="F126" s="2"/>
-      <c r="G126" s="2"/>
-      <c r="H126" s="2"/>
-      <c r="I126" s="2"/>
-      <c r="J126" s="2"/>
-      <c r="K126" s="2"/>
-      <c r="L126" s="2"/>
-      <c r="M126" s="2"/>
-    </row>
-    <row r="127" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B127" s="2"/>
-      <c r="C127" s="2"/>
-      <c r="D127" s="2"/>
-      <c r="E127" s="2"/>
-      <c r="F127" s="2"/>
-      <c r="G127" s="2"/>
-      <c r="H127" s="2"/>
-      <c r="I127" s="2"/>
-      <c r="J127" s="2"/>
-      <c r="K127" s="2"/>
-      <c r="L127" s="2"/>
-      <c r="M127" s="2"/>
-    </row>
-    <row r="128" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B128" s="2"/>
-      <c r="C128" s="2"/>
-      <c r="D128" s="2"/>
-      <c r="E128" s="2"/>
-      <c r="F128" s="2"/>
-      <c r="G128" s="2"/>
-      <c r="H128" s="2"/>
-      <c r="I128" s="2"/>
-      <c r="J128" s="2"/>
-      <c r="K128" s="2"/>
-      <c r="L128" s="2"/>
-      <c r="M128" s="2"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="8.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.9296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.06640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -8175,7 +8335,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
         <v>105</v>
       </c>
@@ -8195,7 +8355,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
         <v>104</v>
       </c>
@@ -8215,7 +8375,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="6" t="s">
         <v>108</v>
       </c>
@@ -8235,7 +8395,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FEAT: more fixes and improvements to date! parsing FSM.
</commit_message>
<xml_diff>
--- a/docs/lexer/lexer-FSM.xlsx
+++ b/docs/lexer/lexer-FSM.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Red\docs\lexer\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{519605FB-0D00-448F-BE8A-3770BAF54A9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1035" yWindow="105" windowWidth="21270" windowHeight="13635" tabRatio="564" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1040" yWindow="110" windowWidth="21270" windowHeight="13640" tabRatio="564" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="transitions" sheetId="3" r:id="rId1"/>
@@ -22,12 +16,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>dk</author>
   </authors>
   <commentList>
-    <comment ref="D6" authorId="0" shapeId="0" xr:uid="{960FFBA6-8FB5-44E2-B372-614E04387ADE}">
+    <comment ref="D6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -57,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1810" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1844" uniqueCount="181">
   <si>
     <t>S_START</t>
   </si>
@@ -500,12 +494,6 @@
     <t>S_DT_YMON</t>
   </si>
   <si>
-    <t>S_DT_YMD</t>
-  </si>
-  <si>
-    <t>S_DT_YMDD</t>
-  </si>
-  <si>
     <t>F_DT_YMDAY</t>
   </si>
   <si>
@@ -521,48 +509,21 @@
     <t>S_DT_DMON</t>
   </si>
   <si>
-    <t>S_DT_DMY</t>
-  </si>
-  <si>
-    <t>S_DT_DMYY</t>
-  </si>
-  <si>
-    <t>S_DT_DMYYY</t>
-  </si>
-  <si>
-    <t>S_DT_DMYYYY</t>
-  </si>
-  <si>
     <t>F_DT_DMYEAR</t>
   </si>
   <si>
     <t>S_TM_START</t>
   </si>
   <si>
-    <t>S_TM_H</t>
-  </si>
-  <si>
     <t>F_TM_HH</t>
   </si>
   <si>
-    <t>S_TM_M</t>
-  </si>
-  <si>
     <t>F_TM_MM</t>
   </si>
   <si>
-    <t>S_TM_S</t>
-  </si>
-  <si>
     <t>F_TM_SS</t>
   </si>
   <si>
-    <t>S_TM_N</t>
-  </si>
-  <si>
-    <t>F_TM_NNN</t>
-  </si>
-  <si>
     <t>S_TZ_START</t>
   </si>
   <si>
@@ -575,19 +536,70 @@
     <t>S_TZ_M</t>
   </si>
   <si>
-    <t>F_TZ_MM</t>
-  </si>
-  <si>
     <t>F_DT_YEARL2</t>
   </si>
   <si>
     <t>C_DT_LETTER</t>
+  </si>
+  <si>
+    <t>F_DT_YMD</t>
+  </si>
+  <si>
+    <t>F_DT_YMDD</t>
+  </si>
+  <si>
+    <t>F_DT_DMY</t>
+  </si>
+  <si>
+    <t>F_DT_DMYY</t>
+  </si>
+  <si>
+    <t>F_DT_DMYYY</t>
+  </si>
+  <si>
+    <t>F_DT_DMYYYY</t>
+  </si>
+  <si>
+    <t>F_TM_H</t>
+  </si>
+  <si>
+    <t>S_TM_HM</t>
+  </si>
+  <si>
+    <t>F_TM_M</t>
+  </si>
+  <si>
+    <t>S_TM_HMS</t>
+  </si>
+  <si>
+    <t>F_TM_S</t>
+  </si>
+  <si>
+    <t>F_TM_N1</t>
+  </si>
+  <si>
+    <t>F_TM_N</t>
+  </si>
+  <si>
+    <t>T_TM_NZ</t>
+  </si>
+  <si>
+    <t>F_TZ_HM</t>
+  </si>
+  <si>
+    <t>T_TZ_HH</t>
+  </si>
+  <si>
+    <t>T_TZ_H</t>
+  </si>
+  <si>
+    <t>T_TZ_MM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -843,7 +855,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -876,26 +888,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -928,23 +923,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1120,7 +1098,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1128,15 +1106,15 @@
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.73046875" customWidth="1"/>
-    <col min="5" max="5" width="9.73046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="12" width="9.73046875" customWidth="1"/>
-    <col min="13" max="13" width="9.9296875" bestFit="1" customWidth="1"/>
-    <col min="14" max="34" width="9.73046875" customWidth="1"/>
+    <col min="1" max="1" width="10.36328125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" customWidth="1"/>
+    <col min="5" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="9.7265625" customWidth="1"/>
+    <col min="13" max="13" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="34" width="9.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -1241,7 +1219,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
@@ -1345,7 +1323,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A3" s="12" t="s">
         <v>70</v>
       </c>
@@ -1449,7 +1427,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A4" s="12" t="s">
         <v>71</v>
       </c>
@@ -1553,7 +1531,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A5" s="12" t="s">
         <v>1</v>
       </c>
@@ -1657,7 +1635,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A6" s="12" t="s">
         <v>2</v>
       </c>
@@ -1761,7 +1739,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A7" s="12" t="s">
         <v>75</v>
       </c>
@@ -1865,7 +1843,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A8" s="12" t="s">
         <v>3</v>
       </c>
@@ -1969,7 +1947,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A9" s="12" t="s">
         <v>4</v>
       </c>
@@ -2073,7 +2051,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A10" s="12" t="s">
         <v>110</v>
       </c>
@@ -2177,7 +2155,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A11" s="12" t="s">
         <v>111</v>
       </c>
@@ -2281,7 +2259,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A12" s="12" t="s">
         <v>112</v>
       </c>
@@ -2385,7 +2363,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A13" s="12" t="s">
         <v>5</v>
       </c>
@@ -2489,7 +2467,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A14" s="12" t="s">
         <v>6</v>
       </c>
@@ -2593,7 +2571,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A15" s="12" t="s">
         <v>7</v>
       </c>
@@ -2697,7 +2675,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A16" s="12" t="s">
         <v>72</v>
       </c>
@@ -2801,7 +2779,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A17" s="12" t="s">
         <v>8</v>
       </c>
@@ -2905,7 +2883,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A18" s="12" t="s">
         <v>9</v>
       </c>
@@ -3009,7 +2987,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A19" s="12" t="s">
         <v>10</v>
       </c>
@@ -3113,7 +3091,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A20" s="12" t="s">
         <v>11</v>
       </c>
@@ -3217,7 +3195,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A21" s="12" t="s">
         <v>12</v>
       </c>
@@ -3321,7 +3299,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A22" s="12" t="s">
         <v>87</v>
       </c>
@@ -3425,7 +3403,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A23" s="12" t="s">
         <v>13</v>
       </c>
@@ -3529,7 +3507,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A24" s="12" t="s">
         <v>14</v>
       </c>
@@ -3633,7 +3611,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A25" s="12" t="s">
         <v>15</v>
       </c>
@@ -3737,7 +3715,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A26" s="12" t="s">
         <v>16</v>
       </c>
@@ -3841,7 +3819,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A27" s="12" t="s">
         <v>17</v>
       </c>
@@ -3945,7 +3923,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A28" s="12" t="s">
         <v>18</v>
       </c>
@@ -4049,7 +4027,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A29" s="12" t="s">
         <v>19</v>
       </c>
@@ -4153,7 +4131,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A30" s="12" t="s">
         <v>20</v>
       </c>
@@ -4257,7 +4235,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A31" s="12" t="s">
         <v>22</v>
       </c>
@@ -4361,7 +4339,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A32" s="12" t="s">
         <v>23</v>
       </c>
@@ -4465,7 +4443,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A33" s="12" t="s">
         <v>24</v>
       </c>
@@ -4569,7 +4547,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A34" s="12" t="s">
         <v>25</v>
       </c>
@@ -4673,7 +4651,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="35" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A35" s="12" t="s">
         <v>26</v>
       </c>
@@ -4777,7 +4755,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A36" s="12" t="s">
         <v>27</v>
       </c>
@@ -4881,7 +4859,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A37" s="12" t="s">
         <v>28</v>
       </c>
@@ -4985,7 +4963,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="38" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A38" s="12" t="s">
         <v>29</v>
       </c>
@@ -5089,7 +5067,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A39" s="12" t="s">
         <v>30</v>
       </c>
@@ -5193,7 +5171,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A40" s="12" t="s">
         <v>31</v>
       </c>
@@ -5297,7 +5275,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="41" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A41" s="12" t="s">
         <v>32</v>
       </c>
@@ -5401,7 +5379,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="42" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A42" s="12" t="s">
         <v>97</v>
       </c>
@@ -5505,7 +5483,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="43" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A43" s="12" t="s">
         <v>33</v>
       </c>
@@ -5609,7 +5587,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="44" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A44" s="12" t="s">
         <v>21</v>
       </c>
@@ -5713,7 +5691,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="45" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A45" s="13" t="s">
         <v>113</v>
       </c>
@@ -5817,7 +5795,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="46" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A46" s="12" t="s">
         <v>114</v>
       </c>
@@ -5921,7 +5899,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="47" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A47" s="12" t="s">
         <v>115</v>
       </c>
@@ -6025,7 +6003,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="48" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A48" s="12" t="s">
         <v>116</v>
       </c>
@@ -6129,7 +6107,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="49" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A49" s="12" t="s">
         <v>117</v>
       </c>
@@ -6240,27 +6218,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M125"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.3984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="14"/>
       <c r="B1" s="7" t="s">
         <v>118</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>119</v>
@@ -6269,19 +6247,19 @@
         <v>120</v>
       </c>
       <c r="F1" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="H1" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>123</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>125</v>
       </c>
       <c r="K1" s="7" t="s">
         <v>126</v>
@@ -6293,7 +6271,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
         <v>129</v>
       </c>
@@ -6312,7 +6290,7 @@
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
         <v>130</v>
       </c>
@@ -6335,7 +6313,7 @@
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
         <v>131</v>
       </c>
@@ -6358,7 +6336,7 @@
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
         <v>132</v>
       </c>
@@ -6381,7 +6359,7 @@
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="16" t="s">
         <v>133</v>
       </c>
@@ -6395,20 +6373,20 @@
         <v>133</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="F6" s="2"/>
+        <v>161</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>146</v>
+      </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
-      <c r="I6" s="2" t="s">
-        <v>146</v>
-      </c>
+      <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="16" t="s">
         <v>134</v>
       </c>
@@ -6420,28 +6398,28 @@
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
+      <c r="F7" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>140</v>
+      </c>
       <c r="H7" s="2"/>
-      <c r="I7" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>140</v>
-      </c>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="16" t="s">
         <v>135</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -6454,7 +6432,7 @@
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="15" t="s">
         <v>136</v>
       </c>
@@ -6477,7 +6455,7 @@
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="15" t="s">
         <v>137</v>
       </c>
@@ -6500,12 +6478,12 @@
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="16" t="s">
         <v>138</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>147</v>
+        <v>163</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -6519,7 +6497,7 @@
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="16" t="s">
         <v>139</v>
       </c>
@@ -6527,18 +6505,18 @@
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="F12" s="2" t="s">
+        <v>153</v>
+      </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
-      <c r="I12" s="2" t="s">
-        <v>159</v>
-      </c>
+      <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="15" t="s">
         <v>140</v>
       </c>
@@ -6557,7 +6535,7 @@
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="15" t="s">
         <v>141</v>
       </c>
@@ -6578,7 +6556,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="15" t="s">
         <v>142</v>
       </c>
@@ -6588,18 +6566,18 @@
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+      <c r="F15" s="2" t="s">
+        <v>153</v>
+      </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
-      <c r="I15" s="2" t="s">
-        <v>159</v>
-      </c>
+      <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" s="16" t="s">
         <v>143</v>
       </c>
@@ -6616,7 +6594,7 @@
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="15" t="s">
         <v>144</v>
       </c>
@@ -6624,7 +6602,9 @@
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
+      <c r="F17" s="2" t="s">
+        <v>153</v>
+      </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
@@ -6635,7 +6615,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="16" t="s">
         <v>145</v>
       </c>
@@ -6652,7 +6632,7 @@
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="15" t="s">
         <v>146</v>
       </c>
@@ -6666,7 +6646,9 @@
       <c r="E19" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="F19" s="2"/>
+      <c r="F19" s="2" t="s">
+        <v>146</v>
+      </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
@@ -6675,21 +6657,21 @@
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A20" s="15" t="s">
-        <v>147</v>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A20" s="16" t="s">
+        <v>163</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>148</v>
+        <v>164</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="F20" s="2"/>
+        <v>153</v>
+      </c>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2" t="s">
+        <v>153</v>
+      </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
@@ -6697,22 +6679,22 @@
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
       <c r="M20" s="2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A21" s="15" t="s">
-        <v>148</v>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A21" s="16" t="s">
+        <v>164</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="F21" s="2"/>
+        <v>153</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2" t="s">
+        <v>153</v>
+      </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
@@ -6720,43 +6702,43 @@
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A22" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A22" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="E22" s="2"/>
+        <v>150</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>150</v>
+      </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
-      <c r="I22" s="2" t="s">
-        <v>159</v>
-      </c>
+      <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" s="15" t="s">
-        <v>150</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>151</v>
-      </c>
+        <v>149</v>
+      </c>
+      <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
@@ -6767,18 +6749,16 @@
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A24" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="B24" s="2"/>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A24" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>165</v>
+      </c>
       <c r="C24" s="2"/>
-      <c r="D24" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>152</v>
-      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
@@ -6788,17 +6768,23 @@
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A25" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A25" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>151</v>
+      </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
@@ -6807,40 +6793,46 @@
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A26" s="15" t="s">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A26" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2" t="s">
+      <c r="E26" s="2"/>
+      <c r="F26" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
-      <c r="M26" s="2"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A27" s="15" t="s">
-        <v>154</v>
+      <c r="M26" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A27" s="16" t="s">
+        <v>166</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>155</v>
+        <v>166</v>
       </c>
       <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
+      <c r="D27" s="2" t="s">
+        <v>153</v>
+      </c>
       <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
+      <c r="F27" s="2" t="s">
+        <v>153</v>
+      </c>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
@@ -6848,20 +6840,24 @@
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
       <c r="M27" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A28" s="15" t="s">
-        <v>155</v>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A28" s="16" t="s">
+        <v>167</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>155</v>
+        <v>167</v>
       </c>
       <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
+      <c r="D28" s="2" t="s">
+        <v>153</v>
+      </c>
       <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
+      <c r="F28" s="2" t="s">
+        <v>153</v>
+      </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
@@ -6869,20 +6865,22 @@
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
       <c r="M28" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A29" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>156</v>
-      </c>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A29" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="B29" s="2"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
+      <c r="D29" s="2" t="s">
+        <v>153</v>
+      </c>
       <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
+      <c r="F29" s="2" t="s">
+        <v>153</v>
+      </c>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
@@ -6890,18 +6888,18 @@
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
       <c r="M29" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A30" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="B30" s="2"/>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A30" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>169</v>
+      </c>
       <c r="C30" s="2"/>
-      <c r="D30" s="2" t="s">
-        <v>158</v>
-      </c>
+      <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
@@ -6910,15 +6908,15 @@
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
-      <c r="M30" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A31" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="B31" s="2"/>
+      <c r="M30" s="2"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A31" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>154</v>
+      </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -6931,28 +6929,34 @@
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="B32" s="2"/>
+        <v>154</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>171</v>
+      </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
+      <c r="I32" s="2" t="s">
+        <v>170</v>
+      </c>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A33" s="13" t="s">
-        <v>159</v>
-      </c>
-      <c r="B33" s="2"/>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A33" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>171</v>
+      </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -6965,11 +6969,13 @@
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A34" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="B34" s="2"/>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A34" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>155</v>
+      </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
@@ -6982,28 +6988,34 @@
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A35" s="16" t="s">
-        <v>161</v>
-      </c>
-      <c r="B35" s="2"/>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A35" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>173</v>
+      </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
+      <c r="I35" s="2" t="s">
+        <v>172</v>
+      </c>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36" s="16" t="s">
-        <v>161</v>
-      </c>
-      <c r="B36" s="2"/>
+        <v>172</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>173</v>
+      </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -7016,11 +7028,13 @@
       <c r="L36" s="2"/>
       <c r="M36" s="2"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" s="15" t="s">
-        <v>162</v>
-      </c>
-      <c r="B37" s="2"/>
+        <v>173</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>156</v>
+      </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -7033,28 +7047,36 @@
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A38" s="16" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
+      <c r="E38" s="2" t="s">
+        <v>157</v>
+      </c>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
+      <c r="H38" s="2" t="s">
+        <v>157</v>
+      </c>
       <c r="I38" s="2"/>
-      <c r="J38" s="2"/>
+      <c r="J38" s="2" t="s">
+        <v>174</v>
+      </c>
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39" s="15" t="s">
-        <v>164</v>
-      </c>
-      <c r="B39" s="2"/>
+        <v>174</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>175</v>
+      </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
@@ -7067,28 +7089,40 @@
       <c r="L39" s="2"/>
       <c r="M39" s="2"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A40" s="16" t="s">
-        <v>165</v>
-      </c>
-      <c r="B40" s="2"/>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A40" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>175</v>
+      </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
+      <c r="E40" s="2" t="s">
+        <v>157</v>
+      </c>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
+      <c r="H40" s="2" t="s">
+        <v>157</v>
+      </c>
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
-      <c r="K40" s="2"/>
+      <c r="K40" s="2" t="s">
+        <v>176</v>
+      </c>
       <c r="L40" s="2"/>
-      <c r="M40" s="2"/>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="M40" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A41" s="15" t="s">
-        <v>166</v>
-      </c>
-      <c r="B41" s="2"/>
+        <v>157</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>158</v>
+      </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
@@ -7101,26 +7135,32 @@
       <c r="L41" s="2"/>
       <c r="M41" s="2"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A42" s="16" t="s">
-        <v>167</v>
-      </c>
-      <c r="B42" s="2"/>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A42" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>159</v>
+      </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
+      <c r="I42" s="2" t="s">
+        <v>177</v>
+      </c>
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
-      <c r="M42" s="2"/>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A43" s="15" t="s">
-        <v>168</v>
+      <c r="M42" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A43" s="16" t="s">
+        <v>159</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -7129,17 +7169,23 @@
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
-      <c r="I43" s="2"/>
+      <c r="I43" s="2" t="s">
+        <v>177</v>
+      </c>
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
-      <c r="M43" s="2"/>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A44" s="15" t="s">
-        <v>169</v>
-      </c>
-      <c r="B44" s="2"/>
+      <c r="M43" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A44" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>160</v>
+      </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
@@ -7152,11 +7198,13 @@
       <c r="L44" s="2"/>
       <c r="M44" s="2"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A45" s="16" t="s">
-        <v>170</v>
-      </c>
-      <c r="B45" s="2"/>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A45" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>180</v>
+      </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -7167,12 +7215,11 @@
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
       <c r="L45" s="2"/>
-      <c r="M45" s="2"/>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A46" s="15" t="s">
-        <v>171</v>
-      </c>
+      <c r="M45" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
@@ -7186,10 +7233,7 @@
       <c r="L46" s="2"/>
       <c r="M46" s="2"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A47" s="16" t="s">
-        <v>172</v>
-      </c>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
@@ -7203,7 +7247,7 @@
       <c r="L47" s="2"/>
       <c r="M47" s="2"/>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
@@ -7217,7 +7261,7 @@
       <c r="L48" s="2"/>
       <c r="M48" s="2"/>
     </row>
-    <row r="49" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="49" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
@@ -7231,7 +7275,7 @@
       <c r="L49" s="2"/>
       <c r="M49" s="2"/>
     </row>
-    <row r="50" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="50" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
@@ -7245,7 +7289,7 @@
       <c r="L50" s="2"/>
       <c r="M50" s="2"/>
     </row>
-    <row r="51" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="51" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
@@ -7259,7 +7303,7 @@
       <c r="L51" s="2"/>
       <c r="M51" s="2"/>
     </row>
-    <row r="52" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="52" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
@@ -7273,7 +7317,7 @@
       <c r="L52" s="2"/>
       <c r="M52" s="2"/>
     </row>
-    <row r="53" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="53" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
@@ -7287,7 +7331,7 @@
       <c r="L53" s="2"/>
       <c r="M53" s="2"/>
     </row>
-    <row r="54" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="54" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
@@ -7301,7 +7345,7 @@
       <c r="L54" s="2"/>
       <c r="M54" s="2"/>
     </row>
-    <row r="55" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="55" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
@@ -7315,7 +7359,7 @@
       <c r="L55" s="2"/>
       <c r="M55" s="2"/>
     </row>
-    <row r="56" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="56" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
@@ -7329,7 +7373,7 @@
       <c r="L56" s="2"/>
       <c r="M56" s="2"/>
     </row>
-    <row r="57" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="57" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
@@ -7343,7 +7387,7 @@
       <c r="L57" s="2"/>
       <c r="M57" s="2"/>
     </row>
-    <row r="58" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="58" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
@@ -7357,7 +7401,7 @@
       <c r="L58" s="2"/>
       <c r="M58" s="2"/>
     </row>
-    <row r="59" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="59" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
@@ -7371,7 +7415,7 @@
       <c r="L59" s="2"/>
       <c r="M59" s="2"/>
     </row>
-    <row r="60" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="60" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
@@ -7385,7 +7429,7 @@
       <c r="L60" s="2"/>
       <c r="M60" s="2"/>
     </row>
-    <row r="61" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="61" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
@@ -7399,7 +7443,7 @@
       <c r="L61" s="2"/>
       <c r="M61" s="2"/>
     </row>
-    <row r="62" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="62" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
@@ -7413,7 +7457,7 @@
       <c r="L62" s="2"/>
       <c r="M62" s="2"/>
     </row>
-    <row r="63" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="63" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
@@ -7427,7 +7471,7 @@
       <c r="L63" s="2"/>
       <c r="M63" s="2"/>
     </row>
-    <row r="64" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="64" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
@@ -7441,7 +7485,7 @@
       <c r="L64" s="2"/>
       <c r="M64" s="2"/>
     </row>
-    <row r="65" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="65" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
@@ -7455,7 +7499,7 @@
       <c r="L65" s="2"/>
       <c r="M65" s="2"/>
     </row>
-    <row r="66" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="66" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
@@ -7469,7 +7513,7 @@
       <c r="L66" s="2"/>
       <c r="M66" s="2"/>
     </row>
-    <row r="67" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="67" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
@@ -7483,7 +7527,7 @@
       <c r="L67" s="2"/>
       <c r="M67" s="2"/>
     </row>
-    <row r="68" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="68" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
@@ -7497,7 +7541,7 @@
       <c r="L68" s="2"/>
       <c r="M68" s="2"/>
     </row>
-    <row r="69" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="69" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
@@ -7511,7 +7555,7 @@
       <c r="L69" s="2"/>
       <c r="M69" s="2"/>
     </row>
-    <row r="70" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="70" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
@@ -7525,7 +7569,7 @@
       <c r="L70" s="2"/>
       <c r="M70" s="2"/>
     </row>
-    <row r="71" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="71" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
@@ -7539,7 +7583,7 @@
       <c r="L71" s="2"/>
       <c r="M71" s="2"/>
     </row>
-    <row r="72" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="72" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
@@ -7553,7 +7597,7 @@
       <c r="L72" s="2"/>
       <c r="M72" s="2"/>
     </row>
-    <row r="73" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="73" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
@@ -7567,7 +7611,7 @@
       <c r="L73" s="2"/>
       <c r="M73" s="2"/>
     </row>
-    <row r="74" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="74" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
@@ -7581,7 +7625,7 @@
       <c r="L74" s="2"/>
       <c r="M74" s="2"/>
     </row>
-    <row r="75" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="75" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
@@ -7595,7 +7639,7 @@
       <c r="L75" s="2"/>
       <c r="M75" s="2"/>
     </row>
-    <row r="76" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="76" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
       <c r="D76" s="2"/>
@@ -7609,7 +7653,7 @@
       <c r="L76" s="2"/>
       <c r="M76" s="2"/>
     </row>
-    <row r="77" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="77" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
       <c r="D77" s="2"/>
@@ -7623,7 +7667,7 @@
       <c r="L77" s="2"/>
       <c r="M77" s="2"/>
     </row>
-    <row r="78" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="78" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
       <c r="D78" s="2"/>
@@ -7637,7 +7681,7 @@
       <c r="L78" s="2"/>
       <c r="M78" s="2"/>
     </row>
-    <row r="79" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="79" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
       <c r="D79" s="2"/>
@@ -7651,7 +7695,7 @@
       <c r="L79" s="2"/>
       <c r="M79" s="2"/>
     </row>
-    <row r="80" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="80" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
       <c r="D80" s="2"/>
@@ -7665,7 +7709,7 @@
       <c r="L80" s="2"/>
       <c r="M80" s="2"/>
     </row>
-    <row r="81" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="81" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
       <c r="D81" s="2"/>
@@ -7679,7 +7723,7 @@
       <c r="L81" s="2"/>
       <c r="M81" s="2"/>
     </row>
-    <row r="82" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="82" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
       <c r="D82" s="2"/>
@@ -7693,7 +7737,7 @@
       <c r="L82" s="2"/>
       <c r="M82" s="2"/>
     </row>
-    <row r="83" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="83" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
       <c r="D83" s="2"/>
@@ -7707,7 +7751,7 @@
       <c r="L83" s="2"/>
       <c r="M83" s="2"/>
     </row>
-    <row r="84" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="84" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
       <c r="D84" s="2"/>
@@ -7721,7 +7765,7 @@
       <c r="L84" s="2"/>
       <c r="M84" s="2"/>
     </row>
-    <row r="85" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="85" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
       <c r="D85" s="2"/>
@@ -7735,7 +7779,7 @@
       <c r="L85" s="2"/>
       <c r="M85" s="2"/>
     </row>
-    <row r="86" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="86" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
       <c r="D86" s="2"/>
@@ -7749,7 +7793,7 @@
       <c r="L86" s="2"/>
       <c r="M86" s="2"/>
     </row>
-    <row r="87" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="87" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
       <c r="D87" s="2"/>
@@ -7763,7 +7807,7 @@
       <c r="L87" s="2"/>
       <c r="M87" s="2"/>
     </row>
-    <row r="88" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="88" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
       <c r="D88" s="2"/>
@@ -7777,7 +7821,7 @@
       <c r="L88" s="2"/>
       <c r="M88" s="2"/>
     </row>
-    <row r="89" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="89" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
       <c r="D89" s="2"/>
@@ -7791,7 +7835,7 @@
       <c r="L89" s="2"/>
       <c r="M89" s="2"/>
     </row>
-    <row r="90" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="90" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
       <c r="D90" s="2"/>
@@ -7805,7 +7849,7 @@
       <c r="L90" s="2"/>
       <c r="M90" s="2"/>
     </row>
-    <row r="91" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="91" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
       <c r="D91" s="2"/>
@@ -7819,7 +7863,7 @@
       <c r="L91" s="2"/>
       <c r="M91" s="2"/>
     </row>
-    <row r="92" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="92" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
       <c r="D92" s="2"/>
@@ -7833,7 +7877,7 @@
       <c r="L92" s="2"/>
       <c r="M92" s="2"/>
     </row>
-    <row r="93" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="93" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
       <c r="D93" s="2"/>
@@ -7847,7 +7891,7 @@
       <c r="L93" s="2"/>
       <c r="M93" s="2"/>
     </row>
-    <row r="94" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="94" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
       <c r="D94" s="2"/>
@@ -7861,7 +7905,7 @@
       <c r="L94" s="2"/>
       <c r="M94" s="2"/>
     </row>
-    <row r="95" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="95" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
       <c r="D95" s="2"/>
@@ -7875,7 +7919,7 @@
       <c r="L95" s="2"/>
       <c r="M95" s="2"/>
     </row>
-    <row r="96" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="96" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
       <c r="D96" s="2"/>
@@ -7889,7 +7933,7 @@
       <c r="L96" s="2"/>
       <c r="M96" s="2"/>
     </row>
-    <row r="97" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="97" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
       <c r="D97" s="2"/>
@@ -7903,7 +7947,7 @@
       <c r="L97" s="2"/>
       <c r="M97" s="2"/>
     </row>
-    <row r="98" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="98" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
       <c r="D98" s="2"/>
@@ -7917,7 +7961,7 @@
       <c r="L98" s="2"/>
       <c r="M98" s="2"/>
     </row>
-    <row r="99" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="99" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
       <c r="D99" s="2"/>
@@ -7931,7 +7975,7 @@
       <c r="L99" s="2"/>
       <c r="M99" s="2"/>
     </row>
-    <row r="100" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="100" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
       <c r="D100" s="2"/>
@@ -7945,7 +7989,7 @@
       <c r="L100" s="2"/>
       <c r="M100" s="2"/>
     </row>
-    <row r="101" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="101" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
       <c r="D101" s="2"/>
@@ -7959,7 +8003,7 @@
       <c r="L101" s="2"/>
       <c r="M101" s="2"/>
     </row>
-    <row r="102" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="102" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
       <c r="D102" s="2"/>
@@ -7973,7 +8017,7 @@
       <c r="L102" s="2"/>
       <c r="M102" s="2"/>
     </row>
-    <row r="103" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="103" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
       <c r="D103" s="2"/>
@@ -7987,7 +8031,7 @@
       <c r="L103" s="2"/>
       <c r="M103" s="2"/>
     </row>
-    <row r="104" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="104" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
       <c r="D104" s="2"/>
@@ -8001,7 +8045,7 @@
       <c r="L104" s="2"/>
       <c r="M104" s="2"/>
     </row>
-    <row r="105" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="105" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
       <c r="D105" s="2"/>
@@ -8015,7 +8059,7 @@
       <c r="L105" s="2"/>
       <c r="M105" s="2"/>
     </row>
-    <row r="106" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="106" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
       <c r="D106" s="2"/>
@@ -8029,7 +8073,7 @@
       <c r="L106" s="2"/>
       <c r="M106" s="2"/>
     </row>
-    <row r="107" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="107" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
       <c r="D107" s="2"/>
@@ -8043,7 +8087,7 @@
       <c r="L107" s="2"/>
       <c r="M107" s="2"/>
     </row>
-    <row r="108" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="108" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
       <c r="D108" s="2"/>
@@ -8057,7 +8101,7 @@
       <c r="L108" s="2"/>
       <c r="M108" s="2"/>
     </row>
-    <row r="109" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="109" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
       <c r="D109" s="2"/>
@@ -8071,7 +8115,7 @@
       <c r="L109" s="2"/>
       <c r="M109" s="2"/>
     </row>
-    <row r="110" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="110" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
       <c r="D110" s="2"/>
@@ -8085,7 +8129,7 @@
       <c r="L110" s="2"/>
       <c r="M110" s="2"/>
     </row>
-    <row r="111" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="111" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
       <c r="D111" s="2"/>
@@ -8099,7 +8143,7 @@
       <c r="L111" s="2"/>
       <c r="M111" s="2"/>
     </row>
-    <row r="112" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="112" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
       <c r="D112" s="2"/>
@@ -8113,7 +8157,7 @@
       <c r="L112" s="2"/>
       <c r="M112" s="2"/>
     </row>
-    <row r="113" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="113" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
       <c r="D113" s="2"/>
@@ -8127,7 +8171,7 @@
       <c r="L113" s="2"/>
       <c r="M113" s="2"/>
     </row>
-    <row r="114" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="114" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
       <c r="D114" s="2"/>
@@ -8141,7 +8185,7 @@
       <c r="L114" s="2"/>
       <c r="M114" s="2"/>
     </row>
-    <row r="115" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="115" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
       <c r="D115" s="2"/>
@@ -8155,146 +8199,6 @@
       <c r="L115" s="2"/>
       <c r="M115" s="2"/>
     </row>
-    <row r="116" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B116" s="2"/>
-      <c r="C116" s="2"/>
-      <c r="D116" s="2"/>
-      <c r="E116" s="2"/>
-      <c r="F116" s="2"/>
-      <c r="G116" s="2"/>
-      <c r="H116" s="2"/>
-      <c r="I116" s="2"/>
-      <c r="J116" s="2"/>
-      <c r="K116" s="2"/>
-      <c r="L116" s="2"/>
-      <c r="M116" s="2"/>
-    </row>
-    <row r="117" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B117" s="2"/>
-      <c r="C117" s="2"/>
-      <c r="D117" s="2"/>
-      <c r="E117" s="2"/>
-      <c r="F117" s="2"/>
-      <c r="G117" s="2"/>
-      <c r="H117" s="2"/>
-      <c r="I117" s="2"/>
-      <c r="J117" s="2"/>
-      <c r="K117" s="2"/>
-      <c r="L117" s="2"/>
-      <c r="M117" s="2"/>
-    </row>
-    <row r="118" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B118" s="2"/>
-      <c r="C118" s="2"/>
-      <c r="D118" s="2"/>
-      <c r="E118" s="2"/>
-      <c r="F118" s="2"/>
-      <c r="G118" s="2"/>
-      <c r="H118" s="2"/>
-      <c r="I118" s="2"/>
-      <c r="J118" s="2"/>
-      <c r="K118" s="2"/>
-      <c r="L118" s="2"/>
-      <c r="M118" s="2"/>
-    </row>
-    <row r="119" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B119" s="2"/>
-      <c r="C119" s="2"/>
-      <c r="D119" s="2"/>
-      <c r="E119" s="2"/>
-      <c r="F119" s="2"/>
-      <c r="G119" s="2"/>
-      <c r="H119" s="2"/>
-      <c r="I119" s="2"/>
-      <c r="J119" s="2"/>
-      <c r="K119" s="2"/>
-      <c r="L119" s="2"/>
-      <c r="M119" s="2"/>
-    </row>
-    <row r="120" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B120" s="2"/>
-      <c r="C120" s="2"/>
-      <c r="D120" s="2"/>
-      <c r="E120" s="2"/>
-      <c r="F120" s="2"/>
-      <c r="G120" s="2"/>
-      <c r="H120" s="2"/>
-      <c r="I120" s="2"/>
-      <c r="J120" s="2"/>
-      <c r="K120" s="2"/>
-      <c r="L120" s="2"/>
-      <c r="M120" s="2"/>
-    </row>
-    <row r="121" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B121" s="2"/>
-      <c r="C121" s="2"/>
-      <c r="D121" s="2"/>
-      <c r="E121" s="2"/>
-      <c r="F121" s="2"/>
-      <c r="G121" s="2"/>
-      <c r="H121" s="2"/>
-      <c r="I121" s="2"/>
-      <c r="J121" s="2"/>
-      <c r="K121" s="2"/>
-      <c r="L121" s="2"/>
-      <c r="M121" s="2"/>
-    </row>
-    <row r="122" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B122" s="2"/>
-      <c r="C122" s="2"/>
-      <c r="D122" s="2"/>
-      <c r="E122" s="2"/>
-      <c r="F122" s="2"/>
-      <c r="G122" s="2"/>
-      <c r="H122" s="2"/>
-      <c r="I122" s="2"/>
-      <c r="J122" s="2"/>
-      <c r="K122" s="2"/>
-      <c r="L122" s="2"/>
-      <c r="M122" s="2"/>
-    </row>
-    <row r="123" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B123" s="2"/>
-      <c r="C123" s="2"/>
-      <c r="D123" s="2"/>
-      <c r="E123" s="2"/>
-      <c r="F123" s="2"/>
-      <c r="G123" s="2"/>
-      <c r="H123" s="2"/>
-      <c r="I123" s="2"/>
-      <c r="J123" s="2"/>
-      <c r="K123" s="2"/>
-      <c r="L123" s="2"/>
-      <c r="M123" s="2"/>
-    </row>
-    <row r="124" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B124" s="2"/>
-      <c r="C124" s="2"/>
-      <c r="D124" s="2"/>
-      <c r="E124" s="2"/>
-      <c r="F124" s="2"/>
-      <c r="G124" s="2"/>
-      <c r="H124" s="2"/>
-      <c r="I124" s="2"/>
-      <c r="J124" s="2"/>
-      <c r="K124" s="2"/>
-      <c r="L124" s="2"/>
-      <c r="M124" s="2"/>
-    </row>
-    <row r="125" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B125" s="2"/>
-      <c r="C125" s="2"/>
-      <c r="D125" s="2"/>
-      <c r="E125" s="2"/>
-      <c r="F125" s="2"/>
-      <c r="G125" s="2"/>
-      <c r="H125" s="2"/>
-      <c r="I125" s="2"/>
-      <c r="J125" s="2"/>
-      <c r="K125" s="2"/>
-      <c r="L125" s="2"/>
-      <c r="M125" s="2"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -8302,19 +8206,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.9296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.06640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.19921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -8335,7 +8239,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
         <v>105</v>
       </c>
@@ -8355,7 +8259,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
         <v>104</v>
       </c>
@@ -8375,7 +8279,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A4" s="6" t="s">
         <v>108</v>
       </c>
@@ -8395,7 +8299,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A5" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FEAT: adds pipeline for generating date! transitions table.
</commit_message>
<xml_diff>
--- a/docs/lexer/lexer-FSM.xlsx
+++ b/docs/lexer/lexer-FSM.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Red\docs\lexer\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8674A13-C6B5-4039-9935-C28BC8358BB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="110" windowWidth="21270" windowHeight="13640" tabRatio="564" activeTab="1"/>
+    <workbookView xWindow="1035" yWindow="0" windowWidth="21270" windowHeight="14400" tabRatio="564" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="transitions" sheetId="3" r:id="rId1"/>
@@ -16,12 +22,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>dk</author>
   </authors>
   <commentList>
-    <comment ref="D6" authorId="0">
+    <comment ref="D6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -51,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1844" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2272" uniqueCount="181">
   <si>
     <t>S_START</t>
   </si>
@@ -455,9 +461,6 @@
     <t>F_DT_YEARL</t>
   </si>
   <si>
-    <t>F_DT_YEAR2</t>
-  </si>
-  <si>
     <t>F_DT_DAYL</t>
   </si>
   <si>
@@ -494,9 +497,6 @@
     <t>S_DT_YMON</t>
   </si>
   <si>
-    <t>F_DT_YMDAY</t>
-  </si>
-  <si>
     <t>S_DT_DM</t>
   </si>
   <si>
@@ -509,9 +509,6 @@
     <t>S_DT_DMON</t>
   </si>
   <si>
-    <t>F_DT_DMYEAR</t>
-  </si>
-  <si>
     <t>S_TM_START</t>
   </si>
   <si>
@@ -594,13 +591,22 @@
   </si>
   <si>
     <t>T_TZ_MM</t>
+  </si>
+  <si>
+    <t>T_DT_ERROR</t>
+  </si>
+  <si>
+    <t>T_DT_YMDAY</t>
+  </si>
+  <si>
+    <t>T_DT_DMYEAR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -665,6 +671,13 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -747,7 +760,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -793,6 +806,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -855,7 +871,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -888,9 +904,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -923,6 +956,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1098,7 +1148,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1106,15 +1156,15 @@
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.36328125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" customWidth="1"/>
-    <col min="5" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="12" width="9.7265625" customWidth="1"/>
-    <col min="13" max="13" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="14" max="34" width="9.7265625" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.73046875" customWidth="1"/>
+    <col min="5" max="5" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="9.73046875" customWidth="1"/>
+    <col min="13" max="13" width="9.9296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="34" width="9.73046875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -1219,7 +1269,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
@@ -1323,7 +1373,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A3" s="12" t="s">
         <v>70</v>
       </c>
@@ -1427,7 +1477,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A4" s="12" t="s">
         <v>71</v>
       </c>
@@ -1531,7 +1581,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A5" s="12" t="s">
         <v>1</v>
       </c>
@@ -1635,7 +1685,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A6" s="12" t="s">
         <v>2</v>
       </c>
@@ -1739,7 +1789,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A7" s="12" t="s">
         <v>75</v>
       </c>
@@ -1843,7 +1893,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A8" s="12" t="s">
         <v>3</v>
       </c>
@@ -1947,7 +1997,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A9" s="12" t="s">
         <v>4</v>
       </c>
@@ -2051,7 +2101,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A10" s="12" t="s">
         <v>110</v>
       </c>
@@ -2155,7 +2205,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A11" s="12" t="s">
         <v>111</v>
       </c>
@@ -2259,7 +2309,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A12" s="12" t="s">
         <v>112</v>
       </c>
@@ -2363,7 +2413,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A13" s="12" t="s">
         <v>5</v>
       </c>
@@ -2467,7 +2517,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A14" s="12" t="s">
         <v>6</v>
       </c>
@@ -2571,7 +2621,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A15" s="12" t="s">
         <v>7</v>
       </c>
@@ -2675,7 +2725,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A16" s="12" t="s">
         <v>72</v>
       </c>
@@ -2779,7 +2829,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A17" s="12" t="s">
         <v>8</v>
       </c>
@@ -2883,7 +2933,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A18" s="12" t="s">
         <v>9</v>
       </c>
@@ -2987,7 +3037,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A19" s="12" t="s">
         <v>10</v>
       </c>
@@ -3091,7 +3141,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A20" s="12" t="s">
         <v>11</v>
       </c>
@@ -3195,7 +3245,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="21" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A21" s="12" t="s">
         <v>12</v>
       </c>
@@ -3299,7 +3349,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A22" s="12" t="s">
         <v>87</v>
       </c>
@@ -3403,7 +3453,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A23" s="12" t="s">
         <v>13</v>
       </c>
@@ -3507,7 +3557,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="24" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A24" s="12" t="s">
         <v>14</v>
       </c>
@@ -3611,7 +3661,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A25" s="12" t="s">
         <v>15</v>
       </c>
@@ -3715,7 +3765,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A26" s="12" t="s">
         <v>16</v>
       </c>
@@ -3819,7 +3869,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A27" s="12" t="s">
         <v>17</v>
       </c>
@@ -3923,7 +3973,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A28" s="12" t="s">
         <v>18</v>
       </c>
@@ -4027,7 +4077,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A29" s="12" t="s">
         <v>19</v>
       </c>
@@ -4131,7 +4181,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A30" s="12" t="s">
         <v>20</v>
       </c>
@@ -4235,7 +4285,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="31" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A31" s="12" t="s">
         <v>22</v>
       </c>
@@ -4339,7 +4389,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="32" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A32" s="12" t="s">
         <v>23</v>
       </c>
@@ -4443,7 +4493,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A33" s="12" t="s">
         <v>24</v>
       </c>
@@ -4547,7 +4597,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A34" s="12" t="s">
         <v>25</v>
       </c>
@@ -4651,7 +4701,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="35" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A35" s="12" t="s">
         <v>26</v>
       </c>
@@ -4755,7 +4805,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A36" s="12" t="s">
         <v>27</v>
       </c>
@@ -4859,7 +4909,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A37" s="12" t="s">
         <v>28</v>
       </c>
@@ -4963,7 +5013,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="38" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A38" s="12" t="s">
         <v>29</v>
       </c>
@@ -5067,7 +5117,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A39" s="12" t="s">
         <v>30</v>
       </c>
@@ -5171,7 +5221,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A40" s="12" t="s">
         <v>31</v>
       </c>
@@ -5275,7 +5325,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="41" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A41" s="12" t="s">
         <v>32</v>
       </c>
@@ -5379,7 +5429,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="42" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A42" s="12" t="s">
         <v>97</v>
       </c>
@@ -5483,7 +5533,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="43" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A43" s="12" t="s">
         <v>33</v>
       </c>
@@ -5587,7 +5637,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="44" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A44" s="12" t="s">
         <v>21</v>
       </c>
@@ -5691,7 +5741,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="45" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A45" s="13" t="s">
         <v>113</v>
       </c>
@@ -5795,7 +5845,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="46" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A46" s="12" t="s">
         <v>114</v>
       </c>
@@ -5899,7 +5949,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="47" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A47" s="12" t="s">
         <v>115</v>
       </c>
@@ -6003,7 +6053,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="48" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A48" s="12" t="s">
         <v>116</v>
       </c>
@@ -6107,7 +6157,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="49" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A49" s="12" t="s">
         <v>117</v>
       </c>
@@ -6218,27 +6268,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M115"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:M45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.19921875" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="14"/>
       <c r="B1" s="7" t="s">
         <v>118</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>119</v>
@@ -6271,1954 +6321,1831 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" s="13" t="s">
         <v>129</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="C2" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="K2" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="L2" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="M2" s="17" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" s="12" t="s">
         <v>130</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="C3" s="2"/>
+      <c r="C3" s="17" t="s">
+        <v>178</v>
+      </c>
       <c r="D3" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+        <v>134</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="I3" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="J3" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="K3" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="L3" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="M3" s="17" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4" s="12" t="s">
         <v>131</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="C4" s="2"/>
+      <c r="C4" s="17" t="s">
+        <v>178</v>
+      </c>
       <c r="D4" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+        <v>134</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="J4" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="K4" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="L4" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="M4" s="17" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" s="12" t="s">
         <v>132</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="C5" s="2"/>
+      <c r="C5" s="17" t="s">
+        <v>178</v>
+      </c>
       <c r="D5" s="2" t="s">
         <v>133</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="F5" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="I5" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="J5" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="K5" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="L5" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="M5" s="17" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6" s="16" t="s">
         <v>133</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>133</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="I6" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="J6" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="K6" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="L6" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="M6" s="17" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A7" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="I7" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="J7" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="K7" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="L7" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="M7" s="17" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A8" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="H8" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="I8" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="J8" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="K8" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="L8" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="M8" s="17" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A9" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="H9" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="I9" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="J9" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="K9" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="L9" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="M9" s="17" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A10" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="H10" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="I10" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="J10" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="K10" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="L10" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="M10" s="17" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A11" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="H11" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="I11" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="J11" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="K11" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="L11" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="M11" s="17" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A12" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G12" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="H12" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="I12" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="J12" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="K12" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="L12" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="M12" s="17" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A13" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="G13" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="H13" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="I13" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="J13" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="K13" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="L13" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="M13" s="17" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A14" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="G14" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="H14" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="I14" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="J14" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="K14" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="L14" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A15" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G15" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="H15" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="I15" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="J15" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="K15" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="L15" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="M15" s="17" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A16" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="G16" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="H16" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="I16" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="J16" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="K16" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="L16" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="M16" s="17" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A17" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G17" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="H17" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="I17" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="J17" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="K17" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="L17" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A18" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="F18" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="G18" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="H18" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="I18" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="J18" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="K18" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="L18" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="M18" s="17" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A19" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="G19" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="H19" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="I19" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="J19" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="K19" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="L19" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="M19" s="17" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A20" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="C20" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G20" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="H20" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="I20" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="J20" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="K20" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="L20" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A21" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G21" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="H21" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="I21" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="J21" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="K21" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="L21" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A22" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A8" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="B8" s="2" t="s">
+      <c r="B22" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="E22" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="F22" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="G22" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="H22" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="I22" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="J22" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="K22" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="L22" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="M22" s="17" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A23" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="F23" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="G23" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="H23" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="I23" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="J23" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="K23" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="L23" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="M23" s="17" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A24" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="E24" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="F24" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="G24" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="H24" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="I24" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="J24" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="K24" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="L24" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="M24" s="17" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A25" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="G25" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="H25" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="I25" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="J25" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="K25" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="L25" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="M25" s="17" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A26" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G26" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="H26" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="I26" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="J26" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="K26" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="L26" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A27" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E27" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G27" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="H27" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="I27" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="J27" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="K27" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="L27" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A28" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E28" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G28" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="H28" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="I28" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="J28" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="K28" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="L28" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A29" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="C29" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E29" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G29" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="H29" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="I29" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="J29" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="K29" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="L29" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A30" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="D30" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="E30" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="F30" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="G30" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="H30" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="I30" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="J30" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="K30" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="L30" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="M30" s="17" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A31" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A9" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A10" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A11" s="16" t="s">
-        <v>138</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A12" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2" t="s">
+      <c r="C31" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="E31" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="F31" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="G31" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="H31" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="I31" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="J31" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="K31" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="L31" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="M31" s="17" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A32" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C32" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="D32" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="E32" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="F32" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="G32" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="H32" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="J32" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="K32" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="L32" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="M32" s="17" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A33" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C33" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="D33" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="E33" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="F33" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="G33" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="H33" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="I33" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="J33" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="K33" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="L33" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="M33" s="17" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A34" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C34" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="D34" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="E34" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="F34" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="G34" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="H34" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="I34" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="J34" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="K34" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="L34" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="M34" s="17" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A35" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C35" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="D35" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="E35" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="F35" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="G35" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="H35" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="J35" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="K35" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="L35" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="M35" s="17" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A36" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="D36" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="E36" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="F36" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="G36" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="H36" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="I36" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="J36" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="K36" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="L36" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="M36" s="17" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A37" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A13" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A14" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A15" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2" t="s">
+      <c r="C37" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="D37" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="E37" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="F37" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="G37" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="H37" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="I37" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="J37" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="K37" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="L37" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="M37" s="17" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A38" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A16" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A17" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A18" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A19" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A20" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A21" s="16" t="s">
-        <v>164</v>
-      </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A22" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A23" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A24" s="16" t="s">
-        <v>150</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="2"/>
-      <c r="M24" s="2"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A25" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
-      <c r="L25" s="2"/>
-      <c r="M25" s="2"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A26" s="16" t="s">
-        <v>165</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
-      <c r="L26" s="2"/>
-      <c r="M26" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A27" s="16" t="s">
-        <v>166</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
-      <c r="M27" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A28" s="16" t="s">
-        <v>167</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-      <c r="L28" s="2"/>
-      <c r="M28" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A29" s="16" t="s">
-        <v>168</v>
-      </c>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
-      <c r="L29" s="2"/>
-      <c r="M29" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A30" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
-      <c r="L30" s="2"/>
-      <c r="M30" s="2"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A31" s="15" t="s">
-        <v>169</v>
-      </c>
-      <c r="B31" s="2" t="s">
+      <c r="B38" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="D38" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="E38" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="2"/>
-      <c r="M31" s="2"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A32" s="16" t="s">
+      <c r="F38" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="G38" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="H38" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="I38" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="J38" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
-      <c r="L32" s="2"/>
-      <c r="M32" s="2"/>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A33" s="15" t="s">
-        <v>170</v>
-      </c>
-      <c r="B33" s="2" t="s">
+      <c r="K38" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="L38" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="M38" s="17" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A39" s="15" t="s">
         <v>171</v>
       </c>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
-      <c r="L33" s="2"/>
-      <c r="M33" s="2"/>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A34" s="16" t="s">
-        <v>171</v>
-      </c>
-      <c r="B34" s="2" t="s">
+      <c r="B39" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C39" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="D39" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="E39" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="F39" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="G39" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="H39" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="I39" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="J39" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="K39" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="L39" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="M39" s="17" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A40" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="D40" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="F40" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="G40" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="I40" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="J40" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="K40" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="L40" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="M40" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A41" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
-      <c r="L34" s="2"/>
-      <c r="M34" s="2"/>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A35" s="15" t="s">
+      <c r="C41" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="D41" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="E41" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="F41" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="G41" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="H41" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="I41" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="J41" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="K41" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="L41" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="M41" s="17" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A42" s="15" t="s">
         <v>155</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="J35" s="2"/>
-      <c r="K35" s="2"/>
-      <c r="L35" s="2"/>
-      <c r="M35" s="2"/>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A36" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
-      <c r="L36" s="2"/>
-      <c r="M36" s="2"/>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A37" s="15" t="s">
-        <v>173</v>
-      </c>
-      <c r="B37" s="2" t="s">
+      <c r="B42" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
-      <c r="I37" s="2"/>
-      <c r="J37" s="2"/>
-      <c r="K37" s="2"/>
-      <c r="L37" s="2"/>
-      <c r="M37" s="2"/>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A38" s="16" t="s">
+      <c r="C42" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="D42" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="E42" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="F42" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="G42" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="H42" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="J42" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="K42" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="L42" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="M42" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A43" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2" t="s">
+      <c r="B43" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="C43" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="D43" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="E43" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="F43" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="G43" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="H43" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="I43" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="J43" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="K43" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="L43" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="M43" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A44" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="B44" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2" t="s">
+      <c r="C44" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="D44" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="E44" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="F44" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="G44" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="H44" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="I44" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="J44" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="K44" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="L44" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="M44" s="17" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A45" s="15" t="s">
         <v>157</v>
       </c>
-      <c r="I38" s="2"/>
-      <c r="J38" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="K38" s="2"/>
-      <c r="L38" s="2"/>
-      <c r="M38" s="2"/>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A39" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
-      <c r="J39" s="2"/>
-      <c r="K39" s="2"/>
-      <c r="L39" s="2"/>
-      <c r="M39" s="2"/>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A40" s="15" t="s">
-        <v>175</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="I40" s="2"/>
-      <c r="J40" s="2"/>
-      <c r="K40" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="L40" s="2"/>
-      <c r="M40" s="2" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A41" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
-      <c r="I41" s="2"/>
-      <c r="J41" s="2"/>
-      <c r="K41" s="2"/>
-      <c r="L41" s="2"/>
-      <c r="M41" s="2"/>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A42" s="15" t="s">
-        <v>158</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2" t="s">
+      <c r="B45" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="J42" s="2"/>
-      <c r="K42" s="2"/>
-      <c r="L42" s="2"/>
-      <c r="M42" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A43" s="16" t="s">
-        <v>159</v>
-      </c>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
-      <c r="H43" s="2"/>
-      <c r="I43" s="2" t="s">
+      <c r="C45" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="D45" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="E45" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="F45" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="G45" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="H45" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="I45" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="J45" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="K45" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="L45" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="M45" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="J43" s="2"/>
-      <c r="K43" s="2"/>
-      <c r="L43" s="2"/>
-      <c r="M43" s="2" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A44" s="16" t="s">
-        <v>177</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
-      <c r="H44" s="2"/>
-      <c r="I44" s="2"/>
-      <c r="J44" s="2"/>
-      <c r="K44" s="2"/>
-      <c r="L44" s="2"/>
-      <c r="M44" s="2"/>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A45" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
-      <c r="G45" s="2"/>
-      <c r="H45" s="2"/>
-      <c r="I45" s="2"/>
-      <c r="J45" s="2"/>
-      <c r="K45" s="2"/>
-      <c r="L45" s="2"/>
-      <c r="M45" s="2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
-      <c r="H46" s="2"/>
-      <c r="I46" s="2"/>
-      <c r="J46" s="2"/>
-      <c r="K46" s="2"/>
-      <c r="L46" s="2"/>
-      <c r="M46" s="2"/>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
-      <c r="G47" s="2"/>
-      <c r="H47" s="2"/>
-      <c r="I47" s="2"/>
-      <c r="J47" s="2"/>
-      <c r="K47" s="2"/>
-      <c r="L47" s="2"/>
-      <c r="M47" s="2"/>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
-      <c r="D48" s="2"/>
-      <c r="E48" s="2"/>
-      <c r="F48" s="2"/>
-      <c r="G48" s="2"/>
-      <c r="H48" s="2"/>
-      <c r="I48" s="2"/>
-      <c r="J48" s="2"/>
-      <c r="K48" s="2"/>
-      <c r="L48" s="2"/>
-      <c r="M48" s="2"/>
-    </row>
-    <row r="49" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
-      <c r="E49" s="2"/>
-      <c r="F49" s="2"/>
-      <c r="G49" s="2"/>
-      <c r="H49" s="2"/>
-      <c r="I49" s="2"/>
-      <c r="J49" s="2"/>
-      <c r="K49" s="2"/>
-      <c r="L49" s="2"/>
-      <c r="M49" s="2"/>
-    </row>
-    <row r="50" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
-      <c r="E50" s="2"/>
-      <c r="F50" s="2"/>
-      <c r="G50" s="2"/>
-      <c r="H50" s="2"/>
-      <c r="I50" s="2"/>
-      <c r="J50" s="2"/>
-      <c r="K50" s="2"/>
-      <c r="L50" s="2"/>
-      <c r="M50" s="2"/>
-    </row>
-    <row r="51" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
-      <c r="E51" s="2"/>
-      <c r="F51" s="2"/>
-      <c r="G51" s="2"/>
-      <c r="H51" s="2"/>
-      <c r="I51" s="2"/>
-      <c r="J51" s="2"/>
-      <c r="K51" s="2"/>
-      <c r="L51" s="2"/>
-      <c r="M51" s="2"/>
-    </row>
-    <row r="52" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B52" s="2"/>
-      <c r="C52" s="2"/>
-      <c r="D52" s="2"/>
-      <c r="E52" s="2"/>
-      <c r="F52" s="2"/>
-      <c r="G52" s="2"/>
-      <c r="H52" s="2"/>
-      <c r="I52" s="2"/>
-      <c r="J52" s="2"/>
-      <c r="K52" s="2"/>
-      <c r="L52" s="2"/>
-      <c r="M52" s="2"/>
-    </row>
-    <row r="53" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B53" s="2"/>
-      <c r="C53" s="2"/>
-      <c r="D53" s="2"/>
-      <c r="E53" s="2"/>
-      <c r="F53" s="2"/>
-      <c r="G53" s="2"/>
-      <c r="H53" s="2"/>
-      <c r="I53" s="2"/>
-      <c r="J53" s="2"/>
-      <c r="K53" s="2"/>
-      <c r="L53" s="2"/>
-      <c r="M53" s="2"/>
-    </row>
-    <row r="54" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
-      <c r="D54" s="2"/>
-      <c r="E54" s="2"/>
-      <c r="F54" s="2"/>
-      <c r="G54" s="2"/>
-      <c r="H54" s="2"/>
-      <c r="I54" s="2"/>
-      <c r="J54" s="2"/>
-      <c r="K54" s="2"/>
-      <c r="L54" s="2"/>
-      <c r="M54" s="2"/>
-    </row>
-    <row r="55" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B55" s="2"/>
-      <c r="C55" s="2"/>
-      <c r="D55" s="2"/>
-      <c r="E55" s="2"/>
-      <c r="F55" s="2"/>
-      <c r="G55" s="2"/>
-      <c r="H55" s="2"/>
-      <c r="I55" s="2"/>
-      <c r="J55" s="2"/>
-      <c r="K55" s="2"/>
-      <c r="L55" s="2"/>
-      <c r="M55" s="2"/>
-    </row>
-    <row r="56" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
-      <c r="D56" s="2"/>
-      <c r="E56" s="2"/>
-      <c r="F56" s="2"/>
-      <c r="G56" s="2"/>
-      <c r="H56" s="2"/>
-      <c r="I56" s="2"/>
-      <c r="J56" s="2"/>
-      <c r="K56" s="2"/>
-      <c r="L56" s="2"/>
-      <c r="M56" s="2"/>
-    </row>
-    <row r="57" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B57" s="2"/>
-      <c r="C57" s="2"/>
-      <c r="D57" s="2"/>
-      <c r="E57" s="2"/>
-      <c r="F57" s="2"/>
-      <c r="G57" s="2"/>
-      <c r="H57" s="2"/>
-      <c r="I57" s="2"/>
-      <c r="J57" s="2"/>
-      <c r="K57" s="2"/>
-      <c r="L57" s="2"/>
-      <c r="M57" s="2"/>
-    </row>
-    <row r="58" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B58" s="2"/>
-      <c r="C58" s="2"/>
-      <c r="D58" s="2"/>
-      <c r="E58" s="2"/>
-      <c r="F58" s="2"/>
-      <c r="G58" s="2"/>
-      <c r="H58" s="2"/>
-      <c r="I58" s="2"/>
-      <c r="J58" s="2"/>
-      <c r="K58" s="2"/>
-      <c r="L58" s="2"/>
-      <c r="M58" s="2"/>
-    </row>
-    <row r="59" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
-      <c r="D59" s="2"/>
-      <c r="E59" s="2"/>
-      <c r="F59" s="2"/>
-      <c r="G59" s="2"/>
-      <c r="H59" s="2"/>
-      <c r="I59" s="2"/>
-      <c r="J59" s="2"/>
-      <c r="K59" s="2"/>
-      <c r="L59" s="2"/>
-      <c r="M59" s="2"/>
-    </row>
-    <row r="60" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B60" s="2"/>
-      <c r="C60" s="2"/>
-      <c r="D60" s="2"/>
-      <c r="E60" s="2"/>
-      <c r="F60" s="2"/>
-      <c r="G60" s="2"/>
-      <c r="H60" s="2"/>
-      <c r="I60" s="2"/>
-      <c r="J60" s="2"/>
-      <c r="K60" s="2"/>
-      <c r="L60" s="2"/>
-      <c r="M60" s="2"/>
-    </row>
-    <row r="61" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
-      <c r="D61" s="2"/>
-      <c r="E61" s="2"/>
-      <c r="F61" s="2"/>
-      <c r="G61" s="2"/>
-      <c r="H61" s="2"/>
-      <c r="I61" s="2"/>
-      <c r="J61" s="2"/>
-      <c r="K61" s="2"/>
-      <c r="L61" s="2"/>
-      <c r="M61" s="2"/>
-    </row>
-    <row r="62" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B62" s="2"/>
-      <c r="C62" s="2"/>
-      <c r="D62" s="2"/>
-      <c r="E62" s="2"/>
-      <c r="F62" s="2"/>
-      <c r="G62" s="2"/>
-      <c r="H62" s="2"/>
-      <c r="I62" s="2"/>
-      <c r="J62" s="2"/>
-      <c r="K62" s="2"/>
-      <c r="L62" s="2"/>
-      <c r="M62" s="2"/>
-    </row>
-    <row r="63" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B63" s="2"/>
-      <c r="C63" s="2"/>
-      <c r="D63" s="2"/>
-      <c r="E63" s="2"/>
-      <c r="F63" s="2"/>
-      <c r="G63" s="2"/>
-      <c r="H63" s="2"/>
-      <c r="I63" s="2"/>
-      <c r="J63" s="2"/>
-      <c r="K63" s="2"/>
-      <c r="L63" s="2"/>
-      <c r="M63" s="2"/>
-    </row>
-    <row r="64" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B64" s="2"/>
-      <c r="C64" s="2"/>
-      <c r="D64" s="2"/>
-      <c r="E64" s="2"/>
-      <c r="F64" s="2"/>
-      <c r="G64" s="2"/>
-      <c r="H64" s="2"/>
-      <c r="I64" s="2"/>
-      <c r="J64" s="2"/>
-      <c r="K64" s="2"/>
-      <c r="L64" s="2"/>
-      <c r="M64" s="2"/>
-    </row>
-    <row r="65" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B65" s="2"/>
-      <c r="C65" s="2"/>
-      <c r="D65" s="2"/>
-      <c r="E65" s="2"/>
-      <c r="F65" s="2"/>
-      <c r="G65" s="2"/>
-      <c r="H65" s="2"/>
-      <c r="I65" s="2"/>
-      <c r="J65" s="2"/>
-      <c r="K65" s="2"/>
-      <c r="L65" s="2"/>
-      <c r="M65" s="2"/>
-    </row>
-    <row r="66" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B66" s="2"/>
-      <c r="C66" s="2"/>
-      <c r="D66" s="2"/>
-      <c r="E66" s="2"/>
-      <c r="F66" s="2"/>
-      <c r="G66" s="2"/>
-      <c r="H66" s="2"/>
-      <c r="I66" s="2"/>
-      <c r="J66" s="2"/>
-      <c r="K66" s="2"/>
-      <c r="L66" s="2"/>
-      <c r="M66" s="2"/>
-    </row>
-    <row r="67" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B67" s="2"/>
-      <c r="C67" s="2"/>
-      <c r="D67" s="2"/>
-      <c r="E67" s="2"/>
-      <c r="F67" s="2"/>
-      <c r="G67" s="2"/>
-      <c r="H67" s="2"/>
-      <c r="I67" s="2"/>
-      <c r="J67" s="2"/>
-      <c r="K67" s="2"/>
-      <c r="L67" s="2"/>
-      <c r="M67" s="2"/>
-    </row>
-    <row r="68" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B68" s="2"/>
-      <c r="C68" s="2"/>
-      <c r="D68" s="2"/>
-      <c r="E68" s="2"/>
-      <c r="F68" s="2"/>
-      <c r="G68" s="2"/>
-      <c r="H68" s="2"/>
-      <c r="I68" s="2"/>
-      <c r="J68" s="2"/>
-      <c r="K68" s="2"/>
-      <c r="L68" s="2"/>
-      <c r="M68" s="2"/>
-    </row>
-    <row r="69" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B69" s="2"/>
-      <c r="C69" s="2"/>
-      <c r="D69" s="2"/>
-      <c r="E69" s="2"/>
-      <c r="F69" s="2"/>
-      <c r="G69" s="2"/>
-      <c r="H69" s="2"/>
-      <c r="I69" s="2"/>
-      <c r="J69" s="2"/>
-      <c r="K69" s="2"/>
-      <c r="L69" s="2"/>
-      <c r="M69" s="2"/>
-    </row>
-    <row r="70" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B70" s="2"/>
-      <c r="C70" s="2"/>
-      <c r="D70" s="2"/>
-      <c r="E70" s="2"/>
-      <c r="F70" s="2"/>
-      <c r="G70" s="2"/>
-      <c r="H70" s="2"/>
-      <c r="I70" s="2"/>
-      <c r="J70" s="2"/>
-      <c r="K70" s="2"/>
-      <c r="L70" s="2"/>
-      <c r="M70" s="2"/>
-    </row>
-    <row r="71" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B71" s="2"/>
-      <c r="C71" s="2"/>
-      <c r="D71" s="2"/>
-      <c r="E71" s="2"/>
-      <c r="F71" s="2"/>
-      <c r="G71" s="2"/>
-      <c r="H71" s="2"/>
-      <c r="I71" s="2"/>
-      <c r="J71" s="2"/>
-      <c r="K71" s="2"/>
-      <c r="L71" s="2"/>
-      <c r="M71" s="2"/>
-    </row>
-    <row r="72" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B72" s="2"/>
-      <c r="C72" s="2"/>
-      <c r="D72" s="2"/>
-      <c r="E72" s="2"/>
-      <c r="F72" s="2"/>
-      <c r="G72" s="2"/>
-      <c r="H72" s="2"/>
-      <c r="I72" s="2"/>
-      <c r="J72" s="2"/>
-      <c r="K72" s="2"/>
-      <c r="L72" s="2"/>
-      <c r="M72" s="2"/>
-    </row>
-    <row r="73" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B73" s="2"/>
-      <c r="C73" s="2"/>
-      <c r="D73" s="2"/>
-      <c r="E73" s="2"/>
-      <c r="F73" s="2"/>
-      <c r="G73" s="2"/>
-      <c r="H73" s="2"/>
-      <c r="I73" s="2"/>
-      <c r="J73" s="2"/>
-      <c r="K73" s="2"/>
-      <c r="L73" s="2"/>
-      <c r="M73" s="2"/>
-    </row>
-    <row r="74" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B74" s="2"/>
-      <c r="C74" s="2"/>
-      <c r="D74" s="2"/>
-      <c r="E74" s="2"/>
-      <c r="F74" s="2"/>
-      <c r="G74" s="2"/>
-      <c r="H74" s="2"/>
-      <c r="I74" s="2"/>
-      <c r="J74" s="2"/>
-      <c r="K74" s="2"/>
-      <c r="L74" s="2"/>
-      <c r="M74" s="2"/>
-    </row>
-    <row r="75" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B75" s="2"/>
-      <c r="C75" s="2"/>
-      <c r="D75" s="2"/>
-      <c r="E75" s="2"/>
-      <c r="F75" s="2"/>
-      <c r="G75" s="2"/>
-      <c r="H75" s="2"/>
-      <c r="I75" s="2"/>
-      <c r="J75" s="2"/>
-      <c r="K75" s="2"/>
-      <c r="L75" s="2"/>
-      <c r="M75" s="2"/>
-    </row>
-    <row r="76" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B76" s="2"/>
-      <c r="C76" s="2"/>
-      <c r="D76" s="2"/>
-      <c r="E76" s="2"/>
-      <c r="F76" s="2"/>
-      <c r="G76" s="2"/>
-      <c r="H76" s="2"/>
-      <c r="I76" s="2"/>
-      <c r="J76" s="2"/>
-      <c r="K76" s="2"/>
-      <c r="L76" s="2"/>
-      <c r="M76" s="2"/>
-    </row>
-    <row r="77" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B77" s="2"/>
-      <c r="C77" s="2"/>
-      <c r="D77" s="2"/>
-      <c r="E77" s="2"/>
-      <c r="F77" s="2"/>
-      <c r="G77" s="2"/>
-      <c r="H77" s="2"/>
-      <c r="I77" s="2"/>
-      <c r="J77" s="2"/>
-      <c r="K77" s="2"/>
-      <c r="L77" s="2"/>
-      <c r="M77" s="2"/>
-    </row>
-    <row r="78" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B78" s="2"/>
-      <c r="C78" s="2"/>
-      <c r="D78" s="2"/>
-      <c r="E78" s="2"/>
-      <c r="F78" s="2"/>
-      <c r="G78" s="2"/>
-      <c r="H78" s="2"/>
-      <c r="I78" s="2"/>
-      <c r="J78" s="2"/>
-      <c r="K78" s="2"/>
-      <c r="L78" s="2"/>
-      <c r="M78" s="2"/>
-    </row>
-    <row r="79" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B79" s="2"/>
-      <c r="C79" s="2"/>
-      <c r="D79" s="2"/>
-      <c r="E79" s="2"/>
-      <c r="F79" s="2"/>
-      <c r="G79" s="2"/>
-      <c r="H79" s="2"/>
-      <c r="I79" s="2"/>
-      <c r="J79" s="2"/>
-      <c r="K79" s="2"/>
-      <c r="L79" s="2"/>
-      <c r="M79" s="2"/>
-    </row>
-    <row r="80" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B80" s="2"/>
-      <c r="C80" s="2"/>
-      <c r="D80" s="2"/>
-      <c r="E80" s="2"/>
-      <c r="F80" s="2"/>
-      <c r="G80" s="2"/>
-      <c r="H80" s="2"/>
-      <c r="I80" s="2"/>
-      <c r="J80" s="2"/>
-      <c r="K80" s="2"/>
-      <c r="L80" s="2"/>
-      <c r="M80" s="2"/>
-    </row>
-    <row r="81" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B81" s="2"/>
-      <c r="C81" s="2"/>
-      <c r="D81" s="2"/>
-      <c r="E81" s="2"/>
-      <c r="F81" s="2"/>
-      <c r="G81" s="2"/>
-      <c r="H81" s="2"/>
-      <c r="I81" s="2"/>
-      <c r="J81" s="2"/>
-      <c r="K81" s="2"/>
-      <c r="L81" s="2"/>
-      <c r="M81" s="2"/>
-    </row>
-    <row r="82" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B82" s="2"/>
-      <c r="C82" s="2"/>
-      <c r="D82" s="2"/>
-      <c r="E82" s="2"/>
-      <c r="F82" s="2"/>
-      <c r="G82" s="2"/>
-      <c r="H82" s="2"/>
-      <c r="I82" s="2"/>
-      <c r="J82" s="2"/>
-      <c r="K82" s="2"/>
-      <c r="L82" s="2"/>
-      <c r="M82" s="2"/>
-    </row>
-    <row r="83" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B83" s="2"/>
-      <c r="C83" s="2"/>
-      <c r="D83" s="2"/>
-      <c r="E83" s="2"/>
-      <c r="F83" s="2"/>
-      <c r="G83" s="2"/>
-      <c r="H83" s="2"/>
-      <c r="I83" s="2"/>
-      <c r="J83" s="2"/>
-      <c r="K83" s="2"/>
-      <c r="L83" s="2"/>
-      <c r="M83" s="2"/>
-    </row>
-    <row r="84" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B84" s="2"/>
-      <c r="C84" s="2"/>
-      <c r="D84" s="2"/>
-      <c r="E84" s="2"/>
-      <c r="F84" s="2"/>
-      <c r="G84" s="2"/>
-      <c r="H84" s="2"/>
-      <c r="I84" s="2"/>
-      <c r="J84" s="2"/>
-      <c r="K84" s="2"/>
-      <c r="L84" s="2"/>
-      <c r="M84" s="2"/>
-    </row>
-    <row r="85" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B85" s="2"/>
-      <c r="C85" s="2"/>
-      <c r="D85" s="2"/>
-      <c r="E85" s="2"/>
-      <c r="F85" s="2"/>
-      <c r="G85" s="2"/>
-      <c r="H85" s="2"/>
-      <c r="I85" s="2"/>
-      <c r="J85" s="2"/>
-      <c r="K85" s="2"/>
-      <c r="L85" s="2"/>
-      <c r="M85" s="2"/>
-    </row>
-    <row r="86" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B86" s="2"/>
-      <c r="C86" s="2"/>
-      <c r="D86" s="2"/>
-      <c r="E86" s="2"/>
-      <c r="F86" s="2"/>
-      <c r="G86" s="2"/>
-      <c r="H86" s="2"/>
-      <c r="I86" s="2"/>
-      <c r="J86" s="2"/>
-      <c r="K86" s="2"/>
-      <c r="L86" s="2"/>
-      <c r="M86" s="2"/>
-    </row>
-    <row r="87" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B87" s="2"/>
-      <c r="C87" s="2"/>
-      <c r="D87" s="2"/>
-      <c r="E87" s="2"/>
-      <c r="F87" s="2"/>
-      <c r="G87" s="2"/>
-      <c r="H87" s="2"/>
-      <c r="I87" s="2"/>
-      <c r="J87" s="2"/>
-      <c r="K87" s="2"/>
-      <c r="L87" s="2"/>
-      <c r="M87" s="2"/>
-    </row>
-    <row r="88" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B88" s="2"/>
-      <c r="C88" s="2"/>
-      <c r="D88" s="2"/>
-      <c r="E88" s="2"/>
-      <c r="F88" s="2"/>
-      <c r="G88" s="2"/>
-      <c r="H88" s="2"/>
-      <c r="I88" s="2"/>
-      <c r="J88" s="2"/>
-      <c r="K88" s="2"/>
-      <c r="L88" s="2"/>
-      <c r="M88" s="2"/>
-    </row>
-    <row r="89" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B89" s="2"/>
-      <c r="C89" s="2"/>
-      <c r="D89" s="2"/>
-      <c r="E89" s="2"/>
-      <c r="F89" s="2"/>
-      <c r="G89" s="2"/>
-      <c r="H89" s="2"/>
-      <c r="I89" s="2"/>
-      <c r="J89" s="2"/>
-      <c r="K89" s="2"/>
-      <c r="L89" s="2"/>
-      <c r="M89" s="2"/>
-    </row>
-    <row r="90" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B90" s="2"/>
-      <c r="C90" s="2"/>
-      <c r="D90" s="2"/>
-      <c r="E90" s="2"/>
-      <c r="F90" s="2"/>
-      <c r="G90" s="2"/>
-      <c r="H90" s="2"/>
-      <c r="I90" s="2"/>
-      <c r="J90" s="2"/>
-      <c r="K90" s="2"/>
-      <c r="L90" s="2"/>
-      <c r="M90" s="2"/>
-    </row>
-    <row r="91" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B91" s="2"/>
-      <c r="C91" s="2"/>
-      <c r="D91" s="2"/>
-      <c r="E91" s="2"/>
-      <c r="F91" s="2"/>
-      <c r="G91" s="2"/>
-      <c r="H91" s="2"/>
-      <c r="I91" s="2"/>
-      <c r="J91" s="2"/>
-      <c r="K91" s="2"/>
-      <c r="L91" s="2"/>
-      <c r="M91" s="2"/>
-    </row>
-    <row r="92" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B92" s="2"/>
-      <c r="C92" s="2"/>
-      <c r="D92" s="2"/>
-      <c r="E92" s="2"/>
-      <c r="F92" s="2"/>
-      <c r="G92" s="2"/>
-      <c r="H92" s="2"/>
-      <c r="I92" s="2"/>
-      <c r="J92" s="2"/>
-      <c r="K92" s="2"/>
-      <c r="L92" s="2"/>
-      <c r="M92" s="2"/>
-    </row>
-    <row r="93" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B93" s="2"/>
-      <c r="C93" s="2"/>
-      <c r="D93" s="2"/>
-      <c r="E93" s="2"/>
-      <c r="F93" s="2"/>
-      <c r="G93" s="2"/>
-      <c r="H93" s="2"/>
-      <c r="I93" s="2"/>
-      <c r="J93" s="2"/>
-      <c r="K93" s="2"/>
-      <c r="L93" s="2"/>
-      <c r="M93" s="2"/>
-    </row>
-    <row r="94" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B94" s="2"/>
-      <c r="C94" s="2"/>
-      <c r="D94" s="2"/>
-      <c r="E94" s="2"/>
-      <c r="F94" s="2"/>
-      <c r="G94" s="2"/>
-      <c r="H94" s="2"/>
-      <c r="I94" s="2"/>
-      <c r="J94" s="2"/>
-      <c r="K94" s="2"/>
-      <c r="L94" s="2"/>
-      <c r="M94" s="2"/>
-    </row>
-    <row r="95" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B95" s="2"/>
-      <c r="C95" s="2"/>
-      <c r="D95" s="2"/>
-      <c r="E95" s="2"/>
-      <c r="F95" s="2"/>
-      <c r="G95" s="2"/>
-      <c r="H95" s="2"/>
-      <c r="I95" s="2"/>
-      <c r="J95" s="2"/>
-      <c r="K95" s="2"/>
-      <c r="L95" s="2"/>
-      <c r="M95" s="2"/>
-    </row>
-    <row r="96" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B96" s="2"/>
-      <c r="C96" s="2"/>
-      <c r="D96" s="2"/>
-      <c r="E96" s="2"/>
-      <c r="F96" s="2"/>
-      <c r="G96" s="2"/>
-      <c r="H96" s="2"/>
-      <c r="I96" s="2"/>
-      <c r="J96" s="2"/>
-      <c r="K96" s="2"/>
-      <c r="L96" s="2"/>
-      <c r="M96" s="2"/>
-    </row>
-    <row r="97" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B97" s="2"/>
-      <c r="C97" s="2"/>
-      <c r="D97" s="2"/>
-      <c r="E97" s="2"/>
-      <c r="F97" s="2"/>
-      <c r="G97" s="2"/>
-      <c r="H97" s="2"/>
-      <c r="I97" s="2"/>
-      <c r="J97" s="2"/>
-      <c r="K97" s="2"/>
-      <c r="L97" s="2"/>
-      <c r="M97" s="2"/>
-    </row>
-    <row r="98" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B98" s="2"/>
-      <c r="C98" s="2"/>
-      <c r="D98" s="2"/>
-      <c r="E98" s="2"/>
-      <c r="F98" s="2"/>
-      <c r="G98" s="2"/>
-      <c r="H98" s="2"/>
-      <c r="I98" s="2"/>
-      <c r="J98" s="2"/>
-      <c r="K98" s="2"/>
-      <c r="L98" s="2"/>
-      <c r="M98" s="2"/>
-    </row>
-    <row r="99" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B99" s="2"/>
-      <c r="C99" s="2"/>
-      <c r="D99" s="2"/>
-      <c r="E99" s="2"/>
-      <c r="F99" s="2"/>
-      <c r="G99" s="2"/>
-      <c r="H99" s="2"/>
-      <c r="I99" s="2"/>
-      <c r="J99" s="2"/>
-      <c r="K99" s="2"/>
-      <c r="L99" s="2"/>
-      <c r="M99" s="2"/>
-    </row>
-    <row r="100" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B100" s="2"/>
-      <c r="C100" s="2"/>
-      <c r="D100" s="2"/>
-      <c r="E100" s="2"/>
-      <c r="F100" s="2"/>
-      <c r="G100" s="2"/>
-      <c r="H100" s="2"/>
-      <c r="I100" s="2"/>
-      <c r="J100" s="2"/>
-      <c r="K100" s="2"/>
-      <c r="L100" s="2"/>
-      <c r="M100" s="2"/>
-    </row>
-    <row r="101" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B101" s="2"/>
-      <c r="C101" s="2"/>
-      <c r="D101" s="2"/>
-      <c r="E101" s="2"/>
-      <c r="F101" s="2"/>
-      <c r="G101" s="2"/>
-      <c r="H101" s="2"/>
-      <c r="I101" s="2"/>
-      <c r="J101" s="2"/>
-      <c r="K101" s="2"/>
-      <c r="L101" s="2"/>
-      <c r="M101" s="2"/>
-    </row>
-    <row r="102" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B102" s="2"/>
-      <c r="C102" s="2"/>
-      <c r="D102" s="2"/>
-      <c r="E102" s="2"/>
-      <c r="F102" s="2"/>
-      <c r="G102" s="2"/>
-      <c r="H102" s="2"/>
-      <c r="I102" s="2"/>
-      <c r="J102" s="2"/>
-      <c r="K102" s="2"/>
-      <c r="L102" s="2"/>
-      <c r="M102" s="2"/>
-    </row>
-    <row r="103" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B103" s="2"/>
-      <c r="C103" s="2"/>
-      <c r="D103" s="2"/>
-      <c r="E103" s="2"/>
-      <c r="F103" s="2"/>
-      <c r="G103" s="2"/>
-      <c r="H103" s="2"/>
-      <c r="I103" s="2"/>
-      <c r="J103" s="2"/>
-      <c r="K103" s="2"/>
-      <c r="L103" s="2"/>
-      <c r="M103" s="2"/>
-    </row>
-    <row r="104" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B104" s="2"/>
-      <c r="C104" s="2"/>
-      <c r="D104" s="2"/>
-      <c r="E104" s="2"/>
-      <c r="F104" s="2"/>
-      <c r="G104" s="2"/>
-      <c r="H104" s="2"/>
-      <c r="I104" s="2"/>
-      <c r="J104" s="2"/>
-      <c r="K104" s="2"/>
-      <c r="L104" s="2"/>
-      <c r="M104" s="2"/>
-    </row>
-    <row r="105" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B105" s="2"/>
-      <c r="C105" s="2"/>
-      <c r="D105" s="2"/>
-      <c r="E105" s="2"/>
-      <c r="F105" s="2"/>
-      <c r="G105" s="2"/>
-      <c r="H105" s="2"/>
-      <c r="I105" s="2"/>
-      <c r="J105" s="2"/>
-      <c r="K105" s="2"/>
-      <c r="L105" s="2"/>
-      <c r="M105" s="2"/>
-    </row>
-    <row r="106" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B106" s="2"/>
-      <c r="C106" s="2"/>
-      <c r="D106" s="2"/>
-      <c r="E106" s="2"/>
-      <c r="F106" s="2"/>
-      <c r="G106" s="2"/>
-      <c r="H106" s="2"/>
-      <c r="I106" s="2"/>
-      <c r="J106" s="2"/>
-      <c r="K106" s="2"/>
-      <c r="L106" s="2"/>
-      <c r="M106" s="2"/>
-    </row>
-    <row r="107" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B107" s="2"/>
-      <c r="C107" s="2"/>
-      <c r="D107" s="2"/>
-      <c r="E107" s="2"/>
-      <c r="F107" s="2"/>
-      <c r="G107" s="2"/>
-      <c r="H107" s="2"/>
-      <c r="I107" s="2"/>
-      <c r="J107" s="2"/>
-      <c r="K107" s="2"/>
-      <c r="L107" s="2"/>
-      <c r="M107" s="2"/>
-    </row>
-    <row r="108" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B108" s="2"/>
-      <c r="C108" s="2"/>
-      <c r="D108" s="2"/>
-      <c r="E108" s="2"/>
-      <c r="F108" s="2"/>
-      <c r="G108" s="2"/>
-      <c r="H108" s="2"/>
-      <c r="I108" s="2"/>
-      <c r="J108" s="2"/>
-      <c r="K108" s="2"/>
-      <c r="L108" s="2"/>
-      <c r="M108" s="2"/>
-    </row>
-    <row r="109" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B109" s="2"/>
-      <c r="C109" s="2"/>
-      <c r="D109" s="2"/>
-      <c r="E109" s="2"/>
-      <c r="F109" s="2"/>
-      <c r="G109" s="2"/>
-      <c r="H109" s="2"/>
-      <c r="I109" s="2"/>
-      <c r="J109" s="2"/>
-      <c r="K109" s="2"/>
-      <c r="L109" s="2"/>
-      <c r="M109" s="2"/>
-    </row>
-    <row r="110" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B110" s="2"/>
-      <c r="C110" s="2"/>
-      <c r="D110" s="2"/>
-      <c r="E110" s="2"/>
-      <c r="F110" s="2"/>
-      <c r="G110" s="2"/>
-      <c r="H110" s="2"/>
-      <c r="I110" s="2"/>
-      <c r="J110" s="2"/>
-      <c r="K110" s="2"/>
-      <c r="L110" s="2"/>
-      <c r="M110" s="2"/>
-    </row>
-    <row r="111" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B111" s="2"/>
-      <c r="C111" s="2"/>
-      <c r="D111" s="2"/>
-      <c r="E111" s="2"/>
-      <c r="F111" s="2"/>
-      <c r="G111" s="2"/>
-      <c r="H111" s="2"/>
-      <c r="I111" s="2"/>
-      <c r="J111" s="2"/>
-      <c r="K111" s="2"/>
-      <c r="L111" s="2"/>
-      <c r="M111" s="2"/>
-    </row>
-    <row r="112" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B112" s="2"/>
-      <c r="C112" s="2"/>
-      <c r="D112" s="2"/>
-      <c r="E112" s="2"/>
-      <c r="F112" s="2"/>
-      <c r="G112" s="2"/>
-      <c r="H112" s="2"/>
-      <c r="I112" s="2"/>
-      <c r="J112" s="2"/>
-      <c r="K112" s="2"/>
-      <c r="L112" s="2"/>
-      <c r="M112" s="2"/>
-    </row>
-    <row r="113" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B113" s="2"/>
-      <c r="C113" s="2"/>
-      <c r="D113" s="2"/>
-      <c r="E113" s="2"/>
-      <c r="F113" s="2"/>
-      <c r="G113" s="2"/>
-      <c r="H113" s="2"/>
-      <c r="I113" s="2"/>
-      <c r="J113" s="2"/>
-      <c r="K113" s="2"/>
-      <c r="L113" s="2"/>
-      <c r="M113" s="2"/>
-    </row>
-    <row r="114" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B114" s="2"/>
-      <c r="C114" s="2"/>
-      <c r="D114" s="2"/>
-      <c r="E114" s="2"/>
-      <c r="F114" s="2"/>
-      <c r="G114" s="2"/>
-      <c r="H114" s="2"/>
-      <c r="I114" s="2"/>
-      <c r="J114" s="2"/>
-      <c r="K114" s="2"/>
-      <c r="L114" s="2"/>
-      <c r="M114" s="2"/>
-    </row>
-    <row r="115" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B115" s="2"/>
-      <c r="C115" s="2"/>
-      <c r="D115" s="2"/>
-      <c r="E115" s="2"/>
-      <c r="F115" s="2"/>
-      <c r="G115" s="2"/>
-      <c r="H115" s="2"/>
-      <c r="I115" s="2"/>
-      <c r="J115" s="2"/>
-      <c r="K115" s="2"/>
-      <c r="L115" s="2"/>
-      <c r="M115" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="8.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.9296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.06640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -8239,7 +8166,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
         <v>105</v>
       </c>
@@ -8259,7 +8186,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
         <v>104</v>
       </c>
@@ -8279,7 +8206,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="6" t="s">
         <v>108</v>
       </c>
@@ -8299,7 +8226,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FEAT: preliminary work for scanning date! values.
</commit_message>
<xml_diff>
--- a/docs/lexer/lexer-FSM.xlsx
+++ b/docs/lexer/lexer-FSM.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Red\docs\lexer\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8674A13-C6B5-4039-9935-C28BC8358BB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1035" yWindow="0" windowWidth="21270" windowHeight="14400" tabRatio="564" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1040" yWindow="0" windowWidth="21270" windowHeight="14400" tabRatio="564"/>
   </bookViews>
   <sheets>
     <sheet name="transitions" sheetId="3" r:id="rId1"/>
@@ -22,12 +16,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>dk</author>
   </authors>
   <commentList>
-    <comment ref="D6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="D6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -605,7 +599,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -871,7 +865,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -904,26 +898,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -956,23 +933,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1148,23 +1108,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="AH26" sqref="AH26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.73046875" customWidth="1"/>
-    <col min="5" max="5" width="9.73046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="12" width="9.73046875" customWidth="1"/>
-    <col min="13" max="13" width="9.9296875" bestFit="1" customWidth="1"/>
-    <col min="14" max="34" width="9.73046875" customWidth="1"/>
+    <col min="1" max="1" width="10.36328125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" customWidth="1"/>
+    <col min="5" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="9.7265625" customWidth="1"/>
+    <col min="13" max="13" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="34" width="9.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -1269,7 +1229,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
@@ -1373,7 +1333,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A3" s="12" t="s">
         <v>70</v>
       </c>
@@ -1477,7 +1437,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A4" s="12" t="s">
         <v>71</v>
       </c>
@@ -1581,7 +1541,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A5" s="12" t="s">
         <v>1</v>
       </c>
@@ -1685,7 +1645,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A6" s="12" t="s">
         <v>2</v>
       </c>
@@ -1789,7 +1749,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A7" s="12" t="s">
         <v>75</v>
       </c>
@@ -1893,7 +1853,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A8" s="12" t="s">
         <v>3</v>
       </c>
@@ -1997,7 +1957,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A9" s="12" t="s">
         <v>4</v>
       </c>
@@ -2101,7 +2061,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A10" s="12" t="s">
         <v>110</v>
       </c>
@@ -2205,7 +2165,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A11" s="12" t="s">
         <v>111</v>
       </c>
@@ -2309,7 +2269,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A12" s="12" t="s">
         <v>112</v>
       </c>
@@ -2413,7 +2373,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A13" s="12" t="s">
         <v>5</v>
       </c>
@@ -2517,7 +2477,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A14" s="12" t="s">
         <v>6</v>
       </c>
@@ -2621,7 +2581,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A15" s="12" t="s">
         <v>7</v>
       </c>
@@ -2725,7 +2685,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A16" s="12" t="s">
         <v>72</v>
       </c>
@@ -2829,7 +2789,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A17" s="12" t="s">
         <v>8</v>
       </c>
@@ -2933,7 +2893,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A18" s="12" t="s">
         <v>9</v>
       </c>
@@ -3037,7 +2997,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A19" s="12" t="s">
         <v>10</v>
       </c>
@@ -3141,7 +3101,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A20" s="12" t="s">
         <v>11</v>
       </c>
@@ -3245,7 +3205,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A21" s="12" t="s">
         <v>12</v>
       </c>
@@ -3349,7 +3309,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A22" s="12" t="s">
         <v>87</v>
       </c>
@@ -3453,7 +3413,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A23" s="12" t="s">
         <v>13</v>
       </c>
@@ -3557,7 +3517,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A24" s="12" t="s">
         <v>14</v>
       </c>
@@ -3661,7 +3621,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A25" s="12" t="s">
         <v>15</v>
       </c>
@@ -3765,7 +3725,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A26" s="12" t="s">
         <v>16</v>
       </c>
@@ -3866,10 +3826,10 @@
         <v>64</v>
       </c>
       <c r="AH26" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.45">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="27" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A27" s="12" t="s">
         <v>17</v>
       </c>
@@ -3973,7 +3933,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A28" s="12" t="s">
         <v>18</v>
       </c>
@@ -4077,7 +4037,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A29" s="12" t="s">
         <v>19</v>
       </c>
@@ -4181,7 +4141,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A30" s="12" t="s">
         <v>20</v>
       </c>
@@ -4285,7 +4245,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A31" s="12" t="s">
         <v>22</v>
       </c>
@@ -4389,7 +4349,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A32" s="12" t="s">
         <v>23</v>
       </c>
@@ -4493,7 +4453,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A33" s="12" t="s">
         <v>24</v>
       </c>
@@ -4597,7 +4557,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A34" s="12" t="s">
         <v>25</v>
       </c>
@@ -4701,7 +4661,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="35" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A35" s="12" t="s">
         <v>26</v>
       </c>
@@ -4805,7 +4765,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A36" s="12" t="s">
         <v>27</v>
       </c>
@@ -4909,7 +4869,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A37" s="12" t="s">
         <v>28</v>
       </c>
@@ -5013,7 +4973,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="38" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A38" s="12" t="s">
         <v>29</v>
       </c>
@@ -5117,7 +5077,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A39" s="12" t="s">
         <v>30</v>
       </c>
@@ -5221,7 +5181,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A40" s="12" t="s">
         <v>31</v>
       </c>
@@ -5325,7 +5285,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="41" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A41" s="12" t="s">
         <v>32</v>
       </c>
@@ -5429,7 +5389,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="42" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A42" s="12" t="s">
         <v>97</v>
       </c>
@@ -5533,7 +5493,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="43" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A43" s="12" t="s">
         <v>33</v>
       </c>
@@ -5637,7 +5597,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="44" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A44" s="12" t="s">
         <v>21</v>
       </c>
@@ -5741,7 +5701,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="45" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A45" s="13" t="s">
         <v>113</v>
       </c>
@@ -5845,7 +5805,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="46" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A46" s="12" t="s">
         <v>114</v>
       </c>
@@ -5949,7 +5909,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="47" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A47" s="12" t="s">
         <v>115</v>
       </c>
@@ -6053,7 +6013,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="48" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A48" s="12" t="s">
         <v>116</v>
       </c>
@@ -6157,7 +6117,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="49" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A49" s="12" t="s">
         <v>117</v>
       </c>
@@ -6268,18 +6228,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -6321,7 +6281,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A2" s="13" t="s">
         <v>129</v>
       </c>
@@ -6362,7 +6322,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A3" s="12" t="s">
         <v>130</v>
       </c>
@@ -6403,7 +6363,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A4" s="12" t="s">
         <v>131</v>
       </c>
@@ -6444,7 +6404,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A5" s="12" t="s">
         <v>132</v>
       </c>
@@ -6485,7 +6445,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A6" s="16" t="s">
         <v>133</v>
       </c>
@@ -6526,7 +6486,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A7" s="16" t="s">
         <v>158</v>
       </c>
@@ -6567,7 +6527,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A8" s="16" t="s">
         <v>134</v>
       </c>
@@ -6608,7 +6568,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A9" s="15" t="s">
         <v>135</v>
       </c>
@@ -6649,7 +6609,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A10" s="15" t="s">
         <v>136</v>
       </c>
@@ -6690,7 +6650,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A11" s="16" t="s">
         <v>137</v>
       </c>
@@ -6731,7 +6691,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A12" s="16" t="s">
         <v>138</v>
       </c>
@@ -6772,7 +6732,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A13" s="15" t="s">
         <v>139</v>
       </c>
@@ -6813,7 +6773,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A14" s="15" t="s">
         <v>140</v>
       </c>
@@ -6854,7 +6814,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A15" s="15" t="s">
         <v>141</v>
       </c>
@@ -6895,7 +6855,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A16" s="16" t="s">
         <v>142</v>
       </c>
@@ -6936,7 +6896,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A17" s="15" t="s">
         <v>143</v>
       </c>
@@ -6977,7 +6937,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A18" s="16" t="s">
         <v>144</v>
       </c>
@@ -7018,7 +6978,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A19" s="15" t="s">
         <v>145</v>
       </c>
@@ -7059,7 +7019,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A20" s="16" t="s">
         <v>160</v>
       </c>
@@ -7100,7 +7060,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A21" s="16" t="s">
         <v>161</v>
       </c>
@@ -7141,7 +7101,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A22" s="15" t="s">
         <v>146</v>
       </c>
@@ -7182,7 +7142,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A23" s="15" t="s">
         <v>147</v>
       </c>
@@ -7223,7 +7183,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A24" s="16" t="s">
         <v>148</v>
       </c>
@@ -7264,7 +7224,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A25" s="15" t="s">
         <v>149</v>
       </c>
@@ -7305,7 +7265,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A26" s="16" t="s">
         <v>162</v>
       </c>
@@ -7346,7 +7306,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A27" s="16" t="s">
         <v>163</v>
       </c>
@@ -7387,7 +7347,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A28" s="16" t="s">
         <v>164</v>
       </c>
@@ -7428,7 +7388,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A29" s="16" t="s">
         <v>165</v>
       </c>
@@ -7469,7 +7429,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A30" s="13" t="s">
         <v>150</v>
       </c>
@@ -7510,7 +7470,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A31" s="15" t="s">
         <v>166</v>
       </c>
@@ -7551,7 +7511,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A32" s="16" t="s">
         <v>151</v>
       </c>
@@ -7592,7 +7552,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A33" s="15" t="s">
         <v>167</v>
       </c>
@@ -7633,7 +7593,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A34" s="16" t="s">
         <v>168</v>
       </c>
@@ -7674,7 +7634,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A35" s="15" t="s">
         <v>152</v>
       </c>
@@ -7715,7 +7675,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A36" s="16" t="s">
         <v>169</v>
       </c>
@@ -7756,7 +7716,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A37" s="15" t="s">
         <v>170</v>
       </c>
@@ -7797,7 +7757,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A38" s="16" t="s">
         <v>153</v>
       </c>
@@ -7838,7 +7798,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A39" s="15" t="s">
         <v>171</v>
       </c>
@@ -7879,7 +7839,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A40" s="15" t="s">
         <v>172</v>
       </c>
@@ -7920,7 +7880,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A41" s="15" t="s">
         <v>154</v>
       </c>
@@ -7961,7 +7921,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A42" s="15" t="s">
         <v>155</v>
       </c>
@@ -8002,7 +7962,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A43" s="16" t="s">
         <v>156</v>
       </c>
@@ -8043,7 +8003,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A44" s="16" t="s">
         <v>174</v>
       </c>
@@ -8133,19 +8093,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.9296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.06640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.19921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -8166,7 +8126,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
         <v>105</v>
       </c>
@@ -8186,7 +8146,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
         <v>104</v>
       </c>
@@ -8206,7 +8166,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A4" s="6" t="s">
         <v>108</v>
       </c>
@@ -8226,7 +8186,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A5" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FEAT: numerous fixes and improvements to the date! parsing FSM.
</commit_message>
<xml_diff>
--- a/docs/lexer/lexer-FSM.xlsx
+++ b/docs/lexer/lexer-FSM.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Red\docs\lexer\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA719BFA-F441-4081-91D1-9CF8F5E587D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="0" windowWidth="21270" windowHeight="14400" tabRatio="564"/>
+    <workbookView xWindow="-28095" yWindow="150" windowWidth="17025" windowHeight="15015" tabRatio="564" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="transitions" sheetId="3" r:id="rId1"/>
@@ -16,12 +22,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>dk</author>
   </authors>
   <commentList>
-    <comment ref="D6" authorId="0">
+    <comment ref="D6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -51,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2272" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2246" uniqueCount="181">
   <si>
     <t>S_START</t>
   </si>
@@ -479,15 +485,9 @@
     <t>S_DT_YWW</t>
   </si>
   <si>
-    <t>F_DT_WEEK</t>
-  </si>
-  <si>
     <t>S_DT_WD</t>
   </si>
   <si>
-    <t>F_DT_YWWD</t>
-  </si>
-  <si>
     <t>S_DT_YMON</t>
   </si>
   <si>
@@ -594,12 +594,18 @@
   </si>
   <si>
     <t>T_DT_DMYEAR</t>
+  </si>
+  <si>
+    <t>T_DT_YWWD</t>
+  </si>
+  <si>
+    <t>T_DT_WEEK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -865,7 +871,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -898,9 +904,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -933,6 +956,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1108,23 +1148,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="AH26" sqref="AH26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.36328125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" customWidth="1"/>
-    <col min="5" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="12" width="9.7265625" customWidth="1"/>
-    <col min="13" max="13" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="14" max="34" width="9.7265625" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.73046875" customWidth="1"/>
+    <col min="5" max="5" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="9.73046875" customWidth="1"/>
+    <col min="13" max="13" width="9.9296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="34" width="9.73046875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -1229,7 +1269,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
@@ -1333,7 +1373,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A3" s="12" t="s">
         <v>70</v>
       </c>
@@ -1437,7 +1477,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A4" s="12" t="s">
         <v>71</v>
       </c>
@@ -1541,7 +1581,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A5" s="12" t="s">
         <v>1</v>
       </c>
@@ -1645,7 +1685,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A6" s="12" t="s">
         <v>2</v>
       </c>
@@ -1749,7 +1789,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A7" s="12" t="s">
         <v>75</v>
       </c>
@@ -1853,7 +1893,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A8" s="12" t="s">
         <v>3</v>
       </c>
@@ -1957,7 +1997,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A9" s="12" t="s">
         <v>4</v>
       </c>
@@ -2061,7 +2101,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A10" s="12" t="s">
         <v>110</v>
       </c>
@@ -2165,7 +2205,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A11" s="12" t="s">
         <v>111</v>
       </c>
@@ -2269,7 +2309,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A12" s="12" t="s">
         <v>112</v>
       </c>
@@ -2373,7 +2413,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A13" s="12" t="s">
         <v>5</v>
       </c>
@@ -2477,7 +2517,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A14" s="12" t="s">
         <v>6</v>
       </c>
@@ -2581,7 +2621,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A15" s="12" t="s">
         <v>7</v>
       </c>
@@ -2685,7 +2725,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A16" s="12" t="s">
         <v>72</v>
       </c>
@@ -2789,7 +2829,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A17" s="12" t="s">
         <v>8</v>
       </c>
@@ -2893,7 +2933,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A18" s="12" t="s">
         <v>9</v>
       </c>
@@ -2997,7 +3037,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A19" s="12" t="s">
         <v>10</v>
       </c>
@@ -3101,7 +3141,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A20" s="12" t="s">
         <v>11</v>
       </c>
@@ -3205,7 +3245,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="21" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A21" s="12" t="s">
         <v>12</v>
       </c>
@@ -3309,7 +3349,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A22" s="12" t="s">
         <v>87</v>
       </c>
@@ -3413,7 +3453,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A23" s="12" t="s">
         <v>13</v>
       </c>
@@ -3517,7 +3557,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="24" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A24" s="12" t="s">
         <v>14</v>
       </c>
@@ -3621,7 +3661,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A25" s="12" t="s">
         <v>15</v>
       </c>
@@ -3725,7 +3765,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A26" s="12" t="s">
         <v>16</v>
       </c>
@@ -3829,7 +3869,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="27" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A27" s="12" t="s">
         <v>17</v>
       </c>
@@ -3933,7 +3973,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A28" s="12" t="s">
         <v>18</v>
       </c>
@@ -4037,7 +4077,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A29" s="12" t="s">
         <v>19</v>
       </c>
@@ -4141,7 +4181,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A30" s="12" t="s">
         <v>20</v>
       </c>
@@ -4245,7 +4285,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="31" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A31" s="12" t="s">
         <v>22</v>
       </c>
@@ -4349,7 +4389,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="32" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A32" s="12" t="s">
         <v>23</v>
       </c>
@@ -4453,7 +4493,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A33" s="12" t="s">
         <v>24</v>
       </c>
@@ -4557,7 +4597,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A34" s="12" t="s">
         <v>25</v>
       </c>
@@ -4661,7 +4701,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="35" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A35" s="12" t="s">
         <v>26</v>
       </c>
@@ -4765,7 +4805,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A36" s="12" t="s">
         <v>27</v>
       </c>
@@ -4869,7 +4909,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A37" s="12" t="s">
         <v>28</v>
       </c>
@@ -4973,7 +5013,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="38" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A38" s="12" t="s">
         <v>29</v>
       </c>
@@ -5077,7 +5117,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A39" s="12" t="s">
         <v>30</v>
       </c>
@@ -5181,7 +5221,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A40" s="12" t="s">
         <v>31</v>
       </c>
@@ -5285,7 +5325,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="41" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A41" s="12" t="s">
         <v>32</v>
       </c>
@@ -5389,7 +5429,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="42" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A42" s="12" t="s">
         <v>97</v>
       </c>
@@ -5493,7 +5533,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="43" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A43" s="12" t="s">
         <v>33</v>
       </c>
@@ -5597,7 +5637,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="44" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A44" s="12" t="s">
         <v>21</v>
       </c>
@@ -5701,7 +5741,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="45" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A45" s="13" t="s">
         <v>113</v>
       </c>
@@ -5805,7 +5845,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="46" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A46" s="12" t="s">
         <v>114</v>
       </c>
@@ -5909,7 +5949,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="47" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A47" s="12" t="s">
         <v>115</v>
       </c>
@@ -6013,7 +6053,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="48" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A48" s="12" t="s">
         <v>116</v>
       </c>
@@ -6117,7 +6157,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="49" spans="1:34" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A49" s="12" t="s">
         <v>117</v>
       </c>
@@ -6228,18 +6268,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M45"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.19921875" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -6248,7 +6288,7 @@
         <v>118</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>119</v>
@@ -6281,7 +6321,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" s="13" t="s">
         <v>129</v>
       </c>
@@ -6289,40 +6329,40 @@
         <v>130</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="K2" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="L2" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="M2" s="17" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" s="12" t="s">
         <v>130</v>
       </c>
@@ -6330,7 +6370,7 @@
         <v>131</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>134</v>
@@ -6339,31 +6379,31 @@
         <v>134</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G3" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H3" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I3" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="J3" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="K3" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="L3" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="M3" s="17" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4" s="12" t="s">
         <v>131</v>
       </c>
@@ -6371,7 +6411,7 @@
         <v>132</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>134</v>
@@ -6380,31 +6420,31 @@
         <v>134</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H4" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I4" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="J4" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="K4" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="L4" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="M4" s="17" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" s="12" t="s">
         <v>132</v>
       </c>
@@ -6412,7 +6452,7 @@
         <v>133</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>133</v>
@@ -6421,31 +6461,31 @@
         <v>133</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H5" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I5" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="J5" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="K5" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="L5" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="M5" s="17" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6" s="16" t="s">
         <v>133</v>
       </c>
@@ -6453,122 +6493,122 @@
         <v>135</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>133</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H6" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I6" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="J6" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="K6" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="L6" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="M6" s="17" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7" s="16" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>135</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>139</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I7" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="J7" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="K7" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="L7" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="M7" s="17" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" s="16" t="s">
         <v>134</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I8" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="J8" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="K8" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="L8" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="M8" s="17" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9" s="15" t="s">
         <v>135</v>
       </c>
@@ -6576,7 +6616,7 @@
         <v>136</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>137</v>
@@ -6585,31 +6625,31 @@
         <v>137</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H9" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I9" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="J9" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="K9" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="L9" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="M9" s="17" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" s="15" t="s">
         <v>136</v>
       </c>
@@ -6617,7 +6657,7 @@
         <v>138</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>137</v>
@@ -6626,113 +6666,113 @@
         <v>137</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H10" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I10" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="J10" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="K10" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="L10" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="M10" s="17" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11" s="16" t="s">
         <v>137</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H11" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I11" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="J11" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="K11" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="L11" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="M11" s="17" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12" s="16" t="s">
         <v>138</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I12" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="J12" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="K12" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="L12" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="M12" s="17" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13" s="15" t="s">
         <v>139</v>
       </c>
@@ -6740,40 +6780,40 @@
         <v>140</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F13" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H13" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I13" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="J13" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="K13" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="L13" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="M13" s="17" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14" s="15" t="s">
         <v>140</v>
       </c>
@@ -6781,491 +6821,491 @@
         <v>141</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H14" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I14" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="J14" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="K14" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="L14" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15" s="15" t="s">
         <v>141</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H15" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I15" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="J15" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="K15" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="L15" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="M15" s="17" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A16" s="16" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A16" s="15" t="s">
         <v>142</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="F16" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I16" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="J16" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="K16" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="L16" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="M16" s="17" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+        <v>176</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A17" s="15" t="s">
         <v>143</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="E17" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>137</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="G17" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H17" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I17" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="J17" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="K17" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="L17" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="M17" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="M17" s="17" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A18" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="G18" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="H18" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="I18" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="J18" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="K18" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="L18" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A19" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="G19" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="H19" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="I19" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="J19" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="K19" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="L19" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A20" s="15" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A18" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="E18" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="F18" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="G18" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="H18" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="I18" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="J18" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="K18" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="L18" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="M18" s="17" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A19" s="15" t="s">
+      <c r="B20" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="B19" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="C19" s="2" t="s">
+      <c r="C20" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F20" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="G20" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="H20" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="I20" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="J20" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="K20" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="L20" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="M20" s="17" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A21" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="G19" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="H19" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="I19" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="J19" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="K19" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="L19" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="M19" s="17" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A20" s="16" t="s">
+      <c r="B21" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F21" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="G21" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="H21" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="I21" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="J21" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="K21" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="L21" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="M21" s="17" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A22" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="E20" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="G20" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="H20" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="I20" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="J20" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="K20" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="L20" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="M20" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A21" s="16" t="s">
-        <v>161</v>
-      </c>
-      <c r="B21" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="E21" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="G21" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="H21" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="I21" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="J21" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="K21" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="L21" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="M21" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A22" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>147</v>
-      </c>
       <c r="C22" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>148</v>
+        <v>176</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="E22" s="17" t="s">
+        <v>176</v>
       </c>
       <c r="F22" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G22" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H22" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I22" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="J22" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="K22" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="L22" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="M22" s="17" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A23" s="15" t="s">
         <v>147</v>
       </c>
       <c r="B23" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="G23" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="H23" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="I23" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="J23" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="K23" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="L23" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="M23" s="17" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A24" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E24" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="G24" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="H24" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="I24" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="J24" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="K24" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="L24" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="M24" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="C23" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="F23" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="G23" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="H23" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="I23" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="J23" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="K23" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="L23" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="M23" s="17" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A24" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="B24" s="2" t="s">
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A25" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="C24" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="D24" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="E24" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="F24" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="G24" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="H24" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="I24" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="J24" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="K24" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="L24" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="M24" s="17" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A25" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="B25" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>149</v>
+      <c r="C25" s="17" t="s">
+        <v>176</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="E25" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="F25" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="F25" s="2" t="s">
-        <v>149</v>
-      </c>
       <c r="G25" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="H25" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="I25" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="J25" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="K25" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="L25" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="M25" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="H25" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="I25" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="J25" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="K25" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="L25" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="M25" s="17" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A26" s="16" t="s">
         <v>162</v>
       </c>
@@ -7273,816 +7313,734 @@
         <v>163</v>
       </c>
       <c r="C26" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="G26" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="H26" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="I26" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="J26" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="K26" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="L26" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="M26" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="E26" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="G26" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="H26" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="I26" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="J26" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="K26" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="L26" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="M26" s="2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A27" s="16" t="s">
         <v>163</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>163</v>
+      <c r="B27" s="17" t="s">
+        <v>176</v>
       </c>
       <c r="C27" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E27" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="G27" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="H27" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="I27" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="J27" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="K27" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="L27" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="M27" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="D27" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="E27" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="G27" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="H27" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="I27" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="J27" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="K27" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="L27" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="M27" s="2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A28" s="16" t="s">
-        <v>164</v>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A28" s="13" t="s">
+        <v>148</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>164</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>150</v>
+        <v>176</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>176</v>
       </c>
       <c r="E28" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>150</v>
+        <v>176</v>
+      </c>
+      <c r="F28" s="17" t="s">
+        <v>176</v>
       </c>
       <c r="G28" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H28" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I28" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="J28" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="K28" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="L28" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="M28" s="2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A29" s="16" t="s">
-        <v>165</v>
-      </c>
-      <c r="B29" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
+      </c>
+      <c r="M28" s="17" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A29" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>150</v>
+        <v>176</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>176</v>
       </c>
       <c r="E29" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>150</v>
+        <v>176</v>
+      </c>
+      <c r="F29" s="17" t="s">
+        <v>176</v>
       </c>
       <c r="G29" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H29" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I29" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="J29" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="K29" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="L29" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="M29" s="2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A30" s="13" t="s">
-        <v>150</v>
+        <v>176</v>
+      </c>
+      <c r="M29" s="17" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A30" s="16" t="s">
+        <v>149</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>166</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D30" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E30" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F30" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G30" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H30" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="I30" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>165</v>
       </c>
       <c r="J30" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="K30" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="L30" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="M30" s="17" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A31" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>151</v>
-      </c>
       <c r="C31" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E31" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F31" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G31" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H31" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I31" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="J31" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="K31" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="L31" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="M31" s="17" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A32" s="16" t="s">
-        <v>151</v>
+        <v>166</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>168</v>
+        <v>150</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D32" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E32" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F32" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G32" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H32" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="I32" s="2" t="s">
-        <v>167</v>
+        <v>176</v>
+      </c>
+      <c r="I32" s="17" t="s">
+        <v>176</v>
       </c>
       <c r="J32" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="K32" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="L32" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="M32" s="17" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A33" s="15" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>168</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D33" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E33" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F33" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G33" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H33" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="I33" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>167</v>
       </c>
       <c r="J33" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="K33" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="L33" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="M33" s="17" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A34" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="C34" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="D34" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="E34" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="F34" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="G34" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="H34" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="I34" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="J34" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="K34" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="L34" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="M34" s="17" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A35" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C35" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="D35" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="E35" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="F35" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="G35" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="H35" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="I35" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="J35" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="K35" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="L35" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="M35" s="17" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A36" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="B36" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="D36" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="C34" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="D34" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="E34" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="F34" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="G34" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="H34" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="I34" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="J34" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="K34" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="L34" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="M34" s="17" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A35" s="15" t="s">
+      <c r="F36" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="G36" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="H36" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="I36" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="K36" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="L36" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="M36" s="17" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A37" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C35" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="D35" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="E35" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="F35" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="G35" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="H35" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="I35" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="J35" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="K35" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="L35" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="M35" s="17" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A36" s="16" t="s">
-        <v>169</v>
-      </c>
-      <c r="B36" s="2" t="s">
+      <c r="C37" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="D37" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="E37" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="F37" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="G37" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="H37" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="I37" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="J37" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="K37" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="L37" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="M37" s="17" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A38" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="C36" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="D36" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="E36" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="F36" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="G36" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="H36" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="I36" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="J36" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="K36" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="L36" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="M36" s="17" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A37" s="15" t="s">
+      <c r="B38" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="C38" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="D38" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F38" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="G38" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="I38" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="J38" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="L38" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="M38" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A39" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C37" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="D37" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="E37" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="F37" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="G37" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="H37" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="I37" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="J37" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="K37" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="L37" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="M37" s="17" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A38" s="16" t="s">
+      <c r="C39" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="D39" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="E39" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="F39" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="G39" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="H39" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="I39" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="J39" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="K39" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="L39" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="M39" s="17" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A40" s="15" t="s">
         <v>153</v>
       </c>
-      <c r="B38" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="C38" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="D38" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="E38" s="2" t="s">
+      <c r="B40" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="F38" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="G38" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="H38" s="2" t="s">
+      <c r="C40" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="D40" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="E40" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="F40" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="G40" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="H40" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="J40" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="K40" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="L40" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="M40" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A41" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="I38" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="J38" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="K38" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="L38" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="M38" s="17" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A39" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="B39" s="2" t="s">
+      <c r="B41" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="C41" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="D41" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="E41" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="F41" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="G41" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="H41" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="I41" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C39" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="D39" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="E39" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="F39" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="G39" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="H39" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="I39" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="J39" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="K39" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="L39" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="M39" s="17" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A40" s="15" t="s">
+      <c r="J41" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="K41" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="L41" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="M41" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A42" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="C40" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="D40" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="F40" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="G40" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="I40" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="J40" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="K40" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="L40" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="M40" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A41" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="B41" s="2" t="s">
+      <c r="B42" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="C41" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="D41" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="E41" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="F41" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="G41" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="H41" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="I41" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="J41" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="K41" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="L41" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="M41" s="17" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A42" s="15" t="s">
+      <c r="C42" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="D42" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="E42" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="F42" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="G42" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="H42" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="I42" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="J42" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="K42" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="L42" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="M42" s="17" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A43" s="15" t="s">
         <v>155</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="C42" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="D42" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="E42" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="F42" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="G42" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="H42" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="I42" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="J42" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="K42" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="L42" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="M42" s="2" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A43" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="B43" s="17" t="s">
-        <v>178</v>
+      <c r="B43" s="2" t="s">
+        <v>175</v>
       </c>
       <c r="C43" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D43" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E43" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F43" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G43" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H43" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="I43" s="2" t="s">
-        <v>174</v>
+        <v>176</v>
+      </c>
+      <c r="I43" s="17" t="s">
+        <v>176</v>
       </c>
       <c r="J43" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="K43" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="L43" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="M43" s="2" t="s">
         <v>175</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A44" s="16" t="s">
-        <v>174</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="C44" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="D44" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="E44" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="F44" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="G44" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="H44" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="I44" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="J44" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="K44" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="L44" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="M44" s="17" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A45" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="C45" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="D45" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="E45" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="F45" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="G45" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="H45" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="I45" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="J45" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="K45" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="L45" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="M45" s="2" t="s">
-        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -8093,19 +8051,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="8.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.9296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.06640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -8126,7 +8084,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
         <v>105</v>
       </c>
@@ -8146,7 +8104,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
         <v>104</v>
       </c>
@@ -8166,7 +8124,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="6" t="s">
         <v>108</v>
       </c>
@@ -8186,7 +8144,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FIX: adds S_DT_YYYY state to date! FSM to fix head yyyy conversion issue.
</commit_message>
<xml_diff>
--- a/docs/lexer/lexer-FSM.xlsx
+++ b/docs/lexer/lexer-FSM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Red\docs\lexer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA719BFA-F441-4081-91D1-9CF8F5E587D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E97F9C-E75D-4076-BA05-70F24FE77F57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28095" yWindow="150" windowWidth="17025" windowHeight="15015" tabRatio="564" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
     <author>dk</author>
   </authors>
   <commentList>
-    <comment ref="D6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="D7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2246" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2259" uniqueCount="182">
   <si>
     <t>S_START</t>
   </si>
@@ -600,6 +600,9 @@
   </si>
   <si>
     <t>T_DT_WEEK</t>
+  </si>
+  <si>
+    <t>S_DT_YYYY</t>
   </si>
 </sst>
 </file>
@@ -6269,10 +6272,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M43"/>
+  <dimension ref="A1:M44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6449,7 +6452,7 @@
         <v>132</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>133</v>
+        <v>181</v>
       </c>
       <c r="C5" s="17" t="s">
         <v>176</v>
@@ -6486,23 +6489,23 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>143</v>
+      <c r="C6" s="17" t="s">
+        <v>176</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>133</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>143</v>
+        <v>133</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>176</v>
       </c>
       <c r="G6" s="17" t="s">
         <v>176</v>
@@ -6528,7 +6531,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7" s="16" t="s">
-        <v>156</v>
+        <v>133</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>135</v>
@@ -6536,17 +6539,17 @@
       <c r="C7" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="D7" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>176</v>
+      <c r="D7" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>156</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>139</v>
+      <c r="G7" s="17" t="s">
+        <v>176</v>
       </c>
       <c r="H7" s="17" t="s">
         <v>176</v>
@@ -6569,60 +6572,60 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="H8" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="I8" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="J8" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="K8" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="L8" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="M8" s="17" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A9" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="D8" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="G8" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="H8" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="I8" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="J8" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="K8" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="L8" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="M8" s="17" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A9" s="15" t="s">
-        <v>135</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>137</v>
+      <c r="D9" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>176</v>
       </c>
       <c r="F9" s="17" t="s">
         <v>176</v>
@@ -6651,10 +6654,10 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>138</v>
       </c>
       <c r="C10" s="17" t="s">
         <v>176</v>
@@ -6691,20 +6694,20 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="E11" s="17" t="s">
-        <v>176</v>
+      <c r="E11" s="2" t="s">
+        <v>137</v>
       </c>
       <c r="F11" s="17" t="s">
         <v>176</v>
@@ -6733,63 +6736,63 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="G12" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="H12" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="I12" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="J12" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="K12" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="L12" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="M12" s="17" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A13" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="B12" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="E12" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="F12" s="2" t="s">
+      <c r="B13" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>148</v>
-      </c>
-      <c r="G12" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="H12" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="I12" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="J12" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="K12" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="L12" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="M12" s="17" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A13" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="E13" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="F13" s="17" t="s">
-        <v>176</v>
       </c>
       <c r="G13" s="17" t="s">
         <v>176</v>
@@ -6815,11 +6818,11 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>141</v>
-      </c>
       <c r="C14" s="17" t="s">
         <v>176</v>
       </c>
@@ -6850,17 +6853,17 @@
       <c r="L14" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="M14" s="2" t="s">
-        <v>180</v>
+      <c r="M14" s="17" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>142</v>
-      </c>
       <c r="C15" s="17" t="s">
         <v>176</v>
       </c>
@@ -6870,8 +6873,8 @@
       <c r="E15" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="F15" s="2" t="s">
-        <v>148</v>
+      <c r="F15" s="17" t="s">
+        <v>176</v>
       </c>
       <c r="G15" s="17" t="s">
         <v>176</v>
@@ -6891,16 +6894,16 @@
       <c r="L15" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="M15" s="17" t="s">
-        <v>176</v>
+      <c r="M15" s="2" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>176</v>
       </c>
       <c r="C16" s="17" t="s">
         <v>176</v>
@@ -6932,70 +6935,70 @@
       <c r="L16" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="M16" s="2" t="s">
-        <v>179</v>
+      <c r="M16" s="17" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A17" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="G17" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="H17" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="I17" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="J17" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="K17" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="L17" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A18" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="B17" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="C17" s="2" t="s">
+      <c r="B18" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F18" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="G17" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="H17" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="I17" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="J17" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="K17" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="L17" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="M17" s="17" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A18" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="E18" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>148</v>
-      </c>
       <c r="G18" s="17" t="s">
         <v>176</v>
       </c>
@@ -7014,16 +7017,16 @@
       <c r="L18" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="M18" s="2" t="s">
-        <v>177</v>
+      <c r="M18" s="17" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A19" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>159</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>176</v>
       </c>
       <c r="C19" s="17" t="s">
         <v>176</v>
@@ -7060,23 +7063,23 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A20" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>145</v>
+      <c r="A20" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>176</v>
       </c>
       <c r="C20" s="17" t="s">
         <v>176</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="F20" s="17" t="s">
-        <v>176</v>
+        <v>148</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="G20" s="17" t="s">
         <v>176</v>
@@ -7096,16 +7099,16 @@
       <c r="L20" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="M20" s="17" t="s">
-        <v>176</v>
+      <c r="M20" s="2" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A21" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>145</v>
-      </c>
-      <c r="B21" s="17" t="s">
-        <v>176</v>
       </c>
       <c r="C21" s="17" t="s">
         <v>176</v>
@@ -7142,106 +7145,106 @@
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A22" s="16" t="s">
+      <c r="A22" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="E22" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F22" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="G22" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="H22" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="I22" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="J22" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="K22" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="L22" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="M22" s="17" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A23" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="C22" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="D22" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="E22" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="F22" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="G22" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="H22" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="I22" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="J22" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="K22" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="L22" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="M22" s="17" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A23" s="15" t="s">
+      <c r="C23" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="F23" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="G23" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="H23" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="I23" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="J23" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="K23" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="L23" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="M23" s="17" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A24" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="B23" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="C23" s="2" t="s">
+      <c r="B24" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E24" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F24" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="G23" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="H23" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="I23" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="J23" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="K23" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="L23" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="M23" s="17" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A24" s="16" t="s">
-        <v>160</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="E24" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>148</v>
-      </c>
       <c r="G24" s="17" t="s">
         <v>176</v>
       </c>
@@ -7260,16 +7263,16 @@
       <c r="L24" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="M24" s="2" t="s">
-        <v>178</v>
+      <c r="M24" s="17" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A25" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>161</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>162</v>
       </c>
       <c r="C25" s="17" t="s">
         <v>176</v>
@@ -7307,10 +7310,10 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A26" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>162</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>163</v>
       </c>
       <c r="C26" s="17" t="s">
         <v>176</v>
@@ -7348,10 +7351,10 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A27" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>163</v>
-      </c>
-      <c r="B27" s="17" t="s">
-        <v>176</v>
       </c>
       <c r="C27" s="17" t="s">
         <v>176</v>
@@ -7388,131 +7391,131 @@
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A28" s="13" t="s">
+      <c r="A28" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="B28" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="E28" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="G28" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="H28" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="I28" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="J28" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="K28" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="L28" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A29" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="C28" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="D28" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="E28" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="F28" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="G28" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="H28" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="I28" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="J28" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="K28" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="L28" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="M28" s="17" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A29" s="15" t="s">
+      <c r="C29" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="E29" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="F29" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="G29" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="H29" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="I29" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="J29" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="K29" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="L29" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="M29" s="17" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A30" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B30" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="C29" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="D29" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="E29" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="F29" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="G29" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="H29" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="I29" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="J29" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="K29" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="L29" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="M29" s="17" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A30" s="16" t="s">
+      <c r="C30" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="D30" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="E30" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="F30" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="G30" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="H30" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="I30" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="J30" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="K30" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="L30" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="M30" s="17" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A31" s="16" t="s">
         <v>149</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="C30" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="D30" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="E30" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="F30" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="G30" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="H30" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="I30" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="J30" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="K30" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="L30" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="M30" s="17" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A31" s="15" t="s">
-        <v>165</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>166</v>
@@ -7535,8 +7538,8 @@
       <c r="H31" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="I31" s="17" t="s">
-        <v>176</v>
+      <c r="I31" s="2" t="s">
+        <v>165</v>
       </c>
       <c r="J31" s="17" t="s">
         <v>176</v>
@@ -7552,90 +7555,90 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A32" s="16" t="s">
+      <c r="A32" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="C32" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="D32" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="E32" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="F32" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="G32" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="H32" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="I32" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="J32" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="K32" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="L32" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="M32" s="17" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A33" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="C32" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="D32" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="E32" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="F32" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="G32" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="H32" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="I32" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="J32" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="K32" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="L32" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="M32" s="17" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A33" s="15" t="s">
+      <c r="C33" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="D33" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="E33" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="F33" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="G33" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="H33" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="I33" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="J33" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="K33" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="L33" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="M33" s="17" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A34" s="15" t="s">
         <v>150</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="C33" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="D33" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="E33" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="F33" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="G33" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="H33" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="I33" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="J33" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="K33" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="L33" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="M33" s="17" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A34" s="16" t="s">
-        <v>167</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>168</v>
@@ -7658,8 +7661,8 @@
       <c r="H34" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="I34" s="17" t="s">
-        <v>176</v>
+      <c r="I34" s="2" t="s">
+        <v>167</v>
       </c>
       <c r="J34" s="17" t="s">
         <v>176</v>
@@ -7675,117 +7678,117 @@
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A35" s="15" t="s">
+      <c r="A35" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="C35" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="D35" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="E35" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="F35" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="G35" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="H35" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="I35" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="J35" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="K35" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="L35" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="M35" s="17" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A36" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="C35" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="D35" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="E35" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="F35" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="G35" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="H35" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="I35" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="J35" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="K35" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="L35" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="M35" s="17" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A36" s="16" t="s">
+      <c r="C36" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="D36" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="E36" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="F36" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="G36" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="H36" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="I36" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="J36" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="K36" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="L36" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="M36" s="17" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A37" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="B36" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="C36" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="D36" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="E36" s="2" t="s">
+      <c r="B37" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="C37" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="D37" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="E37" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="F36" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="G36" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="H36" s="2" t="s">
+      <c r="F37" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="G37" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="H37" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="I36" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="J36" s="2" t="s">
+      <c r="I37" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="J37" s="2" t="s">
         <v>169</v>
-      </c>
-      <c r="K36" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="L36" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="M36" s="17" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A37" s="15" t="s">
-        <v>169</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="C37" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="D37" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="E37" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="F37" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="G37" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="H37" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="I37" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="J37" s="17" t="s">
-        <v>176</v>
       </c>
       <c r="K37" s="17" t="s">
         <v>176</v>
@@ -7799,7 +7802,7 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A38" s="15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>170</v>
@@ -7810,8 +7813,8 @@
       <c r="D38" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="E38" s="2" t="s">
-        <v>152</v>
+      <c r="E38" s="17" t="s">
+        <v>176</v>
       </c>
       <c r="F38" s="17" t="s">
         <v>176</v>
@@ -7819,8 +7822,8 @@
       <c r="G38" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="H38" s="2" t="s">
-        <v>152</v>
+      <c r="H38" s="17" t="s">
+        <v>176</v>
       </c>
       <c r="I38" s="17" t="s">
         <v>176</v>
@@ -7828,40 +7831,40 @@
       <c r="J38" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="K38" s="2" t="s">
-        <v>171</v>
+      <c r="K38" s="17" t="s">
+        <v>176</v>
       </c>
       <c r="L38" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="M38" s="2" t="s">
-        <v>171</v>
+      <c r="M38" s="17" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A39" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C39" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="D39" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="E39" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="C39" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="D39" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="E39" s="17" t="s">
-        <v>176</v>
-      </c>
       <c r="F39" s="17" t="s">
         <v>176</v>
       </c>
       <c r="G39" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="H39" s="17" t="s">
-        <v>176</v>
+      <c r="H39" s="2" t="s">
+        <v>152</v>
       </c>
       <c r="I39" s="17" t="s">
         <v>176</v>
@@ -7869,63 +7872,63 @@
       <c r="J39" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="K39" s="17" t="s">
-        <v>176</v>
+      <c r="K39" s="2" t="s">
+        <v>171</v>
       </c>
       <c r="L39" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="M39" s="17" t="s">
-        <v>176</v>
+      <c r="M39" s="2" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A40" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="C40" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="D40" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="E40" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="F40" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="G40" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="H40" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="I40" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="J40" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="K40" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="L40" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="M40" s="17" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A41" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="C40" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="D40" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="E40" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="F40" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="G40" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="H40" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="I40" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="J40" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="K40" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="L40" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="M40" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A41" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="B41" s="17" t="s">
-        <v>176</v>
       </c>
       <c r="C41" s="17" t="s">
         <v>176</v>
@@ -7958,88 +7961,129 @@
         <v>176</v>
       </c>
       <c r="M41" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A42" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="B42" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="C42" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="D42" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="E42" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="F42" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="G42" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="H42" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="I42" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="J42" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="K42" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="L42" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="M42" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A43" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="C42" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="D42" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="E42" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="F42" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="G42" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="H42" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="I42" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="J42" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="K42" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="L42" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="M42" s="17" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A43" s="15" t="s">
+      <c r="C43" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="D43" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="E43" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="F43" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="G43" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="H43" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="I43" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="J43" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="K43" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="L43" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="M43" s="17" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A44" s="15" t="s">
         <v>155</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B44" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="C43" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="D43" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="E43" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="F43" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="G43" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="H43" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="I43" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="J43" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="K43" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="L43" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="M43" s="2" t="s">
+      <c r="C44" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="D44" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="E44" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="F44" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="G44" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="H44" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="I44" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="J44" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="K44" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="L44" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="M44" s="2" t="s">
         <v>175</v>
       </c>
     </row>

</xml_diff>

<commit_message>
FEAT: various fixes and improvements in parsing date/time.
</commit_message>
<xml_diff>
--- a/docs/lexer/lexer-FSM.xlsx
+++ b/docs/lexer/lexer-FSM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-28100" yWindow="150" windowWidth="17030" windowHeight="15020" tabRatio="564"/>
+    <workbookView xWindow="-28100" yWindow="150" windowWidth="17030" windowHeight="15020" tabRatio="564" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="transitions" sheetId="3" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2308" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2321" uniqueCount="186">
   <si>
     <t>S_START</t>
   </si>
@@ -600,6 +600,15 @@
   </si>
   <si>
     <t>C_PLUS</t>
+  </si>
+  <si>
+    <t>T_TM_HMS</t>
+  </si>
+  <si>
+    <t>T_TM_HM</t>
+  </si>
+  <si>
+    <t>S_TM_START2</t>
   </si>
 </sst>
 </file>
@@ -1117,9 +1126,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AA25" sqref="AA25"/>
+      <selection pane="bottomLeft" activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3849,8 +3858,8 @@
       <c r="N26" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="O26" s="1" t="s">
-        <v>89</v>
+      <c r="O26" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="P26" s="2" t="s">
         <v>16</v>
@@ -6382,10 +6391,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M44"/>
+  <dimension ref="A1:M45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6393,6 +6402,7 @@
     <col min="1" max="1" width="10.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="10" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -7388,13 +7398,13 @@
         <v>175</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>147</v>
+        <v>185</v>
       </c>
       <c r="E25" s="17" t="s">
         <v>175</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>147</v>
+        <v>185</v>
       </c>
       <c r="G25" s="17" t="s">
         <v>175</v>
@@ -7429,13 +7439,13 @@
         <v>175</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>147</v>
+        <v>185</v>
       </c>
       <c r="E26" s="17" t="s">
         <v>175</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>147</v>
+        <v>185</v>
       </c>
       <c r="G26" s="17" t="s">
         <v>175</v>
@@ -7470,13 +7480,13 @@
         <v>175</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>147</v>
+        <v>185</v>
       </c>
       <c r="E27" s="17" t="s">
         <v>175</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>147</v>
+        <v>185</v>
       </c>
       <c r="G27" s="17" t="s">
         <v>175</v>
@@ -7511,13 +7521,13 @@
         <v>175</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>147</v>
+        <v>185</v>
       </c>
       <c r="E28" s="17" t="s">
         <v>175</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>147</v>
+        <v>185</v>
       </c>
       <c r="G28" s="17" t="s">
         <v>175</v>
@@ -7541,7 +7551,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" s="13" t="s">
         <v>147</v>
       </c>
@@ -7582,91 +7592,91 @@
         <v>175</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="C30" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="D30" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="E30" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="F30" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="G30" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="H30" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="I30" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="J30" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="K30" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="L30" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="M30" s="17" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A31" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="C30" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="D30" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="E30" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="F30" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="G30" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="H30" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="I30" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="J30" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="K30" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="L30" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="M30" s="17" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A31" s="16" t="s">
+      <c r="C31" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="E31" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="F31" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="G31" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="H31" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="I31" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="J31" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="K31" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="L31" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="M31" s="17" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A32" s="16" t="s">
         <v>148</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="C31" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="D31" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="E31" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="F31" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="G31" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="H31" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="I31" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="J31" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="K31" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="L31" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="M31" s="17" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A32" s="15" t="s">
-        <v>164</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>165</v>
@@ -7689,8 +7699,8 @@
       <c r="H32" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="I32" s="17" t="s">
-        <v>175</v>
+      <c r="I32" s="2" t="s">
+        <v>164</v>
       </c>
       <c r="J32" s="17" t="s">
         <v>175</v>
@@ -7706,90 +7716,90 @@
       </c>
     </row>
     <row r="33" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A33" s="16" t="s">
+      <c r="A33" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="C33" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="D33" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="E33" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="F33" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="G33" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="H33" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="I33" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="J33" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="K33" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="L33" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="M33" s="17" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A34" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="C33" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="D33" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="E33" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="F33" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="G33" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="H33" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="I33" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="J33" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="K33" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="L33" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="M33" s="17" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A34" s="15" t="s">
+      <c r="C34" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="D34" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="E34" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="F34" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="G34" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="H34" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="I34" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="J34" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="K34" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="L34" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="M34" s="5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A35" s="15" t="s">
         <v>149</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="C34" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="D34" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="E34" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="F34" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="G34" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="H34" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="I34" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="J34" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="K34" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="L34" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="M34" s="17" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A35" s="16" t="s">
-        <v>166</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>167</v>
@@ -7812,8 +7822,8 @@
       <c r="H35" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="I35" s="17" t="s">
-        <v>175</v>
+      <c r="I35" s="2" t="s">
+        <v>166</v>
       </c>
       <c r="J35" s="17" t="s">
         <v>175</v>
@@ -7824,136 +7834,136 @@
       <c r="L35" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="M35" s="17" t="s">
-        <v>175</v>
+      <c r="M35" s="5" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="36" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A36" s="15" t="s">
+      <c r="A36" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="C36" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="D36" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="E36" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="F36" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="G36" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="H36" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="I36" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="J36" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="K36" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="L36" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="M36" s="17" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A37" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="C36" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="D36" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="E36" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="F36" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="G36" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="H36" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="I36" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="J36" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="K36" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="L36" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="M36" s="17" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A37" s="16" t="s">
+      <c r="C37" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="D37" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="E37" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="F37" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="G37" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="H37" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="I37" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="J37" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="K37" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="L37" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="M37" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A38" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="B37" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="C37" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="D37" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="E37" s="2" t="s">
+      <c r="B38" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="D38" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="E38" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="F37" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="G37" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="H37" s="2" t="s">
+      <c r="F38" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="G38" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="H38" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="I37" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="J37" s="2" t="s">
+      <c r="I38" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="J38" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="K37" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="L37" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="M37" s="17" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A38" s="15" t="s">
-        <v>168</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="C38" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="D38" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="E38" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="F38" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="G38" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="H38" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="I38" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="J38" s="17" t="s">
-        <v>175</v>
-      </c>
       <c r="K38" s="17" t="s">
         <v>175</v>
       </c>
       <c r="L38" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="M38" s="17" t="s">
-        <v>175</v>
+      <c r="M38" s="5" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A39" s="15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>169</v>
@@ -7964,8 +7974,8 @@
       <c r="D39" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="E39" s="2" t="s">
-        <v>151</v>
+      <c r="E39" s="17" t="s">
+        <v>175</v>
       </c>
       <c r="F39" s="17" t="s">
         <v>175</v>
@@ -7973,8 +7983,8 @@
       <c r="G39" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="H39" s="2" t="s">
-        <v>151</v>
+      <c r="H39" s="17" t="s">
+        <v>175</v>
       </c>
       <c r="I39" s="17" t="s">
         <v>175</v>
@@ -7982,40 +7992,40 @@
       <c r="J39" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="K39" s="2" t="s">
-        <v>170</v>
+      <c r="K39" s="17" t="s">
+        <v>175</v>
       </c>
       <c r="L39" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="M39" s="2" t="s">
-        <v>170</v>
+      <c r="M39" s="17" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A40" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="D40" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="E40" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="C40" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="D40" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="E40" s="17" t="s">
-        <v>175</v>
-      </c>
       <c r="F40" s="17" t="s">
         <v>175</v>
       </c>
       <c r="G40" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="H40" s="17" t="s">
-        <v>175</v>
+      <c r="H40" s="2" t="s">
+        <v>151</v>
       </c>
       <c r="I40" s="17" t="s">
         <v>175</v>
@@ -8023,63 +8033,63 @@
       <c r="J40" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="K40" s="17" t="s">
-        <v>175</v>
+      <c r="K40" s="2" t="s">
+        <v>170</v>
       </c>
       <c r="L40" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="M40" s="17" t="s">
-        <v>175</v>
+      <c r="M40" s="2" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A41" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="C41" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="D41" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="E41" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="F41" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="G41" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="H41" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="I41" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="J41" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="K41" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="L41" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="M41" s="17" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A42" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>153</v>
-      </c>
-      <c r="C41" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="D41" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="E41" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="F41" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="G41" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="H41" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="I41" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="J41" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="K41" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="L41" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="M41" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A42" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="B42" s="17" t="s">
-        <v>175</v>
       </c>
       <c r="C42" s="17" t="s">
         <v>175</v>
@@ -8112,88 +8122,129 @@
         <v>175</v>
       </c>
       <c r="M42" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A43" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="B43" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="C43" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="D43" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="E43" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="F43" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="G43" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="H43" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="I43" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="J43" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="K43" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="L43" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="M43" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A44" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="B44" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="C43" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="D43" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="E43" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="F43" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="G43" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="H43" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="I43" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="J43" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="K43" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="L43" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="M43" s="17" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A44" s="15" t="s">
+      <c r="C44" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="D44" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="E44" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="F44" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="G44" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="H44" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="I44" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="J44" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="K44" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="L44" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="M44" s="17" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A45" s="15" t="s">
         <v>154</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B45" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C44" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="D44" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="E44" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="F44" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="G44" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="H44" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="I44" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="J44" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="K44" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="L44" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="M44" s="2" t="s">
+      <c r="C45" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="D45" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="E45" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="F45" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="G45" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="H45" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="I45" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="J45" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="K45" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="L45" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="M45" s="2" t="s">
         <v>174</v>
       </c>
     </row>

</xml_diff>

<commit_message>
FEAT: split the date! FSM into date! and time! FSM.
</commit_message>
<xml_diff>
--- a/docs/lexer/lexer-FSM.xlsx
+++ b/docs/lexer/lexer-FSM.xlsx
@@ -1,27 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Red\docs\lexer\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30E163C0-BE51-4329-9C5F-41863A835552}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28100" yWindow="150" windowWidth="17030" windowHeight="15020" tabRatio="564" activeTab="1"/>
+    <workbookView xWindow="2753" yWindow="525" windowWidth="16874" windowHeight="10455" tabRatio="564" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="transitions" sheetId="3" r:id="rId1"/>
     <sheet name="date! transitions" sheetId="5" r:id="rId2"/>
-    <sheet name="bin16 transitions" sheetId="4" r:id="rId3"/>
+    <sheet name="time! transitions" sheetId="6" r:id="rId3"/>
+    <sheet name="bin16 transitions" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>dk</author>
   </authors>
   <commentList>
-    <comment ref="D7" authorId="0">
+    <comment ref="D7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -51,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2321" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2149" uniqueCount="186">
   <si>
     <t>S_START</t>
   </si>
@@ -614,7 +621,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -880,7 +887,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -913,9 +920,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -948,6 +972,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1123,7 +1164,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1131,18 +1172,18 @@
       <selection pane="bottomLeft" activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.36328125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" customWidth="1"/>
-    <col min="5" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="12" width="9.7265625" customWidth="1"/>
-    <col min="13" max="13" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="14" max="35" width="9.7265625" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.73046875" customWidth="1"/>
+    <col min="5" max="5" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="9.73046875" customWidth="1"/>
+    <col min="13" max="13" width="9.9296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="35" width="9.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:35" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="8"/>
       <c r="B1" s="7" t="s">
         <v>37</v>
@@ -1247,7 +1288,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
@@ -1354,7 +1395,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A3" s="12" t="s">
         <v>69</v>
       </c>
@@ -1461,7 +1502,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A4" s="12" t="s">
         <v>70</v>
       </c>
@@ -1568,7 +1609,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A5" s="12" t="s">
         <v>1</v>
       </c>
@@ -1675,7 +1716,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A6" s="12" t="s">
         <v>2</v>
       </c>
@@ -1782,7 +1823,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A7" s="12" t="s">
         <v>74</v>
       </c>
@@ -1889,7 +1930,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A8" s="12" t="s">
         <v>3</v>
       </c>
@@ -1996,7 +2037,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A9" s="12" t="s">
         <v>4</v>
       </c>
@@ -2103,7 +2144,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A10" s="12" t="s">
         <v>109</v>
       </c>
@@ -2210,7 +2251,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A11" s="12" t="s">
         <v>110</v>
       </c>
@@ -2317,7 +2358,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A12" s="12" t="s">
         <v>111</v>
       </c>
@@ -2424,7 +2465,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A13" s="12" t="s">
         <v>5</v>
       </c>
@@ -2531,7 +2572,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A14" s="12" t="s">
         <v>6</v>
       </c>
@@ -2638,7 +2679,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A15" s="12" t="s">
         <v>7</v>
       </c>
@@ -2745,7 +2786,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A16" s="12" t="s">
         <v>71</v>
       </c>
@@ -2852,7 +2893,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A17" s="12" t="s">
         <v>8</v>
       </c>
@@ -2959,7 +3000,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A18" s="12" t="s">
         <v>9</v>
       </c>
@@ -3066,7 +3107,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A19" s="12" t="s">
         <v>10</v>
       </c>
@@ -3173,7 +3214,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A20" s="12" t="s">
         <v>11</v>
       </c>
@@ -3280,7 +3321,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A21" s="12" t="s">
         <v>12</v>
       </c>
@@ -3387,7 +3428,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A22" s="12" t="s">
         <v>86</v>
       </c>
@@ -3494,7 +3535,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A23" s="12" t="s">
         <v>13</v>
       </c>
@@ -3601,7 +3642,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A24" s="12" t="s">
         <v>14</v>
       </c>
@@ -3708,7 +3749,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A25" s="12" t="s">
         <v>15</v>
       </c>
@@ -3815,7 +3856,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A26" s="12" t="s">
         <v>16</v>
       </c>
@@ -3922,7 +3963,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A27" s="12" t="s">
         <v>17</v>
       </c>
@@ -4029,7 +4070,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A28" s="12" t="s">
         <v>18</v>
       </c>
@@ -4136,7 +4177,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A29" s="12" t="s">
         <v>19</v>
       </c>
@@ -4243,7 +4284,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A30" s="12" t="s">
         <v>20</v>
       </c>
@@ -4350,7 +4391,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A31" s="12" t="s">
         <v>22</v>
       </c>
@@ -4457,7 +4498,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A32" s="12" t="s">
         <v>23</v>
       </c>
@@ -4564,7 +4605,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A33" s="12" t="s">
         <v>24</v>
       </c>
@@ -4671,7 +4712,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A34" s="12" t="s">
         <v>25</v>
       </c>
@@ -4778,7 +4819,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A35" s="12" t="s">
         <v>26</v>
       </c>
@@ -4885,7 +4926,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A36" s="12" t="s">
         <v>27</v>
       </c>
@@ -4992,7 +5033,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="37" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A37" s="12" t="s">
         <v>28</v>
       </c>
@@ -5099,7 +5140,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A38" s="12" t="s">
         <v>29</v>
       </c>
@@ -5206,7 +5247,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="39" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A39" s="12" t="s">
         <v>30</v>
       </c>
@@ -5313,7 +5354,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="40" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A40" s="12" t="s">
         <v>31</v>
       </c>
@@ -5420,7 +5461,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="41" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A41" s="12" t="s">
         <v>32</v>
       </c>
@@ -5527,7 +5568,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="42" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A42" s="12" t="s">
         <v>96</v>
       </c>
@@ -5634,7 +5675,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="43" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A43" s="12" t="s">
         <v>33</v>
       </c>
@@ -5741,7 +5782,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="44" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A44" s="12" t="s">
         <v>21</v>
       </c>
@@ -5848,7 +5889,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="45" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A45" s="13" t="s">
         <v>112</v>
       </c>
@@ -5955,7 +5996,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="46" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A46" s="12" t="s">
         <v>113</v>
       </c>
@@ -6062,7 +6103,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="47" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A47" s="12" t="s">
         <v>114</v>
       </c>
@@ -6169,7 +6210,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="48" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A48" s="12" t="s">
         <v>115</v>
       </c>
@@ -6276,7 +6317,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="49" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A49" s="12" t="s">
         <v>116</v>
       </c>
@@ -6390,22 +6431,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M45"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.19921875" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="14"/>
       <c r="B1" s="7" t="s">
         <v>117</v>
@@ -6426,25 +6467,13 @@
         <v>124</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="M1" s="7" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" s="13" t="s">
         <v>128</v>
       </c>
@@ -6472,20 +6501,8 @@
       <c r="I2" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="J2" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="K2" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="L2" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="M2" s="17" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="12" t="s">
         <v>129</v>
       </c>
@@ -6513,20 +6530,8 @@
       <c r="I3" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="J3" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="K3" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="L3" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="M3" s="17" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="12" t="s">
         <v>130</v>
       </c>
@@ -6554,20 +6559,8 @@
       <c r="I4" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="J4" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="K4" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="L4" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="M4" s="17" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="12" t="s">
         <v>131</v>
       </c>
@@ -6595,20 +6588,8 @@
       <c r="I5" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="J5" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="K5" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="L5" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="M5" s="17" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="12" t="s">
         <v>131</v>
       </c>
@@ -6636,20 +6617,8 @@
       <c r="I6" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="J6" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="K6" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="L6" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="M6" s="17" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="16" t="s">
         <v>132</v>
       </c>
@@ -6677,20 +6646,8 @@
       <c r="I7" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="J7" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="K7" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="L7" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="M7" s="17" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" s="16" t="s">
         <v>155</v>
       </c>
@@ -6718,20 +6675,8 @@
       <c r="I8" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="J8" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="K8" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="L8" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="M8" s="17" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" s="16" t="s">
         <v>133</v>
       </c>
@@ -6759,20 +6704,8 @@
       <c r="I9" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="J9" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="K9" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="L9" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="M9" s="17" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" s="15" t="s">
         <v>134</v>
       </c>
@@ -6800,20 +6733,8 @@
       <c r="I10" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="J10" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="K10" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="L10" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="M10" s="17" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" s="15" t="s">
         <v>135</v>
       </c>
@@ -6841,20 +6762,8 @@
       <c r="I11" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="J11" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="K11" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="L11" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="M11" s="17" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" s="16" t="s">
         <v>136</v>
       </c>
@@ -6882,20 +6791,8 @@
       <c r="I12" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="J12" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="K12" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="L12" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="M12" s="17" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" s="16" t="s">
         <v>137</v>
       </c>
@@ -6923,20 +6820,8 @@
       <c r="I13" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="J13" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="K13" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="L13" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="M13" s="17" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" s="15" t="s">
         <v>138</v>
       </c>
@@ -6964,20 +6849,8 @@
       <c r="I14" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="J14" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="K14" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="L14" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="M14" s="17" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" s="15" t="s">
         <v>139</v>
       </c>
@@ -7002,23 +6875,11 @@
       <c r="H15" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="I15" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="J15" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="K15" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="L15" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="M15" s="2" t="s">
+      <c r="I15" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" s="15" t="s">
         <v>140</v>
       </c>
@@ -7046,20 +6907,8 @@
       <c r="I16" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="J16" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="K16" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="L16" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="M16" s="17" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" s="15" t="s">
         <v>141</v>
       </c>
@@ -7084,23 +6933,11 @@
       <c r="H17" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="I17" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="J17" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="K17" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="L17" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="M17" s="2" t="s">
+      <c r="I17" s="2" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" s="15" t="s">
         <v>142</v>
       </c>
@@ -7128,20 +6965,8 @@
       <c r="I18" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="J18" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="K18" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="L18" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="M18" s="17" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" s="16" t="s">
         <v>157</v>
       </c>
@@ -7166,23 +6991,11 @@
       <c r="H19" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="I19" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="J19" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="K19" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="L19" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="M19" s="2" t="s">
+      <c r="I19" s="2" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" s="16" t="s">
         <v>158</v>
       </c>
@@ -7207,23 +7020,11 @@
       <c r="H20" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="I20" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="J20" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="K20" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="L20" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="M20" s="2" t="s">
+      <c r="I20" s="2" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" s="15" t="s">
         <v>143</v>
       </c>
@@ -7251,20 +7052,8 @@
       <c r="I21" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="J21" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="K21" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="L21" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="M21" s="17" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" s="15" t="s">
         <v>144</v>
       </c>
@@ -7292,20 +7081,8 @@
       <c r="I22" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="J22" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="K22" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="L22" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="M22" s="17" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" s="16" t="s">
         <v>145</v>
       </c>
@@ -7333,20 +7110,8 @@
       <c r="I23" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="J23" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="K23" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="L23" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="M23" s="17" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" s="15" t="s">
         <v>146</v>
       </c>
@@ -7374,20 +7139,8 @@
       <c r="I24" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="J24" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="K24" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="L24" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="M24" s="17" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" s="16" t="s">
         <v>159</v>
       </c>
@@ -7412,23 +7165,11 @@
       <c r="H25" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="I25" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="J25" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="K25" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="L25" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="M25" s="2" t="s">
+      <c r="I25" s="2" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" s="16" t="s">
         <v>160</v>
       </c>
@@ -7453,23 +7194,11 @@
       <c r="H26" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="I26" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="J26" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="K26" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="L26" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="M26" s="2" t="s">
+      <c r="I26" s="2" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27" s="16" t="s">
         <v>161</v>
       </c>
@@ -7494,23 +7223,11 @@
       <c r="H27" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="I27" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="J27" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="K27" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="L27" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="M27" s="2" t="s">
+      <c r="I27" s="2" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A28" s="16" t="s">
         <v>162</v>
       </c>
@@ -7535,717 +7252,8 @@
       <c r="H28" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="I28" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="J28" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="K28" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="L28" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="M28" s="2" t="s">
+      <c r="I28" s="2" t="s">
         <v>177</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A29" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="C29" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="D29" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="E29" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="F29" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="G29" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="H29" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="I29" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="J29" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="K29" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="L29" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="M29" s="17" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A30" s="15" t="s">
-        <v>185</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="C30" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="D30" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="E30" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="F30" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="G30" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="H30" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="I30" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="J30" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="K30" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="L30" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="M30" s="17" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A31" s="15" t="s">
-        <v>163</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="C31" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="D31" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="E31" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="F31" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="G31" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="H31" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="I31" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="J31" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="K31" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="L31" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="M31" s="17" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A32" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="C32" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="D32" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="E32" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="F32" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="G32" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="H32" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="I32" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="J32" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="K32" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="L32" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="M32" s="17" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A33" s="15" t="s">
-        <v>164</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="C33" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="D33" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="E33" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="F33" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="G33" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="H33" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="I33" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="J33" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="K33" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="L33" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="M33" s="17" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A34" s="16" t="s">
-        <v>165</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="C34" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="D34" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="E34" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="F34" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="G34" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="H34" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="I34" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="J34" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="K34" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="L34" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="M34" s="5" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A35" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="C35" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="D35" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="E35" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="F35" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="G35" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="H35" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="I35" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="J35" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="K35" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="L35" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="M35" s="5" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A36" s="16" t="s">
-        <v>166</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="C36" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="D36" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="E36" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="F36" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="G36" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="H36" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="I36" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="J36" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="K36" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="L36" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="M36" s="17" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A37" s="15" t="s">
-        <v>167</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="C37" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="D37" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="E37" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="F37" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="G37" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="H37" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="I37" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="J37" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="K37" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="L37" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="M37" s="5" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A38" s="16" t="s">
-        <v>150</v>
-      </c>
-      <c r="B38" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="C38" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="D38" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="F38" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="G38" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="I38" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="J38" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="K38" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="L38" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="M38" s="5" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A39" s="15" t="s">
-        <v>168</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="C39" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="D39" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="E39" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="F39" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="G39" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="H39" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="I39" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="J39" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="K39" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="L39" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="M39" s="17" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A40" s="15" t="s">
-        <v>169</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="C40" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="D40" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="F40" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="G40" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="I40" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="J40" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="K40" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="L40" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="M40" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A41" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="C41" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="D41" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="E41" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="F41" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="G41" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="H41" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="I41" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="J41" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="K41" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="L41" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="M41" s="17" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A42" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="C42" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="D42" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="E42" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="F42" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="G42" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="H42" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="I42" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="J42" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="K42" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="L42" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="M42" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A43" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="B43" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="C43" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="D43" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="E43" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="F43" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="G43" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="H43" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="I43" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="J43" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="K43" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="L43" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="M43" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A44" s="16" t="s">
-        <v>171</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="C44" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="D44" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="E44" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="F44" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="G44" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="H44" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="I44" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="J44" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="K44" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="L44" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="M44" s="17" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A45" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="C45" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="D45" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="E45" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="F45" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="G45" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="H45" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="I45" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="J45" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="K45" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="L45" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="M45" s="2" t="s">
-        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -8256,19 +7264,561 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7189DEF6-EE8B-447E-B57D-16E4D9D72C70}">
+  <dimension ref="A1:I18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:I18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.59765625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="14"/>
+      <c r="B1" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A2" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A3" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="I3" s="17" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A4" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A5" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="I5" s="17" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A6" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="I6" s="17" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A7" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A8" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="H8" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A9" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="H9" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="I9" s="17" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A10" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="H10" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A11" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="H11" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A12" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="G12" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="H12" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="I12" s="17" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A13" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="H13" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A14" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="G14" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="H14" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="I14" s="17" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A15" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="G15" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="H15" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A16" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="G16" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="H16" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A17" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="G17" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="H17" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="I17" s="17" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="F18" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="G18" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="H18" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="8.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.9296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.06640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -8289,7 +7839,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
         <v>104</v>
       </c>
@@ -8309,7 +7859,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
         <v>103</v>
       </c>
@@ -8329,7 +7879,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="6" t="s">
         <v>107</v>
       </c>
@@ -8349,7 +7899,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FEAT: completes the changes on split date/time FSM.
</commit_message>
<xml_diff>
--- a/docs/lexer/lexer-FSM.xlsx
+++ b/docs/lexer/lexer-FSM.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Red\docs\lexer\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30E163C0-BE51-4329-9C5F-41863A835552}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2753" yWindow="525" windowWidth="16874" windowHeight="10455" tabRatio="564" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2750" yWindow="530" windowWidth="16870" windowHeight="10460" tabRatio="564" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="transitions" sheetId="3" r:id="rId1"/>
@@ -23,12 +17,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>dk</author>
   </authors>
   <commentList>
-    <comment ref="D7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="D7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -58,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2149" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2140" uniqueCount="188">
   <si>
     <t>S_START</t>
   </si>
@@ -615,13 +609,19 @@
     <t>T_TM_HM</t>
   </si>
   <si>
-    <t>S_TM_START2</t>
+    <t>T_TM_START</t>
+  </si>
+  <si>
+    <t>T_TM_START2</t>
+  </si>
+  <si>
+    <t>T_TM_ERROR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -887,7 +887,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -920,26 +920,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -972,23 +955,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1164,7 +1130,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1172,15 +1138,15 @@
       <selection pane="bottomLeft" activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.73046875" customWidth="1"/>
-    <col min="5" max="5" width="9.73046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="12" width="9.73046875" customWidth="1"/>
-    <col min="13" max="13" width="9.9296875" bestFit="1" customWidth="1"/>
-    <col min="14" max="35" width="9.73046875" customWidth="1"/>
+    <col min="1" max="1" width="10.36328125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" customWidth="1"/>
+    <col min="5" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="9.7265625" customWidth="1"/>
+    <col min="13" max="13" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="35" width="9.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -1288,7 +1254,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:35" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
@@ -1395,7 +1361,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:35" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A3" s="12" t="s">
         <v>69</v>
       </c>
@@ -1502,7 +1468,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:35" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A4" s="12" t="s">
         <v>70</v>
       </c>
@@ -1609,7 +1575,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:35" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A5" s="12" t="s">
         <v>1</v>
       </c>
@@ -1716,7 +1682,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:35" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A6" s="12" t="s">
         <v>2</v>
       </c>
@@ -1823,7 +1789,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:35" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A7" s="12" t="s">
         <v>74</v>
       </c>
@@ -1930,7 +1896,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:35" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A8" s="12" t="s">
         <v>3</v>
       </c>
@@ -2037,7 +2003,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:35" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A9" s="12" t="s">
         <v>4</v>
       </c>
@@ -2144,7 +2110,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:35" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A10" s="12" t="s">
         <v>109</v>
       </c>
@@ -2251,7 +2217,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:35" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A11" s="12" t="s">
         <v>110</v>
       </c>
@@ -2358,7 +2324,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:35" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A12" s="12" t="s">
         <v>111</v>
       </c>
@@ -2465,7 +2431,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:35" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A13" s="12" t="s">
         <v>5</v>
       </c>
@@ -2572,7 +2538,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:35" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A14" s="12" t="s">
         <v>6</v>
       </c>
@@ -2679,7 +2645,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:35" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A15" s="12" t="s">
         <v>7</v>
       </c>
@@ -2786,7 +2752,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:35" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A16" s="12" t="s">
         <v>71</v>
       </c>
@@ -2893,7 +2859,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:35" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A17" s="12" t="s">
         <v>8</v>
       </c>
@@ -3000,7 +2966,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:35" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A18" s="12" t="s">
         <v>9</v>
       </c>
@@ -3107,7 +3073,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:35" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A19" s="12" t="s">
         <v>10</v>
       </c>
@@ -3214,7 +3180,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:35" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A20" s="12" t="s">
         <v>11</v>
       </c>
@@ -3321,7 +3287,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:35" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A21" s="12" t="s">
         <v>12</v>
       </c>
@@ -3428,7 +3394,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:35" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A22" s="12" t="s">
         <v>86</v>
       </c>
@@ -3535,7 +3501,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:35" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A23" s="12" t="s">
         <v>13</v>
       </c>
@@ -3642,7 +3608,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:35" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A24" s="12" t="s">
         <v>14</v>
       </c>
@@ -3749,7 +3715,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:35" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A25" s="12" t="s">
         <v>15</v>
       </c>
@@ -3856,7 +3822,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:35" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A26" s="12" t="s">
         <v>16</v>
       </c>
@@ -3963,7 +3929,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:35" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A27" s="12" t="s">
         <v>17</v>
       </c>
@@ -4070,7 +4036,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:35" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A28" s="12" t="s">
         <v>18</v>
       </c>
@@ -4177,7 +4143,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:35" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A29" s="12" t="s">
         <v>19</v>
       </c>
@@ -4284,7 +4250,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:35" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A30" s="12" t="s">
         <v>20</v>
       </c>
@@ -4391,7 +4357,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:35" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A31" s="12" t="s">
         <v>22</v>
       </c>
@@ -4498,7 +4464,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:35" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A32" s="12" t="s">
         <v>23</v>
       </c>
@@ -4605,7 +4571,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:35" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A33" s="12" t="s">
         <v>24</v>
       </c>
@@ -4712,7 +4678,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:35" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A34" s="12" t="s">
         <v>25</v>
       </c>
@@ -4819,7 +4785,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:35" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A35" s="12" t="s">
         <v>26</v>
       </c>
@@ -4926,7 +4892,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:35" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A36" s="12" t="s">
         <v>27</v>
       </c>
@@ -5033,7 +4999,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="37" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:35" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A37" s="12" t="s">
         <v>28</v>
       </c>
@@ -5140,7 +5106,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:35" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A38" s="12" t="s">
         <v>29</v>
       </c>
@@ -5247,7 +5213,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="39" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:35" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A39" s="12" t="s">
         <v>30</v>
       </c>
@@ -5354,7 +5320,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="40" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:35" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A40" s="12" t="s">
         <v>31</v>
       </c>
@@ -5461,7 +5427,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="41" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:35" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A41" s="12" t="s">
         <v>32</v>
       </c>
@@ -5568,7 +5534,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="42" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:35" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A42" s="12" t="s">
         <v>96</v>
       </c>
@@ -5675,7 +5641,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="43" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:35" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A43" s="12" t="s">
         <v>33</v>
       </c>
@@ -5782,7 +5748,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="44" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:35" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A44" s="12" t="s">
         <v>21</v>
       </c>
@@ -5889,7 +5855,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="45" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:35" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A45" s="13" t="s">
         <v>112</v>
       </c>
@@ -5996,7 +5962,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="46" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:35" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A46" s="12" t="s">
         <v>113</v>
       </c>
@@ -6103,7 +6069,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="47" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:35" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A47" s="12" t="s">
         <v>114</v>
       </c>
@@ -6210,7 +6176,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="48" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:35" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A48" s="12" t="s">
         <v>115</v>
       </c>
@@ -6317,7 +6283,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="49" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:35" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A49" s="12" t="s">
         <v>116</v>
       </c>
@@ -6431,19 +6397,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -6473,7 +6440,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A2" s="13" t="s">
         <v>128</v>
       </c>
@@ -6502,7 +6469,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A3" s="12" t="s">
         <v>129</v>
       </c>
@@ -6531,7 +6498,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A4" s="12" t="s">
         <v>130</v>
       </c>
@@ -6560,7 +6527,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A5" s="12" t="s">
         <v>131</v>
       </c>
@@ -6589,7 +6556,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A6" s="12" t="s">
         <v>131</v>
       </c>
@@ -6618,7 +6585,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A7" s="16" t="s">
         <v>132</v>
       </c>
@@ -6647,7 +6614,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A8" s="16" t="s">
         <v>155</v>
       </c>
@@ -6676,7 +6643,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A9" s="16" t="s">
         <v>133</v>
       </c>
@@ -6705,7 +6672,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A10" s="15" t="s">
         <v>134</v>
       </c>
@@ -6734,7 +6701,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A11" s="15" t="s">
         <v>135</v>
       </c>
@@ -6763,7 +6730,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A12" s="16" t="s">
         <v>136</v>
       </c>
@@ -6792,7 +6759,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A13" s="16" t="s">
         <v>137</v>
       </c>
@@ -6809,7 +6776,7 @@
         <v>175</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>147</v>
+        <v>185</v>
       </c>
       <c r="G13" s="17" t="s">
         <v>175</v>
@@ -6821,7 +6788,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A14" s="15" t="s">
         <v>138</v>
       </c>
@@ -6850,7 +6817,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A15" s="15" t="s">
         <v>139</v>
       </c>
@@ -6879,7 +6846,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A16" s="15" t="s">
         <v>140</v>
       </c>
@@ -6896,7 +6863,7 @@
         <v>175</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>147</v>
+        <v>185</v>
       </c>
       <c r="G16" s="17" t="s">
         <v>175</v>
@@ -6908,7 +6875,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:9" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A17" s="15" t="s">
         <v>141</v>
       </c>
@@ -6925,7 +6892,7 @@
         <v>175</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>147</v>
+        <v>185</v>
       </c>
       <c r="G17" s="17" t="s">
         <v>175</v>
@@ -6937,7 +6904,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:9" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A18" s="15" t="s">
         <v>142</v>
       </c>
@@ -6966,7 +6933,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:9" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A19" s="16" t="s">
         <v>157</v>
       </c>
@@ -6977,13 +6944,13 @@
         <v>175</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>147</v>
+        <v>185</v>
       </c>
       <c r="E19" s="17" t="s">
         <v>175</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>147</v>
+        <v>185</v>
       </c>
       <c r="G19" s="17" t="s">
         <v>175</v>
@@ -6995,7 +6962,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:9" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A20" s="16" t="s">
         <v>158</v>
       </c>
@@ -7006,13 +6973,13 @@
         <v>175</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>147</v>
+        <v>185</v>
       </c>
       <c r="E20" s="17" t="s">
         <v>175</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>147</v>
+        <v>185</v>
       </c>
       <c r="G20" s="17" t="s">
         <v>175</v>
@@ -7024,7 +6991,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:9" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A21" s="15" t="s">
         <v>143</v>
       </c>
@@ -7053,7 +7020,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:9" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A22" s="15" t="s">
         <v>144</v>
       </c>
@@ -7082,7 +7049,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:9" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A23" s="16" t="s">
         <v>145</v>
       </c>
@@ -7111,7 +7078,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:9" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A24" s="15" t="s">
         <v>146</v>
       </c>
@@ -7140,7 +7107,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:9" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A25" s="16" t="s">
         <v>159</v>
       </c>
@@ -7151,13 +7118,13 @@
         <v>175</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E25" s="17" t="s">
         <v>175</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="G25" s="17" t="s">
         <v>175</v>
@@ -7169,7 +7136,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:9" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A26" s="16" t="s">
         <v>160</v>
       </c>
@@ -7180,13 +7147,13 @@
         <v>175</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E26" s="17" t="s">
         <v>175</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="G26" s="17" t="s">
         <v>175</v>
@@ -7198,7 +7165,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:9" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A27" s="16" t="s">
         <v>161</v>
       </c>
@@ -7209,13 +7176,13 @@
         <v>175</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E27" s="17" t="s">
         <v>175</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="G27" s="17" t="s">
         <v>175</v>
@@ -7227,7 +7194,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:9" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A28" s="16" t="s">
         <v>162</v>
       </c>
@@ -7238,13 +7205,13 @@
         <v>175</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E28" s="17" t="s">
         <v>175</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="G28" s="17" t="s">
         <v>175</v>
@@ -7264,19 +7231,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7189DEF6-EE8B-447E-B57D-16E4D9D72C70}">
-  <dimension ref="A1:I18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:I18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -7306,7 +7274,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
         <v>147</v>
       </c>
@@ -7314,488 +7282,459 @@
         <v>163</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
-        <v>185</v>
+        <v>163</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="G3" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="H3" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="I3" s="17" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A4" s="15" t="s">
-        <v>163</v>
+        <v>187</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A4" s="16" t="s">
+        <v>148</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>148</v>
+        <v>165</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>164</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="H4" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="I4" s="17" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A5" s="16" t="s">
-        <v>148</v>
+        <v>187</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A5" s="15" t="s">
+        <v>164</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>165</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>164</v>
+        <v>187</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>187</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="H5" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="I5" s="17" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A6" s="15" t="s">
-        <v>164</v>
+        <v>187</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A6" s="16" t="s">
+        <v>165</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>165</v>
+        <v>149</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="H6" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="I6" s="17" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A7" s="16" t="s">
-        <v>165</v>
+        <v>187</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A7" s="15" t="s">
+        <v>149</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>149</v>
+        <v>167</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>166</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="I7" s="5" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A8" s="15" t="s">
-        <v>149</v>
+    <row r="8" spans="1:9" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A8" s="16" t="s">
+        <v>166</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>167</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>166</v>
+        <v>187</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>187</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A9" s="16" t="s">
-        <v>166</v>
+        <v>187</v>
+      </c>
+      <c r="I8" s="17" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A9" s="15" t="s">
+        <v>167</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="H9" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="I9" s="17" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A10" s="15" t="s">
-        <v>167</v>
-      </c>
-      <c r="B10" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A10" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="C10" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>175</v>
+      <c r="B10" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>151</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="F10" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>168</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="H10" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="I10" s="5" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A11" s="16" t="s">
-        <v>150</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>151</v>
+    <row r="11" spans="1:9" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A11" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>187</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>168</v>
+        <v>187</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>187</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="H11" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+        <v>187</v>
+      </c>
+      <c r="I11" s="17" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A12" s="15" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="C12" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>175</v>
+      <c r="C12" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>151</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="F12" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="G12" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>170</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="I12" s="17" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+        <v>187</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A13" s="15" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>187</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="F13" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>170</v>
+        <v>187</v>
+      </c>
+      <c r="G13" s="17" t="s">
+        <v>187</v>
       </c>
       <c r="H13" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+        <v>187</v>
+      </c>
+      <c r="I13" s="17" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A14" s="15" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="E14" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>171</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="H14" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="I14" s="17" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A15" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="B15" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A15" s="16" t="s">
         <v>153</v>
       </c>
+      <c r="B15" s="17" t="s">
+        <v>187</v>
+      </c>
       <c r="C15" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>171</v>
       </c>
       <c r="F15" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="H15" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A16" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>175</v>
+        <v>171</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>154</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>171</v>
+        <v>187</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>187</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A17" s="16" t="s">
-        <v>171</v>
+        <v>187</v>
+      </c>
+      <c r="I16" s="17" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="15" t="s">
+        <v>154</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="G17" s="17" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="H17" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="I17" s="17" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="E18" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="F18" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="G18" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="H18" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="I18" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="I17" s="2" t="s">
         <v>174</v>
       </c>
     </row>
@@ -7806,19 +7745,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.9296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.06640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.19921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -7839,7 +7778,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
         <v>104</v>
       </c>
@@ -7859,7 +7798,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
         <v>103</v>
       </c>
@@ -7879,7 +7818,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A4" s="6" t="s">
         <v>107</v>
       </c>
@@ -7899,7 +7838,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A5" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FEAT: adds support for scanning time! values.
</commit_message>
<xml_diff>
--- a/docs/lexer/lexer-FSM.xlsx
+++ b/docs/lexer/lexer-FSM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-28100" yWindow="150" windowWidth="17030" windowHeight="15020" tabRatio="564" activeTab="1"/>
+    <workbookView xWindow="-28100" yWindow="150" windowWidth="17030" windowHeight="15020" tabRatio="564"/>
   </bookViews>
   <sheets>
     <sheet name="transitions" sheetId="3" r:id="rId1"/>
@@ -1126,9 +1126,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O26" sqref="O26"/>
+      <selection pane="bottomLeft" activeCell="AI28" sqref="AI28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4133,7 +4133,7 @@
         <v>63</v>
       </c>
       <c r="AI28" s="1" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
     </row>
     <row r="29" spans="1:35" x14ac:dyDescent="0.35">
@@ -6393,7 +6393,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
FEAT: completes support for basic date! formats.
Some ISO formats still need more work.
</commit_message>
<xml_diff>
--- a/docs/lexer/lexer-FSM.xlsx
+++ b/docs/lexer/lexer-FSM.xlsx
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2422" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2435" uniqueCount="193">
   <si>
     <t>S_START</t>
   </si>
@@ -627,6 +627,9 @@
   </si>
   <si>
     <t>T_DT_YDDD</t>
+  </si>
+  <si>
+    <t>T_TZ_M</t>
   </si>
 </sst>
 </file>
@@ -6556,10 +6559,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M49"/>
+  <dimension ref="A1:M50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6776,10 +6779,10 @@
     </row>
     <row r="6" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A6" s="12" t="s">
-        <v>131</v>
+        <v>179</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C6" s="17" t="s">
         <v>174</v>
@@ -6984,7 +6987,7 @@
         <v>135</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>136</v>
+        <v>156</v>
       </c>
       <c r="C11" s="17" t="s">
         <v>174</v>
@@ -8076,8 +8079,8 @@
       <c r="J37" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="K37" s="17" t="s">
-        <v>174</v>
+      <c r="K37" s="5" t="s">
+        <v>183</v>
       </c>
       <c r="L37" s="17" t="s">
         <v>174</v>
@@ -8460,7 +8463,7 @@
         <v>152</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="C47" s="17" t="s">
         <v>174</v>
@@ -8534,10 +8537,10 @@
         <v>174</v>
       </c>
       <c r="M48" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="15" t="s">
         <v>153</v>
       </c>
@@ -8576,6 +8579,47 @@
       </c>
       <c r="M49" s="2" t="s">
         <v>173</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="B50" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="C50" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D50" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="E50" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="F50" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="G50" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="H50" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="I50" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="J50" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="K50" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="L50" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="M50" s="17" t="s">
+        <v>174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FEAT: now all date! formats are recognized properly.
</commit_message>
<xml_diff>
--- a/docs/lexer/lexer-FSM.xlsx
+++ b/docs/lexer/lexer-FSM.xlsx
@@ -15,43 +15,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>dk</author>
-  </authors>
-  <commentList>
-    <comment ref="D7" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>dk:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
- FIXME: /////...
-</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2435" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2448" uniqueCount="194">
   <si>
     <t>S_START</t>
   </si>
@@ -630,13 +595,16 @@
   </si>
   <si>
     <t>T_TZ_M</t>
+  </si>
+  <si>
+    <t>S_DT_YWD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -688,19 +656,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="8"/>
@@ -838,7 +793,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1149,7 +1104,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q21" sqref="Q21"/>
+      <selection pane="bottomLeft" activeCell="U52" sqref="U52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6558,11 +6513,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M50"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6750,7 +6705,7 @@
         <v>132</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>132</v>
+        <v>154</v>
       </c>
       <c r="F5" s="17" t="s">
         <v>174</v>
@@ -6791,7 +6746,7 @@
         <v>132</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>132</v>
+        <v>154</v>
       </c>
       <c r="F6" s="17" t="s">
         <v>174</v>
@@ -6818,7 +6773,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="16" t="s">
         <v>132</v>
       </c>
@@ -6828,11 +6783,11 @@
       <c r="C7" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>154</v>
+      <c r="D7" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>174</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>142</v>
@@ -7269,12 +7224,12 @@
         <v>178</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>141</v>
+      <c r="B18" s="17" t="s">
+        <v>174</v>
       </c>
       <c r="C18" s="17" t="s">
         <v>174</v>
@@ -7282,8 +7237,8 @@
       <c r="D18" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="E18" s="17" t="s">
-        <v>174</v>
+      <c r="E18" s="5" t="s">
+        <v>193</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>147</v>
@@ -7306,16 +7261,16 @@
       <c r="L18" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="M18" s="17" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="M18" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>141</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>174</v>
       </c>
       <c r="C19" s="17" t="s">
         <v>174</v>
@@ -7347,70 +7302,70 @@
       <c r="L19" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="M19" s="2" t="s">
+      <c r="M19" s="17" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A20" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="G20" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="H20" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="I20" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="J20" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="K20" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="L20" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="M20" s="2" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A20" s="15" t="s">
+    <row r="21" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A21" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="B20" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="C20" s="2" t="s">
+      <c r="B21" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F21" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="G20" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H20" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="I20" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="J20" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K20" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="L20" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="M20" s="17" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A21" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="E21" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>147</v>
-      </c>
       <c r="G21" s="17" t="s">
         <v>174</v>
       </c>
@@ -7429,16 +7384,16 @@
       <c r="L21" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="M21" s="2" t="s">
-        <v>175</v>
+      <c r="M21" s="17" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A22" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>157</v>
-      </c>
-      <c r="B22" s="17" t="s">
-        <v>174</v>
       </c>
       <c r="C22" s="17" t="s">
         <v>174</v>
@@ -7475,52 +7430,52 @@
       </c>
     </row>
     <row r="23" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A23" s="15" t="s">
+      <c r="A23" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="G23" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="H23" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="I23" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="J23" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="K23" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="L23" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A24" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B24" s="2" t="s">
         <v>144</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F23" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="G23" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H23" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="I23" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="J23" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K23" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="L23" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="M23" s="17" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A24" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="B24" s="17" t="s">
-        <v>174</v>
       </c>
       <c r="C24" s="17" t="s">
         <v>174</v>
@@ -7557,106 +7512,106 @@
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A25" s="16" t="s">
+      <c r="A25" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="E25" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F25" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="G25" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="H25" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="I25" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="J25" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="K25" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="L25" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="M25" s="17" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A26" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="C25" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D25" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="E25" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="F25" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="G25" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H25" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="I25" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="J25" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K25" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="L25" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="M25" s="17" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A26" s="15" t="s">
+      <c r="C26" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="F26" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="G26" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="H26" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="I26" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="J26" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="K26" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="L26" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="M26" s="17" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A27" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="B26" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="C26" s="2" t="s">
+      <c r="B27" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="E27" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="F27" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="G26" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H26" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="I26" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="J26" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K26" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="L26" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="M26" s="17" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A27" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="C27" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="E27" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>184</v>
-      </c>
       <c r="G27" s="17" t="s">
         <v>174</v>
       </c>
@@ -7675,16 +7630,16 @@
       <c r="L27" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="M27" s="2" t="s">
-        <v>176</v>
+      <c r="M27" s="17" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A28" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>159</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>160</v>
       </c>
       <c r="C28" s="17" t="s">
         <v>174</v>
@@ -7722,10 +7677,10 @@
     </row>
     <row r="29" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A29" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="C29" s="17" t="s">
         <v>174</v>
@@ -7763,10 +7718,10 @@
     </row>
     <row r="30" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A30" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>161</v>
-      </c>
-      <c r="B30" s="17" t="s">
-        <v>174</v>
       </c>
       <c r="C30" s="17" t="s">
         <v>174</v>
@@ -7802,50 +7757,50 @@
         <v>176</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A31" s="13" t="s">
+    <row r="31" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A31" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="C31" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="E31" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="G31" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="H31" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="I31" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="J31" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="K31" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="L31" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="M31" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A32" s="13" t="s">
         <v>147</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="C31" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D31" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="E31" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="F31" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="G31" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H31" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="I31" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="J31" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K31" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="L31" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="M31" s="17" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A32" s="15" t="s">
-        <v>184</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>162</v>
@@ -7886,51 +7841,51 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="C33" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D33" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="E33" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="F33" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="G33" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="H33" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="I33" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="J33" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="K33" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="L33" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="M33" s="17" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A34" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>148</v>
-      </c>
-      <c r="C33" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D33" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="E33" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="F33" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="G33" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H33" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="I33" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="J33" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K33" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="L33" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="M33" s="17" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A34" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>164</v>
       </c>
       <c r="C34" s="17" t="s">
         <v>174</v>
@@ -7967,8 +7922,8 @@
       </c>
     </row>
     <row r="35" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A35" s="15" t="s">
-        <v>163</v>
+      <c r="A35" s="16" t="s">
+        <v>148</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>164</v>
@@ -7991,8 +7946,8 @@
       <c r="H35" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="I35" s="17" t="s">
-        <v>174</v>
+      <c r="I35" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="J35" s="17" t="s">
         <v>174</v>
@@ -8007,53 +7962,53 @@
         <v>174</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A36" s="16" t="s">
+    <row r="36" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A36" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="C36" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D36" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="E36" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="F36" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="G36" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="H36" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="I36" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="J36" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="K36" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="L36" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="M36" s="17" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A37" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>149</v>
-      </c>
-      <c r="C36" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D36" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="F36" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="G36" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H36" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="I36" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="J36" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K36" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="L36" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="M36" s="5" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A37" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>166</v>
       </c>
       <c r="C37" s="17" t="s">
         <v>174</v>
@@ -8079,8 +8034,8 @@
       <c r="J37" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="K37" s="5" t="s">
-        <v>183</v>
+      <c r="K37" s="17" t="s">
+        <v>174</v>
       </c>
       <c r="L37" s="17" t="s">
         <v>174</v>
@@ -8089,9 +8044,9 @@
         <v>183</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A38" s="16" t="s">
-        <v>165</v>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A38" s="15" t="s">
+        <v>149</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>166</v>
@@ -8102,8 +8057,8 @@
       <c r="D38" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="E38" s="17" t="s">
-        <v>174</v>
+      <c r="E38" s="5" t="s">
+        <v>186</v>
       </c>
       <c r="F38" s="17" t="s">
         <v>174</v>
@@ -8111,72 +8066,72 @@
       <c r="G38" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="H38" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="I38" s="17" t="s">
-        <v>174</v>
+      <c r="H38" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>165</v>
       </c>
       <c r="J38" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="K38" s="17" t="s">
-        <v>174</v>
+      <c r="K38" s="5" t="s">
+        <v>183</v>
       </c>
       <c r="L38" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="M38" s="17" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A39" s="15" t="s">
+      <c r="M38" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A39" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="C39" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D39" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="E39" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="F39" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="G39" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="H39" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="I39" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="J39" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="K39" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="L39" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="M39" s="17" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A40" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>150</v>
-      </c>
-      <c r="C39" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D39" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="F39" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="G39" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="I39" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="J39" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K39" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="L39" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="M39" s="5" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A40" s="16" t="s">
-        <v>150</v>
-      </c>
-      <c r="B40" s="17" t="s">
-        <v>174</v>
       </c>
       <c r="C40" s="17" t="s">
         <v>174</v>
@@ -8199,11 +8154,11 @@
       <c r="I40" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="J40" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="K40" s="5" t="s">
-        <v>182</v>
+      <c r="J40" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="K40" s="17" t="s">
+        <v>174</v>
       </c>
       <c r="L40" s="17" t="s">
         <v>174</v>
@@ -8212,50 +8167,50 @@
         <v>182</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A41" s="15" t="s">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A41" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="B41" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="C41" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D41" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="F41" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="G41" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="I41" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="J41" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="C41" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D41" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="E41" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="F41" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="G41" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H41" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="I41" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="J41" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K41" s="17" t="s">
-        <v>174</v>
+      <c r="K41" s="5" t="s">
+        <v>182</v>
       </c>
       <c r="L41" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="M41" s="17" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M41" s="5" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A42" s="15" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>168</v>
@@ -8266,8 +8221,8 @@
       <c r="D42" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="E42" s="2" t="s">
-        <v>188</v>
+      <c r="E42" s="17" t="s">
+        <v>174</v>
       </c>
       <c r="F42" s="17" t="s">
         <v>174</v>
@@ -8275,8 +8230,8 @@
       <c r="G42" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="H42" s="2" t="s">
-        <v>188</v>
+      <c r="H42" s="17" t="s">
+        <v>174</v>
       </c>
       <c r="I42" s="17" t="s">
         <v>174</v>
@@ -8284,22 +8239,22 @@
       <c r="J42" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="K42" s="2" t="s">
-        <v>169</v>
+      <c r="K42" s="17" t="s">
+        <v>174</v>
       </c>
       <c r="L42" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="M42" s="2" t="s">
-        <v>169</v>
+      <c r="M42" s="17" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A43" s="15" t="s">
-        <v>186</v>
+        <v>168</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>151</v>
+        <v>168</v>
       </c>
       <c r="C43" s="17" t="s">
         <v>174</v>
@@ -8307,8 +8262,8 @@
       <c r="D43" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="E43" s="17" t="s">
-        <v>174</v>
+      <c r="E43" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="F43" s="17" t="s">
         <v>174</v>
@@ -8316,8 +8271,8 @@
       <c r="G43" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="H43" s="17" t="s">
-        <v>174</v>
+      <c r="H43" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="I43" s="17" t="s">
         <v>174</v>
@@ -8325,19 +8280,19 @@
       <c r="J43" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="K43" s="17" t="s">
-        <v>174</v>
+      <c r="K43" s="2" t="s">
+        <v>169</v>
       </c>
       <c r="L43" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="M43" s="17" t="s">
-        <v>174</v>
+      <c r="M43" s="2" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A44" s="15" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>151</v>
@@ -8378,7 +8333,7 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A45" s="15" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>151</v>
@@ -8417,53 +8372,53 @@
         <v>174</v>
       </c>
     </row>
-    <row r="46" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A46" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="C46" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D46" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="E46" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="F46" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="G46" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="H46" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="I46" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="J46" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="K46" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="L46" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="M46" s="17" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A47" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>152</v>
-      </c>
-      <c r="C46" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D46" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="E46" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="F46" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="G46" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H46" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="I46" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="J46" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K46" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="L46" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="M46" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A47" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>153</v>
       </c>
       <c r="C47" s="17" t="s">
         <v>174</v>
@@ -8496,12 +8451,12 @@
         <v>174</v>
       </c>
       <c r="M47" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A48" s="16" t="s">
-        <v>170</v>
+        <v>152</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>153</v>
@@ -8524,8 +8479,8 @@
       <c r="H48" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="I48" s="17" t="s">
-        <v>174</v>
+      <c r="I48" s="2" t="s">
+        <v>170</v>
       </c>
       <c r="J48" s="17" t="s">
         <v>174</v>
@@ -8537,56 +8492,56 @@
         <v>174</v>
       </c>
       <c r="M48" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A49" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C49" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D49" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="E49" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="F49" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="G49" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="H49" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="I49" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="J49" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="K49" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="L49" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="M49" s="2" t="s">
         <v>192</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="C49" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D49" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="E49" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="F49" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="G49" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H49" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="I49" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="J49" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K49" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="L49" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="M49" s="2" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="50" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="B50" s="17" t="s">
-        <v>174</v>
+        <v>153</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>173</v>
       </c>
       <c r="C50" s="17" t="s">
         <v>174</v>
@@ -8618,14 +8573,54 @@
       <c r="L50" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="M50" s="17" t="s">
+      <c r="M50" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="B51" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="C51" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D51" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="E51" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="F51" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="G51" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="H51" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="I51" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="J51" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="K51" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="L51" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="M51" s="17" t="s">
         <v>174</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
FIX: removes unnecessary states in date! FSM.
</commit_message>
<xml_diff>
--- a/docs/lexer/lexer-FSM.xlsx
+++ b/docs/lexer/lexer-FSM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2448" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2409" uniqueCount="191">
   <si>
     <t>S_START</t>
   </si>
@@ -570,19 +570,10 @@
     <t>T_TM_HM</t>
   </si>
   <si>
-    <t>S_TM_START2</t>
-  </si>
-  <si>
     <t>C_T</t>
   </si>
   <si>
     <t>S_TM_HMZ</t>
-  </si>
-  <si>
-    <t>S_TM_HMSZ</t>
-  </si>
-  <si>
-    <t>S_TM_HMSNZ</t>
   </si>
   <si>
     <t>S_DT_YM2</t>
@@ -1166,7 +1157,7 @@
         <v>47</v>
       </c>
       <c r="Q1" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="R1" s="7" t="s">
         <v>48</v>
@@ -6514,10 +6505,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M51"/>
+  <dimension ref="A1:M48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6819,7 +6810,7 @@
         <v>154</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>142</v>
@@ -6980,10 +6971,10 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="15" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C12" s="17" t="s">
         <v>174</v>
@@ -7021,7 +7012,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="15" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>137</v>
@@ -7139,7 +7130,7 @@
         <v>174</v>
       </c>
       <c r="M15" s="5" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.35">
@@ -7238,7 +7229,7 @@
         <v>174</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>147</v>
@@ -7267,7 +7258,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="15" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>141</v>
@@ -7645,13 +7636,13 @@
         <v>174</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>184</v>
+        <v>147</v>
       </c>
       <c r="E28" s="17" t="s">
         <v>174</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>184</v>
+        <v>147</v>
       </c>
       <c r="G28" s="17" t="s">
         <v>174</v>
@@ -7686,13 +7677,13 @@
         <v>174</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>184</v>
+        <v>147</v>
       </c>
       <c r="E29" s="17" t="s">
         <v>174</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>184</v>
+        <v>147</v>
       </c>
       <c r="G29" s="17" t="s">
         <v>174</v>
@@ -7727,13 +7718,13 @@
         <v>174</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>184</v>
+        <v>147</v>
       </c>
       <c r="E30" s="17" t="s">
         <v>174</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>184</v>
+        <v>147</v>
       </c>
       <c r="G30" s="17" t="s">
         <v>174</v>
@@ -7768,13 +7759,13 @@
         <v>174</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>184</v>
+        <v>147</v>
       </c>
       <c r="E31" s="17" t="s">
         <v>174</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>184</v>
+        <v>147</v>
       </c>
       <c r="G31" s="17" t="s">
         <v>174</v>
@@ -7841,10 +7832,10 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" s="15" t="s">
-        <v>184</v>
+        <v>162</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="C33" s="17" t="s">
         <v>174</v>
@@ -7864,8 +7855,8 @@
       <c r="H33" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="I33" s="17" t="s">
-        <v>174</v>
+      <c r="I33" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="J33" s="17" t="s">
         <v>174</v>
@@ -7880,12 +7871,12 @@
         <v>174</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A34" s="15" t="s">
-        <v>162</v>
+    <row r="34" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A34" s="16" t="s">
+        <v>148</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>148</v>
+        <v>164</v>
       </c>
       <c r="C34" s="17" t="s">
         <v>174</v>
@@ -7922,8 +7913,8 @@
       </c>
     </row>
     <row r="35" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A35" s="16" t="s">
-        <v>148</v>
+      <c r="A35" s="15" t="s">
+        <v>163</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>164</v>
@@ -7946,8 +7937,8 @@
       <c r="H35" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="I35" s="2" t="s">
-        <v>163</v>
+      <c r="I35" s="17" t="s">
+        <v>174</v>
       </c>
       <c r="J35" s="17" t="s">
         <v>174</v>
@@ -7962,12 +7953,12 @@
         <v>174</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A36" s="15" t="s">
-        <v>163</v>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A36" s="16" t="s">
+        <v>164</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="C36" s="17" t="s">
         <v>174</v>
@@ -7975,8 +7966,8 @@
       <c r="D36" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="E36" s="17" t="s">
-        <v>174</v>
+      <c r="E36" s="5" t="s">
+        <v>185</v>
       </c>
       <c r="F36" s="17" t="s">
         <v>174</v>
@@ -7984,11 +7975,11 @@
       <c r="G36" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="H36" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="I36" s="17" t="s">
-        <v>174</v>
+      <c r="H36" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>165</v>
       </c>
       <c r="J36" s="17" t="s">
         <v>174</v>
@@ -7999,16 +7990,16 @@
       <c r="L36" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="M36" s="17" t="s">
-        <v>174</v>
+      <c r="M36" s="5" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A37" s="16" t="s">
-        <v>164</v>
+      <c r="A37" s="15" t="s">
+        <v>149</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>149</v>
+        <v>166</v>
       </c>
       <c r="C37" s="17" t="s">
         <v>174</v>
@@ -8017,7 +8008,7 @@
         <v>174</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F37" s="17" t="s">
         <v>174</v>
@@ -8026,7 +8017,7 @@
         <v>174</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I37" s="2" t="s">
         <v>165</v>
@@ -8034,8 +8025,8 @@
       <c r="J37" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="K37" s="17" t="s">
-        <v>174</v>
+      <c r="K37" s="5" t="s">
+        <v>183</v>
       </c>
       <c r="L37" s="17" t="s">
         <v>174</v>
@@ -8044,9 +8035,9 @@
         <v>183</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A38" s="15" t="s">
-        <v>149</v>
+    <row r="38" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A38" s="16" t="s">
+        <v>165</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>166</v>
@@ -8057,8 +8048,8 @@
       <c r="D38" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="E38" s="5" t="s">
-        <v>186</v>
+      <c r="E38" s="17" t="s">
+        <v>174</v>
       </c>
       <c r="F38" s="17" t="s">
         <v>174</v>
@@ -8066,31 +8057,31 @@
       <c r="G38" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="H38" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>165</v>
+      <c r="H38" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="I38" s="17" t="s">
+        <v>174</v>
       </c>
       <c r="J38" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="K38" s="5" t="s">
-        <v>183</v>
+      <c r="K38" s="17" t="s">
+        <v>174</v>
       </c>
       <c r="L38" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="M38" s="5" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A39" s="16" t="s">
-        <v>165</v>
+      <c r="M38" s="17" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A39" s="15" t="s">
+        <v>166</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>166</v>
+        <v>150</v>
       </c>
       <c r="C39" s="17" t="s">
         <v>174</v>
@@ -8098,8 +8089,8 @@
       <c r="D39" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="E39" s="17" t="s">
-        <v>174</v>
+      <c r="E39" s="2" t="s">
+        <v>185</v>
       </c>
       <c r="F39" s="17" t="s">
         <v>174</v>
@@ -8107,8 +8098,8 @@
       <c r="G39" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="H39" s="17" t="s">
-        <v>174</v>
+      <c r="H39" s="2" t="s">
+        <v>185</v>
       </c>
       <c r="I39" s="17" t="s">
         <v>174</v>
@@ -8122,17 +8113,17 @@
       <c r="L39" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="M39" s="17" t="s">
-        <v>174</v>
+      <c r="M39" s="5" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A40" s="15" t="s">
-        <v>166</v>
-      </c>
-      <c r="B40" s="2" t="s">
+      <c r="A40" s="16" t="s">
         <v>150</v>
       </c>
+      <c r="B40" s="17" t="s">
+        <v>174</v>
+      </c>
       <c r="C40" s="17" t="s">
         <v>174</v>
       </c>
@@ -8140,7 +8131,7 @@
         <v>174</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F40" s="17" t="s">
         <v>174</v>
@@ -8149,16 +8140,16 @@
         <v>174</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="I40" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="J40" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K40" s="17" t="s">
-        <v>174</v>
+      <c r="J40" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="K40" s="5" t="s">
+        <v>182</v>
       </c>
       <c r="L40" s="17" t="s">
         <v>174</v>
@@ -8167,12 +8158,12 @@
         <v>182</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A41" s="16" t="s">
-        <v>150</v>
-      </c>
-      <c r="B41" s="17" t="s">
-        <v>174</v>
+    <row r="41" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A41" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>168</v>
       </c>
       <c r="C41" s="17" t="s">
         <v>174</v>
@@ -8180,8 +8171,8 @@
       <c r="D41" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="E41" s="2" t="s">
-        <v>187</v>
+      <c r="E41" s="17" t="s">
+        <v>174</v>
       </c>
       <c r="F41" s="17" t="s">
         <v>174</v>
@@ -8189,28 +8180,28 @@
       <c r="G41" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="H41" s="2" t="s">
-        <v>187</v>
+      <c r="H41" s="17" t="s">
+        <v>174</v>
       </c>
       <c r="I41" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="J41" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="K41" s="5" t="s">
-        <v>182</v>
+      <c r="J41" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="K41" s="17" t="s">
+        <v>174</v>
       </c>
       <c r="L41" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="M41" s="5" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="M41" s="17" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A42" s="15" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>168</v>
@@ -8221,8 +8212,8 @@
       <c r="D42" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="E42" s="17" t="s">
-        <v>174</v>
+      <c r="E42" s="2" t="s">
+        <v>185</v>
       </c>
       <c r="F42" s="17" t="s">
         <v>174</v>
@@ -8230,8 +8221,8 @@
       <c r="G42" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="H42" s="17" t="s">
-        <v>174</v>
+      <c r="H42" s="2" t="s">
+        <v>185</v>
       </c>
       <c r="I42" s="17" t="s">
         <v>174</v>
@@ -8239,22 +8230,22 @@
       <c r="J42" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="K42" s="17" t="s">
-        <v>174</v>
+      <c r="K42" s="2" t="s">
+        <v>169</v>
       </c>
       <c r="L42" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="M42" s="17" t="s">
-        <v>174</v>
+      <c r="M42" s="2" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A43" s="15" t="s">
-        <v>168</v>
+        <v>185</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>168</v>
+        <v>151</v>
       </c>
       <c r="C43" s="17" t="s">
         <v>174</v>
@@ -8262,8 +8253,8 @@
       <c r="D43" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="E43" s="2" t="s">
-        <v>188</v>
+      <c r="E43" s="17" t="s">
+        <v>174</v>
       </c>
       <c r="F43" s="17" t="s">
         <v>174</v>
@@ -8271,8 +8262,8 @@
       <c r="G43" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="H43" s="2" t="s">
-        <v>188</v>
+      <c r="H43" s="17" t="s">
+        <v>174</v>
       </c>
       <c r="I43" s="17" t="s">
         <v>174</v>
@@ -8280,22 +8271,22 @@
       <c r="J43" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="K43" s="2" t="s">
-        <v>169</v>
+      <c r="K43" s="17" t="s">
+        <v>174</v>
       </c>
       <c r="L43" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="M43" s="2" t="s">
-        <v>169</v>
+      <c r="M43" s="17" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A44" s="15" t="s">
-        <v>186</v>
+        <v>151</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C44" s="17" t="s">
         <v>174</v>
@@ -8315,8 +8306,8 @@
       <c r="H44" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="I44" s="17" t="s">
-        <v>174</v>
+      <c r="I44" s="2" t="s">
+        <v>170</v>
       </c>
       <c r="J44" s="17" t="s">
         <v>174</v>
@@ -8327,16 +8318,16 @@
       <c r="L44" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="M44" s="17" t="s">
-        <v>174</v>
+      <c r="M44" s="2" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A45" s="15" t="s">
-        <v>187</v>
+      <c r="A45" s="16" t="s">
+        <v>152</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C45" s="17" t="s">
         <v>174</v>
@@ -8356,8 +8347,8 @@
       <c r="H45" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="I45" s="17" t="s">
-        <v>174</v>
+      <c r="I45" s="2" t="s">
+        <v>170</v>
       </c>
       <c r="J45" s="17" t="s">
         <v>174</v>
@@ -8368,16 +8359,16 @@
       <c r="L45" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="M45" s="17" t="s">
-        <v>174</v>
+      <c r="M45" s="2" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A46" s="15" t="s">
-        <v>188</v>
+      <c r="A46" s="16" t="s">
+        <v>170</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C46" s="17" t="s">
         <v>174</v>
@@ -8409,16 +8400,16 @@
       <c r="L46" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="M46" s="17" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="M46" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="15" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>152</v>
+        <v>173</v>
       </c>
       <c r="C47" s="17" t="s">
         <v>174</v>
@@ -8438,8 +8429,8 @@
       <c r="H47" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="I47" s="2" t="s">
-        <v>170</v>
+      <c r="I47" s="17" t="s">
+        <v>174</v>
       </c>
       <c r="J47" s="17" t="s">
         <v>174</v>
@@ -8451,15 +8442,15 @@
         <v>174</v>
       </c>
       <c r="M47" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A48" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>153</v>
+        <v>173</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="B48" s="17" t="s">
+        <v>174</v>
       </c>
       <c r="C48" s="17" t="s">
         <v>174</v>
@@ -8479,8 +8470,8 @@
       <c r="H48" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="I48" s="2" t="s">
-        <v>170</v>
+      <c r="I48" s="17" t="s">
+        <v>174</v>
       </c>
       <c r="J48" s="17" t="s">
         <v>174</v>
@@ -8491,130 +8482,7 @@
       <c r="L48" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="M48" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A49" s="16" t="s">
-        <v>170</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="C49" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D49" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="E49" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="F49" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="G49" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H49" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="I49" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="J49" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K49" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="L49" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="M49" s="2" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="C50" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D50" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="E50" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="F50" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="G50" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H50" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="I50" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="J50" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K50" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="L50" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="M50" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="B51" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="C51" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D51" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="E51" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="F51" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="G51" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H51" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="I51" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="J51" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K51" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="L51" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="M51" s="17" t="s">
+      <c r="M48" s="17" t="s">
         <v>174</v>
       </c>
     </row>

</xml_diff>

<commit_message>
FIX: excludes C_BIN class from date! literals detection.
</commit_message>
<xml_diff>
--- a/docs/lexer/lexer-FSM.xlsx
+++ b/docs/lexer/lexer-FSM.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Red\docs\lexer\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D28E06D-E77C-422A-A13F-BBFB8BE61B7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28100" yWindow="150" windowWidth="17030" windowHeight="15020" tabRatio="564" activeTab="1"/>
+    <workbookView xWindow="833" yWindow="330" windowWidth="16904" windowHeight="13455" tabRatio="564" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="transitions" sheetId="3" r:id="rId1"/>
@@ -594,7 +600,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -847,7 +853,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -880,9 +886,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -915,6 +938,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1090,26 +1130,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U52" sqref="U52"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AG26" sqref="AG26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.36328125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" customWidth="1"/>
-    <col min="5" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="12" width="9.7265625" customWidth="1"/>
-    <col min="13" max="13" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="14" max="36" width="9.7265625" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.73046875" customWidth="1"/>
+    <col min="5" max="5" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="9.73046875" customWidth="1"/>
+    <col min="13" max="13" width="9.9296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="36" width="9.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:36" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="8"/>
       <c r="B1" s="7" t="s">
         <v>37</v>
@@ -1217,7 +1257,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
@@ -1327,7 +1367,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A3" s="12" t="s">
         <v>69</v>
       </c>
@@ -1437,7 +1477,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A4" s="12" t="s">
         <v>70</v>
       </c>
@@ -1547,7 +1587,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A5" s="12" t="s">
         <v>1</v>
       </c>
@@ -1657,7 +1697,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A6" s="12" t="s">
         <v>2</v>
       </c>
@@ -1767,7 +1807,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A7" s="12" t="s">
         <v>74</v>
       </c>
@@ -1877,7 +1917,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A8" s="12" t="s">
         <v>3</v>
       </c>
@@ -1987,7 +2027,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A9" s="12" t="s">
         <v>4</v>
       </c>
@@ -2097,7 +2137,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A10" s="12" t="s">
         <v>109</v>
       </c>
@@ -2207,7 +2247,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A11" s="12" t="s">
         <v>110</v>
       </c>
@@ -2317,7 +2357,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A12" s="12" t="s">
         <v>111</v>
       </c>
@@ -2427,7 +2467,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A13" s="12" t="s">
         <v>5</v>
       </c>
@@ -2537,7 +2577,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A14" s="12" t="s">
         <v>6</v>
       </c>
@@ -2647,7 +2687,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A15" s="12" t="s">
         <v>7</v>
       </c>
@@ -2757,7 +2797,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A16" s="12" t="s">
         <v>71</v>
       </c>
@@ -2867,7 +2907,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A17" s="12" t="s">
         <v>8</v>
       </c>
@@ -2977,7 +3017,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A18" s="12" t="s">
         <v>9</v>
       </c>
@@ -3087,7 +3127,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A19" s="12" t="s">
         <v>10</v>
       </c>
@@ -3197,7 +3237,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A20" s="12" t="s">
         <v>11</v>
       </c>
@@ -3307,7 +3347,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A21" s="12" t="s">
         <v>12</v>
       </c>
@@ -3417,7 +3457,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A22" s="12" t="s">
         <v>86</v>
       </c>
@@ -3527,7 +3567,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A23" s="12" t="s">
         <v>13</v>
       </c>
@@ -3637,7 +3677,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A24" s="12" t="s">
         <v>14</v>
       </c>
@@ -3747,7 +3787,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A25" s="12" t="s">
         <v>15</v>
       </c>
@@ -3857,7 +3897,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A26" s="12" t="s">
         <v>16</v>
       </c>
@@ -3954,8 +3994,8 @@
       <c r="AF26" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="AG26" s="2" t="s">
-        <v>16</v>
+      <c r="AG26" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="AH26" s="2" t="s">
         <v>16</v>
@@ -3967,7 +4007,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A27" s="12" t="s">
         <v>17</v>
       </c>
@@ -4077,7 +4117,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="28" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A28" s="12" t="s">
         <v>18</v>
       </c>
@@ -4187,7 +4227,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="29" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A29" s="12" t="s">
         <v>19</v>
       </c>
@@ -4297,7 +4337,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="30" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A30" s="12" t="s">
         <v>20</v>
       </c>
@@ -4407,7 +4447,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="31" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A31" s="12" t="s">
         <v>22</v>
       </c>
@@ -4517,7 +4557,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A32" s="12" t="s">
         <v>23</v>
       </c>
@@ -4627,7 +4667,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="33" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A33" s="12" t="s">
         <v>24</v>
       </c>
@@ -4737,7 +4777,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="34" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A34" s="12" t="s">
         <v>25</v>
       </c>
@@ -4847,7 +4887,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="35" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A35" s="12" t="s">
         <v>26</v>
       </c>
@@ -4957,7 +4997,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A36" s="12" t="s">
         <v>27</v>
       </c>
@@ -5067,7 +5107,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="37" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A37" s="12" t="s">
         <v>28</v>
       </c>
@@ -5177,7 +5217,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A38" s="12" t="s">
         <v>29</v>
       </c>
@@ -5287,7 +5327,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="39" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A39" s="12" t="s">
         <v>30</v>
       </c>
@@ -5397,7 +5437,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="40" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A40" s="12" t="s">
         <v>31</v>
       </c>
@@ -5507,7 +5547,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="41" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A41" s="12" t="s">
         <v>32</v>
       </c>
@@ -5617,7 +5657,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="42" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A42" s="12" t="s">
         <v>96</v>
       </c>
@@ -5727,7 +5767,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="43" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A43" s="12" t="s">
         <v>33</v>
       </c>
@@ -5837,7 +5877,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="44" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A44" s="12" t="s">
         <v>21</v>
       </c>
@@ -5947,7 +5987,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="45" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A45" s="13" t="s">
         <v>112</v>
       </c>
@@ -6057,7 +6097,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="46" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A46" s="12" t="s">
         <v>113</v>
       </c>
@@ -6167,7 +6207,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="47" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A47" s="12" t="s">
         <v>114</v>
       </c>
@@ -6277,7 +6317,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="48" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A48" s="12" t="s">
         <v>115</v>
       </c>
@@ -6387,7 +6427,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="49" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A49" s="12" t="s">
         <v>116</v>
       </c>
@@ -6504,20 +6544,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.796875" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -6559,7 +6599,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" s="13" t="s">
         <v>128</v>
       </c>
@@ -6600,7 +6640,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" s="12" t="s">
         <v>129</v>
       </c>
@@ -6641,7 +6681,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4" s="12" t="s">
         <v>130</v>
       </c>
@@ -6682,7 +6722,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" s="12" t="s">
         <v>131</v>
       </c>
@@ -6723,7 +6763,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6" s="12" t="s">
         <v>179</v>
       </c>
@@ -6764,7 +6804,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7" s="16" t="s">
         <v>132</v>
       </c>
@@ -6805,7 +6845,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" s="16" t="s">
         <v>154</v>
       </c>
@@ -6846,7 +6886,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9" s="16" t="s">
         <v>133</v>
       </c>
@@ -6887,7 +6927,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" s="15" t="s">
         <v>134</v>
       </c>
@@ -6928,7 +6968,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11" s="15" t="s">
         <v>135</v>
       </c>
@@ -6969,7 +7009,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12" s="15" t="s">
         <v>186</v>
       </c>
@@ -7010,7 +7050,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13" s="15" t="s">
         <v>187</v>
       </c>
@@ -7051,7 +7091,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14" s="16" t="s">
         <v>136</v>
       </c>
@@ -7092,7 +7132,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15" s="16" t="s">
         <v>137</v>
       </c>
@@ -7133,7 +7173,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16" s="15" t="s">
         <v>138</v>
       </c>
@@ -7174,7 +7214,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A17" s="15" t="s">
         <v>139</v>
       </c>
@@ -7215,7 +7255,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A18" s="15" t="s">
         <v>140</v>
       </c>
@@ -7256,7 +7296,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A19" s="15" t="s">
         <v>190</v>
       </c>
@@ -7297,7 +7337,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A20" s="15" t="s">
         <v>141</v>
       </c>
@@ -7338,7 +7378,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A21" s="15" t="s">
         <v>142</v>
       </c>
@@ -7379,7 +7419,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A22" s="16" t="s">
         <v>156</v>
       </c>
@@ -7420,7 +7460,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A23" s="16" t="s">
         <v>157</v>
       </c>
@@ -7461,7 +7501,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A24" s="15" t="s">
         <v>143</v>
       </c>
@@ -7502,7 +7542,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A25" s="15" t="s">
         <v>144</v>
       </c>
@@ -7543,7 +7583,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A26" s="16" t="s">
         <v>145</v>
       </c>
@@ -7584,7 +7624,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A27" s="15" t="s">
         <v>146</v>
       </c>
@@ -7625,7 +7665,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A28" s="16" t="s">
         <v>158</v>
       </c>
@@ -7666,7 +7706,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A29" s="16" t="s">
         <v>159</v>
       </c>
@@ -7707,7 +7747,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A30" s="16" t="s">
         <v>160</v>
       </c>
@@ -7748,7 +7788,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A31" s="16" t="s">
         <v>161</v>
       </c>
@@ -7789,7 +7829,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A32" s="13" t="s">
         <v>147</v>
       </c>
@@ -7830,7 +7870,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A33" s="15" t="s">
         <v>162</v>
       </c>
@@ -7871,7 +7911,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A34" s="16" t="s">
         <v>148</v>
       </c>
@@ -7912,7 +7952,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A35" s="15" t="s">
         <v>163</v>
       </c>
@@ -7953,7 +7993,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A36" s="16" t="s">
         <v>164</v>
       </c>
@@ -7994,7 +8034,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A37" s="15" t="s">
         <v>149</v>
       </c>
@@ -8035,7 +8075,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A38" s="16" t="s">
         <v>165</v>
       </c>
@@ -8076,7 +8116,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A39" s="15" t="s">
         <v>166</v>
       </c>
@@ -8117,7 +8157,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A40" s="16" t="s">
         <v>150</v>
       </c>
@@ -8158,7 +8198,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A41" s="15" t="s">
         <v>167</v>
       </c>
@@ -8199,7 +8239,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A42" s="15" t="s">
         <v>168</v>
       </c>
@@ -8240,7 +8280,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A43" s="15" t="s">
         <v>185</v>
       </c>
@@ -8281,7 +8321,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A44" s="15" t="s">
         <v>151</v>
       </c>
@@ -8322,7 +8362,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A45" s="16" t="s">
         <v>152</v>
       </c>
@@ -8363,7 +8403,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A46" s="16" t="s">
         <v>170</v>
       </c>
@@ -8404,7 +8444,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47" s="15" t="s">
         <v>153</v>
       </c>
@@ -8445,7 +8485,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="48" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A48" s="15" t="s">
         <v>174</v>
       </c>
@@ -8493,19 +8533,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="8.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.9296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.06640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -8526,7 +8566,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
         <v>104</v>
       </c>
@@ -8546,7 +8586,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
         <v>103</v>
       </c>
@@ -8566,7 +8606,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="6" t="s">
         <v>107</v>
       </c>
@@ -8586,7 +8626,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FEAT: adds support for handling nested brace strings.
</commit_message>
<xml_diff>
--- a/docs/lexer/lexer-FSM.xlsx
+++ b/docs/lexer/lexer-FSM.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Red\docs\lexer\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D28E06D-E77C-422A-A13F-BBFB8BE61B7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="833" yWindow="330" windowWidth="16904" windowHeight="13455" tabRatio="564" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="830" yWindow="330" windowWidth="16900" windowHeight="13460" tabRatio="564"/>
   </bookViews>
   <sheets>
     <sheet name="transitions" sheetId="3" r:id="rId1"/>
@@ -22,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2409" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2409" uniqueCount="193">
   <si>
     <t>S_START</t>
   </si>
@@ -595,12 +589,18 @@
   </si>
   <si>
     <t>S_DT_YWD</t>
+  </si>
+  <si>
+    <t>T_MSTR_OP</t>
+  </si>
+  <si>
+    <t>T_MSTR_CL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -853,7 +853,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -886,26 +886,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -938,23 +921,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1130,23 +1096,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AG26" sqref="AG26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.73046875" customWidth="1"/>
-    <col min="5" max="5" width="9.73046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="12" width="9.73046875" customWidth="1"/>
-    <col min="13" max="13" width="9.9296875" bestFit="1" customWidth="1"/>
-    <col min="14" max="36" width="9.73046875" customWidth="1"/>
+    <col min="1" max="1" width="10.36328125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" customWidth="1"/>
+    <col min="5" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="9.7265625" customWidth="1"/>
+    <col min="13" max="13" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="36" width="9.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -1257,7 +1223,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
@@ -1285,8 +1251,8 @@
       <c r="I2" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>2</v>
+      <c r="J2" s="1" t="s">
+        <v>191</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>63</v>
@@ -1367,7 +1333,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A3" s="12" t="s">
         <v>69</v>
       </c>
@@ -1477,7 +1443,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A4" s="12" t="s">
         <v>70</v>
       </c>
@@ -1587,7 +1553,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
         <v>1</v>
       </c>
@@ -1697,8 +1663,8 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.45">
-      <c r="A6" s="12" t="s">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A6" s="13" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -1725,11 +1691,11 @@
       <c r="I6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J6" s="2" t="s">
-        <v>2</v>
+      <c r="J6" s="1" t="s">
+        <v>191</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>73</v>
+        <v>192</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>2</v>
@@ -1807,7 +1773,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
         <v>74</v>
       </c>
@@ -1917,7 +1883,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A8" s="12" t="s">
         <v>3</v>
       </c>
@@ -2027,7 +1993,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A9" s="12" t="s">
         <v>4</v>
       </c>
@@ -2137,7 +2103,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A10" s="12" t="s">
         <v>109</v>
       </c>
@@ -2247,7 +2213,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A11" s="12" t="s">
         <v>110</v>
       </c>
@@ -2357,7 +2323,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A12" s="12" t="s">
         <v>111</v>
       </c>
@@ -2467,7 +2433,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A13" s="12" t="s">
         <v>5</v>
       </c>
@@ -2577,7 +2543,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A14" s="12" t="s">
         <v>6</v>
       </c>
@@ -2687,7 +2653,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A15" s="12" t="s">
         <v>7</v>
       </c>
@@ -2797,7 +2763,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A16" s="12" t="s">
         <v>71</v>
       </c>
@@ -2907,7 +2873,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A17" s="12" t="s">
         <v>8</v>
       </c>
@@ -3017,7 +2983,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A18" s="12" t="s">
         <v>9</v>
       </c>
@@ -3127,7 +3093,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A19" s="12" t="s">
         <v>10</v>
       </c>
@@ -3237,7 +3203,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A20" s="12" t="s">
         <v>11</v>
       </c>
@@ -3347,7 +3313,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A21" s="12" t="s">
         <v>12</v>
       </c>
@@ -3457,7 +3423,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A22" s="12" t="s">
         <v>86</v>
       </c>
@@ -3567,7 +3533,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A23" s="12" t="s">
         <v>13</v>
       </c>
@@ -3677,7 +3643,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A24" s="12" t="s">
         <v>14</v>
       </c>
@@ -3787,7 +3753,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A25" s="12" t="s">
         <v>15</v>
       </c>
@@ -3897,7 +3863,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A26" s="12" t="s">
         <v>16</v>
       </c>
@@ -4007,7 +3973,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A27" s="12" t="s">
         <v>17</v>
       </c>
@@ -4117,7 +4083,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="28" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A28" s="12" t="s">
         <v>18</v>
       </c>
@@ -4227,7 +4193,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="29" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A29" s="12" t="s">
         <v>19</v>
       </c>
@@ -4337,7 +4303,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="30" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A30" s="12" t="s">
         <v>20</v>
       </c>
@@ -4447,7 +4413,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="31" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A31" s="12" t="s">
         <v>22</v>
       </c>
@@ -4557,7 +4523,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A32" s="12" t="s">
         <v>23</v>
       </c>
@@ -4667,7 +4633,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="33" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A33" s="12" t="s">
         <v>24</v>
       </c>
@@ -4777,7 +4743,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="34" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A34" s="12" t="s">
         <v>25</v>
       </c>
@@ -4887,7 +4853,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="35" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A35" s="12" t="s">
         <v>26</v>
       </c>
@@ -4997,7 +4963,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A36" s="12" t="s">
         <v>27</v>
       </c>
@@ -5107,7 +5073,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="37" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A37" s="12" t="s">
         <v>28</v>
       </c>
@@ -5217,7 +5183,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A38" s="12" t="s">
         <v>29</v>
       </c>
@@ -5327,7 +5293,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="39" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A39" s="12" t="s">
         <v>30</v>
       </c>
@@ -5437,7 +5403,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="40" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A40" s="12" t="s">
         <v>31</v>
       </c>
@@ -5547,7 +5513,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="41" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A41" s="12" t="s">
         <v>32</v>
       </c>
@@ -5657,7 +5623,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="42" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A42" s="12" t="s">
         <v>96</v>
       </c>
@@ -5767,7 +5733,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="43" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A43" s="12" t="s">
         <v>33</v>
       </c>
@@ -5877,7 +5843,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="44" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A44" s="12" t="s">
         <v>21</v>
       </c>
@@ -5987,7 +5953,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="45" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A45" s="13" t="s">
         <v>112</v>
       </c>
@@ -6097,7 +6063,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="46" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A46" s="12" t="s">
         <v>113</v>
       </c>
@@ -6207,7 +6173,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="47" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A47" s="12" t="s">
         <v>114</v>
       </c>
@@ -6317,7 +6283,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="48" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A48" s="12" t="s">
         <v>115</v>
       </c>
@@ -6427,7 +6393,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="49" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A49" s="12" t="s">
         <v>116</v>
       </c>
@@ -6544,20 +6510,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M48"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.19921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -6599,7 +6565,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A2" s="13" t="s">
         <v>128</v>
       </c>
@@ -6640,7 +6606,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A3" s="12" t="s">
         <v>129</v>
       </c>
@@ -6681,7 +6647,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A4" s="12" t="s">
         <v>130</v>
       </c>
@@ -6722,7 +6688,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A5" s="12" t="s">
         <v>131</v>
       </c>
@@ -6763,7 +6729,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A6" s="12" t="s">
         <v>179</v>
       </c>
@@ -6804,7 +6770,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A7" s="16" t="s">
         <v>132</v>
       </c>
@@ -6845,7 +6811,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A8" s="16" t="s">
         <v>154</v>
       </c>
@@ -6886,7 +6852,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A9" s="16" t="s">
         <v>133</v>
       </c>
@@ -6927,7 +6893,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A10" s="15" t="s">
         <v>134</v>
       </c>
@@ -6968,7 +6934,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A11" s="15" t="s">
         <v>135</v>
       </c>
@@ -7009,7 +6975,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A12" s="15" t="s">
         <v>186</v>
       </c>
@@ -7050,7 +7016,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A13" s="15" t="s">
         <v>187</v>
       </c>
@@ -7091,7 +7057,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A14" s="16" t="s">
         <v>136</v>
       </c>
@@ -7132,7 +7098,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A15" s="16" t="s">
         <v>137</v>
       </c>
@@ -7173,7 +7139,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A16" s="15" t="s">
         <v>138</v>
       </c>
@@ -7214,7 +7180,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A17" s="15" t="s">
         <v>139</v>
       </c>
@@ -7255,7 +7221,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A18" s="15" t="s">
         <v>140</v>
       </c>
@@ -7296,7 +7262,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A19" s="15" t="s">
         <v>190</v>
       </c>
@@ -7337,7 +7303,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A20" s="15" t="s">
         <v>141</v>
       </c>
@@ -7378,7 +7344,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A21" s="15" t="s">
         <v>142</v>
       </c>
@@ -7419,7 +7385,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A22" s="16" t="s">
         <v>156</v>
       </c>
@@ -7460,7 +7426,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A23" s="16" t="s">
         <v>157</v>
       </c>
@@ -7501,7 +7467,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A24" s="15" t="s">
         <v>143</v>
       </c>
@@ -7542,7 +7508,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A25" s="15" t="s">
         <v>144</v>
       </c>
@@ -7583,7 +7549,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A26" s="16" t="s">
         <v>145</v>
       </c>
@@ -7624,7 +7590,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A27" s="15" t="s">
         <v>146</v>
       </c>
@@ -7665,7 +7631,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A28" s="16" t="s">
         <v>158</v>
       </c>
@@ -7706,7 +7672,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A29" s="16" t="s">
         <v>159</v>
       </c>
@@ -7747,7 +7713,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A30" s="16" t="s">
         <v>160</v>
       </c>
@@ -7788,7 +7754,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A31" s="16" t="s">
         <v>161</v>
       </c>
@@ -7829,7 +7795,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A32" s="13" t="s">
         <v>147</v>
       </c>
@@ -7870,7 +7836,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A33" s="15" t="s">
         <v>162</v>
       </c>
@@ -7911,7 +7877,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A34" s="16" t="s">
         <v>148</v>
       </c>
@@ -7952,7 +7918,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A35" s="15" t="s">
         <v>163</v>
       </c>
@@ -7993,7 +7959,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A36" s="16" t="s">
         <v>164</v>
       </c>
@@ -8034,7 +8000,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A37" s="15" t="s">
         <v>149</v>
       </c>
@@ -8075,7 +8041,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A38" s="16" t="s">
         <v>165</v>
       </c>
@@ -8116,7 +8082,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A39" s="15" t="s">
         <v>166</v>
       </c>
@@ -8157,7 +8123,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A40" s="16" t="s">
         <v>150</v>
       </c>
@@ -8198,7 +8164,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A41" s="15" t="s">
         <v>167</v>
       </c>
@@ -8239,7 +8205,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A42" s="15" t="s">
         <v>168</v>
       </c>
@@ -8280,7 +8246,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A43" s="15" t="s">
         <v>185</v>
       </c>
@@ -8321,7 +8287,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A44" s="15" t="s">
         <v>151</v>
       </c>
@@ -8362,7 +8328,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A45" s="16" t="s">
         <v>152</v>
       </c>
@@ -8403,7 +8369,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A46" s="16" t="s">
         <v>170</v>
       </c>
@@ -8533,19 +8499,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.9296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.06640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.19921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -8566,7 +8532,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
         <v>104</v>
       </c>
@@ -8586,7 +8552,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
         <v>103</v>
       </c>
@@ -8606,7 +8572,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A4" s="6" t="s">
         <v>107</v>
       </c>
@@ -8626,7 +8592,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A5" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FEAT: supports implicit leading 0 in floats.
</commit_message>
<xml_diff>
--- a/docs/lexer/lexer-FSM.xlsx
+++ b/docs/lexer/lexer-FSM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2409" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2481" uniqueCount="195">
   <si>
     <t>S_START</t>
   </si>
@@ -595,6 +595,12 @@
   </si>
   <si>
     <t>T_MSTR_CL</t>
+  </si>
+  <si>
+    <t>S_DOTWORD</t>
+  </si>
+  <si>
+    <t>S_DOTDEC</t>
   </si>
 </sst>
 </file>
@@ -1097,11 +1103,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ49"/>
+  <dimension ref="A1:AJ51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J6" sqref="J6"/>
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="P42" sqref="P42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1306,7 +1312,7 @@
         <v>63</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>32</v>
+        <v>193</v>
       </c>
       <c r="AC2" s="2" t="s">
         <v>22</v>
@@ -3533,7 +3539,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A23" s="12" t="s">
         <v>13</v>
       </c>
@@ -3570,8 +3576,8 @@
       <c r="L23" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="M23" s="2" t="s">
-        <v>19</v>
+      <c r="M23" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="N23" s="3" t="s">
         <v>63</v>
@@ -3621,11 +3627,11 @@
       <c r="AC23" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="AD23" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AE23" s="3" t="s">
-        <v>63</v>
+      <c r="AD23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE23" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="AF23" s="3" t="s">
         <v>63</v>
@@ -5403,7 +5409,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="40" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A40" s="12" t="s">
         <v>31</v>
       </c>
@@ -5486,7 +5492,7 @@
         <v>32</v>
       </c>
       <c r="AB40" s="2" t="s">
-        <v>32</v>
+        <v>193</v>
       </c>
       <c r="AC40" s="2" t="s">
         <v>32</v>
@@ -5513,9 +5519,9 @@
         <v>75</v>
       </c>
     </row>
-    <row r="41" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A41" s="12" t="s">
-        <v>32</v>
+        <v>193</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>75</v>
@@ -5524,10 +5530,10 @@
         <v>75</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>32</v>
+        <v>194</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>32</v>
+        <v>194</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>75</v>
@@ -5566,7 +5572,7 @@
         <v>32</v>
       </c>
       <c r="R41" s="2" t="s">
-        <v>32</v>
+        <v>194</v>
       </c>
       <c r="S41" s="2" t="s">
         <v>32</v>
@@ -5598,14 +5604,14 @@
       <c r="AB41" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AC41" s="2" t="s">
-        <v>23</v>
+      <c r="AC41" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="AD41" s="2" t="s">
-        <v>32</v>
+        <v>194</v>
       </c>
       <c r="AE41" s="2" t="s">
-        <v>32</v>
+        <v>194</v>
       </c>
       <c r="AF41" s="2" t="s">
         <v>32</v>
@@ -5623,601 +5629,601 @@
         <v>75</v>
       </c>
     </row>
-    <row r="42" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A42" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="L42" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="M42" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="N42" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="O42" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="P42" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q42" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="R42" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="S42" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="T42" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="U42" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="V42" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="W42" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="X42" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="Y42" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z42" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA42" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB42" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC42" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD42" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="AE42" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="AF42" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AG42" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH42" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI42" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ42" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="43" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A43" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="L43" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="M43" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="N43" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="O43" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="I42" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="J42" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="K42" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="L42" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="M42" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="N42" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="O42" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="P42" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q42" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="R42" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="S42" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T42" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U42" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="V42" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="W42" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="X42" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="Y42" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z42" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="AA42" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="AB42" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="AC42" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="AD42" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="AE42" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="AF42" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="AG42" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="AH42" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="AI42" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AJ42" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="43" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A43" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="H43" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="I43" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="J43" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="K43" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="L43" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="M43" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="N43" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="O43" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="P43" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Q43" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="R43" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="S43" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="T43" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="T43" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="U43" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="V43" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="W43" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="X43" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="Y43" s="1" t="s">
-        <v>94</v>
+        <v>75</v>
+      </c>
+      <c r="V43" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="W43" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="X43" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y43" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="Z43" s="1" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="AA43" s="2" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="AB43" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="AC43" s="3" t="s">
-        <v>63</v>
+        <v>32</v>
+      </c>
+      <c r="AC43" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="AD43" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AE43" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="AF43" s="3" t="s">
-        <v>63</v>
+        <v>32</v>
+      </c>
+      <c r="AF43" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="AG43" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AH43" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AI43" s="3" t="s">
         <v>63</v>
       </c>
       <c r="AJ43" s="1" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
     </row>
     <row r="44" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A44" s="12" t="s">
-        <v>21</v>
+        <v>96</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="L44" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="M44" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="N44" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="O44" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="P44" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q44" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="R44" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="S44" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="T44" s="1" t="s">
-        <v>97</v>
+        <v>75</v>
+      </c>
+      <c r="M44" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="N44" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="O44" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="P44" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q44" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="R44" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="S44" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T44" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="U44" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="V44" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="W44" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="X44" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Y44" s="3" t="s">
-        <v>63</v>
+        <v>75</v>
+      </c>
+      <c r="V44" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="W44" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="X44" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y44" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="Z44" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="AA44" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AB44" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AC44" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AD44" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AE44" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AF44" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AG44" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AH44" s="2" t="s">
-        <v>21</v>
+        <v>75</v>
+      </c>
+      <c r="AA44" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB44" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC44" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD44" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE44" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="AF44" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG44" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="AH44" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="AI44" s="3" t="s">
         <v>63</v>
       </c>
       <c r="AJ44" s="1" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
     </row>
     <row r="45" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A45" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>63</v>
+      <c r="A45" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>113</v>
+        <v>33</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G45" s="3" t="s">
-        <v>63</v>
+        <v>33</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>66</v>
+        <v>94</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="J45" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="K45" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="L45" s="2" t="s">
-        <v>70</v>
+        <v>94</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="L45" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="M45" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="N45" s="2" t="s">
-        <v>114</v>
+        <v>33</v>
+      </c>
+      <c r="N45" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="O45" s="2" t="s">
-        <v>114</v>
+        <v>33</v>
       </c>
       <c r="P45" s="2" t="s">
-        <v>114</v>
+        <v>33</v>
       </c>
       <c r="Q45" s="2" t="s">
-        <v>114</v>
+        <v>33</v>
       </c>
       <c r="R45" s="2" t="s">
-        <v>114</v>
+        <v>33</v>
       </c>
       <c r="S45" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="T45" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="U45" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="V45" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="W45" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="X45" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y45" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="Z45" s="3" t="s">
-        <v>63</v>
+        <v>33</v>
+      </c>
+      <c r="T45" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="U45" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="V45" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="W45" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="X45" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y45" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="Z45" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="AA45" s="2" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="AB45" s="2" t="s">
-        <v>114</v>
+        <v>33</v>
       </c>
       <c r="AC45" s="3" t="s">
         <v>63</v>
       </c>
       <c r="AD45" s="2" t="s">
-        <v>116</v>
+        <v>33</v>
       </c>
       <c r="AE45" s="2" t="s">
-        <v>116</v>
+        <v>33</v>
       </c>
       <c r="AF45" s="3" t="s">
         <v>63</v>
       </c>
       <c r="AG45" s="2" t="s">
-        <v>114</v>
+        <v>33</v>
       </c>
       <c r="AH45" s="2" t="s">
-        <v>114</v>
+        <v>33</v>
       </c>
       <c r="AI45" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="AJ45" s="3" t="s">
-        <v>63</v>
+      <c r="AJ45" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="46" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A46" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="L46" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="M46" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="N46" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="O46" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="P46" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q46" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R46" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="S46" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T46" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="U46" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="V46" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="W46" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="X46" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y46" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z46" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AA46" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB46" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AC46" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD46" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE46" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AF46" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AG46" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AH46" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AI46" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ46" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="47" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A47" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D47" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D46" s="2" t="s">
+      <c r="E47" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E46" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="I46" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="J46" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="K46" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="L46" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="M46" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="N46" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="O46" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="P46" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q46" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="R46" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="S46" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="T46" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="U46" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="V46" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="W46" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="X46" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="Y46" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="Z46" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="AA46" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AB46" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="AC46" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AD46" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AE46" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AF46" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AG46" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AH46" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AI46" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AJ46" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="47" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A47" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>75</v>
+      <c r="F47" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="J47" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="K47" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="L47" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="M47" s="3" t="s">
-        <v>63</v>
+        <v>68</v>
+      </c>
+      <c r="J47" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="K47" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="L47" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="M47" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="N47" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="O47" s="1" t="s">
-        <v>75</v>
+      <c r="O47" s="2" t="s">
+        <v>114</v>
       </c>
       <c r="P47" s="2" t="s">
         <v>114</v>
@@ -6231,14 +6237,14 @@
       <c r="S47" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="T47" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="U47" s="1" t="s">
-        <v>75</v>
+      <c r="T47" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="U47" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="V47" s="2" t="s">
-        <v>114</v>
+        <v>25</v>
       </c>
       <c r="W47" s="2" t="s">
         <v>114</v>
@@ -6249,8 +6255,8 @@
       <c r="Y47" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="Z47" s="1" t="s">
-        <v>75</v>
+      <c r="Z47" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="AA47" s="2" t="s">
         <v>21</v>
@@ -6262,13 +6268,13 @@
         <v>63</v>
       </c>
       <c r="AD47" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="AE47" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="AF47" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
+      </c>
+      <c r="AF47" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="AG47" s="2" t="s">
         <v>114</v>
@@ -6279,227 +6285,447 @@
       <c r="AI47" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="AJ47" s="1" t="s">
-        <v>75</v>
+      <c r="AJ47" s="3" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="48" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A48" s="12" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>11</v>
+        <v>113</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G48" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="H48" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="I48" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="J48" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="K48" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="L48" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="M48" s="2" t="s">
-        <v>11</v>
+        <v>113</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="L48" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="M48" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="N48" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="O48" s="3" t="s">
-        <v>63</v>
+        <v>12</v>
+      </c>
+      <c r="O48" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="P48" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q48" s="2" t="s">
-        <v>11</v>
+        <v>19</v>
+      </c>
+      <c r="Q48" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="R48" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="S48" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="T48" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="U48" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="V48" s="3" t="s">
-        <v>63</v>
+        <v>13</v>
+      </c>
+      <c r="S48" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="T48" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="U48" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="V48" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="W48" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="X48" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y48" s="3" t="s">
+      <c r="X48" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="Y48" s="4" t="s">
         <v>63</v>
       </c>
       <c r="Z48" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="AA48" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
+      </c>
+      <c r="AA48" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="AB48" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC48" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AD48" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AE48" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AF48" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AG48" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AH48" s="2" t="s">
-        <v>11</v>
+        <v>86</v>
+      </c>
+      <c r="AC48" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD48" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE48" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF48" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AG48" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH48" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="AI48" s="3" t="s">
         <v>63</v>
       </c>
       <c r="AJ48" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="49" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A49" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="L49" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="M49" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="N49" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="O49" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="P49" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q49" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="R49" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="S49" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="T49" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="U49" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="V49" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="W49" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="X49" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y49" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z49" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA49" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB49" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AC49" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD49" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AE49" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AF49" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AG49" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AH49" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AI49" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ49" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="50" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A50" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H50" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I50" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J50" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="K50" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="L50" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M50" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N50" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O50" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="P50" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q50" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="R50" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="S50" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="T50" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="U50" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="V50" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="W50" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="X50" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y50" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z50" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AA50" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB50" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC50" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD50" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE50" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF50" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AG50" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AH50" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AI50" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ50" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="51" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A51" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D49" s="2" t="s">
+      <c r="B51" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D51" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E49" s="2" t="s">
+      <c r="E51" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="F49" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="H49" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="I49" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="J49" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="K49" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="L49" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="M49" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="N49" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="O49" s="2" t="s">
+      <c r="F51" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J51" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="L51" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="M51" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="N51" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="O51" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="P49" s="2" t="s">
+      <c r="P51" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Q49" s="2" t="s">
+      <c r="Q51" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="R49" s="2" t="s">
+      <c r="R51" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="S49" s="2" t="s">
+      <c r="S51" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="T49" s="2" t="s">
+      <c r="T51" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="U49" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="V49" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="W49" s="2" t="s">
+      <c r="U51" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="V51" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="W51" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="X49" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y49" s="2" t="s">
+      <c r="X51" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y51" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Z49" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="AA49" s="2" t="s">
+      <c r="Z51" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA51" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AB49" s="2" t="s">
+      <c r="AB51" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AC49" s="2" t="s">
+      <c r="AC51" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AD49" s="2" t="s">
+      <c r="AD51" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AE49" s="2" t="s">
+      <c r="AE51" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AF49" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AG49" s="2" t="s">
+      <c r="AF51" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AG51" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AH49" s="2" t="s">
+      <c r="AH51" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AI49" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AJ49" s="1" t="s">
+      <c r="AI51" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ51" s="1" t="s">
         <v>75</v>
       </c>
     </row>

</xml_diff>

<commit_message>
FEAT: adds support for special float values to lexer.
</commit_message>
<xml_diff>
--- a/docs/lexer/lexer-FSM.xlsx
+++ b/docs/lexer/lexer-FSM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2481" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2481" uniqueCount="196">
   <si>
     <t>S_START</t>
   </si>
@@ -601,6 +601,9 @@
   </si>
   <si>
     <t>S_DOTDEC</t>
+  </si>
+  <si>
+    <t>T_FLOAT_SP</t>
   </si>
 </sst>
 </file>
@@ -1106,8 +1109,8 @@
   <dimension ref="A1:AJ51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P42" sqref="P42"/>
+      <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AJ24" sqref="AJ24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3663,37 +3666,37 @@
         <v>87</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>87</v>
+        <v>195</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>87</v>
+        <v>195</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>87</v>
+        <v>195</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>87</v>
+        <v>195</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>87</v>
+        <v>195</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>87</v>
+        <v>195</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>87</v>
+        <v>195</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>87</v>
+        <v>195</v>
       </c>
       <c r="M24" s="2" t="s">
         <v>14</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>87</v>
+        <v>195</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>87</v>
+        <v>195</v>
       </c>
       <c r="P24" s="2" t="s">
         <v>14</v>
@@ -3708,34 +3711,34 @@
         <v>14</v>
       </c>
       <c r="T24" s="1" t="s">
-        <v>87</v>
+        <v>195</v>
       </c>
       <c r="U24" s="1" t="s">
-        <v>87</v>
+        <v>195</v>
       </c>
       <c r="V24" s="1" t="s">
-        <v>87</v>
+        <v>195</v>
       </c>
       <c r="W24" s="2" t="s">
         <v>14</v>
       </c>
       <c r="X24" s="1" t="s">
-        <v>87</v>
+        <v>195</v>
       </c>
       <c r="Y24" s="1" t="s">
-        <v>87</v>
+        <v>195</v>
       </c>
       <c r="Z24" s="1" t="s">
-        <v>87</v>
+        <v>195</v>
       </c>
       <c r="AA24" s="1" t="s">
-        <v>87</v>
+        <v>195</v>
       </c>
       <c r="AB24" s="2" t="s">
         <v>14</v>
       </c>
       <c r="AC24" s="1" t="s">
-        <v>87</v>
+        <v>195</v>
       </c>
       <c r="AD24" s="2" t="s">
         <v>14</v>
@@ -3744,7 +3747,7 @@
         <v>14</v>
       </c>
       <c r="AF24" s="1" t="s">
-        <v>87</v>
+        <v>195</v>
       </c>
       <c r="AG24" s="2" t="s">
         <v>14</v>
@@ -3756,7 +3759,7 @@
         <v>63</v>
       </c>
       <c r="AJ24" s="1" t="s">
-        <v>72</v>
+        <v>195</v>
       </c>
     </row>
     <row r="25" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
FEAT: allows comma as decimal delimiter.
</commit_message>
<xml_diff>
--- a/docs/lexer/lexer-FSM.xlsx
+++ b/docs/lexer/lexer-FSM.xlsx
@@ -671,18 +671,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -751,7 +745,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -760,9 +754,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -781,13 +772,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -796,7 +787,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1110,12 +1101,12 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AJ24" sqref="AJ24"/>
+      <selection pane="topRight" activeCell="Y48" sqref="Y48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.36328125" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.36328125" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.7265625" customWidth="1"/>
     <col min="5" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
@@ -1125,115 +1116,115 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="8"/>
-      <c r="B1" s="7" t="s">
+      <c r="A1" s="7"/>
+      <c r="B1" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="N1" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="O1" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="P1" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="Q1" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="R1" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="S1" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="T1" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="U1" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="V1" s="7" t="s">
+      <c r="V1" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="W1" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="X1" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="Y1" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="Z1" s="7" t="s">
+      <c r="Z1" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="AA1" s="7" t="s">
+      <c r="AA1" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="AB1" s="7" t="s">
+      <c r="AB1" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="AC1" s="7" t="s">
+      <c r="AC1" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="AD1" s="7" t="s">
+      <c r="AD1" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="AE1" s="7" t="s">
+      <c r="AE1" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="AF1" s="7" t="s">
+      <c r="AF1" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="AG1" s="7" t="s">
+      <c r="AG1" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="AH1" s="7" t="s">
+      <c r="AH1" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="AI1" s="7" t="s">
+      <c r="AI1" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="AJ1" s="7" t="s">
+      <c r="AJ1" s="6" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1343,7 +1334,7 @@
       </c>
     </row>
     <row r="3" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="11" t="s">
         <v>69</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1453,7 +1444,7 @@
       </c>
     </row>
     <row r="4" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="11" t="s">
         <v>70</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -1563,7 +1554,7 @@
       </c>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -1673,7 +1664,7 @@
       </c>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="12" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -1783,7 +1774,7 @@
       </c>
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="11" t="s">
         <v>74</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -1893,7 +1884,7 @@
       </c>
     </row>
     <row r="8" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="11" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -2003,7 +1994,7 @@
       </c>
     </row>
     <row r="9" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="11" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -2113,7 +2104,7 @@
       </c>
     </row>
     <row r="10" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="11" t="s">
         <v>109</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -2223,7 +2214,7 @@
       </c>
     </row>
     <row r="11" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="11" t="s">
         <v>110</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -2333,7 +2324,7 @@
       </c>
     </row>
     <row r="12" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="11" t="s">
         <v>111</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -2443,7 +2434,7 @@
       </c>
     </row>
     <row r="13" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="11" t="s">
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -2553,7 +2544,7 @@
       </c>
     </row>
     <row r="14" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -2663,7 +2654,7 @@
       </c>
     </row>
     <row r="15" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="11" t="s">
         <v>7</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -2773,7 +2764,7 @@
       </c>
     </row>
     <row r="16" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="11" t="s">
         <v>71</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -2883,7 +2874,7 @@
       </c>
     </row>
     <row r="17" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="11" t="s">
         <v>8</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -2993,7 +2984,7 @@
       </c>
     </row>
     <row r="18" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="11" t="s">
         <v>9</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -3103,7 +3094,7 @@
       </c>
     </row>
     <row r="19" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="11" t="s">
         <v>10</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -3213,7 +3204,7 @@
       </c>
     </row>
     <row r="20" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A20" s="12" t="s">
+      <c r="A20" s="11" t="s">
         <v>11</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -3322,8 +3313,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A21" s="12" t="s">
+    <row r="21" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A21" s="11" t="s">
         <v>12</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -3395,8 +3386,8 @@
       <c r="X21" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="Y21" s="4" t="s">
-        <v>63</v>
+      <c r="Y21" s="2" t="s">
+        <v>86</v>
       </c>
       <c r="Z21" s="1" t="s">
         <v>84</v>
@@ -3433,7 +3424,7 @@
       </c>
     </row>
     <row r="22" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="11" t="s">
         <v>86</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -3505,7 +3496,7 @@
       <c r="X22" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="Y22" s="4" t="s">
+      <c r="Y22" s="3" t="s">
         <v>63</v>
       </c>
       <c r="Z22" s="1" t="s">
@@ -3543,7 +3534,7 @@
       </c>
     </row>
     <row r="23" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A23" s="12" t="s">
+      <c r="A23" s="11" t="s">
         <v>13</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -3653,7 +3644,7 @@
       </c>
     </row>
     <row r="24" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A24" s="12" t="s">
+      <c r="A24" s="11" t="s">
         <v>14</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -3763,7 +3754,7 @@
       </c>
     </row>
     <row r="25" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A25" s="12" t="s">
+      <c r="A25" s="11" t="s">
         <v>15</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -3873,7 +3864,7 @@
       </c>
     </row>
     <row r="26" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="11" t="s">
         <v>16</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -3983,7 +3974,7 @@
       </c>
     </row>
     <row r="27" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A27" s="12" t="s">
+      <c r="A27" s="11" t="s">
         <v>17</v>
       </c>
       <c r="B27" s="3" t="s">
@@ -4093,7 +4084,7 @@
       </c>
     </row>
     <row r="28" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A28" s="12" t="s">
+      <c r="A28" s="11" t="s">
         <v>18</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -4203,7 +4194,7 @@
       </c>
     </row>
     <row r="29" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A29" s="12" t="s">
+      <c r="A29" s="11" t="s">
         <v>19</v>
       </c>
       <c r="B29" s="3" t="s">
@@ -4313,7 +4304,7 @@
       </c>
     </row>
     <row r="30" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A30" s="12" t="s">
+      <c r="A30" s="11" t="s">
         <v>20</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -4423,7 +4414,7 @@
       </c>
     </row>
     <row r="31" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A31" s="12" t="s">
+      <c r="A31" s="11" t="s">
         <v>22</v>
       </c>
       <c r="B31" s="3" t="s">
@@ -4533,7 +4524,7 @@
       </c>
     </row>
     <row r="32" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A32" s="12" t="s">
+      <c r="A32" s="11" t="s">
         <v>23</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -4643,7 +4634,7 @@
       </c>
     </row>
     <row r="33" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A33" s="12" t="s">
+      <c r="A33" s="11" t="s">
         <v>24</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -4753,7 +4744,7 @@
       </c>
     </row>
     <row r="34" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A34" s="12" t="s">
+      <c r="A34" s="11" t="s">
         <v>25</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -4863,7 +4854,7 @@
       </c>
     </row>
     <row r="35" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A35" s="12" t="s">
+      <c r="A35" s="11" t="s">
         <v>26</v>
       </c>
       <c r="B35" s="2" t="s">
@@ -4973,7 +4964,7 @@
       </c>
     </row>
     <row r="36" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A36" s="12" t="s">
+      <c r="A36" s="11" t="s">
         <v>27</v>
       </c>
       <c r="B36" s="2" t="s">
@@ -5083,7 +5074,7 @@
       </c>
     </row>
     <row r="37" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A37" s="12" t="s">
+      <c r="A37" s="11" t="s">
         <v>28</v>
       </c>
       <c r="B37" s="2" t="s">
@@ -5193,7 +5184,7 @@
       </c>
     </row>
     <row r="38" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A38" s="12" t="s">
+      <c r="A38" s="11" t="s">
         <v>29</v>
       </c>
       <c r="B38" s="2" t="s">
@@ -5303,7 +5294,7 @@
       </c>
     </row>
     <row r="39" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A39" s="12" t="s">
+      <c r="A39" s="11" t="s">
         <v>30</v>
       </c>
       <c r="B39" s="2" t="s">
@@ -5413,7 +5404,7 @@
       </c>
     </row>
     <row r="40" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A40" s="12" t="s">
+      <c r="A40" s="11" t="s">
         <v>31</v>
       </c>
       <c r="B40" s="1" t="s">
@@ -5523,7 +5514,7 @@
       </c>
     </row>
     <row r="41" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A41" s="12" t="s">
+      <c r="A41" s="11" t="s">
         <v>193</v>
       </c>
       <c r="B41" s="1" t="s">
@@ -5633,7 +5624,7 @@
       </c>
     </row>
     <row r="42" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A42" s="12" t="s">
+      <c r="A42" s="11" t="s">
         <v>194</v>
       </c>
       <c r="B42" s="1" t="s">
@@ -5743,7 +5734,7 @@
       </c>
     </row>
     <row r="43" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A43" s="12" t="s">
+      <c r="A43" s="11" t="s">
         <v>32</v>
       </c>
       <c r="B43" s="1" t="s">
@@ -5853,7 +5844,7 @@
       </c>
     </row>
     <row r="44" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A44" s="12" t="s">
+      <c r="A44" s="11" t="s">
         <v>96</v>
       </c>
       <c r="B44" s="1" t="s">
@@ -5889,28 +5880,28 @@
       <c r="L44" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="M44" s="5" t="s">
+      <c r="M44" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="N44" s="5" t="s">
+      <c r="N44" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="O44" s="5" t="s">
+      <c r="O44" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="P44" s="5" t="s">
+      <c r="P44" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="Q44" s="5" t="s">
+      <c r="Q44" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="R44" s="5" t="s">
+      <c r="R44" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="S44" s="5" t="s">
+      <c r="S44" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="T44" s="5" t="s">
+      <c r="T44" s="4" t="s">
         <v>33</v>
       </c>
       <c r="U44" s="1" t="s">
@@ -5919,40 +5910,40 @@
       <c r="V44" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="W44" s="5" t="s">
+      <c r="W44" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="X44" s="5" t="s">
+      <c r="X44" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="Y44" s="5" t="s">
+      <c r="Y44" s="4" t="s">
         <v>33</v>
       </c>
       <c r="Z44" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="AA44" s="5" t="s">
+      <c r="AA44" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AB44" s="5" t="s">
+      <c r="AB44" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AC44" s="5" t="s">
+      <c r="AC44" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AD44" s="5" t="s">
+      <c r="AD44" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AE44" s="5" t="s">
+      <c r="AE44" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AF44" s="5" t="s">
+      <c r="AF44" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AG44" s="5" t="s">
+      <c r="AG44" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AH44" s="5" t="s">
+      <c r="AH44" s="4" t="s">
         <v>33</v>
       </c>
       <c r="AI44" s="3" t="s">
@@ -5963,7 +5954,7 @@
       </c>
     </row>
     <row r="45" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A45" s="12" t="s">
+      <c r="A45" s="11" t="s">
         <v>33</v>
       </c>
       <c r="B45" s="1" t="s">
@@ -6073,7 +6064,7 @@
       </c>
     </row>
     <row r="46" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A46" s="12" t="s">
+      <c r="A46" s="11" t="s">
         <v>21</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -6183,7 +6174,7 @@
       </c>
     </row>
     <row r="47" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A47" s="13" t="s">
+      <c r="A47" s="12" t="s">
         <v>112</v>
       </c>
       <c r="B47" s="3" t="s">
@@ -6292,8 +6283,8 @@
         <v>63</v>
       </c>
     </row>
-    <row r="48" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A48" s="12" t="s">
+    <row r="48" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A48" s="11" t="s">
         <v>113</v>
       </c>
       <c r="B48" s="1" t="s">
@@ -6365,8 +6356,8 @@
       <c r="X48" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="Y48" s="4" t="s">
-        <v>63</v>
+      <c r="Y48" s="2" t="s">
+        <v>86</v>
       </c>
       <c r="Z48" s="1" t="s">
         <v>84</v>
@@ -6403,7 +6394,7 @@
       </c>
     </row>
     <row r="49" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A49" s="12" t="s">
+      <c r="A49" s="11" t="s">
         <v>114</v>
       </c>
       <c r="B49" s="1" t="s">
@@ -6513,7 +6504,7 @@
       </c>
     </row>
     <row r="50" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A50" s="12" t="s">
+      <c r="A50" s="11" t="s">
         <v>115</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -6623,7 +6614,7 @@
       </c>
     </row>
     <row r="51" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A51" s="12" t="s">
+      <c r="A51" s="11" t="s">
         <v>116</v>
       </c>
       <c r="B51" s="1" t="s">
@@ -6756,93 +6747,93 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="14"/>
-      <c r="B1" s="7" t="s">
+      <c r="A1" s="13"/>
+      <c r="B1" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="6" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>128</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C2" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="F2" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H2" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="I2" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="J2" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K2" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="L2" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="M2" s="17" t="s">
+      <c r="C2" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="I2" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="J2" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="K2" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="L2" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="M2" s="16" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="11" t="s">
         <v>129</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="16" t="s">
         <v>174</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -6851,39 +6842,39 @@
       <c r="E3" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="F3" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="G3" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H3" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="I3" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="J3" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K3" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="L3" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="M3" s="17" t="s">
+      <c r="F3" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="J3" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="K3" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="L3" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="M3" s="16" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="11" t="s">
         <v>130</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="16" t="s">
         <v>174</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -6892,39 +6883,39 @@
       <c r="E4" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="F4" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="G4" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H4" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="I4" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="J4" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K4" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="L4" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="M4" s="17" t="s">
+      <c r="F4" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="I4" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="J4" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="K4" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="L4" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="M4" s="16" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="11" t="s">
         <v>131</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="16" t="s">
         <v>174</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -6933,39 +6924,39 @@
       <c r="E5" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="F5" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="G5" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H5" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="I5" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="J5" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K5" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="L5" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="M5" s="17" t="s">
+      <c r="F5" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="J5" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="K5" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="L5" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="M5" s="16" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="11" t="s">
         <v>179</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="16" t="s">
         <v>174</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -6974,33 +6965,33 @@
       <c r="E6" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="F6" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="G6" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H6" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="I6" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="J6" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K6" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="L6" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="M6" s="17" t="s">
+      <c r="F6" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="I6" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="K6" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="L6" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="M6" s="16" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="15" t="s">
         <v>132</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -7009,39 +7000,39 @@
       <c r="C7" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="D7" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="E7" s="17" t="s">
+      <c r="D7" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="E7" s="16" t="s">
         <v>174</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="G7" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H7" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="I7" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="J7" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K7" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="L7" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="M7" s="17" t="s">
+      <c r="G7" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="I7" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="J7" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="K7" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="L7" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="M7" s="16" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="15" t="s">
         <v>154</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -7050,10 +7041,10 @@
       <c r="C8" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="D8" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="E8" s="17" t="s">
+      <c r="D8" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="E8" s="16" t="s">
         <v>174</v>
       </c>
       <c r="F8" s="2" t="s">
@@ -7062,27 +7053,27 @@
       <c r="G8" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="H8" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="I8" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="J8" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K8" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="L8" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="M8" s="17" t="s">
+      <c r="H8" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="J8" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="K8" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="L8" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="M8" s="16" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="15" t="s">
         <v>133</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -7091,45 +7082,45 @@
       <c r="C9" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="D9" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="E9" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="F9" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="G9" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H9" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="I9" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="J9" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K9" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="L9" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="M9" s="17" t="s">
+      <c r="D9" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="I9" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="J9" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="K9" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="L9" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="M9" s="16" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="14" t="s">
         <v>134</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="16" t="s">
         <v>174</v>
       </c>
       <c r="D10" s="2" t="s">
@@ -7138,39 +7129,39 @@
       <c r="E10" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="F10" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="G10" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H10" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="I10" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="J10" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K10" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="L10" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="M10" s="17" t="s">
+      <c r="F10" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="H10" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="I10" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="J10" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="K10" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="L10" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="M10" s="16" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="14" t="s">
         <v>135</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="16" t="s">
         <v>174</v>
       </c>
       <c r="D11" s="2" t="s">
@@ -7179,39 +7170,39 @@
       <c r="E11" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="F11" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="G11" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H11" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="I11" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="J11" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K11" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="L11" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="M11" s="17" t="s">
+      <c r="F11" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="I11" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="J11" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="K11" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="L11" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="M11" s="16" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="14" t="s">
         <v>186</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="16" t="s">
         <v>174</v>
       </c>
       <c r="D12" s="2" t="s">
@@ -7220,39 +7211,39 @@
       <c r="E12" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="F12" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="G12" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H12" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="I12" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="J12" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K12" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="L12" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="M12" s="17" t="s">
+      <c r="F12" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="H12" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="I12" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="J12" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="K12" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="L12" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="M12" s="16" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="14" t="s">
         <v>187</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="16" t="s">
         <v>174</v>
       </c>
       <c r="D13" s="2" t="s">
@@ -7261,189 +7252,189 @@
       <c r="E13" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="F13" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="G13" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H13" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="I13" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="J13" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K13" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="L13" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="M13" s="17" t="s">
+      <c r="F13" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="H13" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="I13" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="J13" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="K13" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="L13" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="M13" s="16" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="15" t="s">
         <v>136</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="C14" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="E14" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="F14" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="G14" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H14" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="I14" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="J14" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K14" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="L14" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="M14" s="17" t="s">
+      <c r="C14" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="H14" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="I14" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="J14" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="K14" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="L14" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="M14" s="16" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="B15" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D15" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="E15" s="17" t="s">
+      <c r="B15" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="E15" s="16" t="s">
         <v>174</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="G15" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H15" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="I15" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="J15" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K15" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="L15" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="M15" s="5" t="s">
+      <c r="G15" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="H15" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="I15" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="J15" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="K15" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="L15" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="M15" s="4" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="14" t="s">
         <v>138</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="C16" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="E16" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="F16" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="G16" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H16" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="I16" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="J16" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K16" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="L16" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="M16" s="17" t="s">
+      <c r="C16" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="H16" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="I16" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="J16" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="K16" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="L16" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="M16" s="16" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="14" t="s">
         <v>139</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="C17" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="E17" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="F17" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="G17" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H17" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="I17" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="J17" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K17" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="L17" s="17" t="s">
+      <c r="C17" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="H17" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="I17" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="J17" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="K17" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="L17" s="16" t="s">
         <v>174</v>
       </c>
       <c r="M17" s="2" t="s">
@@ -7451,40 +7442,40 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="B18" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="E18" s="5" t="s">
+      <c r="B18" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="E18" s="4" t="s">
         <v>190</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="G18" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H18" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="I18" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="J18" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K18" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="L18" s="17" t="s">
+      <c r="G18" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="H18" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="I18" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="J18" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="K18" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="L18" s="16" t="s">
         <v>174</v>
       </c>
       <c r="M18" s="2" t="s">
@@ -7492,81 +7483,81 @@
       </c>
     </row>
     <row r="19" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="14" t="s">
         <v>190</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C19" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="E19" s="17" t="s">
+      <c r="C19" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="E19" s="16" t="s">
         <v>174</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="G19" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H19" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="I19" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="J19" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K19" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="L19" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="M19" s="17" t="s">
+      <c r="G19" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="H19" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="I19" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="J19" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="K19" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="L19" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="M19" s="16" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A20" s="15" t="s">
+      <c r="A20" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="B20" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="E20" s="17" t="s">
+      <c r="B20" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="E20" s="16" t="s">
         <v>174</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="G20" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H20" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="I20" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="J20" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K20" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="L20" s="17" t="s">
+      <c r="G20" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="H20" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="I20" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="J20" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="K20" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="L20" s="16" t="s">
         <v>174</v>
       </c>
       <c r="M20" s="2" t="s">
@@ -7574,10 +7565,10 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="16" t="s">
         <v>174</v>
       </c>
       <c r="C21" s="2" t="s">
@@ -7592,63 +7583,63 @@
       <c r="F21" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="G21" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H21" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="I21" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="J21" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K21" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="L21" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="M21" s="17" t="s">
+      <c r="G21" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="H21" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="I21" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="J21" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="K21" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="L21" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="M21" s="16" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A22" s="16" t="s">
+      <c r="A22" s="15" t="s">
         <v>156</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C22" s="16" t="s">
         <v>174</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E22" s="17" t="s">
+      <c r="E22" s="16" t="s">
         <v>174</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="G22" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H22" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="I22" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="J22" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K22" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="L22" s="17" t="s">
+      <c r="G22" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="H22" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="I22" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="J22" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="K22" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="L22" s="16" t="s">
         <v>174</v>
       </c>
       <c r="M22" s="2" t="s">
@@ -7656,40 +7647,40 @@
       </c>
     </row>
     <row r="23" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="15" t="s">
         <v>157</v>
       </c>
-      <c r="B23" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="C23" s="17" t="s">
+      <c r="B23" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="C23" s="16" t="s">
         <v>174</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E23" s="17" t="s">
+      <c r="E23" s="16" t="s">
         <v>174</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="G23" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H23" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="I23" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="J23" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K23" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="L23" s="17" t="s">
+      <c r="G23" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="H23" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="I23" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="J23" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="K23" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="L23" s="16" t="s">
         <v>174</v>
       </c>
       <c r="M23" s="2" t="s">
@@ -7697,13 +7688,13 @@
       </c>
     </row>
     <row r="24" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A24" s="15" t="s">
+      <c r="A24" s="14" t="s">
         <v>143</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="C24" s="17" t="s">
+      <c r="C24" s="16" t="s">
         <v>174</v>
       </c>
       <c r="D24" s="2" t="s">
@@ -7712,39 +7703,39 @@
       <c r="E24" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="F24" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="G24" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H24" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="I24" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="J24" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K24" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="L24" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="M24" s="17" t="s">
+      <c r="F24" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G24" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="H24" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="I24" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="J24" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="K24" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="L24" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="M24" s="16" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A25" s="15" t="s">
+      <c r="A25" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="B25" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="C25" s="17" t="s">
+      <c r="B25" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="C25" s="16" t="s">
         <v>174</v>
       </c>
       <c r="D25" s="2" t="s">
@@ -7753,77 +7744,77 @@
       <c r="E25" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="F25" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="G25" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H25" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="I25" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="J25" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K25" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="L25" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="M25" s="17" t="s">
+      <c r="F25" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G25" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="H25" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="I25" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="J25" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="K25" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="L25" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="M25" s="16" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A26" s="16" t="s">
+      <c r="A26" s="15" t="s">
         <v>145</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="C26" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D26" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="E26" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="F26" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="G26" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H26" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="I26" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="J26" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K26" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="L26" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="M26" s="17" t="s">
+      <c r="C26" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="E26" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="F26" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G26" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="H26" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="I26" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="J26" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="K26" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="L26" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="M26" s="16" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A27" s="15" t="s">
+      <c r="A27" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="16" t="s">
         <v>174</v>
       </c>
       <c r="C27" s="2" t="s">
@@ -7838,63 +7829,63 @@
       <c r="F27" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="G27" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H27" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="I27" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="J27" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K27" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="L27" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="M27" s="17" t="s">
+      <c r="G27" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="H27" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="I27" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="J27" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="K27" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="L27" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="M27" s="16" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A28" s="16" t="s">
+      <c r="A28" s="15" t="s">
         <v>158</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="C28" s="16" t="s">
         <v>174</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E28" s="17" t="s">
+      <c r="E28" s="16" t="s">
         <v>174</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="G28" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H28" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="I28" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="J28" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K28" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="L28" s="17" t="s">
+      <c r="G28" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="H28" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="I28" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="J28" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="K28" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="L28" s="16" t="s">
         <v>174</v>
       </c>
       <c r="M28" s="2" t="s">
@@ -7902,40 +7893,40 @@
       </c>
     </row>
     <row r="29" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A29" s="16" t="s">
+      <c r="A29" s="15" t="s">
         <v>159</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="C29" s="17" t="s">
+      <c r="C29" s="16" t="s">
         <v>174</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E29" s="17" t="s">
+      <c r="E29" s="16" t="s">
         <v>174</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="G29" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H29" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="I29" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="J29" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K29" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="L29" s="17" t="s">
+      <c r="G29" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="H29" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="I29" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="J29" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="K29" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="L29" s="16" t="s">
         <v>174</v>
       </c>
       <c r="M29" s="2" t="s">
@@ -7943,40 +7934,40 @@
       </c>
     </row>
     <row r="30" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A30" s="16" t="s">
+      <c r="A30" s="15" t="s">
         <v>160</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="C30" s="17" t="s">
+      <c r="C30" s="16" t="s">
         <v>174</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E30" s="17" t="s">
+      <c r="E30" s="16" t="s">
         <v>174</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="G30" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H30" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="I30" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="J30" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K30" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="L30" s="17" t="s">
+      <c r="G30" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="H30" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="I30" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="J30" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="K30" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="L30" s="16" t="s">
         <v>174</v>
       </c>
       <c r="M30" s="2" t="s">
@@ -7984,40 +7975,40 @@
       </c>
     </row>
     <row r="31" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A31" s="16" t="s">
+      <c r="A31" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="B31" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="C31" s="17" t="s">
+      <c r="B31" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="C31" s="16" t="s">
         <v>174</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E31" s="17" t="s">
+      <c r="E31" s="16" t="s">
         <v>174</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="G31" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H31" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="I31" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="J31" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K31" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="L31" s="17" t="s">
+      <c r="G31" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="H31" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="I31" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="J31" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="K31" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="L31" s="16" t="s">
         <v>174</v>
       </c>
       <c r="M31" s="2" t="s">
@@ -8025,450 +8016,450 @@
       </c>
     </row>
     <row r="32" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A32" s="13" t="s">
+      <c r="A32" s="12" t="s">
         <v>147</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="C32" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D32" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="E32" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="F32" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="G32" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H32" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="I32" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="J32" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K32" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="L32" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="M32" s="17" t="s">
+      <c r="C32" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="D32" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="E32" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="F32" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G32" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="H32" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="I32" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="J32" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="K32" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="L32" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="M32" s="16" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A33" s="15" t="s">
+      <c r="A33" s="14" t="s">
         <v>162</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="C33" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D33" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="E33" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="F33" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="G33" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H33" s="17" t="s">
+      <c r="C33" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="D33" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="E33" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="F33" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G33" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="H33" s="16" t="s">
         <v>174</v>
       </c>
       <c r="I33" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="J33" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K33" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="L33" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="M33" s="17" t="s">
+      <c r="J33" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="K33" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="L33" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="M33" s="16" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A34" s="16" t="s">
+      <c r="A34" s="15" t="s">
         <v>148</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="C34" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D34" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="E34" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="F34" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="G34" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H34" s="17" t="s">
+      <c r="C34" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="E34" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="F34" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G34" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="H34" s="16" t="s">
         <v>174</v>
       </c>
       <c r="I34" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="J34" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K34" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="L34" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="M34" s="17" t="s">
+      <c r="J34" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="K34" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="L34" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="M34" s="16" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A35" s="15" t="s">
+      <c r="A35" s="14" t="s">
         <v>163</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="C35" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D35" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="E35" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="F35" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="G35" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H35" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="I35" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="J35" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K35" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="L35" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="M35" s="17" t="s">
+      <c r="C35" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="D35" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="E35" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="F35" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G35" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="H35" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="I35" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="J35" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="K35" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="L35" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="M35" s="16" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="36" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A36" s="16" t="s">
+      <c r="A36" s="15" t="s">
         <v>164</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="C36" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D36" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="E36" s="5" t="s">
+      <c r="C36" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="D36" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="E36" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="F36" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="G36" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H36" s="5" t="s">
+      <c r="F36" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G36" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="H36" s="4" t="s">
         <v>185</v>
       </c>
       <c r="I36" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="J36" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K36" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="L36" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="M36" s="5" t="s">
+      <c r="J36" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="K36" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="L36" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="M36" s="4" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A37" s="15" t="s">
+      <c r="A37" s="14" t="s">
         <v>149</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="C37" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D37" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="E37" s="5" t="s">
+      <c r="C37" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="D37" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="E37" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="F37" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="G37" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H37" s="5" t="s">
+      <c r="F37" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G37" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="H37" s="4" t="s">
         <v>185</v>
       </c>
       <c r="I37" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="J37" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K37" s="5" t="s">
+      <c r="J37" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="K37" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="L37" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="M37" s="5" t="s">
+      <c r="L37" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="M37" s="4" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A38" s="16" t="s">
+      <c r="A38" s="15" t="s">
         <v>165</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="C38" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D38" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="E38" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="F38" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="G38" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H38" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="I38" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="J38" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K38" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="L38" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="M38" s="17" t="s">
+      <c r="C38" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="D38" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="E38" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="F38" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G38" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="H38" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="I38" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="J38" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="K38" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="L38" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="M38" s="16" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A39" s="15" t="s">
+      <c r="A39" s="14" t="s">
         <v>166</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="C39" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D39" s="17" t="s">
+      <c r="C39" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="D39" s="16" t="s">
         <v>174</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="F39" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="G39" s="17" t="s">
+      <c r="F39" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G39" s="16" t="s">
         <v>174</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="I39" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="J39" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K39" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="L39" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="M39" s="5" t="s">
+      <c r="I39" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="J39" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="K39" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="L39" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="M39" s="4" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A40" s="16" t="s">
+      <c r="A40" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="B40" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="C40" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D40" s="17" t="s">
+      <c r="B40" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="C40" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="D40" s="16" t="s">
         <v>174</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="F40" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="G40" s="17" t="s">
+      <c r="F40" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G40" s="16" t="s">
         <v>174</v>
       </c>
       <c r="H40" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="I40" s="17" t="s">
+      <c r="I40" s="16" t="s">
         <v>174</v>
       </c>
       <c r="J40" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="K40" s="5" t="s">
+      <c r="K40" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="L40" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="M40" s="5" t="s">
+      <c r="L40" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="M40" s="4" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A41" s="15" t="s">
+      <c r="A41" s="14" t="s">
         <v>167</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="C41" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D41" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="E41" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="F41" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="G41" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H41" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="I41" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="J41" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K41" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="L41" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="M41" s="17" t="s">
+      <c r="C41" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="D41" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="E41" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="F41" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G41" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="H41" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="I41" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="J41" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="K41" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="L41" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="M41" s="16" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A42" s="15" t="s">
+      <c r="A42" s="14" t="s">
         <v>168</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="C42" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D42" s="17" t="s">
+      <c r="C42" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="D42" s="16" t="s">
         <v>174</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="F42" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="G42" s="17" t="s">
+      <c r="F42" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G42" s="16" t="s">
         <v>174</v>
       </c>
       <c r="H42" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="I42" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="J42" s="17" t="s">
+      <c r="I42" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="J42" s="16" t="s">
         <v>174</v>
       </c>
       <c r="K42" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="L42" s="17" t="s">
+      <c r="L42" s="16" t="s">
         <v>174</v>
       </c>
       <c r="M42" s="2" t="s">
@@ -8476,81 +8467,81 @@
       </c>
     </row>
     <row r="43" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A43" s="15" t="s">
+      <c r="A43" s="14" t="s">
         <v>185</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="C43" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D43" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="E43" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="F43" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="G43" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H43" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="I43" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="J43" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K43" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="L43" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="M43" s="17" t="s">
+      <c r="C43" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="D43" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="E43" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="F43" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G43" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="H43" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="I43" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="J43" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="K43" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="L43" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="M43" s="16" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="44" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A44" s="15" t="s">
+      <c r="A44" s="14" t="s">
         <v>151</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="C44" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D44" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="E44" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="F44" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="G44" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H44" s="17" t="s">
+      <c r="C44" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="D44" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="E44" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="F44" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G44" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="H44" s="16" t="s">
         <v>174</v>
       </c>
       <c r="I44" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="J44" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K44" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="L44" s="17" t="s">
+      <c r="J44" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="K44" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="L44" s="16" t="s">
         <v>174</v>
       </c>
       <c r="M44" s="2" t="s">
@@ -8558,40 +8549,40 @@
       </c>
     </row>
     <row r="45" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A45" s="16" t="s">
+      <c r="A45" s="15" t="s">
         <v>152</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C45" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D45" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="E45" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="F45" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="G45" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H45" s="17" t="s">
+      <c r="C45" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="D45" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="E45" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="F45" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G45" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="H45" s="16" t="s">
         <v>174</v>
       </c>
       <c r="I45" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="J45" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K45" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="L45" s="17" t="s">
+      <c r="J45" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="K45" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="L45" s="16" t="s">
         <v>174</v>
       </c>
       <c r="M45" s="2" t="s">
@@ -8599,40 +8590,40 @@
       </c>
     </row>
     <row r="46" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A46" s="16" t="s">
+      <c r="A46" s="15" t="s">
         <v>170</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C46" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D46" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="E46" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="F46" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="G46" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H46" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="I46" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="J46" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K46" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="L46" s="17" t="s">
+      <c r="C46" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="D46" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="E46" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="F46" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G46" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="H46" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="I46" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="J46" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="K46" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="L46" s="16" t="s">
         <v>174</v>
       </c>
       <c r="M46" s="2" t="s">
@@ -8640,40 +8631,40 @@
       </c>
     </row>
     <row r="47" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="15" t="s">
+      <c r="A47" s="14" t="s">
         <v>153</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="C47" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D47" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="E47" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="F47" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="G47" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H47" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="I47" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="J47" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K47" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="L47" s="17" t="s">
+      <c r="C47" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="D47" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="E47" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="F47" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G47" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="H47" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="I47" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="J47" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="K47" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="L47" s="16" t="s">
         <v>174</v>
       </c>
       <c r="M47" s="2" t="s">
@@ -8681,43 +8672,43 @@
       </c>
     </row>
     <row r="48" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A48" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="B48" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="C48" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D48" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="E48" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="F48" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="G48" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H48" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="I48" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="J48" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K48" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="L48" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="M48" s="17" t="s">
+      <c r="A48" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="B48" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="C48" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="D48" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="E48" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="F48" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="G48" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="H48" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="I48" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="J48" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="K48" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="L48" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="M48" s="16" t="s">
         <v>174</v>
       </c>
     </row>
@@ -8744,25 +8735,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="8"/>
-      <c r="B1" s="7" t="s">
+      <c r="A1" s="7"/>
+      <c r="B1" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>104</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -8782,27 +8773,27 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="9" t="s">
         <v>106</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="9" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>107</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -8822,7 +8813,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A5" s="6"/>
+      <c r="A5" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
FEAT: adds hex states to the Excel table and generator script.
</commit_message>
<xml_diff>
--- a/docs/lexer/lexer-FSM.xlsx
+++ b/docs/lexer/lexer-FSM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2481" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2553" uniqueCount="198">
   <si>
     <t>S_START</t>
   </si>
@@ -604,6 +604,12 @@
   </si>
   <si>
     <t>T_FLOAT_SP</t>
+  </si>
+  <si>
+    <t>S_DECX</t>
+  </si>
+  <si>
+    <t>S_HEX</t>
   </si>
 </sst>
 </file>
@@ -1097,11 +1103,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ51"/>
+  <dimension ref="A1:AJ53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Y48" sqref="Y48"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3643,9 +3649,9 @@
         <v>87</v>
       </c>
     </row>
-    <row r="24" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A24" s="11" t="s">
-        <v>14</v>
+        <v>196</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>87</v>
@@ -3653,445 +3659,445 @@
       <c r="C24" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="G24" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="M24" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="N24" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="P24" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q24" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="R24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="S24" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="T24" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="U24" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="V24" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="W24" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="X24" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="Y24" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z24" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA24" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC24" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF24" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AG24" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH24" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI24" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ24" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A25" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="G25" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="H25" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="I24" s="1" t="s">
+      <c r="I25" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="J24" s="1" t="s">
+      <c r="J25" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="K24" s="1" t="s">
+      <c r="K25" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="L24" s="1" t="s">
+      <c r="L25" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="M24" s="2" t="s">
+      <c r="M25" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="N24" s="1" t="s">
+      <c r="N25" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="O24" s="1" t="s">
+      <c r="O25" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="P24" s="2" t="s">
+      <c r="P25" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="Q24" s="2" t="s">
+      <c r="Q25" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="R24" s="2" t="s">
+      <c r="R25" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="S24" s="2" t="s">
+      <c r="S25" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="T24" s="1" t="s">
+      <c r="T25" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="U24" s="1" t="s">
+      <c r="U25" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="V24" s="1" t="s">
+      <c r="V25" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="W24" s="2" t="s">
+      <c r="W25" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="X24" s="1" t="s">
+      <c r="X25" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="Y24" s="1" t="s">
+      <c r="Y25" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="Z24" s="1" t="s">
+      <c r="Z25" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="AA24" s="1" t="s">
+      <c r="AA25" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="AB24" s="2" t="s">
+      <c r="AB25" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="AC24" s="1" t="s">
+      <c r="AC25" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="AD24" s="2" t="s">
+      <c r="AD25" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="AE24" s="2" t="s">
+      <c r="AE25" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="AF24" s="1" t="s">
+      <c r="AF25" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="AG24" s="2" t="s">
+      <c r="AG25" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="AH24" s="2" t="s">
+      <c r="AH25" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="AI24" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AJ24" s="1" t="s">
+      <c r="AI25" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ25" s="1" t="s">
         <v>195</v>
-      </c>
-    </row>
-    <row r="25" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A25" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="L25" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="M25" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="N25" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="O25" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="P25" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q25" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="R25" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="S25" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="T25" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="U25" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="V25" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="W25" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="X25" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y25" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="Z25" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AA25" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AB25" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="AC25" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AD25" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AE25" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AF25" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AG25" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AH25" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AI25" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AJ25" s="1" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A26" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="M26" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="N26" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="O26" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="P26" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q26" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="R26" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="S26" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="T26" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="U26" s="2" t="s">
-        <v>16</v>
+        <v>88</v>
+      </c>
+      <c r="M26" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="N26" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="P26" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q26" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="R26" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="S26" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="T26" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="U26" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="V26" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="W26" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="X26" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="Y26" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="Z26" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="AA26" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
+      </c>
+      <c r="W26" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="X26" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y26" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z26" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA26" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="AB26" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="AC26" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="AD26" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="AE26" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="AF26" s="1" t="s">
-        <v>89</v>
+        <v>15</v>
+      </c>
+      <c r="AC26" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD26" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE26" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF26" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="AG26" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="AH26" s="2" t="s">
-        <v>16</v>
+      <c r="AH26" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="AI26" s="3" t="s">
         <v>63</v>
       </c>
       <c r="AJ26" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="27" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A27" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>63</v>
+        <v>16</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="I27" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="J27" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="K27" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="L27" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="M27" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="N27" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="O27" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="P27" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q27" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="R27" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="S27" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="T27" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="U27" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="V27" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="W27" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="X27" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y27" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="Z27" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AA27" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AB27" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AC27" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AD27" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AE27" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AF27" s="3" t="s">
-        <v>63</v>
+        <v>16</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="P27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="S27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="T27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="U27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="V27" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="W27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="X27" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z27" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA27" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AB27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AC27" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AD27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF27" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="AG27" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="AH27" s="3" t="s">
-        <v>63</v>
+      <c r="AH27" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="AI27" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="AJ27" s="3" t="s">
-        <v>63</v>
+      <c r="AJ27" s="1" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="28" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A28" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>90</v>
+        <v>17</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>18</v>
@@ -4099,26 +4105,26 @@
       <c r="E28" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F28" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="L28" s="1" t="s">
-        <v>90</v>
+      <c r="F28" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="L28" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="M28" s="3" t="s">
         <v>63</v>
@@ -4126,8 +4132,8 @@
       <c r="N28" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="O28" s="2" t="s">
-        <v>18</v>
+      <c r="O28" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="P28" s="3" t="s">
         <v>63</v>
@@ -4141,14 +4147,14 @@
       <c r="S28" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="T28" s="1" t="s">
-        <v>90</v>
+      <c r="T28" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="U28" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="V28" s="1" t="s">
-        <v>90</v>
+      <c r="V28" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="W28" s="3" t="s">
         <v>63</v>
@@ -4159,14 +4165,14 @@
       <c r="Y28" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="Z28" s="1" t="s">
-        <v>90</v>
+      <c r="Z28" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="AA28" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="AB28" s="2" t="s">
-        <v>18</v>
+      <c r="AB28" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="AC28" s="3" t="s">
         <v>63</v>
@@ -4189,46 +4195,46 @@
       <c r="AI28" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="AJ28" s="1" t="s">
-        <v>90</v>
+      <c r="AJ28" s="3" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A29" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>63</v>
+        <v>18</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="I29" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="J29" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="K29" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="L29" s="3" t="s">
-        <v>63</v>
+        <v>18</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="M29" s="3" t="s">
         <v>63</v>
@@ -4236,8 +4242,8 @@
       <c r="N29" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="O29" s="3" t="s">
-        <v>63</v>
+      <c r="O29" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="P29" s="3" t="s">
         <v>63</v>
@@ -4251,14 +4257,14 @@
       <c r="S29" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="T29" s="3" t="s">
-        <v>63</v>
+      <c r="T29" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="U29" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="V29" s="3" t="s">
-        <v>63</v>
+      <c r="V29" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="W29" s="3" t="s">
         <v>63</v>
@@ -4269,14 +4275,14 @@
       <c r="Y29" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="Z29" s="3" t="s">
-        <v>63</v>
+      <c r="Z29" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="AA29" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="AB29" s="3" t="s">
-        <v>63</v>
+      <c r="AB29" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="AC29" s="3" t="s">
         <v>63</v>
@@ -4299,19 +4305,19 @@
       <c r="AI29" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="AJ29" s="3" t="s">
-        <v>63</v>
+      <c r="AJ29" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="30" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A30" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>91</v>
+        <v>19</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>20</v>
@@ -4319,26 +4325,26 @@
       <c r="E30" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F30" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="J30" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="K30" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="L30" s="1" t="s">
-        <v>91</v>
+      <c r="F30" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J30" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="L30" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="M30" s="3" t="s">
         <v>63</v>
@@ -4346,8 +4352,8 @@
       <c r="N30" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="O30" s="1" t="s">
-        <v>91</v>
+      <c r="O30" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="P30" s="3" t="s">
         <v>63</v>
@@ -4355,20 +4361,20 @@
       <c r="Q30" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="R30" s="2" t="s">
-        <v>20</v>
+      <c r="R30" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="S30" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="T30" s="1" t="s">
-        <v>91</v>
+      <c r="T30" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="U30" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="V30" s="1" t="s">
-        <v>91</v>
+      <c r="V30" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="W30" s="3" t="s">
         <v>63</v>
@@ -4379,14 +4385,14 @@
       <c r="Y30" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="Z30" s="1" t="s">
-        <v>91</v>
+      <c r="Z30" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="AA30" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="AB30" s="2" t="s">
-        <v>20</v>
+      <c r="AB30" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="AC30" s="3" t="s">
         <v>63</v>
@@ -4409,46 +4415,46 @@
       <c r="AI30" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="AJ30" s="1" t="s">
-        <v>91</v>
+      <c r="AJ30" s="3" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A31" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>63</v>
+        <v>20</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>91</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="I31" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="J31" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="K31" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="L31" s="3" t="s">
-        <v>63</v>
+        <v>20</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>91</v>
       </c>
       <c r="M31" s="3" t="s">
         <v>63</v>
@@ -4456,8 +4462,8 @@
       <c r="N31" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="O31" s="3" t="s">
-        <v>63</v>
+      <c r="O31" s="1" t="s">
+        <v>91</v>
       </c>
       <c r="P31" s="3" t="s">
         <v>63</v>
@@ -4465,20 +4471,20 @@
       <c r="Q31" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="R31" s="3" t="s">
-        <v>63</v>
+      <c r="R31" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="S31" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="T31" s="3" t="s">
-        <v>63</v>
+      <c r="T31" s="1" t="s">
+        <v>91</v>
       </c>
       <c r="U31" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="V31" s="3" t="s">
-        <v>63</v>
+      <c r="V31" s="1" t="s">
+        <v>91</v>
       </c>
       <c r="W31" s="3" t="s">
         <v>63</v>
@@ -4489,14 +4495,14 @@
       <c r="Y31" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="Z31" s="3" t="s">
-        <v>63</v>
+      <c r="Z31" s="1" t="s">
+        <v>91</v>
       </c>
       <c r="AA31" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="AB31" s="3" t="s">
-        <v>63</v>
+      <c r="AB31" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="AC31" s="3" t="s">
         <v>63</v>
@@ -4519,19 +4525,19 @@
       <c r="AI31" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="AJ31" s="3" t="s">
-        <v>63</v>
+      <c r="AJ31" s="1" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="32" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A32" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>93</v>
+        <v>22</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>23</v>
@@ -4539,35 +4545,35 @@
       <c r="E32" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F32" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="J32" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="K32" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="L32" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="M32" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="N32" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="O32" s="1" t="s">
-        <v>93</v>
+      <c r="F32" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J32" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="K32" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="L32" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="M32" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="N32" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="O32" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="P32" s="3" t="s">
         <v>63</v>
@@ -4581,14 +4587,14 @@
       <c r="S32" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="T32" s="1" t="s">
-        <v>93</v>
+      <c r="T32" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="U32" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="V32" s="1" t="s">
-        <v>93</v>
+      <c r="V32" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="W32" s="3" t="s">
         <v>63</v>
@@ -4599,14 +4605,14 @@
       <c r="Y32" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="Z32" s="1" t="s">
-        <v>93</v>
+      <c r="Z32" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="AA32" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="AB32" s="2" t="s">
-        <v>24</v>
+      <c r="AB32" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="AC32" s="3" t="s">
         <v>63</v>
@@ -4629,13 +4635,13 @@
       <c r="AI32" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="AJ32" s="1" t="s">
-        <v>72</v>
+      <c r="AJ32" s="3" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A33" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>93</v>
@@ -4644,10 +4650,10 @@
         <v>93</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>93</v>
@@ -4674,7 +4680,7 @@
         <v>93</v>
       </c>
       <c r="N33" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O33" s="1" t="s">
         <v>93</v>
@@ -4715,8 +4721,8 @@
       <c r="AA33" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="AB33" s="3" t="s">
-        <v>63</v>
+      <c r="AB33" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="AC33" s="3" t="s">
         <v>63</v>
@@ -4743,438 +4749,438 @@
         <v>72</v>
       </c>
     </row>
-    <row r="34" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A34" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="N34" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="O34" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="P34" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q34" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="R34" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="S34" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="T34" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="U34" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="V34" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="W34" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="X34" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y34" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z34" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AA34" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB34" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC34" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD34" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE34" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF34" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AG34" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH34" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI34" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ34" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="35" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A35" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="M35" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="N35" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="O35" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="P35" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q35" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="R35" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="S35" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="T35" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="U35" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="V35" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="W35" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="X35" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y35" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z35" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA35" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB35" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC35" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD35" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE35" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF35" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AG35" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH35" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI35" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ35" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="36" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A36" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D34" s="2" t="s">
+      <c r="B36" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="E36" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F34" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="I34" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="J34" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="K34" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="L34" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="M34" s="2" t="s">
+      <c r="F36" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="M36" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N34" s="2" t="s">
+      <c r="N36" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="O34" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="P34" s="2" t="s">
+      <c r="O36" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="P36" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="Q34" s="2" t="s">
+      <c r="Q36" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="R34" s="2" t="s">
+      <c r="R36" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="S34" s="2" t="s">
+      <c r="S36" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="T34" s="2" t="s">
+      <c r="T36" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="U34" s="2" t="s">
+      <c r="U36" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="V34" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="W34" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="X34" s="2" t="s">
+      <c r="V36" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="W36" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="X36" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="Y34" s="2" t="s">
+      <c r="Y36" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="Z34" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="AA34" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="AB34" s="2" t="s">
+      <c r="Z36" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA36" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB36" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AC34" s="2" t="s">
+      <c r="AC36" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AD34" s="2" t="s">
+      <c r="AD36" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AE34" s="2" t="s">
+      <c r="AE36" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AF34" s="2" t="s">
+      <c r="AF36" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AG34" s="2" t="s">
+      <c r="AG36" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AH34" s="2" t="s">
+      <c r="AH36" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AI34" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AJ34" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="35" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A35" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I35" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="J35" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="K35" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="L35" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="M35" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N35" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="O35" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="P35" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q35" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="R35" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="S35" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="T35" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="U35" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="V35" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="W35" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="X35" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y35" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z35" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AA35" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB35" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC35" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AD35" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AE35" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AF35" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AG35" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AH35" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AI35" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AJ35" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="36" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A36" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I36" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="J36" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="K36" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="L36" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M36" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="N36" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="O36" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="P36" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q36" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="R36" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="S36" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="T36" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="U36" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="V36" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="W36" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="X36" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y36" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z36" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA36" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="AB36" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC36" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="AD36" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="AE36" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="AF36" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="AG36" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="AH36" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="AI36" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="AJ36" s="3" t="s">
-        <v>63</v>
+      <c r="AJ36" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="37" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A37" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L37" s="2" t="s">
         <v>27</v>
       </c>
       <c r="M37" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N37" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O37" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="P37" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q37" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R37" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S37" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T37" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="U37" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="V37" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="W37" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="W37" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="X37" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Y37" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Z37" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AA37" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AB37" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AC37" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AD37" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AE37" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AF37" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AG37" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AH37" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AI37" s="3" t="s">
         <v>63</v>
@@ -5185,106 +5191,106 @@
     </row>
     <row r="38" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A38" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="M38" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N38" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="O38" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P38" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="Q38" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="R38" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="S38" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="T38" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="U38" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="V38" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="W38" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="X38" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="Y38" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="Z38" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="AA38" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="AB38" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="AC38" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="AD38" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="AE38" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="AF38" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AG38" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="AH38" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="AI38" s="3" t="s">
         <v>63</v>
@@ -5295,370 +5301,370 @@
     </row>
     <row r="39" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A39" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K39" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L39" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M39" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N39" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O39" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="P39" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q39" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="R39" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="S39" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="T39" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="U39" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="V39" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="W39" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="X39" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y39" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z39" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA39" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB39" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC39" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD39" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE39" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF39" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG39" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH39" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AI39" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ39" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A40" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J40" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K40" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L40" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M40" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="N40" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="O40" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P40" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q40" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="R40" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="S40" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T40" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="U40" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="V40" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="W40" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="X40" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y40" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z40" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA40" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB40" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC40" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD40" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE40" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF40" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AG40" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH40" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AI40" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ40" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A41" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B41" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C41" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D41" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E39" s="2" t="s">
+      <c r="E41" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F39" s="2" t="s">
+      <c r="F41" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G39" s="2" t="s">
+      <c r="G41" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H39" s="2" t="s">
+      <c r="H41" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I39" s="2" t="s">
+      <c r="I41" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J39" s="2" t="s">
+      <c r="J41" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K39" s="2" t="s">
+      <c r="K41" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="L39" s="2" t="s">
+      <c r="L41" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="M39" s="2" t="s">
+      <c r="M41" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="N39" s="2" t="s">
+      <c r="N41" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="O39" s="2" t="s">
+      <c r="O41" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="P39" s="2" t="s">
+      <c r="P41" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="Q39" s="2" t="s">
+      <c r="Q41" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="R39" s="2" t="s">
+      <c r="R41" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="S39" s="2" t="s">
+      <c r="S41" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="T39" s="2" t="s">
+      <c r="T41" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="U39" s="2" t="s">
+      <c r="U41" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="V39" s="2" t="s">
+      <c r="V41" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="W39" s="2" t="s">
+      <c r="W41" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="X39" s="2" t="s">
+      <c r="X41" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="Y39" s="2" t="s">
+      <c r="Y41" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="Z39" s="2" t="s">
+      <c r="Z41" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AA39" s="2" t="s">
+      <c r="AA41" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AB39" s="2" t="s">
+      <c r="AB41" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AC39" s="2" t="s">
+      <c r="AC41" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AD39" s="2" t="s">
+      <c r="AD41" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AE39" s="2" t="s">
+      <c r="AE41" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AF39" s="2" t="s">
+      <c r="AF41" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AG39" s="2" t="s">
+      <c r="AG41" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AH39" s="2" t="s">
+      <c r="AH41" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AI39" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AJ39" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="40" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A40" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="I40" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="J40" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="K40" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="L40" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="M40" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="N40" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="O40" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="P40" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q40" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="R40" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="S40" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="T40" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="U40" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="V40" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="W40" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="X40" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y40" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="Z40" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="AA40" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB40" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="AC40" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AD40" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AE40" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AF40" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AG40" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AH40" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI40" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AJ40" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="41" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A41" s="11" t="s">
-        <v>193</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="I41" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="J41" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="K41" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="L41" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="M41" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="N41" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="O41" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="P41" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q41" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="R41" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="S41" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="T41" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="U41" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="V41" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="W41" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="X41" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y41" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="Z41" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="AA41" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AB41" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AC41" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AD41" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="AE41" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="AF41" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AG41" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AH41" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="AI41" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="AJ41" s="1" t="s">
-        <v>75</v>
+      <c r="AJ41" s="3" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="42" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A42" s="11" t="s">
-        <v>194</v>
+        <v>31</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>194</v>
+        <v>12</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>194</v>
+        <v>12</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="L42" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="M42" s="3" t="s">
         <v>63</v>
@@ -5666,76 +5672,76 @@
       <c r="N42" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="O42" s="1" t="s">
-        <v>87</v>
+      <c r="O42" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="P42" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q42" s="3" t="s">
-        <v>63</v>
+        <v>32</v>
+      </c>
+      <c r="Q42" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="R42" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="S42" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="T42" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="U42" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="V42" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="W42" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="X42" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="Y42" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="Z42" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AA42" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AB42" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AC42" s="3" t="s">
-        <v>63</v>
+        <v>32</v>
+      </c>
+      <c r="S42" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="T42" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="U42" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="V42" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="W42" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="X42" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y42" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z42" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA42" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB42" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="AC42" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="AD42" s="2" t="s">
-        <v>194</v>
+        <v>32</v>
       </c>
       <c r="AE42" s="2" t="s">
-        <v>194</v>
+        <v>32</v>
       </c>
       <c r="AF42" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="AG42" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AH42" s="3" t="s">
-        <v>63</v>
+      <c r="AG42" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH42" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="AI42" s="3" t="s">
         <v>63</v>
       </c>
       <c r="AJ42" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
     </row>
     <row r="43" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A43" s="11" t="s">
-        <v>32</v>
+        <v>193</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>75</v>
@@ -5744,10 +5750,10 @@
         <v>75</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>32</v>
+        <v>194</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>32</v>
+        <v>194</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>75</v>
@@ -5786,7 +5792,7 @@
         <v>32</v>
       </c>
       <c r="R43" s="2" t="s">
-        <v>32</v>
+        <v>194</v>
       </c>
       <c r="S43" s="2" t="s">
         <v>32</v>
@@ -5818,14 +5824,14 @@
       <c r="AB43" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AC43" s="2" t="s">
-        <v>23</v>
+      <c r="AC43" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="AD43" s="2" t="s">
-        <v>32</v>
+        <v>194</v>
       </c>
       <c r="AE43" s="2" t="s">
-        <v>32</v>
+        <v>194</v>
       </c>
       <c r="AF43" s="2" t="s">
         <v>32</v>
@@ -5843,601 +5849,601 @@
         <v>75</v>
       </c>
     </row>
-    <row r="44" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A44" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="M44" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="N44" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="O44" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="P44" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q44" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="R44" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="S44" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="T44" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="U44" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="V44" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="W44" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="X44" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="Y44" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z44" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA44" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB44" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC44" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD44" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="AE44" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="AF44" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AG44" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH44" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI44" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ44" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="45" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A45" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="L45" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="M45" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="N45" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="O45" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="H44" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="I44" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="J44" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="K44" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="L44" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="M44" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="N44" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="O44" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="P44" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q44" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="R44" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="S44" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="T44" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="U44" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="V44" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="W44" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="X44" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="Y44" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z44" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="AA44" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="AB44" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="AC44" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="AD44" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="AE44" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="AF44" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="AG44" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="AH44" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="AI44" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AJ44" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="45" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A45" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="I45" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="J45" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="K45" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="L45" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="M45" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="N45" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="O45" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="P45" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Q45" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="R45" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="S45" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="T45" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="T45" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="U45" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="V45" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="W45" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="X45" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="Y45" s="1" t="s">
-        <v>94</v>
+        <v>75</v>
+      </c>
+      <c r="V45" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="W45" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="X45" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y45" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="Z45" s="1" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="AA45" s="2" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="AB45" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="AC45" s="3" t="s">
-        <v>63</v>
+        <v>32</v>
+      </c>
+      <c r="AC45" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="AD45" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AE45" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="AF45" s="3" t="s">
-        <v>63</v>
+        <v>32</v>
+      </c>
+      <c r="AF45" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="AG45" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AH45" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AI45" s="3" t="s">
         <v>63</v>
       </c>
       <c r="AJ45" s="1" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
     </row>
     <row r="46" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A46" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="L46" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="M46" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="N46" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="O46" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="P46" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q46" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="R46" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="S46" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="T46" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="U46" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="V46" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="W46" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="X46" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y46" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z46" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA46" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB46" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC46" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD46" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE46" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AF46" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG46" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AH46" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI46" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ46" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="47" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A47" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="L47" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="M47" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N47" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="O47" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P47" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q47" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="R47" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="S47" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="T47" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="U47" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="V47" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="W47" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="X47" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y47" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="Z47" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AA47" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB47" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC47" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD47" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE47" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AF47" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AG47" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AH47" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI47" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ47" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="48" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A48" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B48" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C48" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="D48" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E46" s="2" t="s">
+      <c r="E48" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F46" s="1" t="s">
+      <c r="F48" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="G46" s="1" t="s">
+      <c r="G48" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="H46" s="1" t="s">
+      <c r="H48" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="I46" s="1" t="s">
+      <c r="I48" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="J46" s="1" t="s">
+      <c r="J48" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="K46" s="1" t="s">
+      <c r="K48" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="L46" s="1" t="s">
+      <c r="L48" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="M46" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="N46" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="O46" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="P46" s="2" t="s">
+      <c r="M48" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="N48" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="O48" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="P48" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="Q46" s="2" t="s">
+      <c r="Q48" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="R46" s="2" t="s">
+      <c r="R48" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="S46" s="2" t="s">
+      <c r="S48" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="T46" s="1" t="s">
+      <c r="T48" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="U46" s="1" t="s">
+      <c r="U48" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="V46" s="1" t="s">
+      <c r="V48" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="W46" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="X46" s="2" t="s">
+      <c r="W48" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="X48" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="Y46" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="Z46" s="1" t="s">
+      <c r="Y48" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z48" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="AA46" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AB46" s="2" t="s">
+      <c r="AA48" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB48" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AC46" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AD46" s="2" t="s">
+      <c r="AC48" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD48" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AE46" s="2" t="s">
+      <c r="AE48" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AF46" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AG46" s="2" t="s">
+      <c r="AF48" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AG48" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AH46" s="2" t="s">
+      <c r="AH48" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AI46" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AJ46" s="1" t="s">
+      <c r="AI48" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ48" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="47" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A47" s="12" t="s">
+    <row r="49" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A49" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="B47" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D47" s="2" t="s">
+      <c r="B49" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D49" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E47" s="2" t="s">
+      <c r="E49" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="F47" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G47" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="H47" s="1" t="s">
+      <c r="F49" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H49" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="I47" s="1" t="s">
+      <c r="I49" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="J47" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="K47" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="L47" s="2" t="s">
+      <c r="J49" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="K49" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="L49" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="M47" s="2" t="s">
+      <c r="M49" s="2" t="s">
         <v>115</v>
-      </c>
-      <c r="N47" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="O47" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="P47" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="Q47" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="R47" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="S47" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="T47" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="U47" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="V47" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="W47" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="X47" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y47" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="Z47" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AA47" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AB47" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="AC47" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AD47" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="AE47" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="AF47" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AG47" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="AH47" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="AI47" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AJ47" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="48" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A48" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="H48" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="I48" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="J48" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="K48" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="L48" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="M48" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="N48" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="O48" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="P48" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q48" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="R48" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="S48" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="T48" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="U48" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="V48" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="W48" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="X48" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="Y48" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="Z48" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="AA48" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AB48" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="AC48" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AD48" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AE48" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AF48" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AG48" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AH48" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AI48" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AJ48" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="49" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A49" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="H49" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="I49" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="J49" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="K49" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="L49" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="M49" s="3" t="s">
-        <v>63</v>
       </c>
       <c r="N49" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="O49" s="1" t="s">
-        <v>75</v>
+      <c r="O49" s="2" t="s">
+        <v>114</v>
       </c>
       <c r="P49" s="2" t="s">
         <v>114</v>
@@ -6451,14 +6457,14 @@
       <c r="S49" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="T49" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="U49" s="1" t="s">
-        <v>75</v>
+      <c r="T49" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="U49" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="V49" s="2" t="s">
-        <v>114</v>
+        <v>25</v>
       </c>
       <c r="W49" s="2" t="s">
         <v>114</v>
@@ -6469,8 +6475,8 @@
       <c r="Y49" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="Z49" s="1" t="s">
-        <v>75</v>
+      <c r="Z49" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="AA49" s="2" t="s">
         <v>21</v>
@@ -6482,13 +6488,13 @@
         <v>63</v>
       </c>
       <c r="AD49" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="AE49" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="AF49" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
+      </c>
+      <c r="AF49" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="AG49" s="2" t="s">
         <v>114</v>
@@ -6499,227 +6505,447 @@
       <c r="AI49" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="AJ49" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="50" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="AJ49" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="50" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A50" s="11" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>11</v>
+        <v>113</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G50" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="H50" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="I50" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="J50" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="K50" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="L50" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="M50" s="2" t="s">
-        <v>11</v>
+        <v>113</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="K50" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="L50" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="M50" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="N50" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="O50" s="3" t="s">
-        <v>63</v>
+        <v>12</v>
+      </c>
+      <c r="O50" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="P50" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q50" s="2" t="s">
-        <v>11</v>
+        <v>19</v>
+      </c>
+      <c r="Q50" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="R50" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="S50" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="T50" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="U50" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="V50" s="3" t="s">
-        <v>63</v>
+        <v>13</v>
+      </c>
+      <c r="S50" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="T50" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="U50" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="V50" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="W50" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="X50" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y50" s="3" t="s">
-        <v>63</v>
+      <c r="X50" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="Y50" s="2" t="s">
+        <v>86</v>
       </c>
       <c r="Z50" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="AA50" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
+      </c>
+      <c r="AA50" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="AB50" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC50" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AD50" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AE50" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AF50" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AG50" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AH50" s="2" t="s">
-        <v>11</v>
+        <v>86</v>
+      </c>
+      <c r="AC50" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD50" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE50" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF50" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AG50" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH50" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="AI50" s="3" t="s">
         <v>63</v>
       </c>
       <c r="AJ50" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="51" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A51" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J51" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="L51" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="M51" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="N51" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="O51" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="P51" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q51" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="R51" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="S51" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="T51" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="U51" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="V51" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="W51" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="X51" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y51" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z51" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA51" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB51" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AC51" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD51" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AE51" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AF51" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AG51" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AH51" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AI51" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ51" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="52" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A52" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H52" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I52" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J52" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="K52" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="L52" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M52" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N52" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O52" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="P52" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q52" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="R52" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="S52" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="T52" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="U52" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="V52" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="W52" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="X52" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y52" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z52" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AA52" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB52" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC52" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD52" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE52" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF52" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AG52" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AH52" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AI52" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ52" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="53" spans="1:36" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A53" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D51" s="2" t="s">
+      <c r="B53" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D53" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E51" s="2" t="s">
+      <c r="E53" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="F51" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="H51" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="I51" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="J51" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="K51" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="L51" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="M51" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="N51" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="O51" s="2" t="s">
+      <c r="F53" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J53" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K53" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="L53" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="M53" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="N53" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="O53" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="P51" s="2" t="s">
+      <c r="P53" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Q51" s="2" t="s">
+      <c r="Q53" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="R51" s="2" t="s">
+      <c r="R53" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="S51" s="2" t="s">
+      <c r="S53" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="T51" s="2" t="s">
+      <c r="T53" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="U51" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="V51" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="W51" s="2" t="s">
+      <c r="U53" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="V53" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="W53" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="X51" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y51" s="2" t="s">
+      <c r="X53" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y53" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Z51" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="AA51" s="2" t="s">
+      <c r="Z53" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA53" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AB51" s="2" t="s">
+      <c r="AB53" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AC51" s="2" t="s">
+      <c r="AC53" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AD51" s="2" t="s">
+      <c r="AD53" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AE51" s="2" t="s">
+      <c r="AE53" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AF51" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AG51" s="2" t="s">
+      <c r="AF53" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AG53" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AH51" s="2" t="s">
+      <c r="AH53" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AI51" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AJ51" s="1" t="s">
+      <c r="AI53" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ53" s="1" t="s">
         <v>75</v>
       </c>
     </row>

</xml_diff>

<commit_message>
FEAT: make comments first-class in lexer.
Will allow extracting comments from input.
</commit_message>
<xml_diff>
--- a/docs/lexer/lexer-FSM.xlsx
+++ b/docs/lexer/lexer-FSM.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Red\docs\lexer\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9583133C-4400-432C-806B-CB720071809A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="564" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="564"/>
   </bookViews>
   <sheets>
     <sheet name="transitions" sheetId="3" r:id="rId1"/>
@@ -22,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2712" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2712" uniqueCount="203">
   <si>
     <t>S_START</t>
   </si>
@@ -628,12 +622,15 @@
   </si>
   <si>
     <t>T_HEX</t>
+  </si>
+  <si>
+    <t>T_CMT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -877,7 +874,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -910,26 +907,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -962,23 +942,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1154,23 +1117,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1:AG1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.73046875" customWidth="1"/>
-    <col min="5" max="5" width="9.73046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="12" width="9.73046875" customWidth="1"/>
-    <col min="13" max="13" width="9.9296875" bestFit="1" customWidth="1"/>
-    <col min="14" max="39" width="9.73046875" customWidth="1"/>
+    <col min="1" max="1" width="10.36328125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" customWidth="1"/>
+    <col min="5" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="9.7265625" customWidth="1"/>
+    <col min="13" max="13" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="39" width="9.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:39" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -1290,7 +1253,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
@@ -1409,15 +1372,15 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
         <v>68</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>0</v>
+      <c r="C3" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>68</v>
@@ -1528,7 +1491,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A4" s="11" t="s">
         <v>69</v>
       </c>
@@ -1647,7 +1610,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -1766,7 +1729,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A6" s="12" t="s">
         <v>2</v>
       </c>
@@ -1885,7 +1848,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A7" s="11" t="s">
         <v>73</v>
       </c>
@@ -2004,7 +1967,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A8" s="11" t="s">
         <v>3</v>
       </c>
@@ -2123,7 +2086,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A9" s="11" t="s">
         <v>4</v>
       </c>
@@ -2242,7 +2205,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A10" s="11" t="s">
         <v>107</v>
       </c>
@@ -2361,7 +2324,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A11" s="11" t="s">
         <v>108</v>
       </c>
@@ -2480,7 +2443,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A12" s="11" t="s">
         <v>109</v>
       </c>
@@ -2599,7 +2562,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A13" s="11" t="s">
         <v>5</v>
       </c>
@@ -2718,7 +2681,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A14" s="11" t="s">
         <v>6</v>
       </c>
@@ -2837,7 +2800,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A15" s="11" t="s">
         <v>7</v>
       </c>
@@ -2956,7 +2919,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A16" s="11" t="s">
         <v>70</v>
       </c>
@@ -3075,7 +3038,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A17" s="11" t="s">
         <v>8</v>
       </c>
@@ -3194,7 +3157,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A18" s="11" t="s">
         <v>9</v>
       </c>
@@ -3313,7 +3276,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A19" s="11" t="s">
         <v>10</v>
       </c>
@@ -3432,7 +3395,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A20" s="11" t="s">
         <v>11</v>
       </c>
@@ -3551,7 +3514,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A21" s="11" t="s">
         <v>12</v>
       </c>
@@ -3670,7 +3633,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A22" s="11" t="s">
         <v>84</v>
       </c>
@@ -3789,7 +3752,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A23" s="11" t="s">
         <v>13</v>
       </c>
@@ -3908,7 +3871,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A24" s="11" t="s">
         <v>194</v>
       </c>
@@ -4027,7 +3990,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A25" s="11" t="s">
         <v>14</v>
       </c>
@@ -4146,7 +4109,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A26" s="11" t="s">
         <v>15</v>
       </c>
@@ -4265,7 +4228,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A27" s="11" t="s">
         <v>16</v>
       </c>
@@ -4384,7 +4347,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="28" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A28" s="11" t="s">
         <v>17</v>
       </c>
@@ -4503,7 +4466,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A29" s="11" t="s">
         <v>18</v>
       </c>
@@ -4622,7 +4585,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="30" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A30" s="11" t="s">
         <v>19</v>
       </c>
@@ -4741,7 +4704,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A31" s="11" t="s">
         <v>20</v>
       </c>
@@ -4860,7 +4823,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="32" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A32" s="11" t="s">
         <v>22</v>
       </c>
@@ -4979,7 +4942,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A33" s="11" t="s">
         <v>23</v>
       </c>
@@ -5098,7 +5061,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="34" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A34" s="11" t="s">
         <v>24</v>
       </c>
@@ -5217,7 +5180,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="35" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A35" s="11" t="s">
         <v>195</v>
       </c>
@@ -5336,7 +5299,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="36" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A36" s="11" t="s">
         <v>25</v>
       </c>
@@ -5455,7 +5418,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="37" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A37" s="11" t="s">
         <v>26</v>
       </c>
@@ -5574,7 +5537,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="38" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A38" s="11" t="s">
         <v>27</v>
       </c>
@@ -5693,7 +5656,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="39" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A39" s="11" t="s">
         <v>28</v>
       </c>
@@ -5812,7 +5775,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A40" s="11" t="s">
         <v>29</v>
       </c>
@@ -5931,7 +5894,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="41" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A41" s="11" t="s">
         <v>30</v>
       </c>
@@ -6050,7 +6013,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="42" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A42" s="11" t="s">
         <v>31</v>
       </c>
@@ -6169,7 +6132,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="43" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A43" s="11" t="s">
         <v>191</v>
       </c>
@@ -6288,7 +6251,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="44" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A44" s="11" t="s">
         <v>192</v>
       </c>
@@ -6407,7 +6370,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A45" s="11" t="s">
         <v>32</v>
       </c>
@@ -6526,7 +6489,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="46" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A46" s="11" t="s">
         <v>94</v>
       </c>
@@ -6645,7 +6608,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="47" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A47" s="11" t="s">
         <v>33</v>
       </c>
@@ -6764,7 +6727,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="48" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A48" s="11" t="s">
         <v>21</v>
       </c>
@@ -6883,7 +6846,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="49" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A49" s="12" t="s">
         <v>110</v>
       </c>
@@ -7002,7 +6965,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="50" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A50" s="11" t="s">
         <v>111</v>
       </c>
@@ -7121,7 +7084,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="51" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A51" s="11" t="s">
         <v>112</v>
       </c>
@@ -7240,7 +7203,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="52" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A52" s="11" t="s">
         <v>113</v>
       </c>
@@ -7359,7 +7322,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="53" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A53" s="11" t="s">
         <v>114</v>
       </c>
@@ -7485,20 +7448,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M48"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.19921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -7540,7 +7503,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A2" s="12" t="s">
         <v>126</v>
       </c>
@@ -7581,7 +7544,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A3" s="11" t="s">
         <v>127</v>
       </c>
@@ -7622,7 +7585,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A4" s="11" t="s">
         <v>128</v>
       </c>
@@ -7663,7 +7626,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A5" s="11" t="s">
         <v>129</v>
       </c>
@@ -7704,7 +7667,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A6" s="11" t="s">
         <v>177</v>
       </c>
@@ -7745,7 +7708,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A7" s="15" t="s">
         <v>130</v>
       </c>
@@ -7786,7 +7749,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A8" s="15" t="s">
         <v>152</v>
       </c>
@@ -7827,7 +7790,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A9" s="15" t="s">
         <v>131</v>
       </c>
@@ -7868,7 +7831,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A10" s="14" t="s">
         <v>132</v>
       </c>
@@ -7909,7 +7872,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A11" s="14" t="s">
         <v>133</v>
       </c>
@@ -7950,7 +7913,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A12" s="14" t="s">
         <v>184</v>
       </c>
@@ -7991,7 +7954,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A13" s="14" t="s">
         <v>185</v>
       </c>
@@ -8032,7 +7995,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A14" s="15" t="s">
         <v>134</v>
       </c>
@@ -8073,7 +8036,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A15" s="15" t="s">
         <v>135</v>
       </c>
@@ -8114,7 +8077,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A16" s="14" t="s">
         <v>136</v>
       </c>
@@ -8155,7 +8118,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A17" s="14" t="s">
         <v>137</v>
       </c>
@@ -8196,7 +8159,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A18" s="14" t="s">
         <v>138</v>
       </c>
@@ -8237,7 +8200,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A19" s="14" t="s">
         <v>188</v>
       </c>
@@ -8278,7 +8241,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A20" s="14" t="s">
         <v>139</v>
       </c>
@@ -8319,7 +8282,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A21" s="14" t="s">
         <v>140</v>
       </c>
@@ -8360,7 +8323,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A22" s="15" t="s">
         <v>154</v>
       </c>
@@ -8401,7 +8364,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A23" s="15" t="s">
         <v>155</v>
       </c>
@@ -8442,7 +8405,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A24" s="14" t="s">
         <v>141</v>
       </c>
@@ -8483,7 +8446,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A25" s="14" t="s">
         <v>142</v>
       </c>
@@ -8524,7 +8487,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A26" s="15" t="s">
         <v>143</v>
       </c>
@@ -8565,7 +8528,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A27" s="14" t="s">
         <v>144</v>
       </c>
@@ -8606,7 +8569,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A28" s="15" t="s">
         <v>156</v>
       </c>
@@ -8647,7 +8610,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A29" s="15" t="s">
         <v>157</v>
       </c>
@@ -8688,7 +8651,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A30" s="15" t="s">
         <v>158</v>
       </c>
@@ -8729,7 +8692,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A31" s="15" t="s">
         <v>159</v>
       </c>
@@ -8770,7 +8733,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A32" s="12" t="s">
         <v>145</v>
       </c>
@@ -8811,7 +8774,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A33" s="14" t="s">
         <v>160</v>
       </c>
@@ -8852,7 +8815,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A34" s="15" t="s">
         <v>146</v>
       </c>
@@ -8893,7 +8856,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A35" s="14" t="s">
         <v>161</v>
       </c>
@@ -8934,7 +8897,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A36" s="15" t="s">
         <v>162</v>
       </c>
@@ -8975,7 +8938,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A37" s="14" t="s">
         <v>147</v>
       </c>
@@ -9016,7 +8979,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A38" s="15" t="s">
         <v>163</v>
       </c>
@@ -9057,7 +9020,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A39" s="14" t="s">
         <v>164</v>
       </c>
@@ -9098,7 +9061,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A40" s="15" t="s">
         <v>148</v>
       </c>
@@ -9139,7 +9102,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A41" s="14" t="s">
         <v>165</v>
       </c>
@@ -9180,7 +9143,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A42" s="14" t="s">
         <v>166</v>
       </c>
@@ -9221,7 +9184,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A43" s="14" t="s">
         <v>183</v>
       </c>
@@ -9262,7 +9225,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A44" s="14" t="s">
         <v>149</v>
       </c>
@@ -9303,7 +9266,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A45" s="15" t="s">
         <v>150</v>
       </c>
@@ -9344,7 +9307,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A46" s="15" t="s">
         <v>168</v>
       </c>
@@ -9474,19 +9437,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.9296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.06640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.19921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -9507,7 +9470,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
         <v>102</v>
       </c>
@@ -9527,7 +9490,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A3" s="5" t="s">
         <v>101</v>
       </c>
@@ -9547,7 +9510,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A4" s="5" t="s">
         <v>105</v>
       </c>
@@ -9567,7 +9530,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A5" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FIX: eE lexical classes were excluded from encoded hexa values in files.
</commit_message>
<xml_diff>
--- a/docs/lexer/lexer-FSM.xlsx
+++ b/docs/lexer/lexer-FSM.xlsx
@@ -1122,7 +1122,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomLeft" activeCell="S36" sqref="S36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2205,7 +2205,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
         <v>107</v>
       </c>
@@ -2260,11 +2260,11 @@
       <c r="R10" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="S10" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="T10" s="3" t="s">
-        <v>62</v>
+      <c r="S10" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="T10" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="U10" s="2" t="s">
         <v>108</v>
@@ -2324,7 +2324,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
         <v>108</v>
       </c>
@@ -2379,11 +2379,11 @@
       <c r="R11" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="S11" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="T11" s="3" t="s">
-        <v>62</v>
+      <c r="S11" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="T11" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="U11" s="2" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
FEAT: proper support for words starting with <, like << and <=
</commit_message>
<xml_diff>
--- a/docs/lexer/lexer-FSM.xlsx
+++ b/docs/lexer/lexer-FSM.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Red\docs\lexer\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{276A0501-51D9-4FCF-804F-3C672F966E7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="564"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="564" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="transitions" sheetId="3" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2712" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2765" uniqueCount="204">
   <si>
     <t>S_START</t>
   </si>
@@ -625,12 +631,15 @@
   </si>
   <si>
     <t>T_CMT</t>
+  </si>
+  <si>
+    <t>C_EQUAL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -874,7 +883,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -907,9 +916,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -942,6 +968,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1117,26 +1160,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM53"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AN53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S36" sqref="S36"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AA37" sqref="AA37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.36328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" customWidth="1"/>
-    <col min="5" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="12" width="9.7265625" customWidth="1"/>
-    <col min="13" max="13" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="14" max="39" width="9.7265625" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.73046875" customWidth="1"/>
+    <col min="5" max="5" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="9.73046875" customWidth="1"/>
+    <col min="13" max="13" width="9.9296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="40" width="9.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:40" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="7"/>
       <c r="B1" s="6" t="s">
         <v>37</v>
@@ -1214,46 +1257,49 @@
         <v>51</v>
       </c>
       <c r="AA1" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="AB1" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="AB1" s="6" t="s">
+      <c r="AC1" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="AC1" s="6" t="s">
+      <c r="AD1" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="AD1" s="6" t="s">
+      <c r="AE1" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="AE1" s="6" t="s">
+      <c r="AF1" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="AF1" s="6" t="s">
+      <c r="AG1" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="AG1" s="6" t="s">
+      <c r="AH1" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="AH1" s="6" t="s">
+      <c r="AI1" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="AI1" s="6" t="s">
+      <c r="AJ1" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="AJ1" s="6" t="s">
+      <c r="AK1" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="AK1" s="6" t="s">
+      <c r="AL1" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="AL1" s="6" t="s">
+      <c r="AM1" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="AM1" s="6" t="s">
+      <c r="AN1" s="6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
@@ -1333,46 +1379,49 @@
         <v>32</v>
       </c>
       <c r="AA2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="AB2" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AC2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD2" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="AD2" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE2" s="2" t="s">
+      <c r="AE2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF2" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="AF2" s="2" t="s">
+      <c r="AG2" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="AG2" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="AH2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AI2" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AJ2" s="2" t="s">
-        <v>32</v>
+      <c r="AI2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AJ2" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="AK2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AL2" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM2" s="1" t="s">
+      <c r="AL2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AM2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN2" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A3" s="11" t="s">
         <v>68</v>
       </c>
@@ -1484,14 +1533,17 @@
       <c r="AK3" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="AL3" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM3" s="1" t="s">
+      <c r="AL3" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AM3" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN3" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A4" s="11" t="s">
         <v>69</v>
       </c>
@@ -1595,22 +1647,25 @@
         <v>69</v>
       </c>
       <c r="AI4" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AJ4" s="2" t="s">
         <v>1</v>
-      </c>
-      <c r="AJ4" s="2" t="s">
-        <v>69</v>
       </c>
       <c r="AK4" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="AL4" s="3" t="s">
-        <v>62</v>
+      <c r="AL4" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="AM4" s="3" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="5" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="AN4" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -1722,14 +1777,17 @@
       <c r="AK5" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="AL5" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM5" s="1" t="s">
+      <c r="AL5" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AM5" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN5" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A6" s="12" t="s">
         <v>2</v>
       </c>
@@ -1833,22 +1891,25 @@
         <v>2</v>
       </c>
       <c r="AI6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ6" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="AJ6" s="2" t="s">
-        <v>2</v>
       </c>
       <c r="AK6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="AL6" s="3" t="s">
-        <v>62</v>
+      <c r="AL6" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="AM6" s="3" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="7" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="AN6" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A7" s="11" t="s">
         <v>73</v>
       </c>
@@ -1960,14 +2021,17 @@
       <c r="AK7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="AL7" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM7" s="1" t="s">
+      <c r="AL7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AM7" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN7" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A8" s="11" t="s">
         <v>3</v>
       </c>
@@ -2052,14 +2116,14 @@
       <c r="AB8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="AC8" s="1" t="s">
-        <v>74</v>
+      <c r="AC8" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="AD8" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="AE8" s="2" t="s">
-        <v>4</v>
+      <c r="AE8" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="AF8" s="2" t="s">
         <v>4</v>
@@ -2079,14 +2143,17 @@
       <c r="AK8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="AL8" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM8" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="9" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="AL8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AM8" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN8" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A9" s="11" t="s">
         <v>4</v>
       </c>
@@ -2166,19 +2233,19 @@
         <v>4</v>
       </c>
       <c r="AA9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB9" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="AB9" s="2" t="s">
+      <c r="AC9" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="AC9" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="AD9" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="AE9" s="2" t="s">
-        <v>4</v>
+      <c r="AE9" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="AF9" s="2" t="s">
         <v>4</v>
@@ -2198,14 +2265,17 @@
       <c r="AK9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="AL9" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM9" s="1" t="s">
+      <c r="AL9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AM9" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN9" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A10" s="11" t="s">
         <v>107</v>
       </c>
@@ -2323,8 +2393,11 @@
       <c r="AM10" s="3" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.35">
+      <c r="AN10" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A11" s="11" t="s">
         <v>108</v>
       </c>
@@ -2439,11 +2512,14 @@
       <c r="AL11" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AM11" s="1" t="s">
+      <c r="AM11" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN11" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A12" s="11" t="s">
         <v>109</v>
       </c>
@@ -2555,14 +2631,17 @@
       <c r="AK12" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="AL12" s="3" t="s">
-        <v>62</v>
+      <c r="AL12" s="2" t="s">
+        <v>109</v>
       </c>
       <c r="AM12" s="3" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="13" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="AN12" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A13" s="11" t="s">
         <v>5</v>
       </c>
@@ -2647,14 +2726,14 @@
       <c r="AB13" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="AC13" s="1" t="s">
-        <v>76</v>
+      <c r="AC13" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="AD13" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="AE13" s="2" t="s">
-        <v>5</v>
+      <c r="AE13" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="AF13" s="2" t="s">
         <v>5</v>
@@ -2674,14 +2753,17 @@
       <c r="AK13" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="AL13" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM13" s="1" t="s">
+      <c r="AL13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AM13" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN13" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A14" s="11" t="s">
         <v>6</v>
       </c>
@@ -2760,20 +2842,20 @@
       <c r="Z14" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AA14" s="2" t="s">
+      <c r="AA14" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="AB14" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC14" s="1" t="s">
-        <v>81</v>
+      <c r="AC14" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="AD14" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="AE14" s="2" t="s">
-        <v>11</v>
+      <c r="AE14" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="AF14" s="2" t="s">
         <v>11</v>
@@ -2793,14 +2875,17 @@
       <c r="AK14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="AL14" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM14" s="1" t="s">
+      <c r="AL14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AM14" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN14" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A15" s="11" t="s">
         <v>7</v>
       </c>
@@ -2885,12 +2970,12 @@
       <c r="AB15" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AC15" s="2" t="s">
+      <c r="AC15" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD15" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="AD15" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="AE15" s="3" t="s">
         <v>62</v>
       </c>
@@ -2909,17 +2994,20 @@
       <c r="AJ15" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AK15" s="2" t="s">
+      <c r="AK15" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AL15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="AL15" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="AM15" s="3" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="16" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="AN15" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A16" s="11" t="s">
         <v>70</v>
       </c>
@@ -3031,14 +3119,17 @@
       <c r="AK16" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="AL16" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM16" s="1" t="s">
+      <c r="AL16" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AM16" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN16" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A17" s="11" t="s">
         <v>8</v>
       </c>
@@ -3142,22 +3233,25 @@
         <v>8</v>
       </c>
       <c r="AI17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AJ17" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="AJ17" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="AK17" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="AL17" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM17" s="1" t="s">
+      <c r="AL17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AM17" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN17" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A18" s="11" t="s">
         <v>9</v>
       </c>
@@ -3269,14 +3363,17 @@
       <c r="AK18" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="AL18" s="3" t="s">
-        <v>62</v>
+      <c r="AL18" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="AM18" s="3" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="19" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="AN18" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A19" s="11" t="s">
         <v>10</v>
       </c>
@@ -3388,14 +3485,17 @@
       <c r="AK19" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="AL19" s="3" t="s">
-        <v>62</v>
+      <c r="AL19" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="AM19" s="3" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="20" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="AN19" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A20" s="11" t="s">
         <v>11</v>
       </c>
@@ -3480,14 +3580,14 @@
       <c r="AB20" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="AC20" s="1" t="s">
-        <v>81</v>
+      <c r="AC20" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="AD20" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="AE20" s="2" t="s">
-        <v>11</v>
+      <c r="AE20" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="AF20" s="2" t="s">
         <v>11</v>
@@ -3507,14 +3607,17 @@
       <c r="AK20" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="AL20" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM20" s="1" t="s">
+      <c r="AL20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AM20" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN20" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A21" s="11" t="s">
         <v>12</v>
       </c>
@@ -3593,33 +3696,33 @@
       <c r="Z21" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AA21" s="1" t="s">
+      <c r="AA21" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB21" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="AB21" s="2" t="s">
+      <c r="AC21" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="AC21" s="1" t="s">
+      <c r="AD21" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="AD21" s="2" t="s">
+      <c r="AE21" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AE21" s="2" t="s">
+      <c r="AF21" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="AF21" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="AG21" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AH21" s="2" t="s">
+      <c r="AH21" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AI21" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="AI21" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="AJ21" s="3" t="s">
         <v>62</v>
       </c>
@@ -3629,11 +3732,14 @@
       <c r="AL21" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AM21" s="1" t="s">
+      <c r="AM21" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN21" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="22" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A22" s="11" t="s">
         <v>84</v>
       </c>
@@ -3712,18 +3818,18 @@
       <c r="Z22" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AA22" s="1" t="s">
+      <c r="AA22" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB22" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="AB22" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC22" s="1" t="s">
+      <c r="AC22" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD22" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="AD22" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="AE22" s="3" t="s">
         <v>62</v>
       </c>
@@ -3748,11 +3854,14 @@
       <c r="AL22" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AM22" s="1" t="s">
+      <c r="AM22" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN22" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A23" s="11" t="s">
         <v>13</v>
       </c>
@@ -3831,32 +3940,32 @@
       <c r="Z23" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AA23" s="1" t="s">
+      <c r="AA23" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB23" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="AB23" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="AC23" s="3" t="s">
         <v>62</v>
       </c>
       <c r="AD23" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AE23" s="2" t="s">
+      <c r="AE23" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF23" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="AF23" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AG23" s="2" t="s">
-        <v>13</v>
+      <c r="AG23" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="AH23" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="AI23" s="3" t="s">
-        <v>62</v>
+      <c r="AI23" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="AJ23" s="3" t="s">
         <v>62</v>
@@ -3867,11 +3976,14 @@
       <c r="AL23" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AM23" s="1" t="s">
+      <c r="AM23" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN23" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A24" s="11" t="s">
         <v>194</v>
       </c>
@@ -3950,32 +4062,32 @@
       <c r="Z24" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AA24" s="1" t="s">
+      <c r="AA24" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB24" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="AB24" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="AC24" s="3" t="s">
         <v>62</v>
       </c>
       <c r="AD24" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AE24" s="2" t="s">
+      <c r="AE24" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF24" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="AF24" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AG24" s="2" t="s">
-        <v>13</v>
+      <c r="AG24" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="AH24" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="AI24" s="3" t="s">
-        <v>62</v>
+      <c r="AI24" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="AJ24" s="3" t="s">
         <v>62</v>
@@ -3986,11 +4098,14 @@
       <c r="AL24" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AM24" s="1" t="s">
+      <c r="AM24" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN24" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A25" s="11" t="s">
         <v>14</v>
       </c>
@@ -4069,8 +4184,8 @@
       <c r="Z25" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="AA25" s="1" t="s">
-        <v>193</v>
+      <c r="AA25" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="AB25" s="1" t="s">
         <v>193</v>
@@ -4081,35 +4196,38 @@
       <c r="AD25" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="AE25" s="2" t="s">
+      <c r="AE25" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="AF25" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="AF25" s="1" t="s">
+      <c r="AG25" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="AG25" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="AH25" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="AI25" s="1" t="s">
+      <c r="AI25" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AJ25" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="AJ25" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="AK25" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="AL25" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM25" s="1" t="s">
+      <c r="AL25" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AM25" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN25" s="1" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="26" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A26" s="11" t="s">
         <v>15</v>
       </c>
@@ -4200,12 +4318,12 @@
       <c r="AD26" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AE26" s="2" t="s">
+      <c r="AE26" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF26" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="AF26" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="AG26" s="3" t="s">
         <v>62</v>
       </c>
@@ -4224,11 +4342,14 @@
       <c r="AL26" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AM26" s="1" t="s">
+      <c r="AM26" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN26" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A27" s="11" t="s">
         <v>16</v>
       </c>
@@ -4307,47 +4428,50 @@
       <c r="Z27" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="AA27" s="1" t="s">
+      <c r="AA27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB27" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="AB27" s="2" t="s">
+      <c r="AC27" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="AC27" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="AD27" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="AE27" s="2" t="s">
+      <c r="AE27" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AF27" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="AF27" s="1" t="s">
+      <c r="AG27" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="AG27" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="AH27" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="AI27" s="1" t="s">
+      <c r="AI27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AJ27" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="AJ27" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AK27" s="2" t="s">
+      <c r="AK27" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AL27" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="AL27" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM27" s="1" t="s">
+      <c r="AM27" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN27" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="28" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A28" s="11" t="s">
         <v>17</v>
       </c>
@@ -4465,8 +4589,11 @@
       <c r="AM28" s="3" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="29" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="AN28" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A29" s="11" t="s">
         <v>18</v>
       </c>
@@ -4551,18 +4678,18 @@
       <c r="AB29" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AC29" s="1" t="s">
+      <c r="AC29" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD29" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="AD29" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE29" s="2" t="s">
+      <c r="AE29" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF29" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AF29" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="AG29" s="3" t="s">
         <v>62</v>
       </c>
@@ -4581,11 +4708,14 @@
       <c r="AL29" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AM29" s="1" t="s">
+      <c r="AM29" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN29" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="30" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A30" s="11" t="s">
         <v>19</v>
       </c>
@@ -4703,8 +4833,11 @@
       <c r="AM30" s="3" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="31" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="AN30" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A31" s="11" t="s">
         <v>20</v>
       </c>
@@ -4789,18 +4922,18 @@
       <c r="AB31" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AC31" s="1" t="s">
+      <c r="AC31" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD31" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="AD31" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE31" s="2" t="s">
+      <c r="AE31" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF31" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="AF31" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="AG31" s="3" t="s">
         <v>62</v>
       </c>
@@ -4819,11 +4952,14 @@
       <c r="AL31" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AM31" s="1" t="s">
+      <c r="AM31" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN31" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="32" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A32" s="11" t="s">
         <v>22</v>
       </c>
@@ -4941,8 +5077,11 @@
       <c r="AM32" s="3" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="33" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="AN32" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="33" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A33" s="11" t="s">
         <v>23</v>
       </c>
@@ -5027,18 +5166,18 @@
       <c r="AB33" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AC33" s="1" t="s">
+      <c r="AC33" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD33" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="AD33" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE33" s="2" t="s">
+      <c r="AE33" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF33" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="AF33" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="AG33" s="3" t="s">
         <v>62</v>
       </c>
@@ -5057,11 +5196,14 @@
       <c r="AL33" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AM33" s="1" t="s">
+      <c r="AM33" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN33" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="34" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A34" s="11" t="s">
         <v>24</v>
       </c>
@@ -5146,12 +5288,12 @@
       <c r="AB34" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AC34" s="1" t="s">
+      <c r="AC34" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD34" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="AD34" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="AE34" s="3" t="s">
         <v>62</v>
       </c>
@@ -5176,11 +5318,14 @@
       <c r="AL34" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AM34" s="1" t="s">
+      <c r="AM34" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN34" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="35" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A35" s="11" t="s">
         <v>195</v>
       </c>
@@ -5259,26 +5404,26 @@
       <c r="Z35" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AA35" s="3" t="s">
-        <v>62</v>
+      <c r="AA35" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="AB35" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AC35" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AD35" s="2" t="s">
+      <c r="AC35" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD35" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AE35" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AE35" s="2" t="s">
+      <c r="AF35" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AF35" s="2" t="s">
+      <c r="AG35" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="AG35" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="AH35" s="2" t="s">
         <v>32</v>
@@ -5292,14 +5437,17 @@
       <c r="AK35" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AL35" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM35" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="36" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="AL35" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AM35" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN35" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A36" s="11" t="s">
         <v>25</v>
       </c>
@@ -5372,26 +5520,26 @@
       <c r="X36" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="Y36" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="Z36" s="1" t="s">
-        <v>74</v>
+      <c r="Y36" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z36" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="AA36" s="2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="AB36" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AC36" s="1" t="s">
-        <v>74</v>
+      <c r="AC36" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="AD36" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="AE36" s="2" t="s">
-        <v>26</v>
+      <c r="AE36" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="AF36" s="2" t="s">
         <v>26</v>
@@ -5411,14 +5559,17 @@
       <c r="AK36" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AL36" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM36" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="37" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="AL36" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AM36" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN36" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="37" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A37" s="11" t="s">
         <v>26</v>
       </c>
@@ -5530,14 +5681,17 @@
       <c r="AK37" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AL37" s="3" t="s">
-        <v>62</v>
+      <c r="AL37" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="AM37" s="3" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="38" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="AN37" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A38" s="11" t="s">
         <v>27</v>
       </c>
@@ -5641,22 +5795,25 @@
         <v>27</v>
       </c>
       <c r="AI38" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AJ38" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="AJ38" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="AK38" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AL38" s="3" t="s">
-        <v>62</v>
+      <c r="AL38" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="AM38" s="3" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="39" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="AN38" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A39" s="11" t="s">
         <v>28</v>
       </c>
@@ -5768,14 +5925,17 @@
       <c r="AK39" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AL39" s="3" t="s">
-        <v>62</v>
+      <c r="AL39" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="AM39" s="3" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="40" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="AN39" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="40" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A40" s="11" t="s">
         <v>29</v>
       </c>
@@ -5887,14 +6047,17 @@
       <c r="AK40" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AL40" s="3" t="s">
-        <v>62</v>
+      <c r="AL40" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="AM40" s="3" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="41" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="AN40" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="41" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A41" s="11" t="s">
         <v>30</v>
       </c>
@@ -6006,14 +6169,17 @@
       <c r="AK41" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AL41" s="3" t="s">
-        <v>62</v>
+      <c r="AL41" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="AM41" s="3" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="42" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="AN41" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="42" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A42" s="11" t="s">
         <v>31</v>
       </c>
@@ -6092,23 +6258,23 @@
       <c r="Z42" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AA42" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AB42" s="2" t="s">
+      <c r="AA42" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AC42" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AD42" s="2" t="s">
+      <c r="AB42" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC42" s="2" t="s">
         <v>32</v>
       </c>
+      <c r="AD42" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="AE42" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF42" s="2" t="s">
         <v>191</v>
-      </c>
-      <c r="AF42" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="AG42" s="2" t="s">
         <v>32</v>
@@ -6116,23 +6282,26 @@
       <c r="AH42" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AI42" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AJ42" s="2" t="s">
+      <c r="AI42" s="2" t="s">
         <v>32</v>
+      </c>
+      <c r="AJ42" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="AK42" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AL42" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM42" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="43" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="AL42" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AM42" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN42" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="43" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A43" s="11" t="s">
         <v>191</v>
       </c>
@@ -6211,32 +6380,32 @@
       <c r="Z43" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AA43" s="3" t="s">
-        <v>62</v>
+      <c r="AA43" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="AB43" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AC43" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AD43" s="2" t="s">
+      <c r="AC43" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD43" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AE43" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AE43" s="2" t="s">
+      <c r="AF43" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AF43" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AG43" s="2" t="s">
-        <v>192</v>
+      <c r="AG43" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="AH43" s="2" t="s">
         <v>192</v>
       </c>
       <c r="AI43" s="2" t="s">
-        <v>32</v>
+        <v>192</v>
       </c>
       <c r="AJ43" s="2" t="s">
         <v>32</v>
@@ -6244,14 +6413,17 @@
       <c r="AK43" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AL43" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM43" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="44" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="AL43" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AM43" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN43" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="44" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A44" s="11" t="s">
         <v>192</v>
       </c>
@@ -6330,12 +6502,12 @@
       <c r="Z44" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AA44" s="1" t="s">
+      <c r="AA44" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB44" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="AB44" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="AC44" s="3" t="s">
         <v>62</v>
       </c>
@@ -6348,14 +6520,14 @@
       <c r="AF44" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AG44" s="2" t="s">
-        <v>192</v>
+      <c r="AG44" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="AH44" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="AI44" s="3" t="s">
-        <v>62</v>
+      <c r="AI44" s="2" t="s">
+        <v>192</v>
       </c>
       <c r="AJ44" s="3" t="s">
         <v>62</v>
@@ -6366,11 +6538,14 @@
       <c r="AL44" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AM44" s="1" t="s">
+      <c r="AM44" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN44" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A45" s="11" t="s">
         <v>32</v>
       </c>
@@ -6449,26 +6624,26 @@
       <c r="Z45" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AA45" s="3" t="s">
-        <v>62</v>
+      <c r="AA45" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="AB45" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AC45" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AD45" s="2" t="s">
+      <c r="AC45" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD45" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AE45" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AE45" s="2" t="s">
+      <c r="AF45" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AF45" s="2" t="s">
+      <c r="AG45" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="AG45" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="AH45" s="2" t="s">
         <v>32</v>
@@ -6482,14 +6657,17 @@
       <c r="AK45" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AL45" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM45" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="46" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="AL45" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AM45" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN45" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="46" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A46" s="11" t="s">
         <v>94</v>
       </c>
@@ -6574,11 +6752,11 @@
       <c r="AB46" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AC46" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AD46" s="4" t="s">
+      <c r="AC46" s="4" t="s">
         <v>33</v>
+      </c>
+      <c r="AD46" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="AE46" s="4" t="s">
         <v>33</v>
@@ -6601,14 +6779,17 @@
       <c r="AK46" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AL46" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM46" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="47" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="AL46" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AM46" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN46" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="47" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A47" s="11" t="s">
         <v>33</v>
       </c>
@@ -6687,47 +6868,50 @@
       <c r="Z47" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AA47" s="2" t="s">
+      <c r="AA47" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB47" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="AB47" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="AC47" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="AD47" s="2" t="s">
-        <v>33</v>
+      <c r="AD47" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="AE47" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AF47" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AG47" s="2" t="s">
+      <c r="AF47" s="2" t="s">
         <v>33</v>
+      </c>
+      <c r="AG47" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="AH47" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AI47" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AJ47" s="2" t="s">
+      <c r="AI47" s="2" t="s">
         <v>33</v>
+      </c>
+      <c r="AJ47" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="AK47" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AL47" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM47" s="1" t="s">
+      <c r="AL47" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AM47" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN47" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="48" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A48" s="11" t="s">
         <v>21</v>
       </c>
@@ -6806,47 +6990,50 @@
       <c r="Z48" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AA48" s="2" t="s">
+      <c r="AA48" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB48" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AB48" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC48" s="1" t="s">
+      <c r="AC48" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD48" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="AD48" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE48" s="2" t="s">
+      <c r="AE48" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF48" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AF48" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AG48" s="2" t="s">
-        <v>21</v>
+      <c r="AG48" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="AH48" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AI48" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AJ48" s="2" t="s">
+      <c r="AI48" s="2" t="s">
         <v>21</v>
+      </c>
+      <c r="AJ48" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="AK48" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AL48" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM48" s="1" t="s">
+      <c r="AL48" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AM48" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN48" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="49" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A49" s="12" t="s">
         <v>110</v>
       </c>
@@ -6925,8 +7112,8 @@
       <c r="Z49" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="AA49" s="3" t="s">
-        <v>62</v>
+      <c r="AA49" s="2" t="s">
+        <v>112</v>
       </c>
       <c r="AB49" s="3" t="s">
         <v>62</v>
@@ -6934,38 +7121,41 @@
       <c r="AC49" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AD49" s="2" t="s">
+      <c r="AD49" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE49" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AE49" s="2" t="s">
+      <c r="AF49" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="AF49" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AG49" s="2" t="s">
-        <v>114</v>
+      <c r="AG49" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="AH49" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="AI49" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AJ49" s="2" t="s">
-        <v>112</v>
+      <c r="AI49" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AJ49" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="AK49" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="AL49" s="3" t="s">
-        <v>62</v>
+      <c r="AL49" s="2" t="s">
+        <v>112</v>
       </c>
       <c r="AM49" s="3" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="50" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="AN49" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="50" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A50" s="11" t="s">
         <v>111</v>
       </c>
@@ -7044,24 +7234,24 @@
       <c r="Z50" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AA50" s="1" t="s">
+      <c r="AA50" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB50" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="AB50" s="2" t="s">
+      <c r="AC50" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="AC50" s="1" t="s">
+      <c r="AD50" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="AD50" s="2" t="s">
+      <c r="AE50" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AE50" s="2" t="s">
+      <c r="AF50" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="AF50" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="AG50" s="3" t="s">
         <v>62</v>
       </c>
@@ -7080,11 +7270,14 @@
       <c r="AL50" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AM50" s="1" t="s">
+      <c r="AM50" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN50" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="51" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A51" s="11" t="s">
         <v>112</v>
       </c>
@@ -7163,26 +7356,26 @@
       <c r="Z51" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="AA51" s="3" t="s">
-        <v>62</v>
+      <c r="AA51" s="2" t="s">
+        <v>112</v>
       </c>
       <c r="AB51" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AC51" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AD51" s="2" t="s">
+      <c r="AC51" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD51" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AE51" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AE51" s="2" t="s">
+      <c r="AF51" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="AF51" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AG51" s="2" t="s">
-        <v>112</v>
+      <c r="AG51" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="AH51" s="2" t="s">
         <v>112</v>
@@ -7196,14 +7389,17 @@
       <c r="AK51" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="AL51" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM51" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="52" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="AL51" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="AM51" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN51" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="52" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A52" s="11" t="s">
         <v>113</v>
       </c>
@@ -7282,20 +7478,20 @@
       <c r="Z52" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AA52" s="2" t="s">
+      <c r="AA52" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB52" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="AB52" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC52" s="1" t="s">
-        <v>81</v>
+      <c r="AC52" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="AD52" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="AE52" s="2" t="s">
-        <v>11</v>
+      <c r="AE52" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="AF52" s="2" t="s">
         <v>11</v>
@@ -7315,14 +7511,17 @@
       <c r="AK52" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="AL52" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM52" s="1" t="s">
+      <c r="AL52" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AM52" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN52" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="53" spans="1:39" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A53" s="11" t="s">
         <v>114</v>
       </c>
@@ -7401,17 +7600,17 @@
       <c r="Z53" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AA53" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AB53" s="2" t="s">
+      <c r="AA53" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AC53" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AD53" s="2" t="s">
+      <c r="AB53" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC53" s="2" t="s">
         <v>32</v>
+      </c>
+      <c r="AD53" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="AE53" s="2" t="s">
         <v>32</v>
@@ -7425,19 +7624,22 @@
       <c r="AH53" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AI53" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AJ53" s="2" t="s">
+      <c r="AI53" s="2" t="s">
         <v>32</v>
+      </c>
+      <c r="AJ53" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="AK53" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AL53" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM53" s="1" t="s">
+      <c r="AL53" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AM53" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN53" s="1" t="s">
         <v>74</v>
       </c>
     </row>
@@ -7448,20 +7650,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M48"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.796875" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -7503,7 +7705,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" s="12" t="s">
         <v>126</v>
       </c>
@@ -7544,7 +7746,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" s="11" t="s">
         <v>127</v>
       </c>
@@ -7585,7 +7787,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4" s="11" t="s">
         <v>128</v>
       </c>
@@ -7626,7 +7828,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" s="11" t="s">
         <v>129</v>
       </c>
@@ -7667,7 +7869,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6" s="11" t="s">
         <v>177</v>
       </c>
@@ -7708,7 +7910,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7" s="15" t="s">
         <v>130</v>
       </c>
@@ -7749,7 +7951,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" s="15" t="s">
         <v>152</v>
       </c>
@@ -7790,7 +7992,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9" s="15" t="s">
         <v>131</v>
       </c>
@@ -7831,7 +8033,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" s="14" t="s">
         <v>132</v>
       </c>
@@ -7872,7 +8074,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11" s="14" t="s">
         <v>133</v>
       </c>
@@ -7913,7 +8115,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12" s="14" t="s">
         <v>184</v>
       </c>
@@ -7954,7 +8156,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13" s="14" t="s">
         <v>185</v>
       </c>
@@ -7995,7 +8197,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14" s="15" t="s">
         <v>134</v>
       </c>
@@ -8036,7 +8238,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15" s="15" t="s">
         <v>135</v>
       </c>
@@ -8077,7 +8279,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16" s="14" t="s">
         <v>136</v>
       </c>
@@ -8118,7 +8320,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A17" s="14" t="s">
         <v>137</v>
       </c>
@@ -8159,7 +8361,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A18" s="14" t="s">
         <v>138</v>
       </c>
@@ -8200,7 +8402,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A19" s="14" t="s">
         <v>188</v>
       </c>
@@ -8241,7 +8443,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A20" s="14" t="s">
         <v>139</v>
       </c>
@@ -8282,7 +8484,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A21" s="14" t="s">
         <v>140</v>
       </c>
@@ -8323,7 +8525,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A22" s="15" t="s">
         <v>154</v>
       </c>
@@ -8364,7 +8566,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A23" s="15" t="s">
         <v>155</v>
       </c>
@@ -8405,7 +8607,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A24" s="14" t="s">
         <v>141</v>
       </c>
@@ -8446,7 +8648,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A25" s="14" t="s">
         <v>142</v>
       </c>
@@ -8487,7 +8689,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A26" s="15" t="s">
         <v>143</v>
       </c>
@@ -8528,7 +8730,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A27" s="14" t="s">
         <v>144</v>
       </c>
@@ -8569,7 +8771,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A28" s="15" t="s">
         <v>156</v>
       </c>
@@ -8610,7 +8812,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A29" s="15" t="s">
         <v>157</v>
       </c>
@@ -8651,7 +8853,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A30" s="15" t="s">
         <v>158</v>
       </c>
@@ -8692,7 +8894,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A31" s="15" t="s">
         <v>159</v>
       </c>
@@ -8733,7 +8935,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A32" s="12" t="s">
         <v>145</v>
       </c>
@@ -8774,7 +8976,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A33" s="14" t="s">
         <v>160</v>
       </c>
@@ -8815,7 +9017,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A34" s="15" t="s">
         <v>146</v>
       </c>
@@ -8856,7 +9058,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A35" s="14" t="s">
         <v>161</v>
       </c>
@@ -8897,7 +9099,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A36" s="15" t="s">
         <v>162</v>
       </c>
@@ -8938,7 +9140,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A37" s="14" t="s">
         <v>147</v>
       </c>
@@ -8979,7 +9181,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A38" s="15" t="s">
         <v>163</v>
       </c>
@@ -9020,7 +9222,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A39" s="14" t="s">
         <v>164</v>
       </c>
@@ -9061,7 +9263,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A40" s="15" t="s">
         <v>148</v>
       </c>
@@ -9102,7 +9304,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A41" s="14" t="s">
         <v>165</v>
       </c>
@@ -9143,7 +9345,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A42" s="14" t="s">
         <v>166</v>
       </c>
@@ -9184,7 +9386,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A43" s="14" t="s">
         <v>183</v>
       </c>
@@ -9225,7 +9427,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A44" s="14" t="s">
         <v>149</v>
       </c>
@@ -9266,7 +9468,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="45" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A45" s="15" t="s">
         <v>150</v>
       </c>
@@ -9307,7 +9509,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="46" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A46" s="15" t="s">
         <v>168</v>
       </c>
@@ -9437,19 +9639,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="8.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.9296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.06640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -9470,7 +9672,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
         <v>102</v>
       </c>
@@ -9490,7 +9692,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="5" t="s">
         <v>101</v>
       </c>
@@ -9510,7 +9712,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="5" t="s">
         <v>105</v>
       </c>
@@ -9530,7 +9732,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FIX: regression in base64 scanning in lexer.
</commit_message>
<xml_diff>
--- a/docs/lexer/lexer-FSM.xlsx
+++ b/docs/lexer/lexer-FSM.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Red\docs\lexer\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{276A0501-51D9-4FCF-804F-3C672F966E7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="564" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="564"/>
   </bookViews>
   <sheets>
     <sheet name="transitions" sheetId="3" r:id="rId1"/>
@@ -639,7 +633,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -883,7 +877,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -916,26 +910,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -968,23 +945,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1160,23 +1120,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AA37" sqref="AA37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AA15" sqref="AA15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.73046875" customWidth="1"/>
-    <col min="5" max="5" width="9.73046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="12" width="9.73046875" customWidth="1"/>
-    <col min="13" max="13" width="9.9296875" bestFit="1" customWidth="1"/>
-    <col min="14" max="40" width="9.73046875" customWidth="1"/>
+    <col min="1" max="1" width="10.36328125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" customWidth="1"/>
+    <col min="5" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="9.7265625" customWidth="1"/>
+    <col min="13" max="13" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="40" width="9.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -1299,7 +1259,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
@@ -1421,7 +1381,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A3" s="11" t="s">
         <v>68</v>
       </c>
@@ -1543,7 +1503,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A4" s="11" t="s">
         <v>69</v>
       </c>
@@ -1665,7 +1625,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -1787,7 +1747,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A6" s="12" t="s">
         <v>2</v>
       </c>
@@ -1909,7 +1869,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A7" s="11" t="s">
         <v>73</v>
       </c>
@@ -2031,7 +1991,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A8" s="11" t="s">
         <v>3</v>
       </c>
@@ -2153,7 +2113,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A9" s="11" t="s">
         <v>4</v>
       </c>
@@ -2275,7 +2235,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A10" s="11" t="s">
         <v>107</v>
       </c>
@@ -2397,7 +2357,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A11" s="11" t="s">
         <v>108</v>
       </c>
@@ -2519,7 +2479,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A12" s="11" t="s">
         <v>109</v>
       </c>
@@ -2641,7 +2601,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A13" s="11" t="s">
         <v>5</v>
       </c>
@@ -2763,7 +2723,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A14" s="11" t="s">
         <v>6</v>
       </c>
@@ -2885,7 +2845,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A15" s="11" t="s">
         <v>7</v>
       </c>
@@ -2964,8 +2924,8 @@
       <c r="Z15" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AA15" s="3" t="s">
-        <v>62</v>
+      <c r="AA15" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="AB15" s="3" t="s">
         <v>62</v>
@@ -3007,7 +2967,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A16" s="11" t="s">
         <v>70</v>
       </c>
@@ -3129,7 +3089,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A17" s="11" t="s">
         <v>8</v>
       </c>
@@ -3251,7 +3211,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A18" s="11" t="s">
         <v>9</v>
       </c>
@@ -3373,7 +3333,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A19" s="11" t="s">
         <v>10</v>
       </c>
@@ -3495,7 +3455,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A20" s="11" t="s">
         <v>11</v>
       </c>
@@ -3617,7 +3577,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A21" s="11" t="s">
         <v>12</v>
       </c>
@@ -3739,7 +3699,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="22" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A22" s="11" t="s">
         <v>84</v>
       </c>
@@ -3861,7 +3821,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A23" s="11" t="s">
         <v>13</v>
       </c>
@@ -3983,7 +3943,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A24" s="11" t="s">
         <v>194</v>
       </c>
@@ -4105,7 +4065,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A25" s="11" t="s">
         <v>14</v>
       </c>
@@ -4227,7 +4187,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="26" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A26" s="11" t="s">
         <v>15</v>
       </c>
@@ -4349,7 +4309,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A27" s="11" t="s">
         <v>16</v>
       </c>
@@ -4471,7 +4431,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="28" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A28" s="11" t="s">
         <v>17</v>
       </c>
@@ -4593,7 +4553,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A29" s="11" t="s">
         <v>18</v>
       </c>
@@ -4715,7 +4675,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="30" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A30" s="11" t="s">
         <v>19</v>
       </c>
@@ -4837,7 +4797,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A31" s="11" t="s">
         <v>20</v>
       </c>
@@ -4959,7 +4919,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="32" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A32" s="11" t="s">
         <v>22</v>
       </c>
@@ -5081,7 +5041,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A33" s="11" t="s">
         <v>23</v>
       </c>
@@ -5203,7 +5163,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="34" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A34" s="11" t="s">
         <v>24</v>
       </c>
@@ -5325,7 +5285,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="35" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A35" s="11" t="s">
         <v>195</v>
       </c>
@@ -5447,7 +5407,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="36" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A36" s="11" t="s">
         <v>25</v>
       </c>
@@ -5569,7 +5529,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="37" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A37" s="11" t="s">
         <v>26</v>
       </c>
@@ -5691,7 +5651,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="38" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A38" s="11" t="s">
         <v>27</v>
       </c>
@@ -5813,7 +5773,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="39" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A39" s="11" t="s">
         <v>28</v>
       </c>
@@ -5935,7 +5895,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A40" s="11" t="s">
         <v>29</v>
       </c>
@@ -6057,7 +6017,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="41" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A41" s="11" t="s">
         <v>30</v>
       </c>
@@ -6179,7 +6139,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="42" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A42" s="11" t="s">
         <v>31</v>
       </c>
@@ -6301,7 +6261,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="43" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A43" s="11" t="s">
         <v>191</v>
       </c>
@@ -6423,7 +6383,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="44" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A44" s="11" t="s">
         <v>192</v>
       </c>
@@ -6545,7 +6505,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A45" s="11" t="s">
         <v>32</v>
       </c>
@@ -6667,7 +6627,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="46" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A46" s="11" t="s">
         <v>94</v>
       </c>
@@ -6789,7 +6749,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="47" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A47" s="11" t="s">
         <v>33</v>
       </c>
@@ -6911,7 +6871,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="48" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A48" s="11" t="s">
         <v>21</v>
       </c>
@@ -7033,7 +6993,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="49" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A49" s="12" t="s">
         <v>110</v>
       </c>
@@ -7155,7 +7115,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="50" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A50" s="11" t="s">
         <v>111</v>
       </c>
@@ -7277,7 +7237,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="51" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A51" s="11" t="s">
         <v>112</v>
       </c>
@@ -7399,7 +7359,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="52" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A52" s="11" t="s">
         <v>113</v>
       </c>
@@ -7521,7 +7481,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="53" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A53" s="11" t="s">
         <v>114</v>
       </c>
@@ -7650,20 +7610,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M48"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.19921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -7705,7 +7665,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A2" s="12" t="s">
         <v>126</v>
       </c>
@@ -7746,7 +7706,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A3" s="11" t="s">
         <v>127</v>
       </c>
@@ -7787,7 +7747,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A4" s="11" t="s">
         <v>128</v>
       </c>
@@ -7828,7 +7788,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A5" s="11" t="s">
         <v>129</v>
       </c>
@@ -7869,7 +7829,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A6" s="11" t="s">
         <v>177</v>
       </c>
@@ -7910,7 +7870,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A7" s="15" t="s">
         <v>130</v>
       </c>
@@ -7951,7 +7911,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A8" s="15" t="s">
         <v>152</v>
       </c>
@@ -7992,7 +7952,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A9" s="15" t="s">
         <v>131</v>
       </c>
@@ -8033,7 +7993,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A10" s="14" t="s">
         <v>132</v>
       </c>
@@ -8074,7 +8034,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A11" s="14" t="s">
         <v>133</v>
       </c>
@@ -8115,7 +8075,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A12" s="14" t="s">
         <v>184</v>
       </c>
@@ -8156,7 +8116,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A13" s="14" t="s">
         <v>185</v>
       </c>
@@ -8197,7 +8157,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A14" s="15" t="s">
         <v>134</v>
       </c>
@@ -8238,7 +8198,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A15" s="15" t="s">
         <v>135</v>
       </c>
@@ -8279,7 +8239,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A16" s="14" t="s">
         <v>136</v>
       </c>
@@ -8320,7 +8280,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A17" s="14" t="s">
         <v>137</v>
       </c>
@@ -8361,7 +8321,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A18" s="14" t="s">
         <v>138</v>
       </c>
@@ -8402,7 +8362,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A19" s="14" t="s">
         <v>188</v>
       </c>
@@ -8443,7 +8403,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A20" s="14" t="s">
         <v>139</v>
       </c>
@@ -8484,7 +8444,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A21" s="14" t="s">
         <v>140</v>
       </c>
@@ -8525,7 +8485,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A22" s="15" t="s">
         <v>154</v>
       </c>
@@ -8566,7 +8526,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A23" s="15" t="s">
         <v>155</v>
       </c>
@@ -8607,7 +8567,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A24" s="14" t="s">
         <v>141</v>
       </c>
@@ -8648,7 +8608,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A25" s="14" t="s">
         <v>142</v>
       </c>
@@ -8689,7 +8649,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A26" s="15" t="s">
         <v>143</v>
       </c>
@@ -8730,7 +8690,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A27" s="14" t="s">
         <v>144</v>
       </c>
@@ -8771,7 +8731,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A28" s="15" t="s">
         <v>156</v>
       </c>
@@ -8812,7 +8772,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A29" s="15" t="s">
         <v>157</v>
       </c>
@@ -8853,7 +8813,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A30" s="15" t="s">
         <v>158</v>
       </c>
@@ -8894,7 +8854,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A31" s="15" t="s">
         <v>159</v>
       </c>
@@ -8935,7 +8895,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A32" s="12" t="s">
         <v>145</v>
       </c>
@@ -8976,7 +8936,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A33" s="14" t="s">
         <v>160</v>
       </c>
@@ -9017,7 +8977,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A34" s="15" t="s">
         <v>146</v>
       </c>
@@ -9058,7 +9018,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A35" s="14" t="s">
         <v>161</v>
       </c>
@@ -9099,7 +9059,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A36" s="15" t="s">
         <v>162</v>
       </c>
@@ -9140,7 +9100,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A37" s="14" t="s">
         <v>147</v>
       </c>
@@ -9181,7 +9141,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A38" s="15" t="s">
         <v>163</v>
       </c>
@@ -9222,7 +9182,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A39" s="14" t="s">
         <v>164</v>
       </c>
@@ -9263,7 +9223,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A40" s="15" t="s">
         <v>148</v>
       </c>
@@ -9304,7 +9264,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A41" s="14" t="s">
         <v>165</v>
       </c>
@@ -9345,7 +9305,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A42" s="14" t="s">
         <v>166</v>
       </c>
@@ -9386,7 +9346,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A43" s="14" t="s">
         <v>183</v>
       </c>
@@ -9427,7 +9387,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A44" s="14" t="s">
         <v>149</v>
       </c>
@@ -9468,7 +9428,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A45" s="15" t="s">
         <v>150</v>
       </c>
@@ -9509,7 +9469,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A46" s="15" t="s">
         <v>168</v>
       </c>
@@ -9639,19 +9599,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.9296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.06640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.19921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -9672,7 +9632,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
         <v>102</v>
       </c>
@@ -9692,7 +9652,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A3" s="5" t="s">
         <v>101</v>
       </c>
@@ -9712,7 +9672,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A4" s="5" t="s">
         <v>105</v>
       </c>
@@ -9732,7 +9692,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A5" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FIX: accepts / and + in binary! scanning (for base64).
</commit_message>
<xml_diff>
--- a/docs/lexer/lexer-FSM.xlsx
+++ b/docs/lexer/lexer-FSM.xlsx
@@ -1124,8 +1124,8 @@
   <dimension ref="A1:AN53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AA15" sqref="AA15"/>
+      <pane xSplit="1" topLeftCell="S1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AH15" sqref="AH15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2912,8 +2912,8 @@
       <c r="V15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="W15" s="3" t="s">
-        <v>62</v>
+      <c r="W15" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="X15" s="3" t="s">
         <v>62</v>
@@ -2945,8 +2945,8 @@
       <c r="AG15" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AH15" s="3" t="s">
-        <v>62</v>
+      <c r="AH15" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="AI15" s="3" t="s">
         <v>62</v>

</xml_diff>

<commit_message>
FIX: various fixes for scanning binary!, time! and pair! values.
</commit_message>
<xml_diff>
--- a/docs/lexer/lexer-FSM.xlsx
+++ b/docs/lexer/lexer-FSM.xlsx
@@ -1124,8 +1124,8 @@
   <dimension ref="A1:AN53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="S1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AH15" sqref="AH15"/>
+      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Y14" sqref="Y14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2723,7 +2723,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A14" s="11" t="s">
         <v>6</v>
       </c>
@@ -4675,7 +4675,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="30" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A30" s="11" t="s">
         <v>19</v>
       </c>
@@ -4775,11 +4775,11 @@
       <c r="AG30" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AH30" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AI30" s="3" t="s">
-        <v>62</v>
+      <c r="AH30" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AI30" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="AJ30" s="3" t="s">
         <v>62</v>

</xml_diff>

<commit_message>
FIX: some compliant email! forms not accepted by the lexer.
</commit_message>
<xml_diff>
--- a/docs/lexer/lexer-FSM.xlsx
+++ b/docs/lexer/lexer-FSM.xlsx
@@ -1124,8 +1124,8 @@
   <dimension ref="A1:AN53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Y14" sqref="Y14"/>
+      <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AE31" sqref="AE31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3821,7 +3821,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A23" s="11" t="s">
         <v>13</v>
       </c>
@@ -3912,8 +3912,8 @@
       <c r="AD23" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AE23" s="3" t="s">
-        <v>62</v>
+      <c r="AE23" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="AF23" s="2" t="s">
         <v>15</v>
@@ -3943,7 +3943,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A24" s="11" t="s">
         <v>194</v>
       </c>
@@ -4034,8 +4034,8 @@
       <c r="AD24" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AE24" s="3" t="s">
-        <v>62</v>
+      <c r="AE24" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="AF24" s="2" t="s">
         <v>15</v>
@@ -4766,8 +4766,8 @@
       <c r="AD30" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AE30" s="3" t="s">
-        <v>62</v>
+      <c r="AE30" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="AF30" s="3" t="s">
         <v>62</v>
@@ -4797,7 +4797,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A31" s="11" t="s">
         <v>20</v>
       </c>
@@ -4888,8 +4888,8 @@
       <c r="AD31" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="AE31" s="3" t="s">
-        <v>62</v>
+      <c r="AE31" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="AF31" s="2" t="s">
         <v>20</v>
@@ -7481,7 +7481,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="53" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A53" s="11" t="s">
         <v>114</v>
       </c>

</xml_diff>

<commit_message>
FIX: allows C_EQUAL class in url! values.
</commit_message>
<xml_diff>
--- a/docs/lexer/lexer-FSM.xlsx
+++ b/docs/lexer/lexer-FSM.xlsx
@@ -1124,8 +1124,8 @@
   <dimension ref="A1:AN53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AE31" sqref="AE31"/>
+      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AA47" sqref="AA47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6749,7 +6749,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="47" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A47" s="11" t="s">
         <v>33</v>
       </c>
@@ -6828,8 +6828,8 @@
       <c r="Z47" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AA47" s="3" t="s">
-        <v>62</v>
+      <c r="AA47" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="AB47" s="2" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
FEAT: removes date! scanning FSM.
It's replaced by regular code scan-date, which provides faster performance.
</commit_message>
<xml_diff>
--- a/docs/lexer/lexer-FSM.xlsx
+++ b/docs/lexer/lexer-FSM.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Red\docs\lexer\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CD799AF-9E13-41A3-825E-D287EF4C064A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="564"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" tabRatio="564" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="transitions" sheetId="3" r:id="rId1"/>
-    <sheet name="date! transitions" sheetId="5" r:id="rId2"/>
-    <sheet name="bin16 transitions" sheetId="4" r:id="rId3"/>
+    <sheet name="bin16 transitions" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2765" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2142" uniqueCount="133">
   <si>
     <t>S_START</t>
   </si>
@@ -363,226 +368,13 @@
     <t>S_PATH_SIGN</t>
   </si>
   <si>
-    <t>C_DT_DIGIT</t>
-  </si>
-  <si>
-    <t>C_DT_SLASH</t>
-  </si>
-  <si>
-    <t>C_DT_DASH</t>
-  </si>
-  <si>
-    <t>C_DT_PLUS</t>
-  </si>
-  <si>
-    <t>C_DT_COLON</t>
-  </si>
-  <si>
-    <t>C_DT_DOT</t>
-  </si>
-  <si>
-    <t>C_DT_T</t>
-  </si>
-  <si>
-    <t>C_DT_W</t>
-  </si>
-  <si>
-    <t>C_DT_Z</t>
-  </si>
-  <si>
-    <t>C_DT_ILLEGAL</t>
-  </si>
-  <si>
-    <t>C_DT_EOF</t>
-  </si>
-  <si>
-    <t>S_DT_START</t>
-  </si>
-  <si>
-    <t>S_DT_D</t>
-  </si>
-  <si>
-    <t>S_DT_DD</t>
-  </si>
-  <si>
-    <t>S_DT_YYY</t>
-  </si>
-  <si>
-    <t>F_DT_YEARL</t>
-  </si>
-  <si>
-    <t>F_DT_DAYL</t>
-  </si>
-  <si>
-    <t>S_DT_YM</t>
-  </si>
-  <si>
-    <t>S_DT_YMM</t>
-  </si>
-  <si>
-    <t>F_DT_YMONTH</t>
-  </si>
-  <si>
-    <t>F_DT_DDD</t>
-  </si>
-  <si>
-    <t>S_DT_YV</t>
-  </si>
-  <si>
-    <t>S_DT_YW</t>
-  </si>
-  <si>
-    <t>S_DT_YWW</t>
-  </si>
-  <si>
-    <t>S_DT_WD</t>
-  </si>
-  <si>
-    <t>S_DT_YMON</t>
-  </si>
-  <si>
-    <t>S_DT_DM</t>
-  </si>
-  <si>
-    <t>S_DT_DMM</t>
-  </si>
-  <si>
-    <t>F_DT_DMONTH</t>
-  </si>
-  <si>
-    <t>S_DT_DMON</t>
-  </si>
-  <si>
-    <t>S_TM_START</t>
-  </si>
-  <si>
-    <t>F_TM_HH</t>
-  </si>
-  <si>
-    <t>F_TM_MM</t>
-  </si>
-  <si>
-    <t>F_TM_SS</t>
-  </si>
-  <si>
-    <t>S_TZ_H</t>
-  </si>
-  <si>
-    <t>F_TZ_HH</t>
-  </si>
-  <si>
-    <t>S_TZ_M</t>
-  </si>
-  <si>
-    <t>F_DT_YEARL2</t>
-  </si>
-  <si>
-    <t>C_DT_LETTER</t>
-  </si>
-  <si>
-    <t>F_DT_YMD</t>
-  </si>
-  <si>
-    <t>F_DT_YMDD</t>
-  </si>
-  <si>
-    <t>F_DT_DMY</t>
-  </si>
-  <si>
-    <t>F_DT_DMYY</t>
-  </si>
-  <si>
-    <t>F_DT_DMYYY</t>
-  </si>
-  <si>
-    <t>F_DT_DMYYYY</t>
-  </si>
-  <si>
-    <t>F_TM_H</t>
-  </si>
-  <si>
-    <t>S_TM_HM</t>
-  </si>
-  <si>
-    <t>F_TM_M</t>
-  </si>
-  <si>
-    <t>S_TM_HMS</t>
-  </si>
-  <si>
-    <t>F_TM_S</t>
-  </si>
-  <si>
-    <t>F_TM_N1</t>
-  </si>
-  <si>
-    <t>F_TM_N</t>
-  </si>
-  <si>
-    <t>T_TM_NZ</t>
-  </si>
-  <si>
-    <t>F_TZ_HM</t>
-  </si>
-  <si>
-    <t>T_TZ_HH</t>
-  </si>
-  <si>
-    <t>T_TZ_H</t>
-  </si>
-  <si>
-    <t>T_TZ_MM</t>
-  </si>
-  <si>
-    <t>T_DT_ERROR</t>
-  </si>
-  <si>
-    <t>T_DT_YMDAY</t>
-  </si>
-  <si>
-    <t>T_DT_DMYEAR</t>
-  </si>
-  <si>
-    <t>T_DT_YWWD</t>
-  </si>
-  <si>
-    <t>T_DT_WEEK</t>
-  </si>
-  <si>
-    <t>S_DT_YYYY</t>
-  </si>
-  <si>
     <t>C_MINUS</t>
   </si>
   <si>
     <t>C_PLUS</t>
   </si>
   <si>
-    <t>T_TM_HMS</t>
-  </si>
-  <si>
-    <t>T_TM_HM</t>
-  </si>
-  <si>
     <t>C_T</t>
-  </si>
-  <si>
-    <t>S_TM_HMZ</t>
-  </si>
-  <si>
-    <t>S_DT_YM2</t>
-  </si>
-  <si>
-    <t>S_DT_YMM2</t>
-  </si>
-  <si>
-    <t>T_DT_YDDD</t>
-  </si>
-  <si>
-    <t>T_TZ_M</t>
-  </si>
-  <si>
-    <t>S_DT_YWD</t>
   </si>
   <si>
     <t>T_MSTR_OP</t>
@@ -633,8 +425,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -687,15 +479,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -708,14 +493,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -754,22 +533,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -803,18 +571,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -877,7 +633,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -910,9 +666,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -945,6 +718,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1120,7 +910,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AN53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -1128,15 +918,15 @@
       <selection pane="topRight" activeCell="AA47" sqref="AA47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.36328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" customWidth="1"/>
-    <col min="5" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="12" width="9.7265625" customWidth="1"/>
-    <col min="13" max="13" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="14" max="40" width="9.7265625" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.73046875" customWidth="1"/>
+    <col min="5" max="5" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="9.73046875" customWidth="1"/>
+    <col min="13" max="13" width="9.9296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="40" width="9.73046875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -1187,22 +977,22 @@
         <v>47</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>182</v>
+        <v>117</v>
       </c>
       <c r="R1" s="6" t="s">
-        <v>196</v>
+        <v>125</v>
       </c>
       <c r="S1" s="6" t="s">
-        <v>197</v>
+        <v>126</v>
       </c>
       <c r="T1" s="6" t="s">
-        <v>198</v>
+        <v>127</v>
       </c>
       <c r="U1" s="6" t="s">
-        <v>199</v>
+        <v>128</v>
       </c>
       <c r="V1" s="6" t="s">
-        <v>200</v>
+        <v>129</v>
       </c>
       <c r="W1" s="6" t="s">
         <v>48</v>
@@ -1217,7 +1007,7 @@
         <v>51</v>
       </c>
       <c r="AA1" s="6" t="s">
-        <v>203</v>
+        <v>132</v>
       </c>
       <c r="AB1" s="6" t="s">
         <v>52</v>
@@ -1238,10 +1028,10 @@
         <v>57</v>
       </c>
       <c r="AH1" s="6" t="s">
-        <v>179</v>
+        <v>116</v>
       </c>
       <c r="AI1" s="6" t="s">
-        <v>178</v>
+        <v>115</v>
       </c>
       <c r="AJ1" s="6" t="s">
         <v>58</v>
@@ -1259,7 +1049,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
@@ -1288,7 +1078,7 @@
         <v>67</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>189</v>
+        <v>118</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>62</v>
@@ -1318,13 +1108,13 @@
         <v>32</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>195</v>
+        <v>124</v>
       </c>
       <c r="U2" s="2" t="s">
         <v>32</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>195</v>
+        <v>124</v>
       </c>
       <c r="W2" s="2" t="s">
         <v>5</v>
@@ -1354,7 +1144,7 @@
         <v>62</v>
       </c>
       <c r="AF2" s="2" t="s">
-        <v>191</v>
+        <v>120</v>
       </c>
       <c r="AG2" s="2" t="s">
         <v>22</v>
@@ -1381,7 +1171,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A3" s="11" t="s">
         <v>68</v>
       </c>
@@ -1389,7 +1179,7 @@
         <v>68</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>202</v>
+        <v>131</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>68</v>
@@ -1503,7 +1293,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A4" s="11" t="s">
         <v>69</v>
       </c>
@@ -1625,7 +1415,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -1747,7 +1537,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A6" s="12" t="s">
         <v>2</v>
       </c>
@@ -1776,10 +1566,10 @@
         <v>2</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>189</v>
+        <v>118</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>190</v>
+        <v>119</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>2</v>
@@ -1869,7 +1659,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A7" s="11" t="s">
         <v>73</v>
       </c>
@@ -1991,7 +1781,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A8" s="11" t="s">
         <v>3</v>
       </c>
@@ -2113,7 +1903,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A9" s="11" t="s">
         <v>4</v>
       </c>
@@ -2235,7 +2025,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A10" s="11" t="s">
         <v>107</v>
       </c>
@@ -2357,7 +2147,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A11" s="11" t="s">
         <v>108</v>
       </c>
@@ -2479,7 +2269,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A12" s="11" t="s">
         <v>109</v>
       </c>
@@ -2601,7 +2391,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A13" s="11" t="s">
         <v>5</v>
       </c>
@@ -2723,7 +2513,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A14" s="11" t="s">
         <v>6</v>
       </c>
@@ -2845,7 +2635,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A15" s="11" t="s">
         <v>7</v>
       </c>
@@ -2967,7 +2757,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A16" s="11" t="s">
         <v>70</v>
       </c>
@@ -3089,7 +2879,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A17" s="11" t="s">
         <v>8</v>
       </c>
@@ -3211,7 +3001,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A18" s="11" t="s">
         <v>9</v>
       </c>
@@ -3333,7 +3123,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A19" s="11" t="s">
         <v>10</v>
       </c>
@@ -3455,7 +3245,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A20" s="11" t="s">
         <v>11</v>
       </c>
@@ -3577,7 +3367,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A21" s="11" t="s">
         <v>12</v>
       </c>
@@ -3630,19 +3420,19 @@
         <v>16</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>201</v>
+        <v>130</v>
       </c>
       <c r="S21" s="2" t="s">
         <v>13</v>
       </c>
       <c r="T21" s="2" t="s">
-        <v>194</v>
+        <v>123</v>
       </c>
       <c r="U21" s="3" t="s">
         <v>62</v>
       </c>
       <c r="V21" s="2" t="s">
-        <v>195</v>
+        <v>124</v>
       </c>
       <c r="W21" s="2" t="s">
         <v>16</v>
@@ -3699,7 +3489,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="22" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A22" s="11" t="s">
         <v>84</v>
       </c>
@@ -3821,7 +3611,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A23" s="11" t="s">
         <v>13</v>
       </c>
@@ -3943,9 +3733,9 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A24" s="11" t="s">
-        <v>194</v>
+        <v>123</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>85</v>
@@ -3954,10 +3744,10 @@
         <v>85</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>194</v>
+        <v>123</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>194</v>
+        <v>123</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>85</v>
@@ -3996,19 +3786,19 @@
         <v>62</v>
       </c>
       <c r="R24" s="1" t="s">
-        <v>201</v>
+        <v>130</v>
       </c>
       <c r="S24" s="2" t="s">
         <v>13</v>
       </c>
       <c r="T24" s="2" t="s">
-        <v>195</v>
+        <v>124</v>
       </c>
       <c r="U24" s="3" t="s">
         <v>62</v>
       </c>
       <c r="V24" s="2" t="s">
-        <v>195</v>
+        <v>124</v>
       </c>
       <c r="W24" s="1" t="s">
         <v>85</v>
@@ -4065,7 +3855,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A25" s="11" t="s">
         <v>14</v>
       </c>
@@ -4079,37 +3869,37 @@
         <v>85</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>193</v>
+        <v>122</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>193</v>
+        <v>122</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>193</v>
+        <v>122</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>193</v>
+        <v>122</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>193</v>
+        <v>122</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>193</v>
+        <v>122</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>193</v>
+        <v>122</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>193</v>
+        <v>122</v>
       </c>
       <c r="M25" s="2" t="s">
         <v>14</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>193</v>
+        <v>122</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>193</v>
+        <v>122</v>
       </c>
       <c r="P25" s="2" t="s">
         <v>14</v>
@@ -4133,13 +3923,13 @@
         <v>14</v>
       </c>
       <c r="W25" s="1" t="s">
-        <v>193</v>
+        <v>122</v>
       </c>
       <c r="X25" s="1" t="s">
-        <v>193</v>
+        <v>122</v>
       </c>
       <c r="Y25" s="1" t="s">
-        <v>193</v>
+        <v>122</v>
       </c>
       <c r="Z25" s="2" t="s">
         <v>14</v>
@@ -4148,22 +3938,22 @@
         <v>14</v>
       </c>
       <c r="AB25" s="1" t="s">
-        <v>193</v>
+        <v>122</v>
       </c>
       <c r="AC25" s="1" t="s">
-        <v>193</v>
+        <v>122</v>
       </c>
       <c r="AD25" s="1" t="s">
-        <v>193</v>
+        <v>122</v>
       </c>
       <c r="AE25" s="1" t="s">
-        <v>193</v>
+        <v>122</v>
       </c>
       <c r="AF25" s="2" t="s">
         <v>14</v>
       </c>
       <c r="AG25" s="1" t="s">
-        <v>193</v>
+        <v>122</v>
       </c>
       <c r="AH25" s="2" t="s">
         <v>14</v>
@@ -4172,7 +3962,7 @@
         <v>14</v>
       </c>
       <c r="AJ25" s="1" t="s">
-        <v>193</v>
+        <v>122</v>
       </c>
       <c r="AK25" s="2" t="s">
         <v>14</v>
@@ -4184,10 +3974,10 @@
         <v>62</v>
       </c>
       <c r="AN25" s="1" t="s">
-        <v>193</v>
+        <v>122</v>
       </c>
     </row>
-    <row r="26" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A26" s="11" t="s">
         <v>15</v>
       </c>
@@ -4309,7 +4099,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A27" s="11" t="s">
         <v>16</v>
       </c>
@@ -4431,7 +4221,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="28" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A28" s="11" t="s">
         <v>17</v>
       </c>
@@ -4553,7 +4343,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A29" s="11" t="s">
         <v>18</v>
       </c>
@@ -4675,7 +4465,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="30" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A30" s="11" t="s">
         <v>19</v>
       </c>
@@ -4797,7 +4587,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A31" s="11" t="s">
         <v>20</v>
       </c>
@@ -4919,7 +4709,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="32" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A32" s="11" t="s">
         <v>22</v>
       </c>
@@ -5041,7 +4831,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A33" s="11" t="s">
         <v>23</v>
       </c>
@@ -5163,7 +4953,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="34" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A34" s="11" t="s">
         <v>24</v>
       </c>
@@ -5285,9 +5075,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="35" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A35" s="11" t="s">
-        <v>195</v>
+        <v>124</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>74</v>
@@ -5296,10 +5086,10 @@
         <v>74</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>195</v>
+        <v>124</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>195</v>
+        <v>124</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>74</v>
@@ -5338,19 +5128,19 @@
         <v>32</v>
       </c>
       <c r="R35" s="1" t="s">
-        <v>201</v>
+        <v>130</v>
       </c>
       <c r="S35" s="2" t="s">
         <v>32</v>
       </c>
       <c r="T35" s="2" t="s">
-        <v>195</v>
+        <v>124</v>
       </c>
       <c r="U35" s="2" t="s">
         <v>32</v>
       </c>
       <c r="V35" s="2" t="s">
-        <v>195</v>
+        <v>124</v>
       </c>
       <c r="W35" s="1" t="s">
         <v>93</v>
@@ -5407,7 +5197,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="36" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A36" s="11" t="s">
         <v>25</v>
       </c>
@@ -5529,7 +5319,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="37" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A37" s="11" t="s">
         <v>26</v>
       </c>
@@ -5651,7 +5441,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="38" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A38" s="11" t="s">
         <v>27</v>
       </c>
@@ -5773,7 +5563,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="39" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A39" s="11" t="s">
         <v>28</v>
       </c>
@@ -5895,7 +5685,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A40" s="11" t="s">
         <v>29</v>
       </c>
@@ -6017,7 +5807,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="41" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A41" s="11" t="s">
         <v>30</v>
       </c>
@@ -6139,7 +5929,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="42" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A42" s="11" t="s">
         <v>31</v>
       </c>
@@ -6234,7 +6024,7 @@
         <v>32</v>
       </c>
       <c r="AF42" s="2" t="s">
-        <v>191</v>
+        <v>120</v>
       </c>
       <c r="AG42" s="2" t="s">
         <v>32</v>
@@ -6261,9 +6051,9 @@
         <v>74</v>
       </c>
     </row>
-    <row r="43" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A43" s="11" t="s">
-        <v>191</v>
+        <v>120</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>74</v>
@@ -6272,10 +6062,10 @@
         <v>74</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>192</v>
+        <v>121</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>192</v>
+        <v>121</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>74</v>
@@ -6317,10 +6107,10 @@
         <v>32</v>
       </c>
       <c r="S43" s="2" t="s">
-        <v>192</v>
+        <v>121</v>
       </c>
       <c r="T43" s="2" t="s">
-        <v>192</v>
+        <v>121</v>
       </c>
       <c r="U43" s="2" t="s">
         <v>32</v>
@@ -6362,10 +6152,10 @@
         <v>62</v>
       </c>
       <c r="AH43" s="2" t="s">
-        <v>192</v>
+        <v>121</v>
       </c>
       <c r="AI43" s="2" t="s">
-        <v>192</v>
+        <v>121</v>
       </c>
       <c r="AJ43" s="2" t="s">
         <v>32</v>
@@ -6383,9 +6173,9 @@
         <v>74</v>
       </c>
     </row>
-    <row r="44" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A44" s="11" t="s">
-        <v>192</v>
+        <v>121</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>85</v>
@@ -6394,10 +6184,10 @@
         <v>85</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>192</v>
+        <v>121</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>192</v>
+        <v>121</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>85</v>
@@ -6439,10 +6229,10 @@
         <v>62</v>
       </c>
       <c r="S44" s="2" t="s">
-        <v>192</v>
+        <v>121</v>
       </c>
       <c r="T44" s="2" t="s">
-        <v>192</v>
+        <v>121</v>
       </c>
       <c r="U44" s="3" t="s">
         <v>62</v>
@@ -6484,10 +6274,10 @@
         <v>62</v>
       </c>
       <c r="AH44" s="2" t="s">
-        <v>192</v>
+        <v>121</v>
       </c>
       <c r="AI44" s="2" t="s">
-        <v>192</v>
+        <v>121</v>
       </c>
       <c r="AJ44" s="3" t="s">
         <v>62</v>
@@ -6505,7 +6295,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A45" s="11" t="s">
         <v>32</v>
       </c>
@@ -6627,7 +6417,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="46" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A46" s="11" t="s">
         <v>94</v>
       </c>
@@ -6749,7 +6539,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="47" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A47" s="11" t="s">
         <v>33</v>
       </c>
@@ -6871,7 +6661,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="48" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A48" s="11" t="s">
         <v>21</v>
       </c>
@@ -6993,7 +6783,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="49" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A49" s="12" t="s">
         <v>110</v>
       </c>
@@ -7115,7 +6905,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="50" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A50" s="11" t="s">
         <v>111</v>
       </c>
@@ -7237,7 +7027,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="51" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A51" s="11" t="s">
         <v>112</v>
       </c>
@@ -7359,7 +7149,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="52" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A52" s="11" t="s">
         <v>113</v>
       </c>
@@ -7481,7 +7271,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="53" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A53" s="11" t="s">
         <v>114</v>
       </c>
@@ -7610,2008 +7400,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M48"/>
-  <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.6328125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="13"/>
-      <c r="B1" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A2" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="G2" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="H2" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="I2" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="J2" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="K2" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="L2" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="M2" s="16" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A3" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="G3" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="H3" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="I3" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="J3" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="K3" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="L3" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="M3" s="16" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A4" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="F4" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="G4" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="H4" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="I4" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="J4" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="K4" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="L4" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="M4" s="16" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A5" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="G5" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="H5" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="I5" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="J5" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="K5" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="L5" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="M5" s="16" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A6" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="F6" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="G6" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="H6" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="I6" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="J6" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="K6" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="L6" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="M6" s="16" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A7" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="E7" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="G7" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="H7" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="I7" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="J7" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="K7" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="L7" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="M7" s="16" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A8" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="E8" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="H8" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="I8" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="J8" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="K8" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="L8" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="M8" s="16" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A9" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="E9" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="F9" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="G9" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="H9" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="I9" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="J9" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="K9" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="L9" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="M9" s="16" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A10" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="G10" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="H10" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="I10" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="J10" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="K10" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="L10" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="M10" s="16" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A11" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="F11" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="G11" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="H11" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="I11" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="J11" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="K11" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="L11" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="M11" s="16" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A12" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="F12" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="G12" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="H12" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="I12" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="J12" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="K12" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="L12" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="M12" s="16" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A13" s="14" t="s">
-        <v>185</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="G13" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="H13" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="I13" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="J13" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="K13" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="L13" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="M13" s="16" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A14" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="E14" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="F14" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="G14" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="H14" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="I14" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="J14" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="K14" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="L14" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="M14" s="16" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A15" s="15" t="s">
-        <v>135</v>
-      </c>
-      <c r="B15" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="E15" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="G15" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="H15" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="I15" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="J15" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="K15" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="L15" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="M15" s="4" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A16" s="14" t="s">
-        <v>136</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="F16" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="G16" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="H16" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="I16" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="J16" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="K16" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="L16" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="M16" s="16" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A17" s="14" t="s">
-        <v>137</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="E17" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="F17" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="G17" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="H17" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="I17" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="J17" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="K17" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="L17" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="M17" s="2" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A18" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="B18" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="C18" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="D18" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="G18" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="H18" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="I18" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="J18" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="K18" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="L18" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="M18" s="2" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A19" s="14" t="s">
-        <v>188</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="D19" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="E19" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="G19" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="H19" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="I19" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="J19" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="K19" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="L19" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="M19" s="16" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A20" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="B20" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="C20" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="D20" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="E20" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="G20" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="H20" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="I20" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="J20" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="K20" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="L20" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="M20" s="2" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A21" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="B21" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="G21" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="H21" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="I21" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="J21" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="K21" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="L21" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="M21" s="16" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A22" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="C22" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E22" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="G22" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="H22" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="I22" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="J22" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="K22" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="L22" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="M22" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A23" s="15" t="s">
-        <v>155</v>
-      </c>
-      <c r="B23" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="C23" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E23" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="G23" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="H23" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="I23" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="J23" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="K23" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="L23" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="M23" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A24" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="C24" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="F24" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="G24" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="H24" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="I24" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="J24" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="K24" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="L24" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="M24" s="16" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A25" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="B25" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="C25" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="F25" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="G25" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="H25" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="I25" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="J25" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="K25" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="L25" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="M25" s="16" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A26" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="C26" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="D26" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="E26" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="F26" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="G26" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="H26" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="I26" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="J26" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="K26" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="L26" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="M26" s="16" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A27" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="B27" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="G27" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="H27" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="I27" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="J27" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="K27" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="L27" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="M27" s="16" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A28" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="C28" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E28" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="G28" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="H28" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="I28" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="J28" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="K28" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="L28" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="M28" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A29" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="C29" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E29" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="G29" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="H29" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="I29" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="J29" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="K29" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="L29" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="M29" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A30" s="15" t="s">
-        <v>158</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="C30" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E30" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="G30" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="H30" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="I30" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="J30" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="K30" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="L30" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="M30" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A31" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="B31" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="C31" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E31" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="G31" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="H31" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="I31" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="J31" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="K31" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="L31" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="M31" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A32" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="C32" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="D32" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="E32" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="F32" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="G32" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="H32" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="I32" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="J32" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="K32" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="L32" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="M32" s="16" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A33" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="C33" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="D33" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="E33" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="F33" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="G33" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="H33" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="I33" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="J33" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="K33" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="L33" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="M33" s="16" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A34" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="C34" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="D34" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="E34" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="F34" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="G34" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="H34" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="I34" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="J34" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="K34" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="L34" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="M34" s="16" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A35" s="14" t="s">
-        <v>161</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="C35" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="D35" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="E35" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="F35" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="G35" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="H35" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="I35" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="J35" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="K35" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="L35" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="M35" s="16" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A36" s="15" t="s">
-        <v>162</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C36" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="D36" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="F36" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="G36" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="H36" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="I36" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="J36" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="K36" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="L36" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="M36" s="4" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A37" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C37" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="D37" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="F37" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="G37" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="H37" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="I37" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="J37" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="K37" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="L37" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="M37" s="4" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A38" s="15" t="s">
-        <v>163</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C38" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="D38" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="E38" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="F38" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="G38" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="H38" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="I38" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="J38" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="K38" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="L38" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="M38" s="16" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A39" s="14" t="s">
-        <v>164</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="C39" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="D39" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="F39" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="G39" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="I39" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="J39" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="K39" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="L39" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="M39" s="4" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A40" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="B40" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="C40" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="D40" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="F40" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="G40" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="I40" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="J40" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="K40" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="L40" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="M40" s="4" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A41" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="C41" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="D41" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="E41" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="F41" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="G41" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="H41" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="I41" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="J41" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="K41" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="L41" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="M41" s="16" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A42" s="14" t="s">
-        <v>166</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="C42" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="D42" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="F42" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="G42" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="H42" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="I42" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="J42" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="K42" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="L42" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="M42" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A43" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="C43" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="D43" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="E43" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="F43" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="G43" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="H43" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="I43" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="J43" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="K43" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="L43" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="M43" s="16" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A44" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="C44" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="D44" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="E44" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="F44" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="G44" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="H44" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="I44" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="J44" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="K44" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="L44" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="M44" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A45" s="15" t="s">
-        <v>150</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="C45" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="D45" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="E45" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="F45" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="G45" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="H45" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="I45" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="J45" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="K45" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="L45" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="M45" s="2" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A46" s="15" t="s">
-        <v>168</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="C46" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="D46" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="E46" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="F46" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="G46" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="H46" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="I46" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="J46" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="K46" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="L46" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="M46" s="2" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="C47" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="D47" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="E47" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="F47" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="G47" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="H47" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="I47" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="J47" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="K47" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="L47" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="M47" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A48" s="14" t="s">
-        <v>172</v>
-      </c>
-      <c r="B48" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="C48" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="D48" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="E48" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="F48" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="G48" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="H48" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="I48" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="J48" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="K48" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="L48" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="M48" s="16" t="s">
-        <v>172</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="8.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.9296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.06640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -9632,7 +7433,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
         <v>102</v>
       </c>
@@ -9652,7 +7453,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="5" t="s">
         <v>101</v>
       </c>
@@ -9672,7 +7473,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="5" t="s">
         <v>105</v>
       </c>
@@ -9692,7 +7493,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FIX: more accurate detection of any-words starting with a digit.
Examples:
    a/'1  => error
    :1/b  => error
</commit_message>
<xml_diff>
--- a/docs/lexer/lexer-FSM.xlsx
+++ b/docs/lexer/lexer-FSM.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Red\docs\lexer\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CD799AF-9E13-41A3-825E-D287EF4C064A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" tabRatio="564" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-100" yWindow="-100" windowWidth="22700" windowHeight="14600" tabRatio="564"/>
   </bookViews>
   <sheets>
     <sheet name="transitions" sheetId="3" r:id="rId1"/>
@@ -21,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2142" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2222" uniqueCount="135">
   <si>
     <t>S_START</t>
   </si>
@@ -420,12 +414,18 @@
   </si>
   <si>
     <t>C_EQUAL</t>
+  </si>
+  <si>
+    <t>S_WORD_1ST</t>
+  </si>
+  <si>
+    <t>S_PATH_W1ST</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -633,7 +633,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -666,26 +666,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -718,23 +701,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -910,23 +876,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AN53"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AN55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AA47" sqref="AA47"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="W52" sqref="W52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.73046875" customWidth="1"/>
-    <col min="5" max="5" width="9.73046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="12" width="9.73046875" customWidth="1"/>
-    <col min="13" max="13" width="9.9296875" bestFit="1" customWidth="1"/>
-    <col min="14" max="40" width="9.73046875" customWidth="1"/>
+    <col min="1" max="1" width="10.36328125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" customWidth="1"/>
+    <col min="5" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="9.7265625" customWidth="1"/>
+    <col min="13" max="13" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="40" width="9.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -1049,7 +1015,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
@@ -1090,10 +1056,10 @@
         <v>6</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>32</v>
+        <v>133</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>32</v>
+        <v>133</v>
       </c>
       <c r="P2" s="2" t="s">
         <v>32</v>
@@ -1171,7 +1137,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A3" s="11" t="s">
         <v>68</v>
       </c>
@@ -1293,7 +1259,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A4" s="11" t="s">
         <v>69</v>
       </c>
@@ -1415,7 +1381,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -1537,7 +1503,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A6" s="12" t="s">
         <v>2</v>
       </c>
@@ -1659,7 +1625,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A7" s="11" t="s">
         <v>73</v>
       </c>
@@ -1781,7 +1747,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A8" s="11" t="s">
         <v>3</v>
       </c>
@@ -1903,7 +1869,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A9" s="11" t="s">
         <v>4</v>
       </c>
@@ -2025,7 +1991,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A10" s="11" t="s">
         <v>107</v>
       </c>
@@ -2147,7 +2113,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A11" s="11" t="s">
         <v>108</v>
       </c>
@@ -2269,7 +2235,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A12" s="11" t="s">
         <v>109</v>
       </c>
@@ -2391,7 +2357,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A13" s="11" t="s">
         <v>5</v>
       </c>
@@ -2513,7 +2479,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A14" s="11" t="s">
         <v>6</v>
       </c>
@@ -2635,7 +2601,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A15" s="11" t="s">
         <v>7</v>
       </c>
@@ -2757,7 +2723,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A16" s="11" t="s">
         <v>70</v>
       </c>
@@ -2879,7 +2845,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A17" s="11" t="s">
         <v>8</v>
       </c>
@@ -3001,7 +2967,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A18" s="11" t="s">
         <v>9</v>
       </c>
@@ -3123,7 +3089,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A19" s="11" t="s">
         <v>10</v>
       </c>
@@ -3245,7 +3211,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A20" s="11" t="s">
         <v>11</v>
       </c>
@@ -3367,7 +3333,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A21" s="11" t="s">
         <v>12</v>
       </c>
@@ -3489,7 +3455,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="22" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A22" s="11" t="s">
         <v>84</v>
       </c>
@@ -3611,7 +3577,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A23" s="11" t="s">
         <v>13</v>
       </c>
@@ -3733,7 +3699,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A24" s="11" t="s">
         <v>123</v>
       </c>
@@ -3855,7 +3821,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A25" s="11" t="s">
         <v>14</v>
       </c>
@@ -3977,7 +3943,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="26" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A26" s="11" t="s">
         <v>15</v>
       </c>
@@ -4099,7 +4065,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A27" s="11" t="s">
         <v>16</v>
       </c>
@@ -4221,7 +4187,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="28" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A28" s="11" t="s">
         <v>17</v>
       </c>
@@ -4343,7 +4309,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A29" s="11" t="s">
         <v>18</v>
       </c>
@@ -4465,7 +4431,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="30" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A30" s="11" t="s">
         <v>19</v>
       </c>
@@ -4587,7 +4553,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A31" s="11" t="s">
         <v>20</v>
       </c>
@@ -4709,7 +4675,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="32" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A32" s="11" t="s">
         <v>22</v>
       </c>
@@ -4831,7 +4797,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A33" s="11" t="s">
         <v>23</v>
       </c>
@@ -4953,7 +4919,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="34" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A34" s="11" t="s">
         <v>24</v>
       </c>
@@ -5075,7 +5041,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="35" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A35" s="11" t="s">
         <v>124</v>
       </c>
@@ -5197,7 +5163,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="36" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A36" s="11" t="s">
         <v>25</v>
       </c>
@@ -5319,7 +5285,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="37" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A37" s="11" t="s">
         <v>26</v>
       </c>
@@ -5441,7 +5407,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="38" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A38" s="11" t="s">
         <v>27</v>
       </c>
@@ -5563,7 +5529,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="39" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A39" s="11" t="s">
         <v>28</v>
       </c>
@@ -5685,7 +5651,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A40" s="11" t="s">
         <v>29</v>
       </c>
@@ -5807,7 +5773,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="41" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A41" s="11" t="s">
         <v>30</v>
       </c>
@@ -5929,7 +5895,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="42" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A42" s="11" t="s">
         <v>31</v>
       </c>
@@ -6051,7 +6017,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="43" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A43" s="11" t="s">
         <v>120</v>
       </c>
@@ -6173,7 +6139,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="44" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A44" s="11" t="s">
         <v>121</v>
       </c>
@@ -6295,259 +6261,259 @@
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A45" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I45" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="J45" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="K45" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="L45" s="1" t="s">
-        <v>74</v>
+        <v>133</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="I45" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J45" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="K45" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="L45" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="M45" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="N45" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="O45" s="2" t="s">
+      <c r="N45" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="O45" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="P45" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q45" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="R45" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="S45" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="T45" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="U45" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="V45" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="W45" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="X45" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y45" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z45" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA45" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB45" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC45" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD45" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE45" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF45" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AG45" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH45" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI45" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AJ45" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AK45" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AL45" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AM45" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN45" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="46" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="A46" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="L46" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="M46" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="N46" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="O46" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="P45" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q45" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="R45" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="S45" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="T45" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="U45" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="V45" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="W45" s="1" t="s">
+      <c r="P46" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q46" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="R46" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="S46" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="T46" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="U46" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="V46" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="W46" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="X45" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="Y45" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="Z45" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AA45" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB45" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC45" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AD45" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AE45" s="2" t="s">
+      <c r="X46" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y46" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z46" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA46" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB46" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC46" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD46" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AE46" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AF45" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AG45" s="2" t="s">
+      <c r="AF46" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AG46" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="AH45" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI45" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AJ45" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AK45" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AL45" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AM45" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN45" s="1" t="s">
+      <c r="AH46" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI46" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AJ46" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AK46" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AL46" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AM46" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN46" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="46" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A46" s="11" t="s">
+    <row r="47" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A47" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I46" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="J46" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="K46" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="L46" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="M46" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="N46" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="O46" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="P46" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q46" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="R46" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="S46" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="T46" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="U46" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="V46" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="W46" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="X46" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="Y46" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="Z46" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA46" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="AB46" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="AC46" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="AD46" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AE46" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="AF46" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="AG46" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="AH46" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="AI46" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="AJ46" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="AK46" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="AL46" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="AM46" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN46" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="47" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A47" s="11" t="s">
-        <v>33</v>
-      </c>
       <c r="B47" s="1" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>33</v>
@@ -6556,364 +6522,364 @@
         <v>33</v>
       </c>
       <c r="F47" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="L47" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="M47" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="N47" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="O47" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="P47" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q47" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="R47" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="S47" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="T47" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="U47" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="V47" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="W47" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="X47" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y47" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z47" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA47" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB47" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC47" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD47" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AE47" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AF47" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG47" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AH47" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI47" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ47" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK47" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AL47" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AM47" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN47" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="48" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A48" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="G47" s="1" t="s">
+      <c r="C48" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="H47" s="1" t="s">
+      <c r="D48" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F48" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="I47" s="1" t="s">
+      <c r="G48" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="J47" s="1" t="s">
+      <c r="H48" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="K47" s="1" t="s">
+      <c r="I48" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="L47" s="1" t="s">
+      <c r="J48" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="M47" s="2" t="s">
+      <c r="K48" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L48" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M48" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="N47" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="O47" s="2" t="s">
+      <c r="N48" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="O48" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="P47" s="2" t="s">
+      <c r="P48" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="Q47" s="2" t="s">
+      <c r="Q48" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="R47" s="2" t="s">
+      <c r="R48" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="S47" s="2" t="s">
+      <c r="S48" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="T47" s="2" t="s">
+      <c r="T48" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="U47" s="2" t="s">
+      <c r="U48" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="V47" s="2" t="s">
+      <c r="V48" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="W47" s="2" t="s">
+      <c r="W48" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="X47" s="1" t="s">
+      <c r="X48" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="Y47" s="1" t="s">
+      <c r="Y48" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="Z47" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AA47" s="2" t="s">
+      <c r="Z48" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA48" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AB47" s="2" t="s">
+      <c r="AB48" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AC47" s="1" t="s">
+      <c r="AC48" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="AD47" s="1" t="s">
+      <c r="AD48" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="AE47" s="2" t="s">
+      <c r="AE48" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AF47" s="2" t="s">
+      <c r="AF48" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AG47" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AH47" s="2" t="s">
+      <c r="AG48" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH48" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AI47" s="2" t="s">
+      <c r="AI48" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AJ47" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AK47" s="2" t="s">
+      <c r="AJ48" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AK48" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AL47" s="2" t="s">
+      <c r="AL48" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AM47" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN47" s="1" t="s">
+      <c r="AM48" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN48" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="48" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A48" s="11" t="s">
+    <row r="49" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A49" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B49" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C49" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D48" s="2" t="s">
+      <c r="D49" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E48" s="2" t="s">
+      <c r="E49" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F48" s="1" t="s">
+      <c r="F49" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="G48" s="1" t="s">
+      <c r="G49" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="H48" s="1" t="s">
+      <c r="H49" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="I48" s="1" t="s">
+      <c r="I49" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="J48" s="1" t="s">
+      <c r="J49" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="K48" s="1" t="s">
+      <c r="K49" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="L48" s="1" t="s">
+      <c r="L49" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="M48" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="N48" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="O48" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="P48" s="2" t="s">
+      <c r="M49" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="N49" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="O49" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="P49" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="Q48" s="2" t="s">
+      <c r="Q49" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="R48" s="2" t="s">
+      <c r="R49" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="S48" s="2" t="s">
+      <c r="S49" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="T48" s="2" t="s">
+      <c r="T49" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="U48" s="2" t="s">
+      <c r="U49" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="V48" s="2" t="s">
+      <c r="V49" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W48" s="1" t="s">
+      <c r="W49" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="X48" s="1" t="s">
+      <c r="X49" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="Y48" s="1" t="s">
+      <c r="Y49" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="Z48" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AA48" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AB48" s="2" t="s">
+      <c r="Z49" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA49" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB49" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AC48" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AD48" s="1" t="s">
+      <c r="AC49" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD49" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="AE48" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AF48" s="2" t="s">
+      <c r="AE49" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF49" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AG48" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AH48" s="2" t="s">
+      <c r="AG49" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH49" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AI48" s="2" t="s">
+      <c r="AI49" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AJ48" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AK48" s="2" t="s">
+      <c r="AJ49" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AK49" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AL48" s="2" t="s">
+      <c r="AL49" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AM48" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN48" s="1" t="s">
+      <c r="AM49" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN49" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="49" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A49" s="12" t="s">
+    <row r="50" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A50" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="B49" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="F49" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G49" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="H49" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="I49" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="J49" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="K49" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="L49" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="M49" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="N49" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="O49" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="P49" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q49" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="R49" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="S49" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="T49" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="U49" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="V49" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="W49" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="X49" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="Y49" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="Z49" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="AA49" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="AB49" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC49" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AD49" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE49" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AF49" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="AG49" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AH49" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="AI49" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="AJ49" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AK49" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="AL49" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="AM49" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN49" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="50" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A50" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>82</v>
+      <c r="B50" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>111</v>
@@ -6921,475 +6887,719 @@
       <c r="E50" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="F50" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>82</v>
+      <c r="F50" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="J50" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="K50" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="L50" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="M50" s="3" t="s">
-        <v>62</v>
+        <v>67</v>
+      </c>
+      <c r="J50" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="K50" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="L50" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="M50" s="2" t="s">
+        <v>113</v>
       </c>
       <c r="N50" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="O50" s="1" t="s">
-        <v>82</v>
+        <v>134</v>
+      </c>
+      <c r="O50" s="2" t="s">
+        <v>134</v>
       </c>
       <c r="P50" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q50" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="R50" s="3" t="s">
-        <v>62</v>
+        <v>112</v>
+      </c>
+      <c r="Q50" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="R50" s="2" t="s">
+        <v>112</v>
       </c>
       <c r="S50" s="2" t="s">
-        <v>13</v>
+        <v>112</v>
       </c>
       <c r="T50" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="U50" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="V50" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="W50" s="1" t="s">
-        <v>82</v>
+        <v>112</v>
+      </c>
+      <c r="U50" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="V50" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="W50" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="X50" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="Y50" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="Z50" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AA50" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AB50" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="AC50" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="AD50" s="1" t="s">
-        <v>82</v>
+      <c r="Y50" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z50" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA50" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="AB50" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC50" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD50" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="AE50" s="2" t="s">
         <v>21</v>
       </c>
       <c r="AF50" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG50" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH50" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AI50" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AJ50" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AK50" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="AL50" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="AM50" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN50" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="51" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="A51" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="J51" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="L51" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="M51" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="N51" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O51" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="P51" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q51" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="R51" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="S51" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T51" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="U51" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="V51" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="W51" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="X51" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y51" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Z51" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA51" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB51" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AC51" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="AG50" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AH50" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AI50" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AJ50" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AK50" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AL50" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM50" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN50" s="1" t="s">
+      <c r="AD51" s="1" t="s">
         <v>82</v>
-      </c>
-    </row>
-    <row r="51" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A51" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="H51" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I51" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="J51" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="K51" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="L51" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="M51" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="N51" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="O51" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="P51" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q51" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="R51" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="S51" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="T51" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="U51" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="V51" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="W51" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="X51" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="Y51" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="Z51" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="AA51" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="AB51" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC51" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AD51" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="AE51" s="2" t="s">
         <v>21</v>
       </c>
       <c r="AF51" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="AG51" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH51" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AI51" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ51" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AK51" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AL51" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AM51" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN51" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="52" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="A52" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H52" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="I52" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J52" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="K52" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="L52" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="M52" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="N52" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="O52" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="P52" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="AG51" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AH51" s="2" t="s">
+      <c r="Q52" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="AI51" s="2" t="s">
+      <c r="R52" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="AJ51" s="2" t="s">
+      <c r="S52" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="AK51" s="2" t="s">
+      <c r="T52" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="AL51" s="2" t="s">
+      <c r="U52" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="AM51" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN51" s="1" t="s">
-        <v>74</v>
+      <c r="V52" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="W52" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="X52" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y52" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z52" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA52" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="AB52" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC52" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD52" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE52" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF52" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG52" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH52" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="AI52" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="AJ52" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AK52" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="AL52" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="AM52" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN52" s="3" t="s">
+        <v>62</v>
       </c>
     </row>
-    <row r="52" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A52" s="11" t="s">
+    <row r="53" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="A53" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J53" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K53" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="L53" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="M53" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="N53" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="O53" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="P53" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q53" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="R53" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="S53" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="T53" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="U53" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="V53" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="W53" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="X53" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y53" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z53" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA53" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="AB53" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC53" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD53" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AE53" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AF53" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG53" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH53" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="AI53" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="AJ53" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="AK53" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="AL53" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="AM53" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN53" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="54" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A54" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B54" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C54" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D52" s="2" t="s">
+      <c r="D54" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E52" s="2" t="s">
+      <c r="E54" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F52" s="2" t="s">
+      <c r="F54" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G52" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="H52" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="I52" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="J52" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="K52" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="L52" s="2" t="s">
+      <c r="G54" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H54" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="I54" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J54" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="K54" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="L54" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="M52" s="2" t="s">
+      <c r="M54" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N52" s="2" t="s">
+      <c r="N54" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="O52" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="P52" s="2" t="s">
+      <c r="O54" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="P54" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="Q52" s="2" t="s">
+      <c r="Q54" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="R52" s="2" t="s">
+      <c r="R54" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="S52" s="2" t="s">
+      <c r="S54" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="T52" s="2" t="s">
+      <c r="T54" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="U52" s="2" t="s">
+      <c r="U54" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="V52" s="2" t="s">
+      <c r="V54" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="W52" s="2" t="s">
+      <c r="W54" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="X52" s="2" t="s">
+      <c r="X54" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="Y52" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="Z52" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AA52" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AB52" s="2" t="s">
+      <c r="Y54" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z54" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA54" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB54" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="AC52" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AD52" s="1" t="s">
+      <c r="AC54" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD54" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="AE52" s="1" t="s">
+      <c r="AE54" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="AF52" s="2" t="s">
+      <c r="AF54" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="AG52" s="2" t="s">
+      <c r="AG54" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="AH52" s="2" t="s">
+      <c r="AH54" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="AI52" s="2" t="s">
+      <c r="AI54" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="AJ52" s="2" t="s">
+      <c r="AJ54" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="AK52" s="2" t="s">
+      <c r="AK54" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="AL52" s="2" t="s">
+      <c r="AL54" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="AM52" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN52" s="1" t="s">
+      <c r="AM54" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN54" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="53" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A53" s="11" t="s">
+    <row r="55" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A55" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="B53" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D53" s="2" t="s">
+      <c r="B55" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D55" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="E53" s="2" t="s">
+      <c r="E55" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="F53" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="H53" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I53" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="J53" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="K53" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="L53" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="M53" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="N53" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="O53" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="P53" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q53" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="R53" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="S53" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="T53" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="U53" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="V53" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="W53" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="X53" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="Y53" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="Z53" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AA53" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB53" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC53" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AD53" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AE53" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AF53" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AG53" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AH53" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI53" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AJ53" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AK53" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AL53" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AM53" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN53" s="1" t="s">
+      <c r="F55" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J55" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K55" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="L55" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="M55" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="N55" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="O55" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="P55" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q55" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="R55" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="S55" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="T55" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="U55" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="V55" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="W55" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="X55" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y55" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z55" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA55" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB55" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC55" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD55" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AE55" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF55" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AG55" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH55" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI55" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AJ55" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AK55" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AL55" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AM55" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN55" s="1" t="s">
         <v>74</v>
       </c>
     </row>
@@ -7400,19 +7610,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.9296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.06640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.19921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -7433,7 +7643,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
         <v>102</v>
       </c>
@@ -7453,7 +7663,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A3" s="5" t="s">
         <v>101</v>
       </c>
@@ -7473,7 +7683,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A4" s="5" t="s">
         <v>105</v>
       </c>
@@ -7493,7 +7703,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A5" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FEAT: lexer FSM adjustments for handling //... forms.
</commit_message>
<xml_diff>
--- a/docs/lexer/lexer-FSM.xlsx
+++ b/docs/lexer/lexer-FSM.xlsx
@@ -880,8 +880,8 @@
   <dimension ref="A1:AN55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="W52" sqref="W52"/>
+      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="W46" sqref="W46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2425,7 +2425,7 @@
         <v>5</v>
       </c>
       <c r="W13" s="2" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="X13" s="2" t="s">
         <v>5</v>
@@ -6329,7 +6329,7 @@
         <v>32</v>
       </c>
       <c r="W45" s="2" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="X45" s="3" t="s">
         <v>62</v>

</xml_diff>

<commit_message>
FIX: improves hex literal values scanning support.
</commit_message>
<xml_diff>
--- a/docs/lexer/lexer-FSM.xlsx
+++ b/docs/lexer/lexer-FSM.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Red\docs\lexer\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93FE0032-B15F-46E8-8A07-400445CAAC66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-100" yWindow="-100" windowWidth="22700" windowHeight="14600" tabRatio="564"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" tabRatio="564" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="transitions" sheetId="3" r:id="rId1"/>
@@ -15,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2222" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2262" uniqueCount="136">
   <si>
     <t>S_START</t>
   </si>
@@ -420,12 +426,15 @@
   </si>
   <si>
     <t>S_PATH_W1ST</t>
+  </si>
+  <si>
+    <t>S_HEX_END</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -633,7 +642,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -666,9 +675,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -701,6 +727,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -876,23 +919,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AN55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AN56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="W46" sqref="W46"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J36" sqref="A36:XFD36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.36328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" customWidth="1"/>
-    <col min="5" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="12" width="9.7265625" customWidth="1"/>
-    <col min="13" max="13" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="14" max="40" width="9.7265625" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.73046875" customWidth="1"/>
+    <col min="5" max="5" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="9.73046875" customWidth="1"/>
+    <col min="13" max="13" width="9.9296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="40" width="9.73046875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -1015,7 +1058,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
@@ -1137,7 +1180,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A3" s="11" t="s">
         <v>68</v>
       </c>
@@ -1259,7 +1302,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A4" s="11" t="s">
         <v>69</v>
       </c>
@@ -1381,7 +1424,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -1503,7 +1546,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A6" s="12" t="s">
         <v>2</v>
       </c>
@@ -1625,7 +1668,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A7" s="11" t="s">
         <v>73</v>
       </c>
@@ -1747,7 +1790,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A8" s="11" t="s">
         <v>3</v>
       </c>
@@ -1869,7 +1912,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A9" s="11" t="s">
         <v>4</v>
       </c>
@@ -1991,7 +2034,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A10" s="11" t="s">
         <v>107</v>
       </c>
@@ -2113,7 +2156,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A11" s="11" t="s">
         <v>108</v>
       </c>
@@ -2235,7 +2278,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A12" s="11" t="s">
         <v>109</v>
       </c>
@@ -2357,7 +2400,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A13" s="11" t="s">
         <v>5</v>
       </c>
@@ -2479,7 +2522,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A14" s="11" t="s">
         <v>6</v>
       </c>
@@ -2601,7 +2644,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A15" s="11" t="s">
         <v>7</v>
       </c>
@@ -2723,7 +2766,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A16" s="11" t="s">
         <v>70</v>
       </c>
@@ -2845,7 +2888,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A17" s="11" t="s">
         <v>8</v>
       </c>
@@ -2967,7 +3010,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A18" s="11" t="s">
         <v>9</v>
       </c>
@@ -3089,7 +3132,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A19" s="11" t="s">
         <v>10</v>
       </c>
@@ -3211,7 +3254,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A20" s="11" t="s">
         <v>11</v>
       </c>
@@ -3333,7 +3376,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A21" s="11" t="s">
         <v>12</v>
       </c>
@@ -3455,7 +3498,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="22" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A22" s="11" t="s">
         <v>84</v>
       </c>
@@ -3577,7 +3620,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A23" s="11" t="s">
         <v>13</v>
       </c>
@@ -3699,7 +3742,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A24" s="11" t="s">
         <v>123</v>
       </c>
@@ -3821,7 +3864,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A25" s="11" t="s">
         <v>14</v>
       </c>
@@ -3943,7 +3986,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="26" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A26" s="11" t="s">
         <v>15</v>
       </c>
@@ -4065,7 +4108,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A27" s="11" t="s">
         <v>16</v>
       </c>
@@ -4187,7 +4230,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="28" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A28" s="11" t="s">
         <v>17</v>
       </c>
@@ -4309,7 +4352,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A29" s="11" t="s">
         <v>18</v>
       </c>
@@ -4431,7 +4474,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="30" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A30" s="11" t="s">
         <v>19</v>
       </c>
@@ -4553,7 +4596,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A31" s="11" t="s">
         <v>20</v>
       </c>
@@ -4675,7 +4718,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="32" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A32" s="11" t="s">
         <v>22</v>
       </c>
@@ -4797,7 +4840,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A33" s="11" t="s">
         <v>23</v>
       </c>
@@ -4919,7 +4962,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="34" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A34" s="11" t="s">
         <v>24</v>
       </c>
@@ -5041,7 +5084,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="35" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A35" s="11" t="s">
         <v>124</v>
       </c>
@@ -5093,8 +5136,8 @@
       <c r="Q35" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="R35" s="1" t="s">
-        <v>130</v>
+      <c r="R35" s="2" t="s">
+        <v>135</v>
       </c>
       <c r="S35" s="2" t="s">
         <v>32</v>
@@ -5163,137 +5206,137 @@
         <v>74</v>
       </c>
     </row>
-    <row r="36" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A36" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="M36" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="N36" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="O36" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="P36" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q36" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="R36" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="S36" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="T36" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="U36" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="V36" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="W36" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="X36" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="Y36" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z36" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA36" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB36" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC36" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD36" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="AE36" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AF36" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AG36" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH36" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI36" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AJ36" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AK36" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AL36" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AM36" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN36" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="37" spans="1:40" x14ac:dyDescent="0.45">
+      <c r="A37" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I36" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="J36" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="K36" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="L36" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="M36" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N36" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="O36" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="P36" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q36" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="R36" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="S36" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="T36" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="U36" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="V36" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="W36" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="X36" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y36" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="Z36" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AA36" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB36" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC36" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AD36" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AE36" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AF36" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AG36" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AH36" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AI36" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AJ36" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AK36" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AL36" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AM36" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN36" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="37" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A37" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>26</v>
+      <c r="B37" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>26</v>
@@ -5301,26 +5344,26 @@
       <c r="E37" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F37" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I37" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="J37" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="K37" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="L37" s="2" t="s">
-        <v>27</v>
+      <c r="F37" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="L37" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="M37" s="2" t="s">
         <v>26</v>
@@ -5328,8 +5371,8 @@
       <c r="N37" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="O37" s="2" t="s">
-        <v>29</v>
+      <c r="O37" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="P37" s="2" t="s">
         <v>26</v>
@@ -5359,13 +5402,13 @@
         <v>26</v>
       </c>
       <c r="Y37" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z37" s="1" t="s">
-        <v>90</v>
+        <v>32</v>
+      </c>
+      <c r="Z37" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="AA37" s="2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="AB37" s="2" t="s">
         <v>26</v>
@@ -5373,11 +5416,11 @@
       <c r="AC37" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AD37" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AE37" s="2" t="s">
-        <v>26</v>
+      <c r="AD37" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AE37" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="AF37" s="2" t="s">
         <v>26</v>
@@ -5403,135 +5446,135 @@
       <c r="AM37" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AN37" s="3" t="s">
-        <v>62</v>
+      <c r="AN37" s="1" t="s">
+        <v>74</v>
       </c>
     </row>
-    <row r="38" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A38" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L38" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="M38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O38" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="P38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="R38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="S38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="T38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="U38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="V38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="W38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="X38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z38" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AA38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AE38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AG38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AH38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AI38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AJ38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AK38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AL38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AM38" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN38" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="1:40" x14ac:dyDescent="0.45">
+      <c r="A39" s="11" t="s">
         <v>27</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="J38" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="K38" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="L38" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M38" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="N38" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="O38" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="P38" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q38" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="R38" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="S38" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="T38" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="U38" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="V38" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="W38" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="X38" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y38" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z38" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA38" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="AB38" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC38" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="AD38" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="AE38" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="AF38" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="AG38" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="AH38" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="AI38" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="AJ38" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="AK38" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="AL38" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="AM38" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN38" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="39" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A39" s="11" t="s">
-        <v>28</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>27</v>
@@ -5564,7 +5607,7 @@
         <v>27</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M39" s="2" t="s">
         <v>27</v>
@@ -5636,7 +5679,7 @@
         <v>27</v>
       </c>
       <c r="AJ39" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AK39" s="2" t="s">
         <v>27</v>
@@ -5651,131 +5694,131 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A40" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J40" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K40" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L40" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M40" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N40" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O40" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="P40" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q40" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="R40" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="S40" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="T40" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="U40" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="V40" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="W40" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="X40" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y40" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z40" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA40" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB40" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC40" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD40" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE40" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF40" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG40" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH40" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AI40" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AJ40" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AK40" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AL40" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AM40" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN40" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="41" spans="1:40" x14ac:dyDescent="0.45">
+      <c r="A41" s="11" t="s">
         <v>29</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="I40" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J40" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="K40" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="L40" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="M40" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="N40" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="O40" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="P40" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q40" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="R40" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="S40" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="T40" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="U40" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="V40" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="W40" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="X40" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y40" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z40" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA40" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AB40" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AC40" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AD40" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE40" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AF40" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AG40" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AH40" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AI40" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AJ40" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AK40" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AL40" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AM40" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN40" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="41" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A41" s="11" t="s">
-        <v>30</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>29</v>
@@ -5817,7 +5860,7 @@
         <v>29</v>
       </c>
       <c r="O41" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="P41" s="2" t="s">
         <v>29</v>
@@ -5895,259 +5938,259 @@
         <v>62</v>
       </c>
     </row>
-    <row r="42" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A42" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K42" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L42" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M42" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="N42" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="O42" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="P42" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q42" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="R42" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="S42" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T42" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="U42" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="V42" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="W42" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="X42" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y42" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z42" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA42" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB42" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC42" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD42" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE42" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF42" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AG42" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH42" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AI42" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ42" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK42" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AL42" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AM42" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN42" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="43" spans="1:40" x14ac:dyDescent="0.45">
+      <c r="A43" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D42" s="2" t="s">
+      <c r="B43" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D43" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E42" s="2" t="s">
+      <c r="E43" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F42" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I42" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="J42" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="K42" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="L42" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="M42" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="N42" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="O42" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="P42" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q42" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="R42" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="S42" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="T42" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="U42" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="V42" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="W42" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="X42" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="Y42" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="Z42" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AA42" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB42" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC42" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AD42" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AE42" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AF42" s="2" t="s">
+      <c r="F43" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="L43" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="M43" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="N43" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="O43" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="P43" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q43" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="R43" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="S43" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="T43" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="U43" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="V43" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="W43" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="X43" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y43" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z43" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA43" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB43" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC43" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD43" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AE43" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF43" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="AG42" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AH42" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI42" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AJ42" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AK42" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AL42" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AM42" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN42" s="1" t="s">
+      <c r="AG43" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH43" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI43" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AJ43" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AK43" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AL43" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AM43" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN43" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="43" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A43" s="11" t="s">
+    <row r="44" spans="1:40" x14ac:dyDescent="0.45">
+      <c r="A44" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="H43" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I43" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="J43" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="K43" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="L43" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="M43" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="N43" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="O43" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="P43" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q43" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="R43" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="S43" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="T43" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="U43" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="V43" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="W43" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="X43" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="Y43" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="Z43" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AA43" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB43" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC43" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AD43" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AE43" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AF43" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AG43" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AH43" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="AI43" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="AJ43" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AK43" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AL43" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AM43" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN43" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="44" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A44" s="11" t="s">
-        <v>121</v>
-      </c>
       <c r="B44" s="1" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>121</v>
@@ -6156,43 +6199,43 @@
         <v>121</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="L44" s="1" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="M44" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="N44" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="O44" s="1" t="s">
-        <v>85</v>
+      <c r="N44" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="O44" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="P44" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q44" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="R44" s="3" t="s">
-        <v>62</v>
+        <v>32</v>
+      </c>
+      <c r="Q44" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="R44" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="S44" s="2" t="s">
         <v>121</v>
@@ -6200,41 +6243,41 @@
       <c r="T44" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="U44" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="V44" s="3" t="s">
-        <v>62</v>
+      <c r="U44" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="V44" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="W44" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="X44" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="Y44" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="Z44" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AA44" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AB44" s="1" t="s">
-        <v>83</v>
+        <v>93</v>
+      </c>
+      <c r="X44" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y44" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z44" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA44" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB44" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="AC44" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AD44" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE44" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AF44" s="3" t="s">
-        <v>62</v>
+      <c r="AD44" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AE44" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AF44" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="AG44" s="3" t="s">
         <v>62</v>
@@ -6245,397 +6288,397 @@
       <c r="AI44" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="AJ44" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AK44" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AL44" s="3" t="s">
-        <v>62</v>
+      <c r="AJ44" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AK44" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AL44" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="AM44" s="3" t="s">
         <v>62</v>
       </c>
       <c r="AN44" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="45" spans="1:40" x14ac:dyDescent="0.45">
+      <c r="A45" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>85</v>
       </c>
+      <c r="C45" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="L45" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="M45" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="N45" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="O45" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="P45" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q45" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="R45" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="S45" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="T45" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="U45" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="V45" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="W45" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="X45" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y45" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z45" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA45" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB45" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AC45" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD45" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE45" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF45" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AG45" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH45" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="AI45" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="AJ45" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AK45" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AL45" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AM45" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN45" s="1" t="s">
+        <v>85</v>
+      </c>
     </row>
-    <row r="45" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A45" s="11" t="s">
+    <row r="46" spans="1:40" x14ac:dyDescent="0.45">
+      <c r="A46" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="B45" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G45" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="H45" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="I45" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="J45" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="K45" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="L45" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="M45" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="N45" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="O45" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="P45" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q45" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="R45" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="S45" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="T45" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="U45" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="V45" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="W45" s="2" t="s">
+      <c r="B46" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="I46" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J46" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="K46" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="L46" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="M46" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="N46" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="O46" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="P46" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q46" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="R46" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="S46" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="T46" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="U46" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="V46" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="W46" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="X45" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="Y45" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="Z45" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AA45" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB45" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC45" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AD45" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE45" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AF45" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AG45" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AH45" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI45" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AJ45" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AK45" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AL45" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AM45" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN45" s="3" t="s">
+      <c r="X46" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y46" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z46" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA46" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB46" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC46" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD46" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE46" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF46" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AG46" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH46" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI46" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AJ46" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AK46" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AL46" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AM46" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN46" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="46" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A46" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I46" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="J46" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="K46" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="L46" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="M46" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="N46" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="O46" s="2" t="s">
+    <row r="47" spans="1:40" x14ac:dyDescent="0.45">
+      <c r="A47" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="L47" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="M47" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="N47" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="O47" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="P46" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q46" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="R46" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="S46" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="T46" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="U46" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="V46" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="W46" s="1" t="s">
+      <c r="P47" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q47" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="R47" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="S47" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="T47" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="U47" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="V47" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="W47" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="X46" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="Y46" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="Z46" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AA46" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB46" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC46" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AD46" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AE46" s="2" t="s">
+      <c r="X47" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y47" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z47" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA47" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB47" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC47" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD47" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AE47" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AF46" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AG46" s="2" t="s">
+      <c r="AF47" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AG47" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="AH46" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI46" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AJ46" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AK46" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AL46" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AM46" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN46" s="1" t="s">
+      <c r="AH47" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI47" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AJ47" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AK47" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AL47" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AM47" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN47" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="47" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A47" s="11" t="s">
+    <row r="48" spans="1:40" x14ac:dyDescent="0.45">
+      <c r="A48" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="H47" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I47" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="J47" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="K47" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="L47" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="M47" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="N47" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="O47" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="P47" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q47" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="R47" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="S47" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="T47" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="U47" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="V47" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="W47" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="X47" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="Y47" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="Z47" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA47" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="AB47" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="AC47" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="AD47" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AE47" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="AF47" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="AG47" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="AH47" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="AI47" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="AJ47" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="AK47" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="AL47" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="AM47" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN47" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="48" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A48" s="11" t="s">
-        <v>33</v>
-      </c>
       <c r="B48" s="1" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>33</v>
@@ -6644,364 +6687,364 @@
         <v>33</v>
       </c>
       <c r="F48" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="L48" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="M48" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="N48" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="O48" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="P48" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q48" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="R48" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="S48" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="T48" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="U48" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="V48" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="W48" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="X48" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y48" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z48" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA48" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB48" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC48" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD48" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AE48" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AF48" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG48" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AH48" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI48" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ48" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK48" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AL48" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AM48" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN48" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="49" spans="1:40" x14ac:dyDescent="0.45">
+      <c r="A49" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="G48" s="1" t="s">
+      <c r="C49" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="H48" s="1" t="s">
+      <c r="D49" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F49" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="I48" s="1" t="s">
+      <c r="G49" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="J48" s="1" t="s">
+      <c r="H49" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="K48" s="1" t="s">
+      <c r="I49" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="L48" s="1" t="s">
+      <c r="J49" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="M48" s="2" t="s">
+      <c r="K49" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L49" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M49" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="N48" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="O48" s="2" t="s">
+      <c r="N49" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="O49" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="P48" s="2" t="s">
+      <c r="P49" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="Q48" s="2" t="s">
+      <c r="Q49" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="R48" s="2" t="s">
+      <c r="R49" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="S48" s="2" t="s">
+      <c r="S49" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="T48" s="2" t="s">
+      <c r="T49" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="U48" s="2" t="s">
+      <c r="U49" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="V48" s="2" t="s">
+      <c r="V49" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="W48" s="2" t="s">
+      <c r="W49" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="X48" s="1" t="s">
+      <c r="X49" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="Y48" s="1" t="s">
+      <c r="Y49" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="Z48" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AA48" s="2" t="s">
+      <c r="Z49" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA49" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AB48" s="2" t="s">
+      <c r="AB49" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AC48" s="1" t="s">
+      <c r="AC49" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="AD48" s="1" t="s">
+      <c r="AD49" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="AE48" s="2" t="s">
+      <c r="AE49" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AF48" s="2" t="s">
+      <c r="AF49" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AG48" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AH48" s="2" t="s">
+      <c r="AG49" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH49" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AI48" s="2" t="s">
+      <c r="AI49" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AJ48" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AK48" s="2" t="s">
+      <c r="AJ49" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AK49" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AL48" s="2" t="s">
+      <c r="AL49" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AM48" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN48" s="1" t="s">
+      <c r="AM49" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN49" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="49" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A49" s="11" t="s">
+    <row r="50" spans="1:40" x14ac:dyDescent="0.45">
+      <c r="A50" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B50" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C50" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D49" s="2" t="s">
+      <c r="D50" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E49" s="2" t="s">
+      <c r="E50" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F49" s="1" t="s">
+      <c r="F50" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="G49" s="1" t="s">
+      <c r="G50" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="H49" s="1" t="s">
+      <c r="H50" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="I49" s="1" t="s">
+      <c r="I50" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="J49" s="1" t="s">
+      <c r="J50" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="K49" s="1" t="s">
+      <c r="K50" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="L49" s="1" t="s">
+      <c r="L50" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="M49" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="N49" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="O49" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="P49" s="2" t="s">
+      <c r="M50" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="N50" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="O50" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="P50" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="Q49" s="2" t="s">
+      <c r="Q50" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="R49" s="2" t="s">
+      <c r="R50" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="S49" s="2" t="s">
+      <c r="S50" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="T49" s="2" t="s">
+      <c r="T50" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="U49" s="2" t="s">
+      <c r="U50" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="V49" s="2" t="s">
+      <c r="V50" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W49" s="1" t="s">
+      <c r="W50" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="X49" s="1" t="s">
+      <c r="X50" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="Y49" s="1" t="s">
+      <c r="Y50" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="Z49" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AA49" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AB49" s="2" t="s">
+      <c r="Z50" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA50" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB50" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AC49" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AD49" s="1" t="s">
+      <c r="AC50" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD50" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="AE49" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AF49" s="2" t="s">
+      <c r="AE50" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF50" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AG49" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AH49" s="2" t="s">
+      <c r="AG50" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH50" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AI49" s="2" t="s">
+      <c r="AI50" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AJ49" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AK49" s="2" t="s">
+      <c r="AJ50" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AK50" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AL49" s="2" t="s">
+      <c r="AL50" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AM49" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN49" s="1" t="s">
+      <c r="AM50" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN50" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="50" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A50" s="12" t="s">
+    <row r="51" spans="1:40" x14ac:dyDescent="0.45">
+      <c r="A51" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="B50" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="F50" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G50" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="H50" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="I50" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="J50" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="K50" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="L50" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="M50" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="N50" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="O50" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="P50" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q50" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="R50" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="S50" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="T50" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="U50" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="V50" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="W50" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="X50" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="Y50" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="Z50" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="AA50" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="AB50" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC50" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AD50" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE50" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AF50" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="AG50" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AH50" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="AI50" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="AJ50" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AK50" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="AL50" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="AM50" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN50" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="51" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A51" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>82</v>
+      <c r="B51" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>111</v>
@@ -7009,279 +7052,279 @@
       <c r="E51" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="F51" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>82</v>
+      <c r="F51" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="J51" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="K51" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="L51" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="M51" s="3" t="s">
-        <v>62</v>
+        <v>67</v>
+      </c>
+      <c r="J51" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="K51" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="L51" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="M51" s="2" t="s">
+        <v>113</v>
       </c>
       <c r="N51" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="O51" s="1" t="s">
-        <v>82</v>
+        <v>134</v>
+      </c>
+      <c r="O51" s="2" t="s">
+        <v>134</v>
       </c>
       <c r="P51" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q51" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="R51" s="3" t="s">
-        <v>62</v>
+        <v>112</v>
+      </c>
+      <c r="Q51" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="R51" s="2" t="s">
+        <v>112</v>
       </c>
       <c r="S51" s="2" t="s">
-        <v>13</v>
+        <v>112</v>
       </c>
       <c r="T51" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="U51" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="V51" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="W51" s="1" t="s">
-        <v>82</v>
+        <v>112</v>
+      </c>
+      <c r="U51" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="V51" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="W51" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="X51" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="Y51" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="Z51" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AA51" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AB51" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="AC51" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="AD51" s="1" t="s">
-        <v>82</v>
+      <c r="Y51" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z51" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA51" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="AB51" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC51" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD51" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="AE51" s="2" t="s">
         <v>21</v>
       </c>
       <c r="AF51" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG51" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH51" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AI51" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AJ51" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AK51" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="AL51" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="AM51" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN51" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="52" spans="1:40" x14ac:dyDescent="0.45">
+      <c r="A52" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="J52" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="K52" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="L52" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="M52" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="N52" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O52" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="P52" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q52" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="R52" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="S52" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T52" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="U52" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="V52" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="W52" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="X52" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y52" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Z52" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA52" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB52" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AC52" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="AG51" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AH51" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AI51" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AJ51" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AK51" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AL51" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AM51" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN51" s="1" t="s">
+      <c r="AD52" s="1" t="s">
         <v>82</v>
       </c>
+      <c r="AE52" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AF52" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="AG52" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH52" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AI52" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ52" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AK52" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AL52" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AM52" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN52" s="1" t="s">
+        <v>82</v>
+      </c>
     </row>
-    <row r="52" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A52" s="11" t="s">
+    <row r="53" spans="1:40" x14ac:dyDescent="0.45">
+      <c r="A53" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="B52" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E52" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F52" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G52" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="H52" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="I52" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="J52" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="K52" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="L52" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="M52" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="N52" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="O52" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="P52" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q52" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="R52" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="S52" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="T52" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="U52" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="V52" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="W52" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="X52" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="Y52" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="Z52" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="AA52" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="AB52" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC52" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AD52" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE52" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AF52" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="AG52" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AH52" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="AI52" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="AJ52" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AK52" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="AL52" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="AM52" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN52" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="53" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A53" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="H53" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I53" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="J53" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="K53" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="L53" s="1" t="s">
-        <v>74</v>
+      <c r="B53" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H53" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="I53" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J53" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="K53" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="L53" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="M53" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="N53" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="O53" s="1" t="s">
-        <v>74</v>
+      <c r="N53" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="O53" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="P53" s="2" t="s">
         <v>112</v>
@@ -7304,11 +7347,11 @@
       <c r="V53" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="W53" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="X53" s="1" t="s">
-        <v>74</v>
+      <c r="W53" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="X53" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="Y53" s="2" t="s">
         <v>112</v>
@@ -7325,11 +7368,11 @@
       <c r="AC53" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AD53" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AE53" s="2" t="s">
-        <v>21</v>
+      <c r="AD53" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE53" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="AF53" s="2" t="s">
         <v>112</v>
@@ -7343,8 +7386,8 @@
       <c r="AI53" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="AJ53" s="2" t="s">
-        <v>112</v>
+      <c r="AJ53" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="AK53" s="2" t="s">
         <v>112</v>
@@ -7355,251 +7398,373 @@
       <c r="AM53" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AN53" s="1" t="s">
-        <v>74</v>
+      <c r="AN53" s="3" t="s">
+        <v>62</v>
       </c>
     </row>
-    <row r="54" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A54" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J54" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K54" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="L54" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="M54" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="N54" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="O54" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="P54" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q54" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="R54" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="S54" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="T54" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="U54" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="V54" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="W54" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="X54" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y54" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z54" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA54" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="AB54" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC54" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD54" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AE54" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AF54" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG54" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH54" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="AI54" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="AJ54" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="AK54" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="AL54" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="AM54" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN54" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="55" spans="1:40" x14ac:dyDescent="0.45">
+      <c r="A55" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B55" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="C55" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D54" s="2" t="s">
+      <c r="D55" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E54" s="2" t="s">
+      <c r="E55" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F54" s="2" t="s">
+      <c r="F55" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G54" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="H54" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="I54" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="J54" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="K54" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="L54" s="2" t="s">
+      <c r="G55" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H55" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="I55" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J55" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="K55" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="L55" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="M54" s="2" t="s">
+      <c r="M55" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N54" s="2" t="s">
+      <c r="N55" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="O54" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="P54" s="2" t="s">
+      <c r="O55" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="P55" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="Q54" s="2" t="s">
+      <c r="Q55" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="R54" s="2" t="s">
+      <c r="R55" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="S54" s="2" t="s">
+      <c r="S55" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="T54" s="2" t="s">
+      <c r="T55" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="U54" s="2" t="s">
+      <c r="U55" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="V54" s="2" t="s">
+      <c r="V55" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="W54" s="2" t="s">
+      <c r="W55" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="X54" s="2" t="s">
+      <c r="X55" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="Y54" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="Z54" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AA54" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AB54" s="2" t="s">
+      <c r="Y55" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z55" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA55" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB55" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="AC54" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AD54" s="1" t="s">
+      <c r="AC55" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD55" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="AE54" s="1" t="s">
+      <c r="AE55" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="AF54" s="2" t="s">
+      <c r="AF55" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="AG54" s="2" t="s">
+      <c r="AG55" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="AH54" s="2" t="s">
+      <c r="AH55" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="AI54" s="2" t="s">
+      <c r="AI55" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="AJ54" s="2" t="s">
+      <c r="AJ55" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="AK54" s="2" t="s">
+      <c r="AK55" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="AL54" s="2" t="s">
+      <c r="AL55" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="AM54" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN54" s="1" t="s">
+      <c r="AM55" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN55" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="55" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A55" s="11" t="s">
+    <row r="56" spans="1:40" x14ac:dyDescent="0.45">
+      <c r="A56" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="B55" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D55" s="2" t="s">
+      <c r="B56" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D56" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="E55" s="2" t="s">
+      <c r="E56" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="F55" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="G55" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="H55" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I55" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="J55" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="K55" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="L55" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="M55" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="N55" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="O55" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="P55" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q55" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="R55" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="S55" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="T55" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="U55" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="V55" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="W55" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="X55" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="Y55" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="Z55" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AA55" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB55" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC55" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AD55" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AE55" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AF55" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AG55" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AH55" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI55" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AJ55" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AK55" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AL55" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AM55" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN55" s="1" t="s">
+      <c r="F56" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K56" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="L56" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="M56" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="N56" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="O56" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="P56" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q56" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="R56" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="S56" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="T56" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="U56" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="V56" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="W56" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="X56" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y56" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z56" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA56" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB56" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC56" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD56" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AE56" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF56" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AG56" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH56" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI56" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AJ56" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AK56" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AL56" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AM56" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN56" s="1" t="s">
         <v>74</v>
       </c>
     </row>
@@ -7610,19 +7775,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="8.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.9296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.06640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -7643,7 +7808,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
         <v>102</v>
       </c>
@@ -7663,7 +7828,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="5" t="s">
         <v>101</v>
       </c>
@@ -7683,7 +7848,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="5" t="s">
         <v>105</v>
       </c>
@@ -7703,7 +7868,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FIX: incomplete error management for base-16 binaries loading.
</commit_message>
<xml_diff>
--- a/docs/lexer/lexer-FSM.xlsx
+++ b/docs/lexer/lexer-FSM.xlsx
@@ -1,22 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Red\docs\lexer\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93FE0032-B15F-46E8-8A07-400445CAAC66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" tabRatio="564" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-100" yWindow="-40" windowWidth="22700" windowHeight="14540" tabRatio="564" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="transitions" sheetId="3" r:id="rId1"/>
     <sheet name="bin16 transitions" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -314,9 +308,6 @@
     <t>C_BIN</t>
   </si>
   <si>
-    <t>C_BIN_SKIP</t>
-  </si>
-  <si>
     <t>C_BIN_BLANK</t>
   </si>
   <si>
@@ -429,12 +420,15 @@
   </si>
   <si>
     <t>S_HEX_END</t>
+  </si>
+  <si>
+    <t>C_BIN_ILLEGAL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -642,7 +636,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -675,26 +669,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -727,23 +704,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -919,23 +879,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J36" sqref="A36:XFD36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.73046875" customWidth="1"/>
-    <col min="5" max="5" width="9.73046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="12" width="9.73046875" customWidth="1"/>
-    <col min="13" max="13" width="9.9296875" bestFit="1" customWidth="1"/>
-    <col min="14" max="40" width="9.73046875" customWidth="1"/>
+    <col min="1" max="1" width="10.36328125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" customWidth="1"/>
+    <col min="5" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="9.7265625" customWidth="1"/>
+    <col min="13" max="13" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="40" width="9.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -986,22 +946,22 @@
         <v>47</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="R1" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="S1" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="T1" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="U1" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="V1" s="6" t="s">
         <v>128</v>
-      </c>
-      <c r="V1" s="6" t="s">
-        <v>129</v>
       </c>
       <c r="W1" s="6" t="s">
         <v>48</v>
@@ -1016,7 +976,7 @@
         <v>51</v>
       </c>
       <c r="AA1" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AB1" s="6" t="s">
         <v>52</v>
@@ -1037,10 +997,10 @@
         <v>57</v>
       </c>
       <c r="AH1" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AI1" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AJ1" s="6" t="s">
         <v>58</v>
@@ -1058,7 +1018,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
@@ -1087,7 +1047,7 @@
         <v>67</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>62</v>
@@ -1099,10 +1059,10 @@
         <v>6</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="P2" s="2" t="s">
         <v>32</v>
@@ -1117,13 +1077,13 @@
         <v>32</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="U2" s="2" t="s">
         <v>32</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="W2" s="2" t="s">
         <v>5</v>
@@ -1153,7 +1113,7 @@
         <v>62</v>
       </c>
       <c r="AF2" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AG2" s="2" t="s">
         <v>22</v>
@@ -1180,7 +1140,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A3" s="11" t="s">
         <v>68</v>
       </c>
@@ -1188,7 +1148,7 @@
         <v>68</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>68</v>
@@ -1302,7 +1262,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A4" s="11" t="s">
         <v>69</v>
       </c>
@@ -1424,7 +1384,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -1546,7 +1506,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A6" s="12" t="s">
         <v>2</v>
       </c>
@@ -1575,10 +1535,10 @@
         <v>2</v>
       </c>
       <c r="J6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>2</v>
@@ -1668,7 +1628,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A7" s="11" t="s">
         <v>73</v>
       </c>
@@ -1790,7 +1750,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A8" s="11" t="s">
         <v>3</v>
       </c>
@@ -1825,7 +1785,7 @@
         <v>74</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M8" s="2" t="s">
         <v>4</v>
@@ -1912,7 +1872,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A9" s="11" t="s">
         <v>4</v>
       </c>
@@ -1995,7 +1955,7 @@
         <v>4</v>
       </c>
       <c r="AB9" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AC9" s="2" t="s">
         <v>4</v>
@@ -2034,9 +1994,9 @@
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A10" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>4</v>
@@ -2045,10 +2005,10 @@
         <v>4</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>62</v>
@@ -2090,16 +2050,16 @@
         <v>62</v>
       </c>
       <c r="S10" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="T10" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="U10" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="V10" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="W10" s="3" t="s">
         <v>62</v>
@@ -2156,9 +2116,9 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A11" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>4</v>
@@ -2212,10 +2172,10 @@
         <v>62</v>
       </c>
       <c r="S11" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="T11" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="U11" s="2" t="s">
         <v>4</v>
@@ -2278,120 +2238,120 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A12" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>75</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="R12" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="S12" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="T12" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="U12" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="V12" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="W12" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="X12" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="Y12" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="Z12" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AA12" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AB12" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AC12" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AD12" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AE12" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AF12" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AG12" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AH12" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AI12" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AJ12" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AK12" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AL12" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AM12" s="3" t="s">
         <v>62</v>
@@ -2400,7 +2360,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A13" s="11" t="s">
         <v>5</v>
       </c>
@@ -2522,7 +2482,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A14" s="11" t="s">
         <v>6</v>
       </c>
@@ -2644,7 +2604,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A15" s="11" t="s">
         <v>7</v>
       </c>
@@ -2766,7 +2726,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A16" s="11" t="s">
         <v>70</v>
       </c>
@@ -2888,7 +2848,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A17" s="11" t="s">
         <v>8</v>
       </c>
@@ -3010,7 +2970,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A18" s="11" t="s">
         <v>9</v>
       </c>
@@ -3132,7 +3092,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A19" s="11" t="s">
         <v>10</v>
       </c>
@@ -3254,7 +3214,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A20" s="11" t="s">
         <v>11</v>
       </c>
@@ -3376,7 +3336,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A21" s="11" t="s">
         <v>12</v>
       </c>
@@ -3429,19 +3389,19 @@
         <v>16</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="S21" s="2" t="s">
         <v>13</v>
       </c>
       <c r="T21" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="U21" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="V21" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="U21" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="V21" s="2" t="s">
-        <v>124</v>
       </c>
       <c r="W21" s="2" t="s">
         <v>16</v>
@@ -3498,7 +3458,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="22" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A22" s="11" t="s">
         <v>84</v>
       </c>
@@ -3620,7 +3580,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A23" s="11" t="s">
         <v>13</v>
       </c>
@@ -3742,9 +3702,9 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A24" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>85</v>
@@ -3753,10 +3713,10 @@
         <v>85</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>85</v>
@@ -3795,19 +3755,19 @@
         <v>62</v>
       </c>
       <c r="R24" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="S24" s="2" t="s">
         <v>13</v>
       </c>
       <c r="T24" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="U24" s="3" t="s">
         <v>62</v>
       </c>
       <c r="V24" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="W24" s="1" t="s">
         <v>85</v>
@@ -3864,7 +3824,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A25" s="11" t="s">
         <v>14</v>
       </c>
@@ -3878,37 +3838,37 @@
         <v>85</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M25" s="2" t="s">
         <v>14</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P25" s="2" t="s">
         <v>14</v>
@@ -3932,13 +3892,13 @@
         <v>14</v>
       </c>
       <c r="W25" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="X25" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Y25" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Z25" s="2" t="s">
         <v>14</v>
@@ -3947,22 +3907,22 @@
         <v>14</v>
       </c>
       <c r="AB25" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AC25" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AD25" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AE25" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AF25" s="2" t="s">
         <v>14</v>
       </c>
       <c r="AG25" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AH25" s="2" t="s">
         <v>14</v>
@@ -3971,7 +3931,7 @@
         <v>14</v>
       </c>
       <c r="AJ25" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AK25" s="2" t="s">
         <v>14</v>
@@ -3983,10 +3943,10 @@
         <v>62</v>
       </c>
       <c r="AN25" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
-    <row r="26" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A26" s="11" t="s">
         <v>15</v>
       </c>
@@ -4108,7 +4068,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A27" s="11" t="s">
         <v>16</v>
       </c>
@@ -4230,7 +4190,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="28" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A28" s="11" t="s">
         <v>17</v>
       </c>
@@ -4352,7 +4312,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A29" s="11" t="s">
         <v>18</v>
       </c>
@@ -4474,7 +4434,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="30" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A30" s="11" t="s">
         <v>19</v>
       </c>
@@ -4596,7 +4556,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A31" s="11" t="s">
         <v>20</v>
       </c>
@@ -4718,7 +4678,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="32" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A32" s="11" t="s">
         <v>22</v>
       </c>
@@ -4840,7 +4800,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A33" s="11" t="s">
         <v>23</v>
       </c>
@@ -4962,7 +4922,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="34" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A34" s="11" t="s">
         <v>24</v>
       </c>
@@ -5084,9 +5044,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="35" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A35" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>74</v>
@@ -5095,10 +5055,10 @@
         <v>74</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>74</v>
@@ -5137,19 +5097,19 @@
         <v>32</v>
       </c>
       <c r="R35" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="S35" s="2" t="s">
         <v>32</v>
       </c>
       <c r="T35" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="U35" s="2" t="s">
         <v>32</v>
       </c>
       <c r="V35" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="W35" s="1" t="s">
         <v>93</v>
@@ -5206,15 +5166,15 @@
         <v>74</v>
       </c>
     </row>
-    <row r="36" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A36" s="11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>32</v>
@@ -5223,25 +5183,25 @@
         <v>32</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="M36" s="3" t="s">
         <v>62</v>
@@ -5277,7 +5237,7 @@
         <v>93</v>
       </c>
       <c r="X36" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="Y36" s="2" t="s">
         <v>32</v>
@@ -5295,7 +5255,7 @@
         <v>62</v>
       </c>
       <c r="AD36" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AE36" s="2" t="s">
         <v>21</v>
@@ -5325,10 +5285,10 @@
         <v>62</v>
       </c>
       <c r="AN36" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
-    <row r="37" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A37" s="11" t="s">
         <v>25</v>
       </c>
@@ -5450,7 +5410,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="38" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A38" s="11" t="s">
         <v>26</v>
       </c>
@@ -5572,7 +5532,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="39" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A39" s="11" t="s">
         <v>27</v>
       </c>
@@ -5694,7 +5654,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A40" s="11" t="s">
         <v>28</v>
       </c>
@@ -5816,7 +5776,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="41" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A41" s="11" t="s">
         <v>29</v>
       </c>
@@ -5938,7 +5898,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="42" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A42" s="11" t="s">
         <v>30</v>
       </c>
@@ -6060,7 +6020,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="43" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A43" s="11" t="s">
         <v>31</v>
       </c>
@@ -6155,48 +6115,48 @@
         <v>32</v>
       </c>
       <c r="AF43" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="AG43" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH43" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI43" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AJ43" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AK43" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AL43" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AM43" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN43" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="44" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A44" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D44" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="AG43" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AH43" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI43" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AJ43" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AK43" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AL43" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AM43" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN43" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="44" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A44" s="11" t="s">
+      <c r="E44" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>121</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>74</v>
@@ -6238,10 +6198,10 @@
         <v>32</v>
       </c>
       <c r="S44" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="T44" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="U44" s="2" t="s">
         <v>32</v>
@@ -6283,10 +6243,10 @@
         <v>62</v>
       </c>
       <c r="AH44" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AI44" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AJ44" s="2" t="s">
         <v>32</v>
@@ -6304,9 +6264,9 @@
         <v>74</v>
       </c>
     </row>
-    <row r="45" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A45" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>85</v>
@@ -6315,10 +6275,10 @@
         <v>85</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>85</v>
@@ -6360,10 +6320,10 @@
         <v>62</v>
       </c>
       <c r="S45" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="T45" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="U45" s="3" t="s">
         <v>62</v>
@@ -6405,10 +6365,10 @@
         <v>62</v>
       </c>
       <c r="AH45" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AI45" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AJ45" s="3" t="s">
         <v>62</v>
@@ -6426,9 +6386,9 @@
         <v>85</v>
       </c>
     </row>
-    <row r="46" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A46" s="11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>62</v>
@@ -6548,7 +6508,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="47" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A47" s="11" t="s">
         <v>32</v>
       </c>
@@ -6670,7 +6630,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="48" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A48" s="11" t="s">
         <v>94</v>
       </c>
@@ -6792,7 +6752,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="49" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A49" s="11" t="s">
         <v>33</v>
       </c>
@@ -6914,7 +6874,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="50" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A50" s="11" t="s">
         <v>21</v>
       </c>
@@ -7036,21 +6996,21 @@
         <v>95</v>
       </c>
     </row>
-    <row r="51" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A51" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D51" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B51" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>111</v>
-      </c>
       <c r="E51" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F51" s="3" t="s">
         <v>62</v>
@@ -7074,34 +7034,34 @@
         <v>69</v>
       </c>
       <c r="M51" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N51" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O51" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="P51" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Q51" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="R51" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S51" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="T51" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="U51" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="V51" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="W51" s="3" t="s">
         <v>62</v>
@@ -7113,10 +7073,10 @@
         <v>25</v>
       </c>
       <c r="Z51" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AA51" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AB51" s="3" t="s">
         <v>62</v>
@@ -7131,25 +7091,25 @@
         <v>21</v>
       </c>
       <c r="AF51" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AG51" s="3" t="s">
         <v>62</v>
       </c>
       <c r="AH51" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AI51" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AJ51" s="3" t="s">
         <v>62</v>
       </c>
       <c r="AK51" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AL51" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AM51" s="3" t="s">
         <v>62</v>
@@ -7158,9 +7118,9 @@
         <v>62</v>
       </c>
     </row>
-    <row r="52" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A52" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>82</v>
@@ -7169,10 +7129,10 @@
         <v>82</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>82</v>
@@ -7280,9 +7240,9 @@
         <v>82</v>
       </c>
     </row>
-    <row r="53" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A53" s="11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>62</v>
@@ -7327,25 +7287,25 @@
         <v>62</v>
       </c>
       <c r="P53" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Q53" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="R53" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S53" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="T53" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="U53" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="V53" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="W53" s="3" t="s">
         <v>62</v>
@@ -7354,13 +7314,13 @@
         <v>62</v>
       </c>
       <c r="Y53" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Z53" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AA53" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AB53" s="3" t="s">
         <v>62</v>
@@ -7375,25 +7335,25 @@
         <v>62</v>
       </c>
       <c r="AF53" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AG53" s="3" t="s">
         <v>62</v>
       </c>
       <c r="AH53" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AI53" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AJ53" s="3" t="s">
         <v>62</v>
       </c>
       <c r="AK53" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AL53" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AM53" s="3" t="s">
         <v>62</v>
@@ -7402,9 +7362,9 @@
         <v>62</v>
       </c>
     </row>
-    <row r="54" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A54" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>74</v>
@@ -7413,10 +7373,10 @@
         <v>74</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>74</v>
@@ -7443,31 +7403,31 @@
         <v>62</v>
       </c>
       <c r="N54" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="O54" s="1" t="s">
         <v>74</v>
       </c>
       <c r="P54" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Q54" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="R54" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S54" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="T54" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="U54" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="V54" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="W54" s="1" t="s">
         <v>74</v>
@@ -7476,13 +7436,13 @@
         <v>74</v>
       </c>
       <c r="Y54" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Z54" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AA54" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AB54" s="3" t="s">
         <v>62</v>
@@ -7497,36 +7457,36 @@
         <v>21</v>
       </c>
       <c r="AF54" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="AG54" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH54" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="AI54" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="AJ54" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="AK54" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="AL54" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="AM54" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN54" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="55" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A55" s="11" t="s">
         <v>112</v>
-      </c>
-      <c r="AG54" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AH54" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="AI54" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="AJ54" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="AK54" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="AL54" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="AM54" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN54" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="55" spans="1:40" x14ac:dyDescent="0.45">
-      <c r="A55" s="11" t="s">
-        <v>113</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>81</v>
@@ -7646,9 +7606,9 @@
         <v>81</v>
       </c>
     </row>
-    <row r="56" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A56" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>74</v>
@@ -7657,10 +7617,10 @@
         <v>74</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>74</v>
@@ -7775,100 +7735,100 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.9296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.06640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.19921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="7"/>
       <c r="B1" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>106</v>
+      <c r="F2" s="2" t="s">
+        <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" s="5" t="s">
+    <row r="3" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A3" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="F3" s="9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A4" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>105</v>
+      <c r="E4" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A5" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FEAT: removes the bin16 FSM table.
Missing change from last commit.
</commit_message>
<xml_diff>
--- a/docs/lexer/lexer-FSM.xlsx
+++ b/docs/lexer/lexer-FSM.xlsx
@@ -8,14 +8,13 @@
   </bookViews>
   <sheets>
     <sheet name="transitions" sheetId="3" r:id="rId1"/>
-    <sheet name="bin16 transitions" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2182" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2159" uniqueCount="124">
   <si>
     <t>S_START</t>
   </si>
@@ -302,33 +301,6 @@
     <t>C_BIN</t>
   </si>
   <si>
-    <t>C_BIN_BLANK</t>
-  </si>
-  <si>
-    <t>C_BIN_LINE</t>
-  </si>
-  <si>
-    <t>C_BIN_HEXA</t>
-  </si>
-  <si>
-    <t>S_BIN_1ST</t>
-  </si>
-  <si>
-    <t>S_BIN_START</t>
-  </si>
-  <si>
-    <t>T_BIN_BYTE</t>
-  </si>
-  <si>
-    <t>T_BIN_ERROR</t>
-  </si>
-  <si>
-    <t>S_BIN_CMT</t>
-  </si>
-  <si>
-    <t>C_BIN_CMT</t>
-  </si>
-  <si>
     <t>S_FILE_HEX1</t>
   </si>
   <si>
@@ -414,16 +386,13 @@
   </si>
   <si>
     <t>S_HEX_END</t>
-  </si>
-  <si>
-    <t>C_BIN_ILLEGAL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -464,14 +433,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -534,7 +495,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -548,17 +509,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -883,7 +838,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.36328125" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.36328125" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.7265625" customWidth="1"/>
     <col min="5" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
@@ -893,127 +848,127 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="7"/>
-      <c r="B1" s="6" t="s">
+      <c r="A1" s="6"/>
+      <c r="B1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="Q1" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="S1" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="R1" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="S1" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="T1" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="U1" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="V1" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="W1" s="6" t="s">
+      <c r="T1" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="W1" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="X1" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="Y1" s="6" t="s">
+      <c r="Y1" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="Z1" s="6" t="s">
+      <c r="Z1" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="AA1" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="AB1" s="6" t="s">
+      <c r="AA1" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="AB1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="AC1" s="6" t="s">
+      <c r="AC1" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="AD1" s="6" t="s">
+      <c r="AD1" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="AE1" s="6" t="s">
+      <c r="AE1" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="AF1" s="6" t="s">
+      <c r="AF1" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="AG1" s="6" t="s">
+      <c r="AG1" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="AH1" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="AI1" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="AJ1" s="6" t="s">
+      <c r="AH1" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="AI1" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="AJ1" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="AK1" s="6" t="s">
+      <c r="AK1" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="AL1" s="6" t="s">
+      <c r="AL1" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="AM1" s="6" t="s">
+      <c r="AM1" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="AN1" s="6" t="s">
+      <c r="AN1" s="5" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1041,7 +996,7 @@
         <v>65</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>60</v>
@@ -1053,10 +1008,10 @@
         <v>6</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="P2" s="2" t="s">
         <v>30</v>
@@ -1071,13 +1026,13 @@
         <v>30</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="U2" s="2" t="s">
         <v>30</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="W2" s="2" t="s">
         <v>5</v>
@@ -1107,7 +1062,7 @@
         <v>60</v>
       </c>
       <c r="AF2" s="2" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="AG2" s="2" t="s">
         <v>22</v>
@@ -1135,14 +1090,14 @@
       </c>
     </row>
     <row r="3" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="9" t="s">
         <v>66</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>66</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>66</v>
@@ -1257,7 +1212,7 @@
       </c>
     </row>
     <row r="4" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="9" t="s">
         <v>67</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -1379,7 +1334,7 @@
       </c>
     </row>
     <row r="5" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -1501,7 +1456,7 @@
       </c>
     </row>
     <row r="6" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="10" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -1529,10 +1484,10 @@
         <v>2</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>2</v>
@@ -1623,7 +1578,7 @@
       </c>
     </row>
     <row r="7" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="9" t="s">
         <v>71</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -1745,7 +1700,7 @@
       </c>
     </row>
     <row r="8" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="9" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1779,7 +1734,7 @@
         <v>72</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="M8" s="2" t="s">
         <v>4</v>
@@ -1867,7 +1822,7 @@
       </c>
     </row>
     <row r="9" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="9" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1949,7 +1904,7 @@
         <v>4</v>
       </c>
       <c r="AB9" s="2" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="AC9" s="2" t="s">
         <v>4</v>
@@ -1989,8 +1944,8 @@
       </c>
     </row>
     <row r="10" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A10" s="11" t="s">
-        <v>104</v>
+      <c r="A10" s="9" t="s">
+        <v>95</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>4</v>
@@ -1999,10 +1954,10 @@
         <v>4</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>60</v>
@@ -2044,16 +1999,16 @@
         <v>60</v>
       </c>
       <c r="S10" s="2" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="T10" s="2" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="U10" s="2" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="V10" s="2" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="W10" s="3" t="s">
         <v>60</v>
@@ -2111,8 +2066,8 @@
       </c>
     </row>
     <row r="11" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A11" s="11" t="s">
-        <v>105</v>
+      <c r="A11" s="9" t="s">
+        <v>96</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>4</v>
@@ -2166,10 +2121,10 @@
         <v>60</v>
       </c>
       <c r="S11" s="2" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="T11" s="2" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="U11" s="2" t="s">
         <v>4</v>
@@ -2233,119 +2188,119 @@
       </c>
     </row>
     <row r="12" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A12" s="11" t="s">
-        <v>106</v>
+      <c r="A12" s="9" t="s">
+        <v>97</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>73</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="R12" s="2" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="S12" s="2" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="T12" s="2" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="U12" s="2" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="V12" s="2" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="W12" s="2" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="X12" s="2" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="Y12" s="2" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="Z12" s="2" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="AA12" s="2" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="AB12" s="2" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="AC12" s="2" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="AD12" s="2" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="AE12" s="2" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="AF12" s="2" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="AG12" s="2" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="AH12" s="2" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="AI12" s="2" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="AJ12" s="2" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="AK12" s="2" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="AL12" s="2" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="AM12" s="3" t="s">
         <v>60</v>
@@ -2355,7 +2310,7 @@
       </c>
     </row>
     <row r="13" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -2477,7 +2432,7 @@
       </c>
     </row>
     <row r="14" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -2599,7 +2554,7 @@
       </c>
     </row>
     <row r="15" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="9" t="s">
         <v>7</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -2721,7 +2676,7 @@
       </c>
     </row>
     <row r="16" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="9" t="s">
         <v>68</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -2843,7 +2798,7 @@
       </c>
     </row>
     <row r="17" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -2965,7 +2920,7 @@
       </c>
     </row>
     <row r="18" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="9" t="s">
         <v>9</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -3087,7 +3042,7 @@
       </c>
     </row>
     <row r="19" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="9" t="s">
         <v>10</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -3209,7 +3164,7 @@
       </c>
     </row>
     <row r="20" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -3331,7 +3286,7 @@
       </c>
     </row>
     <row r="21" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="9" t="s">
         <v>12</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -3383,19 +3338,19 @@
         <v>16</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="S21" s="2" t="s">
         <v>13</v>
       </c>
       <c r="T21" s="2" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="U21" s="3" t="s">
         <v>60</v>
       </c>
       <c r="V21" s="2" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="W21" s="2" t="s">
         <v>16</v>
@@ -3453,7 +3408,7 @@
       </c>
     </row>
     <row r="22" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="9" t="s">
         <v>82</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -3575,7 +3530,7 @@
       </c>
     </row>
     <row r="23" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="9" t="s">
         <v>13</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -3697,8 +3652,8 @@
       </c>
     </row>
     <row r="24" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A24" s="11" t="s">
-        <v>120</v>
+      <c r="A24" s="9" t="s">
+        <v>111</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>83</v>
@@ -3707,10 +3662,10 @@
         <v>83</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>83</v>
@@ -3749,19 +3704,19 @@
         <v>60</v>
       </c>
       <c r="R24" s="1" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="S24" s="2" t="s">
         <v>13</v>
       </c>
       <c r="T24" s="2" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="U24" s="3" t="s">
         <v>60</v>
       </c>
       <c r="V24" s="2" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="W24" s="1" t="s">
         <v>83</v>
@@ -3819,7 +3774,7 @@
       </c>
     </row>
     <row r="25" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A25" s="11" t="s">
+      <c r="A25" s="9" t="s">
         <v>14</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -3832,37 +3787,37 @@
         <v>83</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="M25" s="2" t="s">
         <v>14</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="P25" s="2" t="s">
         <v>14</v>
@@ -3886,13 +3841,13 @@
         <v>14</v>
       </c>
       <c r="W25" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="X25" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="Y25" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="Z25" s="2" t="s">
         <v>14</v>
@@ -3901,22 +3856,22 @@
         <v>14</v>
       </c>
       <c r="AB25" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="AC25" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="AD25" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="AE25" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="AF25" s="2" t="s">
         <v>14</v>
       </c>
       <c r="AG25" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="AH25" s="2" t="s">
         <v>14</v>
@@ -3925,7 +3880,7 @@
         <v>14</v>
       </c>
       <c r="AJ25" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="AK25" s="2" t="s">
         <v>14</v>
@@ -3937,11 +3892,11 @@
         <v>60</v>
       </c>
       <c r="AN25" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="26" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A26" s="11" t="s">
+      <c r="A26" s="9" t="s">
         <v>15</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -4063,7 +4018,7 @@
       </c>
     </row>
     <row r="27" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A27" s="11" t="s">
+      <c r="A27" s="9" t="s">
         <v>16</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -4185,7 +4140,7 @@
       </c>
     </row>
     <row r="28" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A28" s="11" t="s">
+      <c r="A28" s="9" t="s">
         <v>17</v>
       </c>
       <c r="B28" s="3" t="s">
@@ -4307,7 +4262,7 @@
       </c>
     </row>
     <row r="29" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A29" s="11" t="s">
+      <c r="A29" s="9" t="s">
         <v>18</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -4429,7 +4384,7 @@
       </c>
     </row>
     <row r="30" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A30" s="11" t="s">
+      <c r="A30" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B30" s="3" t="s">
@@ -4551,7 +4506,7 @@
       </c>
     </row>
     <row r="31" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A31" s="11" t="s">
+      <c r="A31" s="9" t="s">
         <v>20</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -4673,7 +4628,7 @@
       </c>
     </row>
     <row r="32" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A32" s="11" t="s">
+      <c r="A32" s="9" t="s">
         <v>22</v>
       </c>
       <c r="B32" s="3" t="s">
@@ -4795,7 +4750,7 @@
       </c>
     </row>
     <row r="33" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A33" s="11" t="s">
+      <c r="A33" s="9" t="s">
         <v>23</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -4917,7 +4872,7 @@
       </c>
     </row>
     <row r="34" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A34" s="11" t="s">
+      <c r="A34" s="9" t="s">
         <v>24</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -5039,8 +4994,8 @@
       </c>
     </row>
     <row r="35" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A35" s="11" t="s">
-        <v>121</v>
+      <c r="A35" s="9" t="s">
+        <v>112</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>72</v>
@@ -5049,10 +5004,10 @@
         <v>72</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>72</v>
@@ -5091,19 +5046,19 @@
         <v>30</v>
       </c>
       <c r="R35" s="2" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="S35" s="2" t="s">
         <v>30</v>
       </c>
       <c r="T35" s="2" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="U35" s="2" t="s">
         <v>30</v>
       </c>
       <c r="V35" s="2" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="W35" s="1" t="s">
         <v>91</v>
@@ -5161,14 +5116,14 @@
       </c>
     </row>
     <row r="36" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A36" s="11" t="s">
-        <v>132</v>
+      <c r="A36" s="9" t="s">
+        <v>123</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>30</v>
@@ -5177,25 +5132,25 @@
         <v>30</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="M36" s="3" t="s">
         <v>60</v>
@@ -5231,7 +5186,7 @@
         <v>91</v>
       </c>
       <c r="X36" s="1" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="Y36" s="2" t="s">
         <v>30</v>
@@ -5249,7 +5204,7 @@
         <v>60</v>
       </c>
       <c r="AD36" s="1" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="AE36" s="2" t="s">
         <v>21</v>
@@ -5279,11 +5234,11 @@
         <v>60</v>
       </c>
       <c r="AN36" s="1" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
     </row>
     <row r="37" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A37" s="11" t="s">
+      <c r="A37" s="9" t="s">
         <v>25</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -5405,7 +5360,7 @@
       </c>
     </row>
     <row r="38" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A38" s="11" t="s">
+      <c r="A38" s="9" t="s">
         <v>26</v>
       </c>
       <c r="B38" s="2" t="s">
@@ -5527,7 +5482,7 @@
       </c>
     </row>
     <row r="39" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A39" s="11" t="s">
+      <c r="A39" s="9" t="s">
         <v>27</v>
       </c>
       <c r="B39" s="2" t="s">
@@ -5649,7 +5604,7 @@
       </c>
     </row>
     <row r="40" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A40" s="11" t="s">
+      <c r="A40" s="9" t="s">
         <v>28</v>
       </c>
       <c r="B40" s="2" t="s">
@@ -5771,7 +5726,7 @@
       </c>
     </row>
     <row r="41" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A41" s="11" t="s">
+      <c r="A41" s="9" t="s">
         <v>29</v>
       </c>
       <c r="B41" s="1" t="s">
@@ -5865,7 +5820,7 @@
         <v>30</v>
       </c>
       <c r="AF41" s="2" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="AG41" s="2" t="s">
         <v>30</v>
@@ -5893,8 +5848,8 @@
       </c>
     </row>
     <row r="42" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A42" s="11" t="s">
-        <v>117</v>
+      <c r="A42" s="9" t="s">
+        <v>108</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>72</v>
@@ -5903,10 +5858,10 @@
         <v>72</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>72</v>
@@ -5948,10 +5903,10 @@
         <v>30</v>
       </c>
       <c r="S42" s="2" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="T42" s="2" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="U42" s="2" t="s">
         <v>30</v>
@@ -5993,10 +5948,10 @@
         <v>60</v>
       </c>
       <c r="AH42" s="2" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="AI42" s="2" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="AJ42" s="2" t="s">
         <v>30</v>
@@ -6015,8 +5970,8 @@
       </c>
     </row>
     <row r="43" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A43" s="11" t="s">
-        <v>118</v>
+      <c r="A43" s="9" t="s">
+        <v>109</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>83</v>
@@ -6025,10 +5980,10 @@
         <v>83</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>83</v>
@@ -6070,10 +6025,10 @@
         <v>60</v>
       </c>
       <c r="S43" s="2" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="T43" s="2" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="U43" s="3" t="s">
         <v>60</v>
@@ -6115,10 +6070,10 @@
         <v>60</v>
       </c>
       <c r="AH43" s="2" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="AI43" s="2" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="AJ43" s="3" t="s">
         <v>60</v>
@@ -6137,8 +6092,8 @@
       </c>
     </row>
     <row r="44" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A44" s="11" t="s">
-        <v>130</v>
+      <c r="A44" s="9" t="s">
+        <v>121</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>60</v>
@@ -6259,7 +6214,7 @@
       </c>
     </row>
     <row r="45" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A45" s="11" t="s">
+      <c r="A45" s="9" t="s">
         <v>30</v>
       </c>
       <c r="B45" s="1" t="s">
@@ -6381,7 +6336,7 @@
       </c>
     </row>
     <row r="46" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A46" s="11" t="s">
+      <c r="A46" s="9" t="s">
         <v>92</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -6503,7 +6458,7 @@
       </c>
     </row>
     <row r="47" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A47" s="11" t="s">
+      <c r="A47" s="9" t="s">
         <v>31</v>
       </c>
       <c r="B47" s="1" t="s">
@@ -6625,7 +6580,7 @@
       </c>
     </row>
     <row r="48" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A48" s="11" t="s">
+      <c r="A48" s="9" t="s">
         <v>21</v>
       </c>
       <c r="B48" s="1" t="s">
@@ -6747,8 +6702,8 @@
       </c>
     </row>
     <row r="49" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A49" s="12" t="s">
-        <v>107</v>
+      <c r="A49" s="10" t="s">
+        <v>98</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>60</v>
@@ -6757,10 +6712,10 @@
         <v>60</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="F49" s="3" t="s">
         <v>60</v>
@@ -6784,34 +6739,34 @@
         <v>67</v>
       </c>
       <c r="M49" s="2" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="N49" s="2" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="O49" s="2" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="P49" s="2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="Q49" s="2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="R49" s="2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="S49" s="2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="T49" s="2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="U49" s="2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="V49" s="2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="W49" s="3" t="s">
         <v>60</v>
@@ -6823,10 +6778,10 @@
         <v>25</v>
       </c>
       <c r="Z49" s="2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="AA49" s="2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="AB49" s="3" t="s">
         <v>60</v>
@@ -6841,25 +6796,25 @@
         <v>21</v>
       </c>
       <c r="AF49" s="2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="AG49" s="3" t="s">
         <v>60</v>
       </c>
       <c r="AH49" s="2" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="AI49" s="2" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="AJ49" s="3" t="s">
         <v>60</v>
       </c>
       <c r="AK49" s="2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="AL49" s="2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="AM49" s="3" t="s">
         <v>60</v>
@@ -6869,8 +6824,8 @@
       </c>
     </row>
     <row r="50" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A50" s="11" t="s">
-        <v>108</v>
+      <c r="A50" s="9" t="s">
+        <v>99</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>80</v>
@@ -6879,10 +6834,10 @@
         <v>80</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>80</v>
@@ -6990,9 +6945,9 @@
         <v>80</v>
       </c>
     </row>
-    <row r="51" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A51" s="11" t="s">
-        <v>131</v>
+    <row r="51" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="A51" s="9" t="s">
+        <v>122</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>60</v>
@@ -7037,25 +6992,25 @@
         <v>60</v>
       </c>
       <c r="P51" s="2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="Q51" s="2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="R51" s="2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="S51" s="2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="T51" s="2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="U51" s="2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="V51" s="2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="W51" s="3" t="s">
         <v>60</v>
@@ -7064,13 +7019,13 @@
         <v>60</v>
       </c>
       <c r="Y51" s="2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="Z51" s="2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="AA51" s="2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="AB51" s="3" t="s">
         <v>60</v>
@@ -7085,25 +7040,25 @@
         <v>60</v>
       </c>
       <c r="AF51" s="2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="AG51" s="3" t="s">
         <v>60</v>
       </c>
       <c r="AH51" s="2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="AI51" s="2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="AJ51" s="3" t="s">
         <v>60</v>
       </c>
       <c r="AK51" s="2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="AL51" s="2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="AM51" s="3" t="s">
         <v>60</v>
@@ -7112,9 +7067,9 @@
         <v>60</v>
       </c>
     </row>
-    <row r="52" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A52" s="11" t="s">
-        <v>109</v>
+    <row r="52" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="A52" s="9" t="s">
+        <v>100</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>72</v>
@@ -7123,10 +7078,10 @@
         <v>72</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>72</v>
@@ -7153,31 +7108,31 @@
         <v>60</v>
       </c>
       <c r="N52" s="2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="O52" s="1" t="s">
         <v>72</v>
       </c>
       <c r="P52" s="2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="Q52" s="2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="R52" s="2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="S52" s="2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="T52" s="2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="U52" s="2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="V52" s="2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="W52" s="1" t="s">
         <v>72</v>
@@ -7186,13 +7141,13 @@
         <v>72</v>
       </c>
       <c r="Y52" s="2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="Z52" s="2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="AA52" s="2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="AB52" s="3" t="s">
         <v>60</v>
@@ -7207,25 +7162,25 @@
         <v>21</v>
       </c>
       <c r="AF52" s="2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="AG52" s="3" t="s">
         <v>60</v>
       </c>
       <c r="AH52" s="2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="AI52" s="2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="AJ52" s="2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="AK52" s="2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="AL52" s="2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="AM52" s="3" t="s">
         <v>60</v>
@@ -7234,9 +7189,9 @@
         <v>72</v>
       </c>
     </row>
-    <row r="53" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A53" s="11" t="s">
-        <v>110</v>
+    <row r="53" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="A53" s="9" t="s">
+        <v>101</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>79</v>
@@ -7356,9 +7311,9 @@
         <v>79</v>
       </c>
     </row>
-    <row r="54" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A54" s="11" t="s">
-        <v>111</v>
+    <row r="54" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="A54" s="9" t="s">
+        <v>102</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>72</v>
@@ -7367,10 +7322,10 @@
         <v>72</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>72</v>
@@ -7477,109 +7432,6 @@
       <c r="AN54" s="1" t="s">
         <v>72</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="8.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.1796875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="7"/>
-      <c r="B1" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A3" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A4" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A5" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
FIX: hex literals ending not always checked for illegal characters.
</commit_message>
<xml_diff>
--- a/docs/lexer/lexer-FSM.xlsx
+++ b/docs/lexer/lexer-FSM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2159" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2199" uniqueCount="125">
   <si>
     <t>S_START</t>
   </si>
@@ -386,6 +386,9 @@
   </si>
   <si>
     <t>S_HEX_END</t>
+  </si>
+  <si>
+    <t>S_HEX_END2</t>
   </si>
 </sst>
 </file>
@@ -829,11 +832,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AN54"/>
+  <dimension ref="A1:AN55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O40" sqref="O40"/>
+      <selection pane="bottomLeft" activeCell="AL37" sqref="AL37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3285,7 +3288,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="21" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
         <v>12</v>
       </c>
@@ -3337,8 +3340,8 @@
       <c r="Q21" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R21" s="1" t="s">
-        <v>118</v>
+      <c r="R21" s="2" t="s">
+        <v>124</v>
       </c>
       <c r="S21" s="2" t="s">
         <v>13</v>
@@ -3651,7 +3654,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A24" s="9" t="s">
         <v>111</v>
       </c>
@@ -3703,8 +3706,8 @@
       <c r="Q24" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="R24" s="1" t="s">
-        <v>118</v>
+      <c r="R24" s="2" t="s">
+        <v>124</v>
       </c>
       <c r="S24" s="2" t="s">
         <v>13</v>
@@ -5115,7 +5118,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="36" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A36" s="9" t="s">
         <v>123</v>
       </c>
@@ -5237,137 +5240,137 @@
         <v>118</v>
       </c>
     </row>
-    <row r="37" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A37" s="9" t="s">
-        <v>25</v>
+        <v>124</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>72</v>
+        <v>118</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>26</v>
+        <v>118</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>72</v>
+        <v>118</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>72</v>
+        <v>118</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>72</v>
+        <v>118</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>72</v>
+        <v>118</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>72</v>
+        <v>118</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>72</v>
+        <v>118</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="M37" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N37" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="O37" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="P37" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q37" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="R37" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="S37" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="T37" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="U37" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="V37" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="W37" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="X37" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y37" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="Z37" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AA37" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AB37" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC37" s="2" t="s">
-        <v>26</v>
+        <v>118</v>
+      </c>
+      <c r="M37" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="N37" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="O37" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="P37" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q37" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="R37" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="S37" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="T37" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="U37" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="V37" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="W37" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="X37" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="Y37" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="Z37" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA37" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB37" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC37" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="AD37" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AE37" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AF37" s="2" t="s">
-        <v>26</v>
+        <v>118</v>
+      </c>
+      <c r="AE37" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AF37" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="AG37" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AH37" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AI37" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AJ37" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AK37" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AL37" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
+      </c>
+      <c r="AH37" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AI37" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AJ37" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK37" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AL37" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="AM37" s="3" t="s">
         <v>60</v>
       </c>
       <c r="AN37" s="1" t="s">
-        <v>72</v>
+        <v>118</v>
       </c>
     </row>
     <row r="38" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A38" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>72</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>26</v>
@@ -5375,35 +5378,35 @@
       <c r="E38" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F38" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="J38" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="K38" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="L38" s="2" t="s">
-        <v>27</v>
+      <c r="F38" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="L38" s="1" t="s">
+        <v>72</v>
       </c>
       <c r="M38" s="2" t="s">
         <v>26</v>
       </c>
       <c r="N38" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="O38" s="2" t="s">
         <v>26</v>
+      </c>
+      <c r="O38" s="1" t="s">
+        <v>72</v>
       </c>
       <c r="P38" s="2" t="s">
         <v>26</v>
@@ -5433,13 +5436,13 @@
         <v>26</v>
       </c>
       <c r="Y38" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z38" s="1" t="s">
-        <v>88</v>
+        <v>30</v>
+      </c>
+      <c r="Z38" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="AA38" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="AB38" s="2" t="s">
         <v>26</v>
@@ -5447,11 +5450,11 @@
       <c r="AC38" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AD38" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AE38" s="2" t="s">
-        <v>26</v>
+      <c r="AD38" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE38" s="1" t="s">
+        <v>72</v>
       </c>
       <c r="AF38" s="2" t="s">
         <v>26</v>
@@ -5477,124 +5480,124 @@
       <c r="AM38" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="AN38" s="3" t="s">
-        <v>60</v>
+      <c r="AN38" s="1" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="39" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A39" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K39" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L39" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I39" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="J39" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="K39" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="L39" s="2" t="s">
+      <c r="M39" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="M39" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="N39" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O39" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P39" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q39" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R39" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S39" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T39" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="U39" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="V39" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W39" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X39" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Y39" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z39" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="Z39" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="AA39" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AB39" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AC39" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AD39" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AE39" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AF39" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AG39" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AH39" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AI39" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AJ39" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AK39" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AL39" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AM39" s="3" t="s">
         <v>60</v>
@@ -5605,118 +5608,118 @@
     </row>
     <row r="40" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A40" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L40" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="M40" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N40" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O40" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P40" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q40" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R40" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S40" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="T40" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="U40" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="V40" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="W40" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="X40" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Y40" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Z40" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AA40" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AB40" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AC40" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AD40" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AE40" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AF40" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AG40" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AH40" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AI40" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AJ40" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AK40" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AL40" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AM40" s="3" t="s">
         <v>60</v>
@@ -5727,234 +5730,234 @@
     </row>
     <row r="41" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A41" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K41" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L41" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M41" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N41" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O41" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="P41" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q41" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="R41" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="S41" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="T41" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="U41" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="V41" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="W41" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="X41" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y41" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z41" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA41" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB41" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC41" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD41" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE41" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF41" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG41" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH41" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AI41" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AJ41" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AK41" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AL41" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AM41" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN41" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="A42" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D41" s="2" t="s">
+      <c r="B42" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E41" s="2" t="s">
+      <c r="E42" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F41" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="I41" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="J41" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="K41" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="L41" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="M41" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="N41" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="O41" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="P41" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q41" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="R41" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="S41" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="T41" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="U41" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="V41" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="W41" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="X41" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="Y41" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="Z41" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AA41" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AB41" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AC41" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AD41" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AE41" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF41" s="2" t="s">
+      <c r="F42" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="L42" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="M42" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="N42" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="O42" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="P42" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q42" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="R42" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="S42" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="T42" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="U42" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="V42" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="W42" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="X42" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y42" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z42" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA42" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB42" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC42" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD42" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE42" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF42" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="AG41" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AH41" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AI41" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AJ41" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AK41" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AL41" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AM41" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AN41" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="42" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A42" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="I42" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="J42" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="K42" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="L42" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="M42" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="N42" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="O42" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="P42" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q42" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="R42" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="S42" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="T42" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="U42" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="V42" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="W42" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="X42" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="Y42" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="Z42" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AA42" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AB42" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AC42" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AD42" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AE42" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AF42" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AG42" s="3" t="s">
-        <v>60</v>
+      <c r="AG42" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="AH42" s="2" t="s">
-        <v>109</v>
+        <v>30</v>
       </c>
       <c r="AI42" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="AJ42" s="2" t="s">
-        <v>30</v>
+        <v>30</v>
+      </c>
+      <c r="AJ42" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="AK42" s="2" t="s">
         <v>30</v>
@@ -5971,13 +5974,13 @@
     </row>
     <row r="43" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A43" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>109</v>
@@ -5986,43 +5989,43 @@
         <v>109</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="L43" s="1" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="M43" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="N43" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="O43" s="1" t="s">
-        <v>83</v>
+      <c r="N43" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="O43" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="P43" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q43" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="R43" s="3" t="s">
-        <v>60</v>
+        <v>30</v>
+      </c>
+      <c r="Q43" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="R43" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="S43" s="2" t="s">
         <v>109</v>
@@ -6030,41 +6033,41 @@
       <c r="T43" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="U43" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="V43" s="3" t="s">
-        <v>60</v>
+      <c r="U43" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="V43" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="W43" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="X43" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="Y43" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="Z43" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AA43" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AB43" s="1" t="s">
-        <v>81</v>
+        <v>91</v>
+      </c>
+      <c r="X43" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y43" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z43" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA43" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB43" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="AC43" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="AD43" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AE43" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AF43" s="3" t="s">
-        <v>60</v>
+      <c r="AD43" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE43" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AF43" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="AG43" s="3" t="s">
         <v>60</v>
@@ -6075,58 +6078,58 @@
       <c r="AI43" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="AJ43" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AK43" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AL43" s="3" t="s">
-        <v>60</v>
+      <c r="AJ43" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AK43" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AL43" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="AM43" s="3" t="s">
         <v>60</v>
       </c>
       <c r="AN43" s="1" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
     </row>
     <row r="44" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A44" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="F44" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G44" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="H44" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="I44" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="J44" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="K44" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="L44" s="3" t="s">
-        <v>60</v>
+        <v>109</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>83</v>
       </c>
       <c r="M44" s="3" t="s">
         <v>60</v>
@@ -6134,47 +6137,47 @@
       <c r="N44" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="O44" s="3" t="s">
-        <v>60</v>
+      <c r="O44" s="1" t="s">
+        <v>83</v>
       </c>
       <c r="P44" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q44" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="R44" s="2" t="s">
-        <v>30</v>
+        <v>19</v>
+      </c>
+      <c r="Q44" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="R44" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="S44" s="2" t="s">
-        <v>30</v>
+        <v>109</v>
       </c>
       <c r="T44" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="U44" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="V44" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="W44" s="2" t="s">
-        <v>5</v>
+        <v>109</v>
+      </c>
+      <c r="U44" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="V44" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="W44" s="1" t="s">
+        <v>83</v>
       </c>
       <c r="X44" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="Y44" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="Z44" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AA44" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AB44" s="3" t="s">
-        <v>60</v>
+      <c r="Y44" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Z44" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA44" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB44" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="AC44" s="3" t="s">
         <v>60</v>
@@ -6185,79 +6188,79 @@
       <c r="AE44" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="AF44" s="2" t="s">
-        <v>30</v>
+      <c r="AF44" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="AG44" s="3" t="s">
         <v>60</v>
       </c>
       <c r="AH44" s="2" t="s">
-        <v>30</v>
+        <v>109</v>
       </c>
       <c r="AI44" s="2" t="s">
-        <v>30</v>
+        <v>109</v>
       </c>
       <c r="AJ44" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="AK44" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AL44" s="2" t="s">
-        <v>30</v>
+      <c r="AK44" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AL44" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="AM44" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="AN44" s="3" t="s">
-        <v>60</v>
+      <c r="AN44" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="45" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A45" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="I45" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="J45" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="K45" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="L45" s="1" t="s">
-        <v>72</v>
+        <v>121</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I45" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="J45" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="K45" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="L45" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="M45" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="N45" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="O45" s="2" t="s">
-        <v>92</v>
+      <c r="N45" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="O45" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="P45" s="2" t="s">
         <v>30</v>
@@ -6280,11 +6283,11 @@
       <c r="V45" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="W45" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="X45" s="1" t="s">
-        <v>72</v>
+      <c r="W45" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="X45" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="Y45" s="2" t="s">
         <v>30</v>
@@ -6301,17 +6304,17 @@
       <c r="AC45" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="AD45" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AE45" s="2" t="s">
-        <v>21</v>
+      <c r="AD45" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE45" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="AF45" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AG45" s="2" t="s">
-        <v>23</v>
+      <c r="AG45" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="AH45" s="2" t="s">
         <v>30</v>
@@ -6319,8 +6322,8 @@
       <c r="AI45" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AJ45" s="2" t="s">
-        <v>30</v>
+      <c r="AJ45" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="AK45" s="2" t="s">
         <v>30</v>
@@ -6331,124 +6334,124 @@
       <c r="AM45" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="AN45" s="1" t="s">
-        <v>72</v>
+      <c r="AN45" s="3" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="46" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A46" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="L46" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="M46" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="N46" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="O46" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="I46" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="J46" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="K46" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="L46" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="M46" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="N46" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="O46" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="P46" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q46" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="R46" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="S46" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="T46" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="U46" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="V46" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="W46" s="4" t="s">
-        <v>31</v>
+      <c r="P46" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q46" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="R46" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="S46" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="T46" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="U46" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="V46" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="W46" s="1" t="s">
+        <v>91</v>
       </c>
       <c r="X46" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="Y46" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="Z46" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AA46" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB46" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AC46" s="4" t="s">
-        <v>31</v>
+      <c r="Y46" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z46" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA46" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB46" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC46" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="AD46" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AE46" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AF46" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG46" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH46" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AI46" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AJ46" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AK46" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL46" s="4" t="s">
-        <v>31</v>
+      <c r="AE46" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AF46" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG46" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH46" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AI46" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AJ46" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AK46" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AL46" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="AM46" s="3" t="s">
         <v>60</v>
@@ -6459,13 +6462,13 @@
     </row>
     <row r="47" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A47" s="9" t="s">
-        <v>31</v>
+        <v>92</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>31</v>
@@ -6474,364 +6477,364 @@
         <v>31</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="M47" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="M47" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="N47" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="O47" s="2" t="s">
+      <c r="N47" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="P47" s="2" t="s">
+      <c r="O47" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="Q47" s="2" t="s">
+      <c r="P47" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="R47" s="2" t="s">
+      <c r="Q47" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="S47" s="2" t="s">
+      <c r="R47" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="T47" s="2" t="s">
+      <c r="S47" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="U47" s="2" t="s">
+      <c r="T47" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="V47" s="2" t="s">
+      <c r="U47" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="W47" s="2" t="s">
+      <c r="V47" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="W47" s="4" t="s">
+        <v>31</v>
+      </c>
       <c r="X47" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="Y47" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="Z47" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AA47" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y47" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z47" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AB47" s="2" t="s">
+      <c r="AA47" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AC47" s="1" t="s">
-        <v>90</v>
+      <c r="AB47" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC47" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="AD47" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="AE47" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE47" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AF47" s="2" t="s">
+      <c r="AF47" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AG47" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AH47" s="2" t="s">
+      <c r="AG47" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AI47" s="2" t="s">
+      <c r="AH47" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AJ47" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AK47" s="2" t="s">
+      <c r="AI47" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AL47" s="2" t="s">
+      <c r="AJ47" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="AK47" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL47" s="4" t="s">
+        <v>31</v>
+      </c>
       <c r="AM47" s="3" t="s">
         <v>60</v>
       </c>
       <c r="AN47" s="1" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
     </row>
     <row r="48" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A48" s="9" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="L48" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="M48" s="3" t="s">
-        <v>60</v>
+        <v>90</v>
+      </c>
+      <c r="M48" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="N48" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="O48" s="3" t="s">
-        <v>60</v>
+      <c r="O48" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="P48" s="2" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="Q48" s="2" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="R48" s="2" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="S48" s="2" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="T48" s="2" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="U48" s="2" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="V48" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="W48" s="1" t="s">
-        <v>93</v>
+        <v>31</v>
+      </c>
+      <c r="W48" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="X48" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="Y48" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="Z48" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="AA48" s="3" t="s">
-        <v>60</v>
+      <c r="AA48" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="AB48" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AC48" s="3" t="s">
-        <v>60</v>
+        <v>31</v>
+      </c>
+      <c r="AC48" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="AD48" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="AE48" s="3" t="s">
-        <v>60</v>
+        <v>90</v>
+      </c>
+      <c r="AE48" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="AF48" s="2" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="AG48" s="3" t="s">
         <v>60</v>
       </c>
       <c r="AH48" s="2" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="AI48" s="2" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="AJ48" s="3" t="s">
         <v>60</v>
       </c>
       <c r="AK48" s="2" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="AL48" s="2" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="AM48" s="3" t="s">
         <v>60</v>
       </c>
       <c r="AN48" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="49" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A49" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>60</v>
+      <c r="A49" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>99</v>
+        <v>21</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="F49" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G49" s="3" t="s">
-        <v>60</v>
+        <v>21</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>63</v>
+        <v>93</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="J49" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="K49" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="L49" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="M49" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="N49" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="O49" s="2" t="s">
-        <v>122</v>
+        <v>93</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="L49" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="M49" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="N49" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="O49" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="P49" s="2" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="Q49" s="2" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="R49" s="2" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="S49" s="2" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="T49" s="2" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="U49" s="2" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="V49" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="W49" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="X49" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="Y49" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="Z49" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="AA49" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="AB49" s="3" t="s">
-        <v>60</v>
+        <v>21</v>
+      </c>
+      <c r="W49" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="X49" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="Y49" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z49" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA49" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB49" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="AC49" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="AD49" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AE49" s="2" t="s">
+      <c r="AD49" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AE49" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF49" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AF49" s="2" t="s">
-        <v>100</v>
-      </c>
       <c r="AG49" s="3" t="s">
         <v>60</v>
       </c>
       <c r="AH49" s="2" t="s">
-        <v>102</v>
+        <v>21</v>
       </c>
       <c r="AI49" s="2" t="s">
-        <v>102</v>
+        <v>21</v>
       </c>
       <c r="AJ49" s="3" t="s">
         <v>60</v>
       </c>
       <c r="AK49" s="2" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="AL49" s="2" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="AM49" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="AN49" s="3" t="s">
-        <v>60</v>
+      <c r="AN49" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="50" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A50" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>80</v>
+      <c r="A50" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>99</v>
@@ -6839,279 +6842,279 @@
       <c r="E50" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="F50" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>80</v>
+      <c r="F50" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="J50" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="K50" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="L50" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="M50" s="3" t="s">
-        <v>60</v>
+        <v>65</v>
+      </c>
+      <c r="J50" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="K50" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="L50" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="M50" s="2" t="s">
+        <v>101</v>
       </c>
       <c r="N50" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="O50" s="1" t="s">
-        <v>80</v>
+        <v>122</v>
+      </c>
+      <c r="O50" s="2" t="s">
+        <v>122</v>
       </c>
       <c r="P50" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q50" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="R50" s="3" t="s">
-        <v>60</v>
+        <v>100</v>
+      </c>
+      <c r="Q50" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="R50" s="2" t="s">
+        <v>100</v>
       </c>
       <c r="S50" s="2" t="s">
-        <v>13</v>
+        <v>100</v>
       </c>
       <c r="T50" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="U50" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="V50" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="W50" s="1" t="s">
-        <v>80</v>
+        <v>100</v>
+      </c>
+      <c r="U50" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="V50" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="W50" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="X50" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="Y50" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="Z50" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AA50" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AB50" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="AC50" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="AD50" s="1" t="s">
-        <v>80</v>
+      <c r="Y50" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z50" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA50" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB50" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC50" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AD50" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="AE50" s="2" t="s">
         <v>21</v>
       </c>
       <c r="AF50" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG50" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AH50" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="AI50" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="AJ50" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK50" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="AL50" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="AM50" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN50" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="51" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="A51" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="J51" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="L51" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="M51" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="N51" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O51" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="P51" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q51" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="R51" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="S51" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T51" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="U51" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="V51" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="W51" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="X51" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y51" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z51" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA51" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB51" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC51" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="AG50" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AH50" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AI50" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AJ50" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AK50" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AL50" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AM50" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AN50" s="1" t="s">
+      <c r="AD51" s="1" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="51" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A51" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="F51" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G51" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="H51" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="I51" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="J51" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="K51" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="L51" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="M51" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="N51" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="O51" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="P51" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q51" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="R51" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="S51" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="T51" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="U51" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="V51" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="W51" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="X51" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="Y51" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="Z51" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="AA51" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="AB51" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AC51" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AD51" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AE51" s="3" t="s">
-        <v>60</v>
+      <c r="AE51" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="AF51" s="2" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="AG51" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="AH51" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="AI51" s="2" t="s">
-        <v>100</v>
+      <c r="AH51" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AI51" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="AJ51" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="AK51" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="AL51" s="2" t="s">
-        <v>100</v>
+      <c r="AK51" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AL51" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="AM51" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="AN51" s="3" t="s">
-        <v>60</v>
+      <c r="AN51" s="1" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="52" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A52" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="H52" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="I52" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="J52" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="K52" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="L52" s="1" t="s">
-        <v>72</v>
+        <v>122</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H52" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I52" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="J52" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="K52" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="L52" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="M52" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="N52" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="O52" s="1" t="s">
-        <v>72</v>
+      <c r="N52" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="O52" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="P52" s="2" t="s">
         <v>100</v>
@@ -7134,11 +7137,11 @@
       <c r="V52" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="W52" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="X52" s="1" t="s">
-        <v>72</v>
+      <c r="W52" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="X52" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="Y52" s="2" t="s">
         <v>100</v>
@@ -7155,11 +7158,11 @@
       <c r="AC52" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="AD52" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AE52" s="2" t="s">
-        <v>21</v>
+      <c r="AD52" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE52" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="AF52" s="2" t="s">
         <v>100</v>
@@ -7173,8 +7176,8 @@
       <c r="AI52" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="AJ52" s="2" t="s">
-        <v>100</v>
+      <c r="AJ52" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="AK52" s="2" t="s">
         <v>100</v>
@@ -7185,251 +7188,373 @@
       <c r="AM52" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="AN52" s="1" t="s">
-        <v>72</v>
+      <c r="AN52" s="3" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="53" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A53" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>11</v>
+        <v>100</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G53" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="H53" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="I53" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="J53" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="K53" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="L53" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="M53" s="2" t="s">
-        <v>11</v>
+        <v>100</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J53" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K53" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="L53" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="M53" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="N53" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="O53" s="3" t="s">
-        <v>60</v>
+        <v>100</v>
+      </c>
+      <c r="O53" s="1" t="s">
+        <v>72</v>
       </c>
       <c r="P53" s="2" t="s">
-        <v>11</v>
+        <v>100</v>
       </c>
       <c r="Q53" s="2" t="s">
-        <v>11</v>
+        <v>100</v>
       </c>
       <c r="R53" s="2" t="s">
-        <v>11</v>
+        <v>100</v>
       </c>
       <c r="S53" s="2" t="s">
-        <v>11</v>
+        <v>100</v>
       </c>
       <c r="T53" s="2" t="s">
-        <v>11</v>
+        <v>100</v>
       </c>
       <c r="U53" s="2" t="s">
-        <v>11</v>
+        <v>100</v>
       </c>
       <c r="V53" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="W53" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="X53" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y53" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="Z53" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AA53" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AB53" s="2" t="s">
-        <v>11</v>
+        <v>100</v>
+      </c>
+      <c r="W53" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="X53" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y53" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z53" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA53" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB53" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="AC53" s="3" t="s">
         <v>60</v>
       </c>
       <c r="AD53" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AE53" s="1" t="s">
-        <v>79</v>
+        <v>72</v>
+      </c>
+      <c r="AE53" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="AF53" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AG53" s="2" t="s">
-        <v>11</v>
+        <v>100</v>
+      </c>
+      <c r="AG53" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="AH53" s="2" t="s">
-        <v>11</v>
+        <v>100</v>
       </c>
       <c r="AI53" s="2" t="s">
-        <v>11</v>
+        <v>100</v>
       </c>
       <c r="AJ53" s="2" t="s">
-        <v>11</v>
+        <v>100</v>
       </c>
       <c r="AK53" s="2" t="s">
-        <v>11</v>
+        <v>100</v>
       </c>
       <c r="AL53" s="2" t="s">
-        <v>11</v>
+        <v>100</v>
       </c>
       <c r="AM53" s="3" t="s">
         <v>60</v>
       </c>
       <c r="AN53" s="1" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="54" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A54" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H54" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I54" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="J54" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="K54" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="L54" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M54" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N54" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O54" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="P54" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q54" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="R54" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="S54" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="T54" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="U54" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="V54" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="W54" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="X54" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y54" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z54" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA54" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB54" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC54" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AD54" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE54" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF54" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AG54" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AH54" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AI54" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ54" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AK54" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AL54" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AM54" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN54" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="55" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="A55" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="B54" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D54" s="2" t="s">
+      <c r="B55" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D55" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E54" s="2" t="s">
+      <c r="E55" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="F54" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G54" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="H54" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="I54" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="J54" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="K54" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="L54" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="M54" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="N54" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="O54" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="P54" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q54" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="R54" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="S54" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="T54" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="U54" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="V54" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="W54" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="X54" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="Y54" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="Z54" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AA54" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AB54" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AC54" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AD54" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AE54" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF54" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AG54" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AH54" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AI54" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AJ54" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AK54" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AL54" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AM54" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AN54" s="1" t="s">
+      <c r="F55" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J55" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K55" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="L55" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="M55" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="N55" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="O55" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="P55" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q55" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="R55" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="S55" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="T55" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="U55" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="V55" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="W55" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="X55" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y55" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z55" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA55" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB55" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC55" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD55" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE55" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF55" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG55" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AH55" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AI55" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AJ55" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK55" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AL55" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AM55" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN55" s="1" t="s">
         <v>72</v>
       </c>
     </row>

</xml_diff>

<commit_message>
FEAT: strict format validation on scanning float values.
</commit_message>
<xml_diff>
--- a/docs/lexer/lexer-FSM.xlsx
+++ b/docs/lexer/lexer-FSM.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="transitions" sheetId="3" r:id="rId1"/>
+    <sheet name="float transitions" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2239" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2294" uniqueCount="140">
   <si>
     <t>S_START</t>
   </si>
@@ -392,6 +393,48 @@
   </si>
   <si>
     <t>S_SLASH_N</t>
+  </si>
+  <si>
+    <t>S_FL_START</t>
+  </si>
+  <si>
+    <t>S_FL_NUM</t>
+  </si>
+  <si>
+    <t>S_FL_DEC</t>
+  </si>
+  <si>
+    <t>S_FL_EXP</t>
+  </si>
+  <si>
+    <t>S_FL_EXPS</t>
+  </si>
+  <si>
+    <t>S_FL_EXPD</t>
+  </si>
+  <si>
+    <t>T_FL_FLOAT</t>
+  </si>
+  <si>
+    <t>T_FL_ERROR</t>
+  </si>
+  <si>
+    <t>C_FL_SIGN</t>
+  </si>
+  <si>
+    <t>C_FL_DIGIT</t>
+  </si>
+  <si>
+    <t>C_FL_EXP</t>
+  </si>
+  <si>
+    <t>C_FL_DOT</t>
+  </si>
+  <si>
+    <t>C_FL_ILLEGAL</t>
+  </si>
+  <si>
+    <t>C_FL_EOF</t>
   </si>
 </sst>
 </file>
@@ -501,7 +544,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -529,6 +572,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -839,7 +885,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AN15" sqref="AN15"/>
+      <selection pane="topRight" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7687,4 +7733,202 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="6"/>
+      <c r="B1" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
FIX: regression on tests "load-41" and "load-43".
</commit_message>
<xml_diff>
--- a/docs/lexer/lexer-FSM.xlsx
+++ b/docs/lexer/lexer-FSM.xlsx
@@ -888,7 +888,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AI26" sqref="AI26"/>
+      <selection pane="bottomLeft" activeCell="AI25" sqref="AI25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3928,11 +3928,11 @@
       <c r="AG25" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="AH25" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AI25" s="3" t="s">
-        <v>60</v>
+      <c r="AH25" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="AI25" s="2" t="s">
+        <v>140</v>
       </c>
       <c r="AJ25" s="3" t="s">
         <v>60</v>

</xml_diff>

<commit_message>
FEAT: scan "<-" as word! instead of tag!.
</commit_message>
<xml_diff>
--- a/docs/lexer/lexer-FSM.xlsx
+++ b/docs/lexer/lexer-FSM.xlsx
@@ -886,9 +886,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AI25" sqref="AI25"/>
+      <selection pane="bottomLeft" activeCell="AI40" sqref="AI40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5762,7 +5762,7 @@
         <v>26</v>
       </c>
       <c r="AI40" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="AJ40" s="2" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
FEAT: make opening angle bracket a stricter delimiter.
Solves the "<a > 3" ambiguous patterns.
</commit_message>
<xml_diff>
--- a/docs/lexer/lexer-FSM.xlsx
+++ b/docs/lexer/lexer-FSM.xlsx
@@ -886,9 +886,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AI40" sqref="AI40"/>
+      <selection pane="bottomLeft" activeCell="Y41" sqref="Y41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5732,7 +5732,7 @@
         <v>26</v>
       </c>
       <c r="Y40" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="Z40" s="2" t="s">
         <v>30</v>
@@ -6634,7 +6634,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="48" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A48" s="9" t="s">
         <v>30</v>
       </c>
@@ -6707,8 +6707,8 @@
       <c r="X48" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="Y48" s="2" t="s">
-        <v>30</v>
+      <c r="Y48" s="1" t="s">
+        <v>72</v>
       </c>
       <c r="Z48" s="2" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
FEAT: improves date! values ending validity checking.
</commit_message>
<xml_diff>
--- a/docs/lexer/lexer-FSM.xlsx
+++ b/docs/lexer/lexer-FSM.xlsx
@@ -888,7 +888,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Y41" sqref="Y41"/>
+      <selection pane="bottomLeft" activeCell="AJ29" sqref="AJ29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4316,7 +4316,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="29" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A29" s="9" t="s">
         <v>16</v>
       </c>
@@ -4398,8 +4398,8 @@
       <c r="AA29" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="AB29" s="1" t="s">
-        <v>85</v>
+      <c r="AB29" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="AC29" s="2" t="s">
         <v>16</v>
@@ -4422,8 +4422,8 @@
       <c r="AI29" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="AJ29" s="1" t="s">
-        <v>85</v>
+      <c r="AJ29" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="AK29" s="3" t="s">
         <v>60</v>

</xml_diff>

<commit_message>
FEAT: support comma as decimal separator in money! values.
</commit_message>
<xml_diff>
--- a/docs/lexer/lexer-FSM.xlsx
+++ b/docs/lexer/lexer-FSM.xlsx
@@ -903,7 +903,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K8" sqref="K8"/>
+      <selection pane="bottomLeft" activeCell="AC39" sqref="AC39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5551,7 +5551,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="39" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A39" s="9" t="s">
         <v>23</v>
       </c>
@@ -5636,8 +5636,8 @@
       <c r="AB39" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="AC39" s="3" t="s">
-        <v>60</v>
+      <c r="AC39" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="AD39" s="1" t="s">
         <v>89</v>

</xml_diff>

<commit_message>
FEAT: completes raw strings support.
</commit_message>
<xml_diff>
--- a/docs/lexer/lexer-FSM.xlsx
+++ b/docs/lexer/lexer-FSM.xlsx
@@ -903,7 +903,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AC39" sqref="AC39"/>
+      <selection pane="bottomLeft" activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2407,11 +2407,11 @@
       <c r="I13" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="J13" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="K13" s="2" t="s">
+      <c r="J13" s="2" t="s">
         <v>142</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="L13" s="3" t="s">
         <v>60</v>

</xml_diff>

<commit_message>
FIX: fixes non-passing test "tr-40".
</commit_message>
<xml_diff>
--- a/docs/lexer/lexer-FSM.xlsx
+++ b/docs/lexer/lexer-FSM.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Red\docs\lexer\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{70EDA8A6-BFD7-49AA-9E15-7994E3B776B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-100" yWindow="20" windowWidth="22700" windowHeight="14480" tabRatio="564"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" tabRatio="564" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="transitions" sheetId="3" r:id="rId1"/>
@@ -458,7 +464,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -655,7 +661,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -688,9 +694,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -723,6 +746,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -898,23 +938,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AN61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K13" sqref="K13"/>
+      <selection pane="bottomLeft" activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.36328125" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" customWidth="1"/>
-    <col min="5" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="12" width="9.7265625" customWidth="1"/>
-    <col min="13" max="13" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="14" max="40" width="9.7265625" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.73046875" customWidth="1"/>
+    <col min="5" max="5" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="9.73046875" customWidth="1"/>
+    <col min="13" max="13" width="9.9296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="40" width="9.73046875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -1037,7 +1077,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
@@ -1159,7 +1199,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A3" s="9" t="s">
         <v>66</v>
       </c>
@@ -1281,7 +1321,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A4" s="9" t="s">
         <v>67</v>
       </c>
@@ -1403,7 +1443,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A5" s="9" t="s">
         <v>1</v>
       </c>
@@ -1525,7 +1565,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A6" s="10" t="s">
         <v>2</v>
       </c>
@@ -1647,7 +1687,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A7" s="9" t="s">
         <v>71</v>
       </c>
@@ -1769,7 +1809,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A8" s="9" t="s">
         <v>3</v>
       </c>
@@ -1891,7 +1931,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A9" s="9" t="s">
         <v>4</v>
       </c>
@@ -2013,7 +2053,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A10" s="9" t="s">
         <v>95</v>
       </c>
@@ -2135,7 +2175,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A11" s="9" t="s">
         <v>96</v>
       </c>
@@ -2257,7 +2297,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A12" s="9" t="s">
         <v>97</v>
       </c>
@@ -2379,7 +2419,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A13" s="9" t="s">
         <v>141</v>
       </c>
@@ -2501,7 +2541,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A14" s="9" t="s">
         <v>142</v>
       </c>
@@ -2623,7 +2663,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A15" s="9" t="s">
         <v>143</v>
       </c>
@@ -2655,7 +2695,7 @@
         <v>142</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="L15" s="2" t="s">
         <v>142</v>
@@ -2745,7 +2785,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A16" s="9" t="s">
         <v>144</v>
       </c>
@@ -2867,7 +2907,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="17" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A17" s="9" t="s">
         <v>5</v>
       </c>
@@ -2989,7 +3029,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A18" s="9" t="s">
         <v>125</v>
       </c>
@@ -3111,7 +3151,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A19" s="9" t="s">
         <v>6</v>
       </c>
@@ -3233,7 +3273,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A20" s="9" t="s">
         <v>7</v>
       </c>
@@ -3355,7 +3395,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A21" s="9" t="s">
         <v>68</v>
       </c>
@@ -3477,7 +3517,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A22" s="9" t="s">
         <v>8</v>
       </c>
@@ -3599,7 +3639,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A23" s="9" t="s">
         <v>9</v>
       </c>
@@ -3721,7 +3761,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A24" s="9" t="s">
         <v>10</v>
       </c>
@@ -3843,7 +3883,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A25" s="9" t="s">
         <v>11</v>
       </c>
@@ -3965,7 +4005,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="26" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A26" s="9" t="s">
         <v>12</v>
       </c>
@@ -4087,7 +4127,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="27" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A27" s="9" t="s">
         <v>82</v>
       </c>
@@ -4209,7 +4249,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A28" s="9" t="s">
         <v>13</v>
       </c>
@@ -4331,7 +4371,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="29" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A29" s="9" t="s">
         <v>140</v>
       </c>
@@ -4453,7 +4493,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="30" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A30" s="9" t="s">
         <v>111</v>
       </c>
@@ -4575,7 +4615,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="31" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A31" s="9" t="s">
         <v>14</v>
       </c>
@@ -4697,7 +4737,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="32" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A32" s="9" t="s">
         <v>15</v>
       </c>
@@ -4819,7 +4859,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="33" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A33" s="9" t="s">
         <v>16</v>
       </c>
@@ -4941,7 +4981,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="34" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A34" s="9" t="s">
         <v>17</v>
       </c>
@@ -5063,7 +5103,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A35" s="9" t="s">
         <v>18</v>
       </c>
@@ -5185,7 +5225,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="36" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A36" s="9" t="s">
         <v>19</v>
       </c>
@@ -5307,7 +5347,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="37" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A37" s="9" t="s">
         <v>20</v>
       </c>
@@ -5429,7 +5469,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="38" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A38" s="9" t="s">
         <v>22</v>
       </c>
@@ -5551,7 +5591,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="39" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A39" s="9" t="s">
         <v>23</v>
       </c>
@@ -5673,7 +5713,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="40" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A40" s="9" t="s">
         <v>24</v>
       </c>
@@ -5795,7 +5835,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="41" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A41" s="9" t="s">
         <v>112</v>
       </c>
@@ -5917,7 +5957,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="42" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A42" s="9" t="s">
         <v>123</v>
       </c>
@@ -6039,7 +6079,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="43" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A43" s="9" t="s">
         <v>124</v>
       </c>
@@ -6161,7 +6201,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="44" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A44" s="9" t="s">
         <v>25</v>
       </c>
@@ -6283,7 +6323,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="45" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A45" s="9" t="s">
         <v>26</v>
       </c>
@@ -6405,7 +6445,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="46" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A46" s="9" t="s">
         <v>27</v>
       </c>
@@ -6527,7 +6567,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="47" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A47" s="9" t="s">
         <v>28</v>
       </c>
@@ -6649,7 +6689,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="48" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A48" s="9" t="s">
         <v>29</v>
       </c>
@@ -6771,7 +6811,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="49" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A49" s="9" t="s">
         <v>108</v>
       </c>
@@ -6893,7 +6933,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="50" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A50" s="9" t="s">
         <v>109</v>
       </c>
@@ -7015,7 +7055,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="51" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A51" s="9" t="s">
         <v>121</v>
       </c>
@@ -7137,7 +7177,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="52" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A52" s="9" t="s">
         <v>30</v>
       </c>
@@ -7259,7 +7299,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="53" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A53" s="9" t="s">
         <v>92</v>
       </c>
@@ -7381,7 +7421,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="54" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A54" s="9" t="s">
         <v>31</v>
       </c>
@@ -7503,7 +7543,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="55" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A55" s="9" t="s">
         <v>21</v>
       </c>
@@ -7625,7 +7665,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="56" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A56" s="10" t="s">
         <v>98</v>
       </c>
@@ -7747,7 +7787,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="57" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A57" s="9" t="s">
         <v>99</v>
       </c>
@@ -7869,7 +7909,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="58" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A58" s="9" t="s">
         <v>122</v>
       </c>
@@ -7991,7 +8031,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="59" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A59" s="9" t="s">
         <v>100</v>
       </c>
@@ -8113,7 +8153,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="60" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A60" s="9" t="s">
         <v>101</v>
       </c>
@@ -8235,7 +8275,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="61" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A61" s="9" t="s">
         <v>102</v>
       </c>
@@ -8364,16 +8404,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="6"/>
       <c r="B1" s="5" t="s">
         <v>138</v>
@@ -8394,7 +8434,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="8" t="s">
         <v>126</v>
       </c>
@@ -8417,7 +8457,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="9" t="s">
         <v>127</v>
       </c>
@@ -8440,7 +8480,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="9" t="s">
         <v>128</v>
       </c>
@@ -8463,7 +8503,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="9" t="s">
         <v>129</v>
       </c>
@@ -8486,7 +8526,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="9" t="s">
         <v>130</v>
       </c>
@@ -8509,7 +8549,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="9" t="s">
         <v>131</v>
       </c>
@@ -8532,7 +8572,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="9" t="s">
         <v>133</v>
       </c>

</xml_diff>

<commit_message>
FIX: unbalanced single quotes in tags passing silently in some cases.
Fixes those cases:

>> <'>
== <'>
>> <''>
*** Syntax Error: (line 2) invalid tag at <''>

Now:

>> <'>
*** Syntax Error: (line 2) invalid tag at <'>
*** Where: transcode
*** Stack: load
>> <''>
== <''>
</commit_message>
<xml_diff>
--- a/docs/lexer/lexer-FSM.xlsx
+++ b/docs/lexer/lexer-FSM.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Red\docs\lexer\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{70EDA8A6-BFD7-49AA-9E15-7994E3B776B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" tabRatio="564" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-100" yWindow="-100" windowWidth="22700" windowHeight="14600" tabRatio="564"/>
   </bookViews>
   <sheets>
     <sheet name="transitions" sheetId="3" r:id="rId1"/>
@@ -464,7 +458,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -661,7 +655,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -694,26 +688,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -746,23 +723,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -938,23 +898,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K15" sqref="K15"/>
+      <selection pane="bottomLeft" activeCell="N44" sqref="N44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.73046875" customWidth="1"/>
-    <col min="5" max="5" width="9.73046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="12" width="9.73046875" customWidth="1"/>
-    <col min="13" max="13" width="9.9296875" bestFit="1" customWidth="1"/>
-    <col min="14" max="40" width="9.73046875" customWidth="1"/>
+    <col min="1" max="1" width="10.36328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" customWidth="1"/>
+    <col min="5" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="9.7265625" customWidth="1"/>
+    <col min="13" max="13" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="40" width="9.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -1077,7 +1037,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
@@ -1199,7 +1159,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A3" s="9" t="s">
         <v>66</v>
       </c>
@@ -1321,7 +1281,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:40" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A4" s="9" t="s">
         <v>67</v>
       </